<commit_message>
finished renaming derived variables
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10615"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E1008E-F510-8049-BBE4-1324ACB8A32D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17A1DF1-B2F7-374A-96AA-B14E537B1564}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36840" yWindow="2380" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="210">
   <si>
     <t>Variable #</t>
   </si>
@@ -59,9 +59,6 @@
     <t>recovered</t>
   </si>
   <si>
-    <t>ccc19cat</t>
-  </si>
-  <si>
     <t>hca</t>
   </si>
   <si>
@@ -92,27 +89,18 @@
     <t>Time of followup (if alive) or to death (if dead) in days</t>
   </si>
   <si>
-    <t>Follow-ups</t>
-  </si>
-  <si>
     <t>dead30</t>
   </si>
   <si>
     <t>Median F/U in days</t>
   </si>
   <si>
-    <t>righttime2, lefttime2</t>
-  </si>
-  <si>
     <t>ecogcat</t>
   </si>
   <si>
     <t>Categorical ECOG variable, lumping 1 = 0/1, 2 = 2, and 3 = 3/4, 4 = unknown</t>
   </si>
   <si>
-    <t>age_cph</t>
-  </si>
-  <si>
     <t>o2_ever</t>
   </si>
   <si>
@@ -137,9 +125,6 @@
     <t>who</t>
   </si>
   <si>
-    <t>PE_comp, SVT_comp, DVT_comp, Thrombosis_NOS_comp</t>
-  </si>
-  <si>
     <t>Complications</t>
   </si>
   <si>
@@ -173,24 +158,12 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>not used</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
     <t>Recode other/prefer not to say gender --&gt; unknown</t>
   </si>
   <si>
-    <t>obesitylevel</t>
-  </si>
-  <si>
-    <t>lefttime, righttime</t>
-  </si>
-  <si>
-    <t>cancer_status_v2</t>
-  </si>
-  <si>
     <t>Age with imputation for categoricals</t>
   </si>
   <si>
@@ -245,27 +218,18 @@
     <t>Derived recovery variable</t>
   </si>
   <si>
-    <t>Derived variable indicating complication severity, at diagnosis</t>
-  </si>
-  <si>
     <t>Derived variable for plaquenil/azithro exposure (1 = neither, 2 = plaq only (5521), 3 = azithro only (18631), 4 = both, 5 = unknown)</t>
   </si>
   <si>
     <t>Derived variable coding the obesity status</t>
   </si>
   <si>
-    <t>Derived variable for smoking status collapsing the former smoker variable   #1 = current, 2 = former, 3 = never, 4 = unknown</t>
-  </si>
-  <si>
     <t>Derived variable for whether a patient is on active therapy (within 1 month)</t>
   </si>
   <si>
     <t>Derived variable for race/ethnicity</t>
   </si>
   <si>
-    <t>Derived variable for type of tumor (Solid=0, Heme=1, Both=2, Other=3)</t>
-  </si>
-  <si>
     <t>Derived variable indicating if there has been surgery within 4 weeks</t>
   </si>
   <si>
@@ -275,12 +239,6 @@
     <t>Derived variable indicating cancer status</t>
   </si>
   <si>
-    <t>Derived variables indicating VTE complications</t>
-  </si>
-  <si>
-    <t>Derived variable indicating whether patient has arrhythmia complications</t>
-  </si>
-  <si>
     <t>Derived variable indicating whether patient has diabetes mellitus</t>
   </si>
   <si>
@@ -290,12 +248,6 @@
     <t>Derived variable indicating whether patient has pulmonary comorbidities</t>
   </si>
   <si>
-    <t>Derived variable indicating whether patient has any cardiovascular comorbidities (CAD, CHF, Afib, arrhythmia NOS, PVD, CVA)</t>
-  </si>
-  <si>
-    <t>smokingderived</t>
-  </si>
-  <si>
     <t>Indicates whether patient has ever had supplemental o2 (partial derived)</t>
   </si>
   <si>
@@ -326,15 +278,9 @@
     <t>Hydroxychloroquine as COVID-19 treatment ever</t>
   </si>
   <si>
-    <t>Steroids as COVID-19 treatment ever</t>
-  </si>
-  <si>
     <t>Remdesivir as treatment for COVID-19 ever</t>
   </si>
   <si>
-    <t>other_c19</t>
-  </si>
-  <si>
     <t>COVID-19 treatments other than HCQ, AZ, steroids, remdesivir, or toci</t>
   </si>
   <si>
@@ -384,6 +330,321 @@
   </si>
   <si>
     <t>O11</t>
+  </si>
+  <si>
+    <t>O12</t>
+  </si>
+  <si>
+    <t>PE_comp</t>
+  </si>
+  <si>
+    <t>O13</t>
+  </si>
+  <si>
+    <t>SVT_comp</t>
+  </si>
+  <si>
+    <t>O14</t>
+  </si>
+  <si>
+    <t>DVT_comp</t>
+  </si>
+  <si>
+    <t>O15</t>
+  </si>
+  <si>
+    <t>thrombosis_NOS</t>
+  </si>
+  <si>
+    <t>Thrombosis NOS complications</t>
+  </si>
+  <si>
+    <t>DVT complications</t>
+  </si>
+  <si>
+    <t>SVT complications</t>
+  </si>
+  <si>
+    <t>PE complications</t>
+  </si>
+  <si>
+    <t>O16</t>
+  </si>
+  <si>
+    <t>Arrhythmia complications</t>
+  </si>
+  <si>
+    <t>O17</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>righttime</t>
+  </si>
+  <si>
+    <t>lefttime</t>
+  </si>
+  <si>
+    <t>Time measurements</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>median_fu</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>righttime2</t>
+  </si>
+  <si>
+    <t>lefttime2</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>lefttime3</t>
+  </si>
+  <si>
+    <t>righttime3</t>
+  </si>
+  <si>
+    <t>Latest date that diagnosis was possible</t>
+  </si>
+  <si>
+    <t>Median of date interval of diagnosis</t>
+  </si>
+  <si>
+    <t>Earliest date that diagnosis was possible</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>O18</t>
+  </si>
+  <si>
+    <t>Rx1</t>
+  </si>
+  <si>
+    <t>Rx2</t>
+  </si>
+  <si>
+    <t>Rx3</t>
+  </si>
+  <si>
+    <t>Rx4</t>
+  </si>
+  <si>
+    <t>High-dose steroids as COVID-19 treatment ever</t>
+  </si>
+  <si>
+    <t>Rx5</t>
+  </si>
+  <si>
+    <t>Rx6</t>
+  </si>
+  <si>
+    <t>other_tx_c19</t>
+  </si>
+  <si>
+    <t>Rx7</t>
+  </si>
+  <si>
+    <t>Rx8</t>
+  </si>
+  <si>
+    <t>statins</t>
+  </si>
+  <si>
+    <t>Statins ever (baseline or for COVID-19)</t>
+  </si>
+  <si>
+    <t>Rx9</t>
+  </si>
+  <si>
+    <t>antivirals</t>
+  </si>
+  <si>
+    <t>Antivirals ever (except oseltamivir or remdesivir) for treatment of COVID-19</t>
+  </si>
+  <si>
+    <t>Rx10</t>
+  </si>
+  <si>
+    <t>steroids_ld</t>
+  </si>
+  <si>
+    <t>Low-dose steroids ever (dose up to 20 mg/d)</t>
+  </si>
+  <si>
+    <t>Anticoagulation, aspirin, or APA ever (baseline or treatment for COVID-19)</t>
+  </si>
+  <si>
+    <t>Rx11</t>
+  </si>
+  <si>
+    <t>ac_apa</t>
+  </si>
+  <si>
+    <t>Aspirin or APA ever (baseline or treatment for COVID-19)</t>
+  </si>
+  <si>
+    <t>Rx12</t>
+  </si>
+  <si>
+    <t>as_apa</t>
+  </si>
+  <si>
+    <t>Anticoagulation ever (baseline or treatment for COVID-19)</t>
+  </si>
+  <si>
+    <t>ac</t>
+  </si>
+  <si>
+    <t>Rx13</t>
+  </si>
+  <si>
+    <t>Rx14</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>smoking</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>obesity</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>Cardiovascular comorbidity (CAD, CHF, Afib, arrhythmia NOS, PVD, CVA, cardiac disease NOS)</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>US Census Division</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>htn</t>
+  </si>
+  <si>
+    <t>Hypertension</t>
+  </si>
+  <si>
+    <t>D17</t>
+  </si>
+  <si>
+    <t>smoking2</t>
+  </si>
+  <si>
+    <t>Derived variable for smoking status collapsing the current/former smoker variables</t>
+  </si>
+  <si>
+    <t>Ca1</t>
+  </si>
+  <si>
+    <t>Ca2</t>
+  </si>
+  <si>
+    <t>Derived variable for type of tumor</t>
+  </si>
+  <si>
+    <t>Derived variable for smoking status collapsing the former smoker variable</t>
+  </si>
+  <si>
+    <t>Ca3</t>
+  </si>
+  <si>
+    <t>Ca4</t>
+  </si>
+  <si>
+    <t>Ca5</t>
+  </si>
+  <si>
+    <t>Ca6</t>
+  </si>
+  <si>
+    <t>Ca7</t>
+  </si>
+  <si>
+    <t>cancer_status</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>neg_control</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Negative controls</t>
+  </si>
+  <si>
+    <t>partial variable</t>
   </si>
 </sst>
 </file>
@@ -439,10 +700,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E49" totalsRowShown="0">
-  <autoFilter ref="A1:E49" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E47">
-    <sortCondition ref="B1:B47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E66" totalsRowShown="0">
+  <autoFilter ref="A1:E66" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E65">
+    <sortCondition ref="A1:A65"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -776,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -796,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -805,682 +1066,920 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>10</v>
+      <c r="A2" t="s">
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
       <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>28</v>
+      <c r="A14" t="s">
+        <v>185</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>16</v>
+      <c r="A15" t="s">
+        <v>186</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>187</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>35</v>
+      <c r="A16" t="s">
+        <v>189</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>190</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>7</v>
+      <c r="A17" t="s">
+        <v>192</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>193</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>33</v>
+      <c r="A18" t="s">
+        <v>170</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>173</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>29</v>
+      <c r="A21" t="s">
+        <v>175</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>174</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>176</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>15</v>
+      <c r="A23" t="s">
+        <v>177</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>26</v>
+      <c r="A24" t="s">
+        <v>178</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" t="s">
         <v>116</v>
       </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>12</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>22</v>
-      </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" t="s">
         <v>36</v>
       </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>46</v>
-      </c>
-      <c r="B28" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>25</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" t="s">
-        <v>22</v>
-      </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>11</v>
+      <c r="A31" t="s">
+        <v>109</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" t="s">
         <v>112</v>
       </c>
-      <c r="B32" t="s">
-        <v>13</v>
-      </c>
       <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
         <v>6</v>
       </c>
-      <c r="D32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>40</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>30</v>
-      </c>
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" t="s">
-        <v>16</v>
-      </c>
       <c r="D34" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>38</v>
+      <c r="A35" t="s">
+        <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>42</v>
+      <c r="A36" t="s">
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>8</v>
+      <c r="A39" t="s">
+        <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>39</v>
+      <c r="A40" t="s">
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>9</v>
+      <c r="A41" t="s">
+        <v>98</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>34</v>
+      <c r="A42" t="s">
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" t="s">
         <v>14</v>
       </c>
-      <c r="B43" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>45</v>
-      </c>
-      <c r="B44" t="s">
-        <v>99</v>
-      </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>13</v>
+      <c r="A45" t="s">
+        <v>155</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="C45" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>82</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>160</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>36</v>
+      <c r="A47" t="s">
+        <v>162</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>67</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>166</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="B49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>146</v>
+      </c>
+      <c r="B54" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>148</v>
+      </c>
+      <c r="B55" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>149</v>
+      </c>
+      <c r="B56" t="s">
+        <v>150</v>
+      </c>
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>152</v>
+      </c>
+      <c r="B57" t="s">
+        <v>153</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>120</v>
       </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="B58" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" t="s">
+        <v>124</v>
+      </c>
+      <c r="D58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>121</v>
+      </c>
+      <c r="B59" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60" t="s">
+        <v>124</v>
+      </c>
+      <c r="D60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61" t="s">
+        <v>124</v>
+      </c>
+      <c r="D61" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" t="s">
+        <v>124</v>
+      </c>
+      <c r="D62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" t="s">
+        <v>124</v>
+      </c>
+      <c r="D63" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>137</v>
+      </c>
+      <c r="B64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>138</v>
+      </c>
+      <c r="B65" t="s">
+        <v>133</v>
+      </c>
+      <c r="C65" t="s">
+        <v>124</v>
+      </c>
+      <c r="D65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>205</v>
+      </c>
+      <c r="B66" t="s">
+        <v>206</v>
+      </c>
+      <c r="C66" t="s">
+        <v>207</v>
+      </c>
+      <c r="D66" t="s">
+        <v>208</v>
+      </c>
+      <c r="E66" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added separate heme and solid indicator variables
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17A1DF1-B2F7-374A-96AA-B14E537B1564}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BDF59C-EC88-9541-ABA3-7DA6B72121DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36840" yWindow="2380" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="219">
   <si>
     <t>Variable #</t>
   </si>
@@ -645,6 +645,33 @@
   </si>
   <si>
     <t>partial variable</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>imwg</t>
+  </si>
+  <si>
+    <t>Modified IMWG frailty index</t>
+  </si>
+  <si>
+    <t>Ca8</t>
+  </si>
+  <si>
+    <t>Ca9</t>
+  </si>
+  <si>
+    <t>heme</t>
+  </si>
+  <si>
+    <t>solid</t>
+  </si>
+  <si>
+    <t>Hematologic malignancy indicator</t>
+  </si>
+  <si>
+    <t>Solid tumor indicator</t>
   </si>
 </sst>
 </file>
@@ -700,10 +727,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E66" totalsRowShown="0">
-  <autoFilter ref="A1:E66" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E65">
-    <sortCondition ref="A1:A65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E69" totalsRowShown="0">
+  <autoFilter ref="A1:E69" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E69">
+    <sortCondition ref="A1:A69"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1037,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1169,817 +1196,859 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>216</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B15" t="s">
-        <v>187</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>188</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s">
-        <v>190</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>191</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B17" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="B19" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>174</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>178</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
         <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="C33" t="s">
         <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>155</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>156</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>157</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="B46" t="s">
-        <v>160</v>
+        <v>14</v>
       </c>
       <c r="C46" t="s">
         <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>158</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B47" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C47" t="s">
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B48" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>163</v>
       </c>
       <c r="C49" t="s">
         <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="B50" t="s">
-        <v>32</v>
+        <v>165</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>144</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C53" t="s">
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C54" t="s">
         <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B55" t="s">
-        <v>147</v>
+        <v>59</v>
       </c>
       <c r="C55" t="s">
         <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B56" t="s">
-        <v>150</v>
+        <v>83</v>
       </c>
       <c r="C56" t="s">
         <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>154</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="C58" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="D58" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="C59" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="D59" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C60" t="s">
         <v>124</v>
       </c>
       <c r="D60" t="s">
-        <v>25</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C61" t="s">
         <v>124</v>
       </c>
       <c r="D61" t="s">
-        <v>135</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C62" t="s">
         <v>124</v>
       </c>
       <c r="D62" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B63" t="s">
-        <v>33</v>
+        <v>130</v>
       </c>
       <c r="C63" t="s">
         <v>124</v>
       </c>
       <c r="D63" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B64" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C64" t="s">
         <v>124</v>
       </c>
       <c r="D64" t="s">
-        <v>134</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B65" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
       <c r="C65" t="s">
         <v>124</v>
       </c>
       <c r="D65" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" t="s">
+        <v>124</v>
+      </c>
+      <c r="D66" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" t="s">
+        <v>124</v>
+      </c>
+      <c r="D67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>205</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B68" t="s">
         <v>206</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C68" t="s">
         <v>207</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D68" t="s">
         <v>208</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E68" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>210</v>
+      </c>
+      <c r="B69" t="s">
+        <v>211</v>
+      </c>
+      <c r="C69" t="s">
+        <v>207</v>
+      </c>
+      <c r="D69" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a number of lab derived variables
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680407B3-30CF-B742-A689-B9E8447BBA1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029FDA05-0A14-1149-A144-D3DEF65A4BFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36480" yWindow="1800" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="262">
   <si>
     <t>Variable #</t>
   </si>
@@ -702,6 +702,105 @@
   </si>
   <si>
     <t>Neutrophil:Lymphocyte ratio, categorical</t>
+  </si>
+  <si>
+    <t>Ca10</t>
+  </si>
+  <si>
+    <t>D18</t>
+  </si>
+  <si>
+    <t>surgery2</t>
+  </si>
+  <si>
+    <t>Derived variable indicating if there has been surgery within 3 months</t>
+  </si>
+  <si>
+    <t>anytx</t>
+  </si>
+  <si>
+    <t>Any cancer treatment in the past 3 months</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>ddimer</t>
+  </si>
+  <si>
+    <t>D-Dimer</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>fibrinogen</t>
+  </si>
+  <si>
+    <t>Fibrinogen</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>pt</t>
+  </si>
+  <si>
+    <t>aptt</t>
+  </si>
+  <si>
+    <t>aPTT</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>hs_trop</t>
+  </si>
+  <si>
+    <t>High-sensitivity troponin</t>
+  </si>
+  <si>
+    <t>L7</t>
+  </si>
+  <si>
+    <t>bnp</t>
+  </si>
+  <si>
+    <t>BNP</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+  <si>
+    <t>crp</t>
+  </si>
+  <si>
+    <t>CRP</t>
+  </si>
+  <si>
+    <t>L9</t>
+  </si>
+  <si>
+    <t>ldh</t>
+  </si>
+  <si>
+    <t>LDH</t>
+  </si>
+  <si>
+    <t>L10</t>
+  </si>
+  <si>
+    <t>il6</t>
+  </si>
+  <si>
+    <t>IL-6</t>
   </si>
 </sst>
 </file>
@@ -757,10 +856,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E72" totalsRowShown="0">
-  <autoFilter ref="A1:E72" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E71">
-    <sortCondition ref="A1:A71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E83" totalsRowShown="0">
+  <autoFilter ref="A1:E83" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E73">
+    <sortCondition ref="A1:A73"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1094,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1254,873 +1353,1027 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>229</v>
       </c>
       <c r="B11" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>183</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B17" t="s">
-        <v>187</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>188</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B19" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>193</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>230</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>231</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B23" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>174</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>178</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
         <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
         <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
         <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>219</v>
+        <v>119</v>
       </c>
       <c r="B38" t="s">
-        <v>220</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>221</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>222</v>
+        <v>139</v>
       </c>
       <c r="B39" t="s">
-        <v>223</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>224</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>219</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>220</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>222</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>223</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>155</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>156</v>
+        <v>50</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>157</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="B50" t="s">
-        <v>160</v>
+        <v>14</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>158</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B51" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B52" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>163</v>
       </c>
       <c r="C53" t="s">
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>165</v>
       </c>
       <c r="C54" t="s">
         <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C55" t="s">
         <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C56" t="s">
         <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>144</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C58" t="s">
         <v>15</v>
       </c>
       <c r="D58" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B59" t="s">
-        <v>147</v>
+        <v>59</v>
       </c>
       <c r="C59" t="s">
         <v>15</v>
       </c>
       <c r="D59" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B60" t="s">
-        <v>150</v>
+        <v>83</v>
       </c>
       <c r="C60" t="s">
         <v>15</v>
       </c>
       <c r="D60" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B61" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C61" t="s">
         <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>154</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="C62" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="D62" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="C63" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="D63" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C64" t="s">
         <v>124</v>
       </c>
       <c r="D64" t="s">
-        <v>25</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B65" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C65" t="s">
         <v>124</v>
       </c>
       <c r="D65" t="s">
-        <v>135</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C66" t="s">
         <v>124</v>
       </c>
       <c r="D66" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B67" t="s">
-        <v>33</v>
+        <v>130</v>
       </c>
       <c r="C67" t="s">
         <v>124</v>
       </c>
       <c r="D67" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C68" t="s">
         <v>124</v>
       </c>
       <c r="D68" t="s">
-        <v>134</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
       <c r="C69" t="s">
         <v>124</v>
       </c>
       <c r="D69" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>205</v>
+        <v>137</v>
       </c>
       <c r="B70" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="C70" t="s">
-        <v>207</v>
+        <v>124</v>
       </c>
       <c r="D70" t="s">
-        <v>208</v>
-      </c>
-      <c r="E70" t="s">
-        <v>209</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>210</v>
+        <v>138</v>
       </c>
       <c r="B71" t="s">
-        <v>211</v>
+        <v>133</v>
       </c>
       <c r="C71" t="s">
-        <v>207</v>
+        <v>124</v>
       </c>
       <c r="D71" t="s">
-        <v>212</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>205</v>
+      </c>
+      <c r="B72" t="s">
+        <v>206</v>
+      </c>
+      <c r="C72" t="s">
+        <v>207</v>
+      </c>
+      <c r="D72" t="s">
+        <v>208</v>
+      </c>
+      <c r="E72" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>210</v>
+      </c>
+      <c r="B73" t="s">
+        <v>211</v>
+      </c>
+      <c r="C73" t="s">
+        <v>207</v>
+      </c>
+      <c r="D73" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>225</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B74" t="s">
         <v>226</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C74" t="s">
         <v>227</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D74" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>235</v>
+      </c>
+      <c r="B75" t="s">
+        <v>236</v>
+      </c>
+      <c r="C75" t="s">
+        <v>227</v>
+      </c>
+      <c r="D75" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>238</v>
+      </c>
+      <c r="B76" t="s">
+        <v>239</v>
+      </c>
+      <c r="C76" t="s">
+        <v>227</v>
+      </c>
+      <c r="D76" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>241</v>
+      </c>
+      <c r="B77" t="s">
+        <v>244</v>
+      </c>
+      <c r="C77" t="s">
+        <v>227</v>
+      </c>
+      <c r="D77" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>243</v>
+      </c>
+      <c r="B78" t="s">
+        <v>245</v>
+      </c>
+      <c r="C78" t="s">
+        <v>227</v>
+      </c>
+      <c r="D78" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>247</v>
+      </c>
+      <c r="B79" t="s">
+        <v>248</v>
+      </c>
+      <c r="C79" t="s">
+        <v>227</v>
+      </c>
+      <c r="D79" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>250</v>
+      </c>
+      <c r="B80" t="s">
+        <v>251</v>
+      </c>
+      <c r="C80" t="s">
+        <v>227</v>
+      </c>
+      <c r="D80" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>253</v>
+      </c>
+      <c r="B81" t="s">
+        <v>254</v>
+      </c>
+      <c r="C81" t="s">
+        <v>227</v>
+      </c>
+      <c r="D81" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>256</v>
+      </c>
+      <c r="B82" t="s">
+        <v>257</v>
+      </c>
+      <c r="C82" t="s">
+        <v>227</v>
+      </c>
+      <c r="D82" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>259</v>
+      </c>
+      <c r="B83" t="s">
+        <v>260</v>
+      </c>
+      <c r="C83" t="s">
+        <v>227</v>
+      </c>
+      <c r="D83" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added baseline VTE derived variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029FDA05-0A14-1149-A144-D3DEF65A4BFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E84E2A-E451-024B-A5B6-81023B6B4765}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36480" yWindow="1800" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="265">
   <si>
     <t>Variable #</t>
   </si>
@@ -801,6 +801,15 @@
   </si>
   <si>
     <t>IL-6</t>
+  </si>
+  <si>
+    <t>D19</t>
+  </si>
+  <si>
+    <t>VTE_baseline</t>
+  </si>
+  <si>
+    <t>History of VTE</t>
   </si>
 </sst>
 </file>
@@ -856,10 +865,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E83" totalsRowShown="0">
-  <autoFilter ref="A1:E83" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E73">
-    <sortCondition ref="A1:A73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E84" totalsRowShown="0">
+  <autoFilter ref="A1:E84" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E74">
+    <sortCondition ref="A1:A74"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1193,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1507,872 +1516,886 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>262</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>263</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>198</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>171</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B25" t="s">
-        <v>174</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>174</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
         <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
         <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
         <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
         <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C36" t="s">
         <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>219</v>
+        <v>139</v>
       </c>
       <c r="B40" t="s">
-        <v>220</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>221</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B41" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>222</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>63</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C50" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B51" t="s">
-        <v>156</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>157</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B52" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B53" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C53" t="s">
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C54" t="s">
         <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>165</v>
       </c>
       <c r="C55" t="s">
         <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C56" t="s">
         <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B57" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
         <v>15</v>
       </c>
       <c r="D58" t="s">
-        <v>144</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C59" t="s">
         <v>15</v>
       </c>
       <c r="D59" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="C60" t="s">
         <v>15</v>
       </c>
       <c r="D60" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="C61" t="s">
         <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B62" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C62" t="s">
         <v>15</v>
       </c>
       <c r="D62" t="s">
-        <v>151</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B63" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C63" t="s">
         <v>15</v>
       </c>
       <c r="D63" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="B64" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="C64" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="D64" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C65" t="s">
         <v>124</v>
       </c>
       <c r="D65" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B66" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C66" t="s">
         <v>124</v>
       </c>
       <c r="D66" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B67" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C67" t="s">
         <v>124</v>
       </c>
       <c r="D67" t="s">
-        <v>135</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C68" t="s">
         <v>124</v>
       </c>
       <c r="D68" t="s">
-        <v>23</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B69" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="C69" t="s">
         <v>124</v>
       </c>
       <c r="D69" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B70" t="s">
-        <v>132</v>
+        <v>33</v>
       </c>
       <c r="C70" t="s">
         <v>124</v>
       </c>
       <c r="D70" t="s">
-        <v>134</v>
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C71" t="s">
         <v>124</v>
       </c>
       <c r="D71" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="B72" t="s">
-        <v>206</v>
+        <v>133</v>
       </c>
       <c r="C72" t="s">
-        <v>207</v>
+        <v>124</v>
       </c>
       <c r="D72" t="s">
-        <v>208</v>
-      </c>
-      <c r="E72" t="s">
-        <v>209</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B73" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C73" t="s">
         <v>207</v>
       </c>
       <c r="D73" t="s">
-        <v>212</v>
+        <v>208</v>
+      </c>
+      <c r="E73" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="B74" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="C74" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="D74" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B75" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C75" t="s">
         <v>227</v>
       </c>
       <c r="D75" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B76" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C76" t="s">
         <v>227</v>
       </c>
       <c r="D76" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B77" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C77" t="s">
         <v>227</v>
       </c>
       <c r="D77" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B78" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C78" t="s">
         <v>227</v>
       </c>
       <c r="D78" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B79" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C79" t="s">
         <v>227</v>
       </c>
       <c r="D79" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B80" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C80" t="s">
         <v>227</v>
       </c>
       <c r="D80" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B81" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C81" t="s">
         <v>227</v>
       </c>
       <c r="D81" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B82" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C82" t="s">
         <v>227</v>
       </c>
       <c r="D82" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B83" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C83" t="s">
         <v>227</v>
       </c>
       <c r="D83" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>259</v>
+      </c>
+      <c r="B84" t="s">
+        <v>260</v>
+      </c>
+      <c r="C84" t="s">
+        <v>227</v>
+      </c>
+      <c r="D84" t="s">
         <v>261</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added baseline AC/aspirin variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E84E2A-E451-024B-A5B6-81023B6B4765}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCBA909-202D-864D-ABD5-ABB2E235FE15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36480" yWindow="1800" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="268">
   <si>
     <t>Variable #</t>
   </si>
@@ -810,6 +810,15 @@
   </si>
   <si>
     <t>History of VTE</t>
+  </si>
+  <si>
+    <t>Rx15</t>
+  </si>
+  <si>
+    <t>ac_apa_baseline</t>
+  </si>
+  <si>
+    <t>Baseline anticoagulation, aspirin, or APA</t>
   </si>
 </sst>
 </file>
@@ -865,10 +874,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E84" totalsRowShown="0">
-  <autoFilter ref="A1:E84" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E74">
-    <sortCondition ref="A1:A74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E85" totalsRowShown="0">
+  <autoFilter ref="A1:E85" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E75">
+    <sortCondition ref="A1:A75"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1202,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2006,396 +2015,410 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>141</v>
+        <v>265</v>
       </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>266</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>79</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C58" t="s">
         <v>15</v>
       </c>
       <c r="D58" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
         <v>15</v>
       </c>
       <c r="D59" t="s">
-        <v>144</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C60" t="s">
         <v>15</v>
       </c>
       <c r="D60" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="C61" t="s">
         <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B62" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
         <v>15</v>
       </c>
       <c r="D62" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B63" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C63" t="s">
         <v>15</v>
       </c>
       <c r="D63" t="s">
-        <v>151</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B64" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C64" t="s">
         <v>15</v>
       </c>
       <c r="D64" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="B65" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="C65" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="D65" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B66" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C66" t="s">
         <v>124</v>
       </c>
       <c r="D66" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C67" t="s">
         <v>124</v>
       </c>
       <c r="D67" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B68" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C68" t="s">
         <v>124</v>
       </c>
       <c r="D68" t="s">
-        <v>135</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B69" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C69" t="s">
         <v>124</v>
       </c>
       <c r="D69" t="s">
-        <v>23</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B70" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="C70" t="s">
         <v>124</v>
       </c>
       <c r="D70" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B71" t="s">
-        <v>132</v>
+        <v>33</v>
       </c>
       <c r="C71" t="s">
         <v>124</v>
       </c>
       <c r="D71" t="s">
-        <v>134</v>
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C72" t="s">
         <v>124</v>
       </c>
       <c r="D72" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="B73" t="s">
-        <v>206</v>
+        <v>133</v>
       </c>
       <c r="C73" t="s">
-        <v>207</v>
+        <v>124</v>
       </c>
       <c r="D73" t="s">
-        <v>208</v>
-      </c>
-      <c r="E73" t="s">
-        <v>209</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C74" t="s">
         <v>207</v>
       </c>
       <c r="D74" t="s">
-        <v>212</v>
+        <v>208</v>
+      </c>
+      <c r="E74" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="B75" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="C75" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="D75" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B76" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C76" t="s">
         <v>227</v>
       </c>
       <c r="D76" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B77" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C77" t="s">
         <v>227</v>
       </c>
       <c r="D77" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B78" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C78" t="s">
         <v>227</v>
       </c>
       <c r="D78" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B79" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C79" t="s">
         <v>227</v>
       </c>
       <c r="D79" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B80" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C80" t="s">
         <v>227</v>
       </c>
       <c r="D80" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B81" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C81" t="s">
         <v>227</v>
       </c>
       <c r="D81" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B82" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C82" t="s">
         <v>227</v>
       </c>
       <c r="D82" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B83" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C83" t="s">
         <v>227</v>
       </c>
       <c r="D83" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B84" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C84" t="s">
         <v>227</v>
       </c>
       <c r="D84" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>259</v>
+      </c>
+      <c r="B85" t="s">
+        <v>260</v>
+      </c>
+      <c r="C85" t="s">
+        <v>227</v>
+      </c>
+      <c r="D85" t="s">
         <v>261</v>
       </c>
     </row>

</xml_diff>

<commit_message>
VTE risk derived variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65C3B38-EEB7-E84F-B6C6-B0FA0E615F1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1140C30C-3750-A54D-A749-FD9D4814C241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-44980" yWindow="2420" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="292">
   <si>
     <t>Variable #</t>
   </si>
@@ -882,6 +882,15 @@
   </si>
   <si>
     <t>Indicates whether patient has ever had supplemental o2</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>VTE_risk</t>
+  </si>
+  <si>
+    <t>Risk of VTE based on malignancy diagnosis</t>
   </si>
 </sst>
 </file>
@@ -937,8 +946,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E92" totalsRowShown="0">
-  <autoFilter ref="A1:E92" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E93" totalsRowShown="0">
+  <autoFilter ref="A1:E93" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
   <sortState ref="A2:E82">
     <sortCondition ref="A1:A82"/>
   </sortState>
@@ -1274,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2583,6 +2592,20 @@
         <v>260</v>
       </c>
     </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>289</v>
+      </c>
+      <c r="B93" t="s">
+        <v>290</v>
+      </c>
+      <c r="C93" t="s">
+        <v>206</v>
+      </c>
+      <c r="D93" t="s">
+        <v>291</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
ASCT within 100 days
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1140C30C-3750-A54D-A749-FD9D4814C241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872118DC-AA0A-0546-8C1C-6E810644044C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44980" yWindow="2420" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36300" yWindow="2940" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="301">
   <si>
     <t>Variable #</t>
   </si>
@@ -891,6 +891,33 @@
   </si>
   <si>
     <t>Risk of VTE based on malignancy diagnosis</t>
+  </si>
+  <si>
+    <t>Ca1a</t>
+  </si>
+  <si>
+    <t>activetx3mo</t>
+  </si>
+  <si>
+    <t>Derived variable for whether a patient is on active therapy (within 3 months)</t>
+  </si>
+  <si>
+    <t>Ca12</t>
+  </si>
+  <si>
+    <t>allo365</t>
+  </si>
+  <si>
+    <t>Allogeneic transplant within one year</t>
+  </si>
+  <si>
+    <t>Ca13</t>
+  </si>
+  <si>
+    <t>auto100</t>
+  </si>
+  <si>
+    <t>Autologous transplant within 100 days</t>
   </si>
 </sst>
 </file>
@@ -946,10 +973,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E93" totalsRowShown="0">
-  <autoFilter ref="A1:E93" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E82">
-    <sortCondition ref="A1:A82"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E96" totalsRowShown="0">
+  <autoFilter ref="A1:E96" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E85">
+    <sortCondition ref="A1:A85"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1283,10 +1310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1331,1046 +1358,1046 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>293</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8" t="s">
-        <v>203</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>216</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="B11" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>279</v>
+        <v>228</v>
       </c>
       <c r="B12" t="s">
-        <v>280</v>
+        <v>232</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>281</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B13" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="B15" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>270</v>
       </c>
       <c r="B16" t="s">
-        <v>168</v>
+        <v>271</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>179</v>
+        <v>295</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>296</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>180</v>
+        <v>298</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>299</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>168</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s">
-        <v>186</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B23" t="s">
-        <v>189</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>190</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B24" t="s">
-        <v>192</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>193</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>229</v>
+        <v>185</v>
       </c>
       <c r="B25" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>231</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>261</v>
+        <v>188</v>
       </c>
       <c r="B26" t="s">
-        <v>262</v>
+        <v>189</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>263</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>267</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s">
-        <v>268</v>
+        <v>192</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>269</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>169</v>
+        <v>229</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>230</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>48</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>261</v>
       </c>
       <c r="B29" t="s">
-        <v>170</v>
+        <v>262</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>197</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>267</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>268</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>273</v>
+        <v>169</v>
       </c>
       <c r="B31" t="s">
-        <v>274</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>275</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B32" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C32" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>68</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>176</v>
+        <v>273</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>274</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>275</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="C35" t="s">
         <v>21</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>276</v>
+        <v>175</v>
       </c>
       <c r="B36" t="s">
-        <v>277</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>278</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
         <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>177</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>277</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D39" t="s">
-        <v>102</v>
+        <v>278</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>178</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>115</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C44" t="s">
         <v>36</v>
       </c>
       <c r="D44" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="C45" t="s">
         <v>36</v>
       </c>
       <c r="D45" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D46" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>111</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D47" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>218</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>219</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D48" t="s">
-        <v>220</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>221</v>
+        <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>222</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>223</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>138</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>218</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>219</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
       </c>
       <c r="D51" t="s">
-        <v>64</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>221</v>
       </c>
       <c r="B52" t="s">
-        <v>11</v>
+        <v>222</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>65</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B55" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>288</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B56" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B57" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>67</v>
+        <v>288</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="B59" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>156</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>158</v>
+        <v>99</v>
       </c>
       <c r="B60" t="s">
-        <v>159</v>
+        <v>50</v>
       </c>
       <c r="C60" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>157</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="B61" t="s">
-        <v>162</v>
+        <v>14</v>
       </c>
       <c r="C61" t="s">
         <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>160</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B62" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C62" t="s">
         <v>15</v>
       </c>
       <c r="D62" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>159</v>
       </c>
       <c r="C63" t="s">
         <v>15</v>
       </c>
       <c r="D63" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>264</v>
+        <v>161</v>
       </c>
       <c r="B64" t="s">
-        <v>265</v>
+        <v>162</v>
       </c>
       <c r="C64" t="s">
         <v>15</v>
       </c>
       <c r="D64" t="s">
-        <v>266</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="B65" t="s">
-        <v>32</v>
+        <v>164</v>
       </c>
       <c r="C65" t="s">
         <v>15</v>
       </c>
       <c r="D65" t="s">
-        <v>78</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C66" t="s">
         <v>15</v>
       </c>
       <c r="D66" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>264</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>265</v>
       </c>
       <c r="C67" t="s">
         <v>15</v>
       </c>
       <c r="D67" t="s">
-        <v>143</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C68" t="s">
         <v>15</v>
       </c>
       <c r="D68" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B69" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C69" t="s">
         <v>15</v>
       </c>
       <c r="D69" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B70" t="s">
-        <v>146</v>
+        <v>55</v>
       </c>
       <c r="C70" t="s">
         <v>15</v>
       </c>
       <c r="D70" t="s">
-        <v>87</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B71" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="C71" t="s">
         <v>15</v>
       </c>
       <c r="D71" t="s">
-        <v>150</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B72" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
       <c r="C72" t="s">
         <v>15</v>
       </c>
       <c r="D72" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="B73" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="C73" t="s">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="D73" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="B74" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="C74" t="s">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="D74" t="s">
-        <v>23</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="C75" t="s">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="D75" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B76" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C76" t="s">
         <v>123</v>
       </c>
       <c r="D76" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B77" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C77" t="s">
         <v>123</v>
@@ -2381,38 +2408,38 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B78" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="C78" t="s">
         <v>123</v>
       </c>
       <c r="D78" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B79" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C79" t="s">
         <v>123</v>
       </c>
       <c r="D79" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B80" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C80" t="s">
         <v>123</v>
@@ -2423,186 +2450,228 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>204</v>
+        <v>130</v>
       </c>
       <c r="B81" t="s">
-        <v>205</v>
+        <v>33</v>
       </c>
       <c r="C81" t="s">
-        <v>206</v>
+        <v>123</v>
       </c>
       <c r="D81" t="s">
-        <v>207</v>
-      </c>
-      <c r="E81" t="s">
-        <v>208</v>
+        <v>34</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>209</v>
+        <v>136</v>
       </c>
       <c r="B82" t="s">
-        <v>210</v>
+        <v>131</v>
       </c>
       <c r="C82" t="s">
-        <v>206</v>
+        <v>123</v>
       </c>
       <c r="D82" t="s">
-        <v>211</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>224</v>
+        <v>137</v>
       </c>
       <c r="B83" t="s">
-        <v>225</v>
+        <v>132</v>
       </c>
       <c r="C83" t="s">
-        <v>226</v>
+        <v>123</v>
       </c>
       <c r="D83" t="s">
-        <v>227</v>
+        <v>23</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="B84" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="C84" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="D84" t="s">
-        <v>236</v>
+        <v>207</v>
+      </c>
+      <c r="E84" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
       <c r="B85" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="C85" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="D85" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="B86" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="C86" t="s">
         <v>226</v>
       </c>
       <c r="D86" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B87" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C87" t="s">
         <v>226</v>
       </c>
       <c r="D87" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B88" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C88" t="s">
         <v>226</v>
       </c>
       <c r="D88" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B89" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C89" t="s">
         <v>226</v>
       </c>
       <c r="D89" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="B90" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C90" t="s">
         <v>226</v>
       </c>
       <c r="D90" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B91" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C91" t="s">
         <v>226</v>
       </c>
       <c r="D91" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B92" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C92" t="s">
         <v>226</v>
       </c>
       <c r="D92" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>252</v>
+      </c>
+      <c r="B93" t="s">
+        <v>253</v>
+      </c>
+      <c r="C93" t="s">
+        <v>226</v>
+      </c>
+      <c r="D93" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>255</v>
+      </c>
+      <c r="B94" t="s">
+        <v>256</v>
+      </c>
+      <c r="C94" t="s">
+        <v>226</v>
+      </c>
+      <c r="D94" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>258</v>
+      </c>
+      <c r="B95" t="s">
+        <v>259</v>
+      </c>
+      <c r="C95" t="s">
+        <v>226</v>
+      </c>
+      <c r="D95" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>289</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B96" t="s">
         <v>290</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C96" t="s">
         <v>206</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D96" t="s">
         <v>291</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed a bug in O2 requirement variable
Cases were incorrectly assigned missing instead of no requirement, due to the baseline O2 requirement variable. Fixed now, with almost no missingness for this variable. This will also help the composite variables missingness.
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313A6D3A-2EE4-634A-8FF3-906A32E24A83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD0CCDA-5F09-0F48-BF78-9BF3068F58CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36300" yWindow="2940" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36340" yWindow="2860" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="334">
   <si>
     <t>Variable #</t>
   </si>
@@ -990,6 +990,33 @@
   </si>
   <si>
     <t>Lymphopenia and Neutropenia</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>Quality score</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>problems</t>
+  </si>
+  <si>
+    <t>Enumerated problems that feed quality score</t>
+  </si>
+  <si>
+    <t>X6</t>
+  </si>
+  <si>
+    <t>ccc19cci</t>
+  </si>
+  <si>
+    <t>CCC19 modified Charlson</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1072,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E104" totalsRowShown="0">
-  <autoFilter ref="A1:E104" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E107" totalsRowShown="0">
+  <autoFilter ref="A1:E107" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
   <sortState ref="A2:E104">
     <sortCondition ref="A1:A104"/>
   </sortState>
@@ -1382,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2859,6 +2886,48 @@
         <v>282</v>
       </c>
     </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>325</v>
+      </c>
+      <c r="B105" t="s">
+        <v>326</v>
+      </c>
+      <c r="C105" t="s">
+        <v>206</v>
+      </c>
+      <c r="D105" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>328</v>
+      </c>
+      <c r="B106" t="s">
+        <v>329</v>
+      </c>
+      <c r="C106" t="s">
+        <v>206</v>
+      </c>
+      <c r="D106" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>331</v>
+      </c>
+      <c r="B107" t="s">
+        <v>332</v>
+      </c>
+      <c r="C107" t="s">
+        <v>206</v>
+      </c>
+      <c r="D107" t="s">
+        <v>333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Added CV event derived variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD0CCDA-5F09-0F48-BF78-9BF3068F58CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27147AC-8154-EB43-BAC5-C884BE00F167}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36340" yWindow="2860" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="337">
   <si>
     <t>Variable #</t>
   </si>
@@ -284,39 +284,12 @@
     <t>Variable Name (der_name)</t>
   </si>
   <si>
-    <t>O1</t>
-  </si>
-  <si>
-    <t>O2</t>
-  </si>
-  <si>
-    <t>O3</t>
-  </si>
-  <si>
-    <t>O4</t>
-  </si>
-  <si>
-    <t>O5</t>
-  </si>
-  <si>
-    <t>O6</t>
-  </si>
-  <si>
     <t>days_to_death_combined</t>
   </si>
   <si>
     <t>Combined days to death</t>
   </si>
   <si>
-    <t>O7</t>
-  </si>
-  <si>
-    <t>O8</t>
-  </si>
-  <si>
-    <t>O9</t>
-  </si>
-  <si>
     <t>O10</t>
   </si>
   <si>
@@ -1017,6 +990,42 @@
   </si>
   <si>
     <t>CCC19 modified Charlson</t>
+  </si>
+  <si>
+    <t>O01</t>
+  </si>
+  <si>
+    <t>O02</t>
+  </si>
+  <si>
+    <t>O03</t>
+  </si>
+  <si>
+    <t>O04</t>
+  </si>
+  <si>
+    <t>O05</t>
+  </si>
+  <si>
+    <t>O06</t>
+  </si>
+  <si>
+    <t>O07</t>
+  </si>
+  <si>
+    <t>O08</t>
+  </si>
+  <si>
+    <t>O09</t>
+  </si>
+  <si>
+    <t>O21</t>
+  </si>
+  <si>
+    <t>CV_event</t>
+  </si>
+  <si>
+    <t>Combined cardiovascular event</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1081,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E107" totalsRowShown="0">
-  <autoFilter ref="A1:E107" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E104">
-    <sortCondition ref="A1:A104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E108" totalsRowShown="0">
+  <autoFilter ref="A1:E108" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E108">
+    <sortCondition ref="A1:A108"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1409,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1443,7 +1452,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -1457,119 +1466,119 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B7" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B9" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B10" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
@@ -1578,12 +1587,12 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -1597,7 +1606,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -1611,7 +1620,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B14" t="s">
         <v>80</v>
@@ -1625,7 +1634,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1639,10 +1648,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B16" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -1653,38 +1662,38 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B17" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B19" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1695,7 +1704,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
         <v>42</v>
@@ -1709,7 +1718,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
         <v>44</v>
@@ -1723,7 +1732,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B22" t="s">
         <v>45</v>
@@ -1732,12 +1741,12 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B23" t="s">
         <v>60</v>
@@ -1751,7 +1760,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -1765,77 +1774,77 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B25" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B26" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C26" t="s">
         <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B27" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B28" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B29" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B30" t="s">
         <v>47</v>
@@ -1849,35 +1858,35 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B31" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B32" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B33" t="s">
         <v>18</v>
@@ -1891,24 +1900,24 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B34" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B35" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C35" t="s">
         <v>21</v>
@@ -1919,7 +1928,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B36" t="s">
         <v>22</v>
@@ -1933,7 +1942,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B37" t="s">
         <v>30</v>
@@ -1947,7 +1956,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B38" t="s">
         <v>52</v>
@@ -1961,21 +1970,21 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B39" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C39" t="s">
         <v>21</v>
       </c>
       <c r="D39" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -1989,259 +1998,259 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="B41" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C41" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D41" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B42" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C42" t="s">
+        <v>216</v>
+      </c>
+      <c r="D42" t="s">
         <v>225</v>
-      </c>
-      <c r="D42" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B43" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C43" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D43" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B44" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C44" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D44" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B45" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C45" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D45" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B46" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C46" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D46" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B47" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C47" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D47" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B48" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C48" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D48" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B49" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D49" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B50" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C50" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D50" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B51" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="C51" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D51" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B52" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C52" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D52" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B53" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C53" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D53" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B54" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C54" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D54" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="B55" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="C55" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D55" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="B56" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="C56" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D56" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B57" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C57" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D57" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B58" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="C58" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D58" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>89</v>
+        <v>325</v>
       </c>
       <c r="B59" t="s">
         <v>4</v>
@@ -2255,677 +2264,691 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>100</v>
+        <v>326</v>
       </c>
       <c r="B60" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>103</v>
+        <v>327</v>
       </c>
       <c r="B61" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>104</v>
+        <v>328</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>106</v>
+        <v>329</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D63" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>108</v>
+        <v>330</v>
       </c>
       <c r="B64" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="C64" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D64" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>110</v>
+        <v>331</v>
       </c>
       <c r="B65" t="s">
-        <v>111</v>
+        <v>28</v>
       </c>
       <c r="C65" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>112</v>
+        <v>270</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>116</v>
+        <v>332</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>118</v>
+        <v>333</v>
       </c>
       <c r="B67" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
       <c r="B68" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>218</v>
+        <v>94</v>
       </c>
       <c r="B69" t="s">
-        <v>219</v>
+        <v>35</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
       </c>
       <c r="D69" t="s">
-        <v>220</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D70" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>221</v>
+        <v>97</v>
       </c>
       <c r="B71" t="s">
-        <v>222</v>
+        <v>98</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D71" t="s">
-        <v>223</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D72" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B73" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D73" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B74" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D74" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="B75" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="C75" t="s">
         <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="B76" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>279</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>98</v>
+        <v>209</v>
       </c>
       <c r="B77" t="s">
-        <v>29</v>
+        <v>210</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>77</v>
+        <v>211</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>99</v>
+        <v>212</v>
       </c>
       <c r="B78" t="s">
-        <v>50</v>
+        <v>213</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>51</v>
+        <v>214</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>139</v>
+        <v>334</v>
       </c>
       <c r="B79" t="s">
-        <v>14</v>
+        <v>335</v>
       </c>
       <c r="C79" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>67</v>
+        <v>336</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="B80" t="s">
-        <v>155</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
         <v>15</v>
       </c>
       <c r="D80" t="s">
-        <v>156</v>
+        <v>67</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B81" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C81" t="s">
         <v>15</v>
       </c>
       <c r="D81" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C82" t="s">
         <v>15</v>
       </c>
       <c r="D82" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C83" t="s">
         <v>15</v>
       </c>
       <c r="D83" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B84" t="s">
-        <v>43</v>
+        <v>155</v>
       </c>
       <c r="C84" t="s">
         <v>15</v>
       </c>
       <c r="D84" t="s">
-        <v>86</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>255</v>
+        <v>157</v>
       </c>
       <c r="B85" t="s">
-        <v>256</v>
+        <v>43</v>
       </c>
       <c r="C85" t="s">
         <v>15</v>
       </c>
       <c r="D85" t="s">
-        <v>257</v>
+        <v>86</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>140</v>
+        <v>246</v>
       </c>
       <c r="B86" t="s">
-        <v>32</v>
+        <v>247</v>
       </c>
       <c r="C86" t="s">
         <v>15</v>
       </c>
       <c r="D86" t="s">
-        <v>78</v>
+        <v>248</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B87" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C87" t="s">
         <v>15</v>
       </c>
       <c r="D87" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B88" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C88" t="s">
         <v>15</v>
       </c>
       <c r="D88" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B89" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C89" t="s">
         <v>15</v>
       </c>
       <c r="D89" t="s">
-        <v>84</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B90" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C90" t="s">
         <v>15</v>
       </c>
       <c r="D90" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B91" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="C91" t="s">
         <v>15</v>
       </c>
       <c r="D91" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B92" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C92" t="s">
         <v>15</v>
       </c>
       <c r="D92" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="B93" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C93" t="s">
         <v>15</v>
       </c>
       <c r="D93" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="B94" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="C94" t="s">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="D94" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B95" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C95" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D95" t="s">
-        <v>23</v>
+        <v>126</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B96" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C96" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D96" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B97" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C97" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D97" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B98" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C98" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D98" t="s">
-        <v>23</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B99" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="C99" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D99" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B100" t="s">
-        <v>131</v>
+        <v>33</v>
       </c>
       <c r="C100" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D100" t="s">
-        <v>133</v>
+        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B101" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C101" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D101" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>204</v>
+        <v>128</v>
       </c>
       <c r="B102" t="s">
-        <v>205</v>
+        <v>123</v>
       </c>
       <c r="C102" t="s">
-        <v>206</v>
+        <v>114</v>
       </c>
       <c r="D102" t="s">
-        <v>207</v>
-      </c>
-      <c r="E102" t="s">
-        <v>208</v>
+        <v>23</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B103" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C103" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D103" t="s">
-        <v>211</v>
+        <v>198</v>
+      </c>
+      <c r="E103" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>280</v>
+        <v>200</v>
       </c>
       <c r="B104" t="s">
-        <v>281</v>
+        <v>201</v>
       </c>
       <c r="C104" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D104" t="s">
-        <v>282</v>
+        <v>202</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>325</v>
+        <v>271</v>
       </c>
       <c r="B105" t="s">
-        <v>326</v>
+        <v>272</v>
       </c>
       <c r="C105" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D105" t="s">
-        <v>327</v>
+        <v>273</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="B106" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="C106" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D106" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="B107" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="C107" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D107" t="s">
-        <v>333</v>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>322</v>
+      </c>
+      <c r="B108" t="s">
+        <v>323</v>
+      </c>
+      <c r="C108" t="s">
+        <v>197</v>
+      </c>
+      <c r="D108" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New breast biomarkers derived variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10914"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EBEE08-154F-E747-86CC-39E1344ACF74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2602953D-B6CB-A540-94D6-64ED49ABCB45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5200" yWindow="3520" windowWidth="35840" windowHeight="23680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="340">
   <si>
     <t>Variable #</t>
   </si>
@@ -1026,6 +1026,15 @@
   </si>
   <si>
     <t>Severe composite outcome v2 not including severe hospitalization</t>
+  </si>
+  <si>
+    <t>X7</t>
+  </si>
+  <si>
+    <t>breast_biomarkers</t>
+  </si>
+  <si>
+    <t>Breast biomarkers combined variable</t>
   </si>
 </sst>
 </file>
@@ -1081,8 +1090,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E108" totalsRowShown="0">
-  <autoFilter ref="A1:E108" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E109" totalsRowShown="0">
+  <autoFilter ref="A1:E109" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
   <sortState ref="A2:E108">
     <sortCondition ref="A1:A108"/>
   </sortState>
@@ -1418,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2951,6 +2960,20 @@
         <v>311</v>
       </c>
     </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>337</v>
+      </c>
+      <c r="B109" t="s">
+        <v>338</v>
+      </c>
+      <c r="C109" t="s">
+        <v>186</v>
+      </c>
+      <c r="D109" t="s">
+        <v>339</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Renaming of variables so that they can be sorted in numeric order
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2602953D-B6CB-A540-94D6-64ED49ABCB45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8030163-FED9-F341-81FA-8BE0B4D575C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="3520" windowWidth="35840" windowHeight="23680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,45 +401,18 @@
     <t>O18</t>
   </si>
   <si>
-    <t>Rx1</t>
-  </si>
-  <si>
-    <t>Rx2</t>
-  </si>
-  <si>
-    <t>Rx3</t>
-  </si>
-  <si>
-    <t>Rx4</t>
-  </si>
-  <si>
     <t>High-dose steroids as COVID-19 treatment ever</t>
   </si>
   <si>
-    <t>Rx5</t>
-  </si>
-  <si>
-    <t>Rx6</t>
-  </si>
-  <si>
     <t>other_tx_c19</t>
   </si>
   <si>
-    <t>Rx7</t>
-  </si>
-  <si>
-    <t>Rx8</t>
-  </si>
-  <si>
     <t>statins</t>
   </si>
   <si>
     <t>Statins ever (baseline or for COVID-19)</t>
   </si>
   <si>
-    <t>Rx9</t>
-  </si>
-  <si>
     <t>antivirals</t>
   </si>
   <si>
@@ -539,33 +512,12 @@
     <t>Derived variable for smoking status collapsing the current/former smoker variables</t>
   </si>
   <si>
-    <t>Ca1</t>
-  </si>
-  <si>
-    <t>Ca2</t>
-  </si>
-  <si>
     <t>Derived variable for type of tumor</t>
   </si>
   <si>
     <t>Derived variable for smoking status collapsing the former smoker variable</t>
   </si>
   <si>
-    <t>Ca3</t>
-  </si>
-  <si>
-    <t>Ca4</t>
-  </si>
-  <si>
-    <t>Ca5</t>
-  </si>
-  <si>
-    <t>Ca6</t>
-  </si>
-  <si>
-    <t>Ca7</t>
-  </si>
-  <si>
     <t>cancer_status</t>
   </si>
   <si>
@@ -593,12 +545,6 @@
     <t>Modified IMWG frailty index</t>
   </si>
   <si>
-    <t>Ca8</t>
-  </si>
-  <si>
-    <t>Ca9</t>
-  </si>
-  <si>
     <t>heme</t>
   </si>
   <si>
@@ -800,9 +746,6 @@
     <t>Risk of VTE based on malignancy diagnosis</t>
   </si>
   <si>
-    <t>Ca1a</t>
-  </si>
-  <si>
     <t>activetx3mo</t>
   </si>
   <si>
@@ -1035,6 +978,63 @@
   </si>
   <si>
     <t>Breast biomarkers combined variable</t>
+  </si>
+  <si>
+    <t>Rx01</t>
+  </si>
+  <si>
+    <t>Rx02</t>
+  </si>
+  <si>
+    <t>Rx03</t>
+  </si>
+  <si>
+    <t>Rx04</t>
+  </si>
+  <si>
+    <t>Rx05</t>
+  </si>
+  <si>
+    <t>Rx06</t>
+  </si>
+  <si>
+    <t>Rx07</t>
+  </si>
+  <si>
+    <t>Rx08</t>
+  </si>
+  <si>
+    <t>Rx09</t>
+  </si>
+  <si>
+    <t>Ca01</t>
+  </si>
+  <si>
+    <t>Ca01a</t>
+  </si>
+  <si>
+    <t>Ca02</t>
+  </si>
+  <si>
+    <t>Ca03</t>
+  </si>
+  <si>
+    <t>Ca04</t>
+  </si>
+  <si>
+    <t>Ca05</t>
+  </si>
+  <si>
+    <t>Ca06</t>
+  </si>
+  <si>
+    <t>Ca07</t>
+  </si>
+  <si>
+    <t>Ca08</t>
+  </si>
+  <si>
+    <t>Ca09</t>
   </si>
 </sst>
 </file>
@@ -1092,8 +1092,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E109" totalsRowShown="0">
   <autoFilter ref="A1:E109" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E108">
-    <sortCondition ref="A1:A108"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E109">
+    <sortCondition ref="A1:A109"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1429,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>330</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -1475,234 +1475,234 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>331</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>243</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>212</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>332</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>333</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>253</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>334</v>
       </c>
       <c r="B6" t="s">
-        <v>255</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>256</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>241</v>
+        <v>335</v>
       </c>
       <c r="B7" t="s">
-        <v>242</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>243</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>264</v>
+        <v>336</v>
       </c>
       <c r="B8" t="s">
-        <v>265</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>266</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>267</v>
+        <v>337</v>
       </c>
       <c r="B9" t="s">
-        <v>268</v>
+        <v>167</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>269</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>261</v>
+        <v>338</v>
       </c>
       <c r="B10" t="s">
-        <v>262</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>263</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>339</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>177</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>193</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>231</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>233</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>234</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>236</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>237</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>223</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>224</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>192</v>
+        <v>245</v>
       </c>
       <c r="B17" t="s">
-        <v>194</v>
+        <v>246</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>196</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>193</v>
+        <v>248</v>
       </c>
       <c r="B18" t="s">
-        <v>195</v>
+        <v>249</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>197</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1713,553 +1713,553 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>306</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>307</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>308</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>163</v>
+        <v>309</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>226</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>310</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
       <c r="B25" t="s">
-        <v>166</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>167</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>312</v>
       </c>
       <c r="B26" t="s">
-        <v>169</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
         <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>170</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>313</v>
       </c>
       <c r="B27" t="s">
-        <v>172</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>173</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>208</v>
+        <v>314</v>
       </c>
       <c r="B28" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>232</v>
+        <v>315</v>
       </c>
       <c r="B29" t="s">
-        <v>233</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>234</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>325</v>
+        <v>150</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>238</v>
+        <v>151</v>
       </c>
       <c r="B31" t="s">
-        <v>239</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D31" t="s">
-        <v>240</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>326</v>
+        <v>152</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D32" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>327</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>328</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>244</v>
+        <v>3</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>245</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>329</v>
+        <v>156</v>
       </c>
       <c r="B35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
         <v>158</v>
-      </c>
-      <c r="C35" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>330</v>
+        <v>159</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
       <c r="C36" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D36" t="s">
-        <v>70</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>331</v>
+        <v>162</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>163</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>332</v>
+        <v>190</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>191</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B39" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>334</v>
+        <v>220</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>221</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="B41" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="C41" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D41" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="B42" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="C42" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D42" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="B43" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="C43" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D43" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="B44" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="C44" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D44" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="B45" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="C45" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D45" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="B46" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="C46" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D46" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="B47" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="C47" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D47" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="B48" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="C48" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D48" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="B49" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="C49" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D49" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="B50" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="C50" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D50" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="B51" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="C51" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D51" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="B52" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="C52" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D52" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="B53" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="C53" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D53" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="B54" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="C54" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D54" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="B55" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="C55" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D55" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="B56" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="C56" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D56" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
       <c r="B57" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="C57" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D57" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="B58" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="C58" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D58" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="B59" t="s">
         <v>4</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>313</v>
+        <v>294</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>316</v>
+        <v>297</v>
       </c>
       <c r="B63" t="s">
         <v>13</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="B64" t="s">
         <v>87</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>318</v>
+        <v>299</v>
       </c>
       <c r="B65" t="s">
         <v>28</v>
@@ -2352,12 +2352,12 @@
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="B66" t="s">
         <v>29</v>
@@ -2366,12 +2366,12 @@
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>320</v>
+        <v>301</v>
       </c>
       <c r="B67" t="s">
         <v>50</v>
@@ -2380,7 +2380,7 @@
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2511,49 +2511,49 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="B77" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="B78" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>321</v>
+        <v>302</v>
       </c>
       <c r="B79" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>128</v>
+        <v>321</v>
       </c>
       <c r="B80" t="s">
         <v>14</v>
@@ -2567,198 +2567,198 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>143</v>
+        <v>322</v>
       </c>
       <c r="B81" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="C81" t="s">
         <v>15</v>
       </c>
       <c r="D81" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>323</v>
       </c>
       <c r="B82" t="s">
-        <v>148</v>
+        <v>53</v>
       </c>
       <c r="C82" t="s">
         <v>15</v>
       </c>
       <c r="D82" t="s">
-        <v>146</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>150</v>
+        <v>324</v>
       </c>
       <c r="B83" t="s">
-        <v>151</v>
+        <v>54</v>
       </c>
       <c r="C83" t="s">
         <v>15</v>
       </c>
       <c r="D83" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>154</v>
+        <v>325</v>
       </c>
       <c r="B84" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="C84" t="s">
         <v>15</v>
       </c>
       <c r="D84" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>155</v>
+        <v>326</v>
       </c>
       <c r="B85" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="C85" t="s">
         <v>15</v>
       </c>
       <c r="D85" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>235</v>
+        <v>327</v>
       </c>
       <c r="B86" t="s">
-        <v>236</v>
+        <v>129</v>
       </c>
       <c r="C86" t="s">
         <v>15</v>
       </c>
       <c r="D86" t="s">
-        <v>237</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>129</v>
+        <v>328</v>
       </c>
       <c r="B87" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="C87" t="s">
         <v>15</v>
       </c>
       <c r="D87" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>130</v>
+        <v>329</v>
       </c>
       <c r="B88" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="C88" t="s">
         <v>15</v>
       </c>
       <c r="D88" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B89" t="s">
-        <v>54</v>
+        <v>135</v>
       </c>
       <c r="C89" t="s">
         <v>15</v>
       </c>
       <c r="D89" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B90" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="C90" t="s">
         <v>15</v>
       </c>
       <c r="D90" t="s">
-        <v>82</v>
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B91" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="C91" t="s">
         <v>15</v>
       </c>
       <c r="D91" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B92" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C92" t="s">
         <v>15</v>
       </c>
       <c r="D92" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B93" t="s">
-        <v>138</v>
+        <v>43</v>
       </c>
       <c r="C93" t="s">
         <v>15</v>
       </c>
       <c r="D93" t="s">
-        <v>139</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>140</v>
+        <v>217</v>
       </c>
       <c r="B94" t="s">
-        <v>141</v>
+        <v>218</v>
       </c>
       <c r="C94" t="s">
         <v>15</v>
       </c>
       <c r="D94" t="s">
-        <v>142</v>
+        <v>219</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -2875,103 +2875,103 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B103" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="C103" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D103" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="E103" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="B104" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C104" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D104" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B105" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="C105" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D105" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="B106" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="C106" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D106" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="B107" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="C107" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D107" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="B108" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="C108" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D108" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>337</v>
+        <v>318</v>
       </c>
       <c r="B109" t="s">
-        <v>338</v>
+        <v>319</v>
       </c>
       <c r="C109" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D109" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New derived variable - early ICU admission
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3603D98-5E1D-D64E-B427-162F3EB52CCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCBF618-CC6F-5845-A955-8F0FE1543D48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35940" yWindow="2600" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="352">
   <si>
     <t>Variable #</t>
   </si>
@@ -1062,6 +1062,15 @@
   </si>
   <si>
     <t>Hemi-year of diagnosis, accounting for interval bounds</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>early_icu</t>
+  </si>
+  <si>
+    <t>Early ICU admission (within 48 hours)</t>
   </si>
 </sst>
 </file>
@@ -1117,10 +1126,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E112" totalsRowShown="0">
-  <autoFilter ref="A1:E112" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E112">
-    <sortCondition ref="A1:A112"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E113" totalsRowShown="0">
+  <autoFilter ref="A1:E113" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E113">
+    <sortCondition ref="A1:A113"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1454,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2944,102 +2953,116 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>160</v>
+        <v>349</v>
       </c>
       <c r="B106" t="s">
-        <v>161</v>
+        <v>350</v>
       </c>
       <c r="C106" t="s">
-        <v>162</v>
+        <v>110</v>
       </c>
       <c r="D106" t="s">
-        <v>163</v>
-      </c>
-      <c r="E106" t="s">
-        <v>164</v>
+        <v>351</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B107" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C107" t="s">
         <v>162</v>
       </c>
       <c r="D107" t="s">
-        <v>167</v>
+        <v>163</v>
+      </c>
+      <c r="E107" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>232</v>
+        <v>165</v>
       </c>
       <c r="B108" t="s">
-        <v>233</v>
+        <v>166</v>
       </c>
       <c r="C108" t="s">
         <v>162</v>
       </c>
       <c r="D108" t="s">
-        <v>234</v>
+        <v>167</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
       <c r="B109" t="s">
-        <v>277</v>
+        <v>233</v>
       </c>
       <c r="C109" t="s">
         <v>162</v>
       </c>
       <c r="D109" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B110" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C110" t="s">
         <v>162</v>
       </c>
       <c r="D110" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B111" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C111" t="s">
         <v>162</v>
       </c>
       <c r="D111" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>310</v>
+        <v>282</v>
       </c>
       <c r="B112" t="s">
-        <v>311</v>
+        <v>283</v>
       </c>
       <c r="C112" t="s">
         <v>162</v>
       </c>
       <c r="D112" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>310</v>
+      </c>
+      <c r="B113" t="s">
+        <v>311</v>
+      </c>
+      <c r="C113" t="s">
+        <v>162</v>
+      </c>
+      <c r="D113" t="s">
         <v>312</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add a hospitalized at baseline derived variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F1C5BE-6B3A-0246-AD2E-28F57E20EA8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4970F7ED-2852-904A-AA01-9F9CA79DA915}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35940" yWindow="2600" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="355">
   <si>
     <t>Variable #</t>
   </si>
@@ -1071,6 +1071,15 @@
   </si>
   <si>
     <t>Derived variable indicating whether patients required mechanical ventilation</t>
+  </si>
+  <si>
+    <t>O02a</t>
+  </si>
+  <si>
+    <t>hosp_bl</t>
+  </si>
+  <si>
+    <t>Hospitalized at baseline (within 30 days of diagnosis)</t>
   </si>
 </sst>
 </file>
@@ -1126,10 +1135,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E113" totalsRowShown="0">
-  <autoFilter ref="A1:E113" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E113">
-    <sortCondition ref="A1:A113"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E114" totalsRowShown="0">
+  <autoFilter ref="A1:E114" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E114">
+    <sortCondition ref="A1:A114"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1463,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2323,746 +2332,760 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>285</v>
+        <v>352</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>353</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>62</v>
+        <v>354</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B62" t="s">
-        <v>350</v>
+        <v>10</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>351</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B63" t="s">
-        <v>12</v>
+        <v>350</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63" t="s">
-        <v>63</v>
+        <v>351</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B64" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="C64" t="s">
         <v>6</v>
       </c>
       <c r="D64" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B65" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>229</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>306</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B67" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>87</v>
+        <v>291</v>
       </c>
       <c r="B68" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>89</v>
+        <v>307</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B69" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
       </c>
       <c r="D69" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B70" t="s">
-        <v>92</v>
+        <v>34</v>
       </c>
       <c r="C70" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B71" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C71" t="s">
         <v>35</v>
       </c>
       <c r="D71" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B72" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C72" t="s">
         <v>35</v>
       </c>
       <c r="D72" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B73" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C73" t="s">
         <v>35</v>
       </c>
       <c r="D73" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B74" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="C74" t="s">
         <v>35</v>
       </c>
       <c r="D74" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B75" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C75" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D75" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B76" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>170</v>
+        <v>117</v>
       </c>
       <c r="B77" t="s">
-        <v>171</v>
+        <v>23</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>172</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B78" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>292</v>
+        <v>173</v>
       </c>
       <c r="B79" t="s">
-        <v>293</v>
+        <v>174</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>294</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
       <c r="B80" t="s">
-        <v>13</v>
+        <v>293</v>
       </c>
       <c r="C80" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>64</v>
+        <v>294</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B81" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C81" t="s">
         <v>14</v>
       </c>
       <c r="D81" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B82" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C82" t="s">
         <v>14</v>
       </c>
       <c r="D82" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C83" t="s">
         <v>14</v>
       </c>
       <c r="D83" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B84" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C84" t="s">
         <v>14</v>
       </c>
       <c r="D84" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B85" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="C85" t="s">
         <v>14</v>
       </c>
       <c r="D85" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B86" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="C86" t="s">
         <v>14</v>
       </c>
       <c r="D86" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B87" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C87" t="s">
         <v>14</v>
       </c>
       <c r="D87" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B88" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C88" t="s">
         <v>14</v>
       </c>
       <c r="D88" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>124</v>
+        <v>319</v>
       </c>
       <c r="B89" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C89" t="s">
         <v>14</v>
       </c>
       <c r="D89" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B90" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C90" t="s">
         <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B91" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C91" t="s">
         <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B92" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C92" t="s">
         <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B93" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="C93" t="s">
         <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>82</v>
+        <v>133</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
       <c r="B94" t="s">
-        <v>208</v>
+        <v>42</v>
       </c>
       <c r="C94" t="s">
         <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>209</v>
+        <v>82</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>330</v>
+        <v>207</v>
       </c>
       <c r="B95" t="s">
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="C95" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="D95" t="s">
-        <v>116</v>
+        <v>209</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B96" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C96" t="s">
         <v>108</v>
       </c>
       <c r="D96" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B97" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C97" t="s">
         <v>108</v>
       </c>
       <c r="D97" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B98" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C98" t="s">
         <v>108</v>
       </c>
       <c r="D98" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B99" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C99" t="s">
         <v>108</v>
       </c>
       <c r="D99" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B100" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="C100" t="s">
         <v>108</v>
       </c>
       <c r="D100" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B101" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="C101" t="s">
         <v>108</v>
       </c>
       <c r="D101" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B102" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C102" t="s">
         <v>108</v>
       </c>
       <c r="D102" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B103" t="s">
-        <v>339</v>
+        <v>113</v>
       </c>
       <c r="C103" t="s">
         <v>108</v>
       </c>
       <c r="D103" t="s">
-        <v>340</v>
+        <v>22</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B104" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C104" t="s">
         <v>108</v>
       </c>
       <c r="D104" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B105" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C105" t="s">
         <v>108</v>
       </c>
       <c r="D105" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B106" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C106" t="s">
         <v>108</v>
       </c>
       <c r="D106" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>158</v>
+        <v>347</v>
       </c>
       <c r="B107" t="s">
-        <v>159</v>
+        <v>348</v>
       </c>
       <c r="C107" t="s">
-        <v>160</v>
+        <v>108</v>
       </c>
       <c r="D107" t="s">
-        <v>161</v>
-      </c>
-      <c r="E107" t="s">
-        <v>162</v>
+        <v>349</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B108" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C108" t="s">
         <v>160</v>
       </c>
       <c r="D108" t="s">
-        <v>165</v>
+        <v>161</v>
+      </c>
+      <c r="E108" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>230</v>
+        <v>163</v>
       </c>
       <c r="B109" t="s">
-        <v>231</v>
+        <v>164</v>
       </c>
       <c r="C109" t="s">
         <v>160</v>
       </c>
       <c r="D109" t="s">
-        <v>232</v>
+        <v>165</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>274</v>
+        <v>230</v>
       </c>
       <c r="B110" t="s">
-        <v>275</v>
+        <v>231</v>
       </c>
       <c r="C110" t="s">
         <v>160</v>
       </c>
       <c r="D110" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B111" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C111" t="s">
         <v>160</v>
       </c>
       <c r="D111" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B112" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C112" t="s">
         <v>160</v>
       </c>
       <c r="D112" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>308</v>
+        <v>280</v>
       </c>
       <c r="B113" t="s">
-        <v>309</v>
+        <v>281</v>
       </c>
       <c r="C113" t="s">
         <v>160</v>
       </c>
       <c r="D113" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>308</v>
+      </c>
+      <c r="B114" t="s">
+        <v>309</v>
+      </c>
+      <c r="C114" t="s">
+        <v>160</v>
+      </c>
+      <c r="D114" t="s">
         <v>310</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More minor fixes to derived variables
More refining of what gets defined as unknown vs No
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458DBF9E-ED31-FF45-A5C8-632F6F693DE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0479AB50-D4CF-B84A-8E9D-ABD0347DD22E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35940" yWindow="2600" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="364">
   <si>
     <t>Variable #</t>
   </si>
@@ -1089,6 +1089,24 @@
   </si>
   <si>
     <t>Region of patient residence with ex-US collapsed</t>
+  </si>
+  <si>
+    <t>O22</t>
+  </si>
+  <si>
+    <t>ordinal_v1</t>
+  </si>
+  <si>
+    <t>Custom ordinal outcome ignoring oxygen requirement</t>
+  </si>
+  <si>
+    <t>O23</t>
+  </si>
+  <si>
+    <t>ordinal_v2</t>
+  </si>
+  <si>
+    <t>Custom ordinal including need for oxygen</t>
   </si>
 </sst>
 </file>
@@ -1144,10 +1162,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E115" totalsRowShown="0">
-  <autoFilter ref="A1:E115" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E115">
-    <sortCondition ref="A1:A115"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E117" totalsRowShown="0">
+  <autoFilter ref="A1:E117" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E117">
+    <sortCondition ref="A1:A117"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1481,10 +1499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2635,480 +2653,508 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>311</v>
+        <v>358</v>
       </c>
       <c r="B82" t="s">
-        <v>13</v>
+        <v>359</v>
       </c>
       <c r="C82" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>64</v>
+        <v>360</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>312</v>
+        <v>361</v>
       </c>
       <c r="B83" t="s">
-        <v>31</v>
+        <v>362</v>
       </c>
       <c r="C83" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>74</v>
+        <v>363</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B84" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="C84" t="s">
         <v>14</v>
       </c>
       <c r="D84" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B85" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C85" t="s">
         <v>14</v>
       </c>
       <c r="D85" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B86" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C86" t="s">
         <v>14</v>
       </c>
       <c r="D86" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B87" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C87" t="s">
         <v>14</v>
       </c>
       <c r="D87" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B88" t="s">
-        <v>119</v>
+        <v>57</v>
       </c>
       <c r="C88" t="s">
         <v>14</v>
       </c>
       <c r="D88" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B89" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="C89" t="s">
         <v>14</v>
       </c>
       <c r="D89" t="s">
-        <v>121</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B90" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C90" t="s">
         <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>124</v>
+        <v>318</v>
       </c>
       <c r="B91" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C91" t="s">
         <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>128</v>
+        <v>319</v>
       </c>
       <c r="B92" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C92" t="s">
         <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B93" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C93" t="s">
         <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B94" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C94" t="s">
         <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B95" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="C95" t="s">
         <v>14</v>
       </c>
       <c r="D95" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>207</v>
+        <v>135</v>
       </c>
       <c r="B96" t="s">
-        <v>208</v>
+        <v>134</v>
       </c>
       <c r="C96" t="s">
         <v>14</v>
       </c>
       <c r="D96" t="s">
-        <v>209</v>
+        <v>133</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>330</v>
+        <v>136</v>
       </c>
       <c r="B97" t="s">
-        <v>107</v>
+        <v>42</v>
       </c>
       <c r="C97" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="D97" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>331</v>
+        <v>207</v>
       </c>
       <c r="B98" t="s">
-        <v>106</v>
+        <v>208</v>
       </c>
       <c r="C98" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="D98" t="s">
-        <v>22</v>
+        <v>209</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B99" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C99" t="s">
         <v>108</v>
       </c>
       <c r="D99" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B100" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C100" t="s">
         <v>108</v>
       </c>
       <c r="D100" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B101" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C101" t="s">
         <v>108</v>
       </c>
       <c r="D101" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B102" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="C102" t="s">
         <v>108</v>
       </c>
       <c r="D102" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B103" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C103" t="s">
         <v>108</v>
       </c>
       <c r="D103" t="s">
-        <v>114</v>
+        <v>22</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B104" t="s">
-        <v>113</v>
+        <v>32</v>
       </c>
       <c r="C104" t="s">
         <v>108</v>
       </c>
       <c r="D104" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B105" t="s">
-        <v>339</v>
+        <v>112</v>
       </c>
       <c r="C105" t="s">
         <v>108</v>
       </c>
       <c r="D105" t="s">
-        <v>340</v>
+        <v>114</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B106" t="s">
-        <v>342</v>
+        <v>113</v>
       </c>
       <c r="C106" t="s">
         <v>108</v>
       </c>
       <c r="D106" t="s">
-        <v>343</v>
+        <v>22</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B107" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C107" t="s">
         <v>108</v>
       </c>
       <c r="D107" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="B108" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C108" t="s">
         <v>108</v>
       </c>
       <c r="D108" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>158</v>
+        <v>344</v>
       </c>
       <c r="B109" t="s">
-        <v>159</v>
+        <v>345</v>
       </c>
       <c r="C109" t="s">
-        <v>160</v>
+        <v>108</v>
       </c>
       <c r="D109" t="s">
-        <v>161</v>
-      </c>
-      <c r="E109" t="s">
-        <v>162</v>
+        <v>346</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>163</v>
+        <v>347</v>
       </c>
       <c r="B110" t="s">
-        <v>164</v>
+        <v>348</v>
       </c>
       <c r="C110" t="s">
-        <v>160</v>
+        <v>108</v>
       </c>
       <c r="D110" t="s">
-        <v>165</v>
+        <v>349</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>230</v>
+        <v>158</v>
       </c>
       <c r="B111" t="s">
-        <v>231</v>
+        <v>159</v>
       </c>
       <c r="C111" t="s">
         <v>160</v>
       </c>
       <c r="D111" t="s">
-        <v>232</v>
+        <v>161</v>
+      </c>
+      <c r="E111" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>274</v>
+        <v>163</v>
       </c>
       <c r="B112" t="s">
-        <v>275</v>
+        <v>164</v>
       </c>
       <c r="C112" t="s">
         <v>160</v>
       </c>
       <c r="D112" t="s">
-        <v>276</v>
+        <v>165</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>277</v>
+        <v>230</v>
       </c>
       <c r="B113" t="s">
-        <v>278</v>
+        <v>231</v>
       </c>
       <c r="C113" t="s">
         <v>160</v>
       </c>
       <c r="D113" t="s">
-        <v>279</v>
+        <v>232</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B114" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C114" t="s">
         <v>160</v>
       </c>
       <c r="D114" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>308</v>
+        <v>277</v>
       </c>
       <c r="B115" t="s">
-        <v>309</v>
+        <v>278</v>
       </c>
       <c r="C115" t="s">
         <v>160</v>
       </c>
       <c r="D115" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>280</v>
+      </c>
+      <c r="B116" t="s">
+        <v>281</v>
+      </c>
+      <c r="C116" t="s">
+        <v>160</v>
+      </c>
+      <c r="D116" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>308</v>
+      </c>
+      <c r="B117" t="s">
+        <v>309</v>
+      </c>
+      <c r="C117" t="s">
+        <v>160</v>
+      </c>
+      <c r="D117" t="s">
         <v>310</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New derived variable for steroids
Added a new derived variable for ever/never treatment of COVID-19 with steroids, which does not take into consideration dosing (assuming all COVID-19 treatment is high-dose steroids)
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0479AB50-D4CF-B84A-8E9D-ABD0347DD22E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC68F07-DD07-E444-9429-A8F0A5080720}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35940" yWindow="2600" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="367">
   <si>
     <t>Variable #</t>
   </si>
@@ -176,9 +176,6 @@
     <t>hcq</t>
   </si>
   <si>
-    <t>steroids</t>
-  </si>
-  <si>
     <t>Performance Status</t>
   </si>
   <si>
@@ -1107,6 +1104,18 @@
   </si>
   <si>
     <t>Custom ordinal including need for oxygen</t>
+  </si>
+  <si>
+    <t>Rx04a</t>
+  </si>
+  <si>
+    <t>steroids_hd_c19</t>
+  </si>
+  <si>
+    <t>steroids_c19</t>
+  </si>
+  <si>
+    <t>Steroids as COVID-19 treatment ever</t>
   </si>
 </sst>
 </file>
@@ -1162,10 +1171,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E117" totalsRowShown="0">
-  <autoFilter ref="A1:E117" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E117">
-    <sortCondition ref="A1:A117"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E118" totalsRowShown="0">
+  <autoFilter ref="A1:E118" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E118">
+    <sortCondition ref="A1:A118"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1499,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1519,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1533,7 +1542,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -1542,26 +1551,26 @@
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -1570,18 +1579,18 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
@@ -1589,7 +1598,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -1603,21 +1612,21 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
         <v>76</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -1631,150 +1640,150 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" t="s">
         <v>220</v>
-      </c>
-      <c r="B13" t="s">
-        <v>221</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" t="s">
         <v>223</v>
-      </c>
-      <c r="B14" t="s">
-        <v>224</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B15" t="s">
         <v>226</v>
-      </c>
-      <c r="B15" t="s">
-        <v>227</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" t="s">
         <v>213</v>
-      </c>
-      <c r="B16" t="s">
-        <v>214</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" t="s">
         <v>235</v>
-      </c>
-      <c r="B17" t="s">
-        <v>236</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18" t="s">
         <v>238</v>
-      </c>
-      <c r="B18" t="s">
-        <v>239</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1785,7 +1794,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B20" t="s">
         <v>46</v>
@@ -1799,21 +1808,21 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
@@ -1822,40 +1831,40 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
@@ -1864,12 +1873,12 @@
         <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
@@ -1883,7 +1892,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B27" t="s">
         <v>50</v>
@@ -1897,21 +1906,21 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B29" t="s">
         <v>40</v>
@@ -1920,12 +1929,12 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B30" t="s">
         <v>41</v>
@@ -1934,12 +1943,12 @@
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B31" t="s">
         <v>43</v>
@@ -1948,12 +1957,12 @@
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B32" t="s">
         <v>44</v>
@@ -1962,26 +1971,26 @@
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
@@ -1995,357 +2004,357 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>354</v>
+      </c>
+      <c r="B35" t="s">
         <v>355</v>
-      </c>
-      <c r="B35" t="s">
-        <v>356</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" t="s">
         <v>146</v>
-      </c>
-      <c r="B36" t="s">
-        <v>147</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" t="s">
         <v>149</v>
-      </c>
-      <c r="B37" t="s">
-        <v>150</v>
       </c>
       <c r="C37" t="s">
         <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" t="s">
         <v>152</v>
-      </c>
-      <c r="B38" t="s">
-        <v>153</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>179</v>
+      </c>
+      <c r="B39" t="s">
         <v>180</v>
-      </c>
-      <c r="B39" t="s">
-        <v>181</v>
       </c>
       <c r="C39" t="s">
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>203</v>
+      </c>
+      <c r="B40" t="s">
         <v>204</v>
-      </c>
-      <c r="B40" t="s">
-        <v>205</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>209</v>
+      </c>
+      <c r="B41" t="s">
         <v>210</v>
-      </c>
-      <c r="B41" t="s">
-        <v>211</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B42" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" t="s">
         <v>176</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>177</v>
-      </c>
-      <c r="D42" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B43" t="s">
+        <v>184</v>
+      </c>
+      <c r="C43" t="s">
+        <v>176</v>
+      </c>
+      <c r="D43" t="s">
         <v>185</v>
-      </c>
-      <c r="C43" t="s">
-        <v>177</v>
-      </c>
-      <c r="D43" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B44" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" t="s">
+        <v>176</v>
+      </c>
+      <c r="D44" t="s">
         <v>187</v>
-      </c>
-      <c r="C44" t="s">
-        <v>177</v>
-      </c>
-      <c r="D44" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B46" t="s">
+        <v>190</v>
+      </c>
+      <c r="C46" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" t="s">
         <v>191</v>
-      </c>
-      <c r="C46" t="s">
-        <v>177</v>
-      </c>
-      <c r="D46" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B47" t="s">
+        <v>192</v>
+      </c>
+      <c r="C47" t="s">
+        <v>176</v>
+      </c>
+      <c r="D47" t="s">
         <v>193</v>
-      </c>
-      <c r="C47" t="s">
-        <v>177</v>
-      </c>
-      <c r="D47" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B48" t="s">
+        <v>194</v>
+      </c>
+      <c r="C48" t="s">
+        <v>176</v>
+      </c>
+      <c r="D48" t="s">
         <v>195</v>
-      </c>
-      <c r="C48" t="s">
-        <v>177</v>
-      </c>
-      <c r="D48" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B49" t="s">
+        <v>196</v>
+      </c>
+      <c r="C49" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" t="s">
         <v>197</v>
-      </c>
-      <c r="C49" t="s">
-        <v>177</v>
-      </c>
-      <c r="D49" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B50" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" t="s">
+        <v>176</v>
+      </c>
+      <c r="D50" t="s">
         <v>199</v>
-      </c>
-      <c r="C50" t="s">
-        <v>177</v>
-      </c>
-      <c r="D50" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>200</v>
+      </c>
+      <c r="B51" t="s">
         <v>201</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
+        <v>176</v>
+      </c>
+      <c r="D51" t="s">
         <v>202</v>
-      </c>
-      <c r="C51" t="s">
-        <v>177</v>
-      </c>
-      <c r="D51" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B52" t="s">
+        <v>244</v>
+      </c>
+      <c r="C52" t="s">
+        <v>176</v>
+      </c>
+      <c r="D52" t="s">
         <v>245</v>
-      </c>
-      <c r="C52" t="s">
-        <v>177</v>
-      </c>
-      <c r="D52" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>246</v>
+      </c>
+      <c r="B53" t="s">
         <v>247</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
+        <v>176</v>
+      </c>
+      <c r="D53" t="s">
         <v>248</v>
-      </c>
-      <c r="C53" t="s">
-        <v>177</v>
-      </c>
-      <c r="D53" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>249</v>
+      </c>
+      <c r="B54" t="s">
         <v>250</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
+        <v>176</v>
+      </c>
+      <c r="D54" t="s">
         <v>251</v>
-      </c>
-      <c r="C54" t="s">
-        <v>177</v>
-      </c>
-      <c r="D54" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>252</v>
+      </c>
+      <c r="B55" t="s">
         <v>253</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
+        <v>176</v>
+      </c>
+      <c r="D55" t="s">
         <v>254</v>
-      </c>
-      <c r="C55" t="s">
-        <v>177</v>
-      </c>
-      <c r="D55" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>255</v>
+      </c>
+      <c r="B56" t="s">
         <v>256</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>176</v>
+      </c>
+      <c r="D56" t="s">
         <v>257</v>
-      </c>
-      <c r="C56" t="s">
-        <v>177</v>
-      </c>
-      <c r="D56" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>258</v>
+      </c>
+      <c r="B57" t="s">
         <v>259</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" t="s">
         <v>260</v>
-      </c>
-      <c r="C57" t="s">
-        <v>177</v>
-      </c>
-      <c r="D57" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B58" t="s">
+        <v>241</v>
+      </c>
+      <c r="C58" t="s">
+        <v>176</v>
+      </c>
+      <c r="D58" t="s">
         <v>242</v>
-      </c>
-      <c r="C58" t="s">
-        <v>177</v>
-      </c>
-      <c r="D58" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>270</v>
+      </c>
+      <c r="B59" t="s">
         <v>271</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>176</v>
+      </c>
+      <c r="D59" t="s">
         <v>272</v>
-      </c>
-      <c r="C59" t="s">
-        <v>177</v>
-      </c>
-      <c r="D59" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B60" t="s">
         <v>4</v>
@@ -2354,12 +2363,12 @@
         <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B61" t="s">
         <v>11</v>
@@ -2368,26 +2377,26 @@
         <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>351</v>
+      </c>
+      <c r="B62" t="s">
         <v>352</v>
-      </c>
-      <c r="B62" t="s">
-        <v>353</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
@@ -2396,26 +2405,26 @@
         <v>6</v>
       </c>
       <c r="D63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B64" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C64" t="s">
         <v>6</v>
       </c>
       <c r="D64" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B65" t="s">
         <v>12</v>
@@ -2424,26 +2433,26 @@
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B67" t="s">
         <v>27</v>
@@ -2452,12 +2461,12 @@
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B68" t="s">
         <v>28</v>
@@ -2466,12 +2475,12 @@
         <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B69" t="s">
         <v>49</v>
@@ -2480,26 +2489,26 @@
         <v>6</v>
       </c>
       <c r="D69" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70" t="s">
         <v>87</v>
-      </c>
-      <c r="B70" t="s">
-        <v>88</v>
       </c>
       <c r="C70" t="s">
         <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B71" t="s">
         <v>34</v>
@@ -2508,68 +2517,68 @@
         <v>6</v>
       </c>
       <c r="D71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>90</v>
+      </c>
+      <c r="B72" t="s">
         <v>91</v>
-      </c>
-      <c r="B72" t="s">
-        <v>92</v>
       </c>
       <c r="C72" t="s">
         <v>35</v>
       </c>
       <c r="D72" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" t="s">
         <v>93</v>
-      </c>
-      <c r="B73" t="s">
-        <v>94</v>
       </c>
       <c r="C73" t="s">
         <v>35</v>
       </c>
       <c r="D73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" t="s">
         <v>95</v>
-      </c>
-      <c r="B74" t="s">
-        <v>96</v>
       </c>
       <c r="C74" t="s">
         <v>35</v>
       </c>
       <c r="D74" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>96</v>
+      </c>
+      <c r="B75" t="s">
         <v>97</v>
-      </c>
-      <c r="B75" t="s">
-        <v>98</v>
       </c>
       <c r="C75" t="s">
         <v>35</v>
       </c>
       <c r="D75" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B76" t="s">
         <v>39</v>
@@ -2578,26 +2587,26 @@
         <v>35</v>
       </c>
       <c r="D76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B78" t="s">
         <v>23</v>
@@ -2606,82 +2615,82 @@
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>169</v>
+      </c>
+      <c r="B79" t="s">
         <v>170</v>
-      </c>
-      <c r="B79" t="s">
-        <v>171</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>172</v>
+      </c>
+      <c r="B80" t="s">
         <v>173</v>
-      </c>
-      <c r="B80" t="s">
-        <v>174</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>291</v>
+      </c>
+      <c r="B81" t="s">
         <v>292</v>
-      </c>
-      <c r="B81" t="s">
-        <v>293</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>357</v>
+      </c>
+      <c r="B82" t="s">
         <v>358</v>
-      </c>
-      <c r="B82" t="s">
-        <v>359</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>360</v>
+      </c>
+      <c r="B83" t="s">
         <v>361</v>
-      </c>
-      <c r="B83" t="s">
-        <v>362</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B84" t="s">
         <v>13</v>
@@ -2690,12 +2699,12 @@
         <v>14</v>
       </c>
       <c r="D84" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B85" t="s">
         <v>31</v>
@@ -2704,12 +2713,12 @@
         <v>14</v>
       </c>
       <c r="D85" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B86" t="s">
         <v>52</v>
@@ -2718,43 +2727,43 @@
         <v>14</v>
       </c>
       <c r="D86" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B87" t="s">
-        <v>53</v>
+        <v>364</v>
       </c>
       <c r="C87" t="s">
         <v>14</v>
       </c>
       <c r="D87" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>315</v>
+        <v>363</v>
       </c>
       <c r="B88" t="s">
-        <v>57</v>
+        <v>365</v>
       </c>
       <c r="C88" t="s">
         <v>14</v>
       </c>
       <c r="D88" t="s">
-        <v>80</v>
+        <v>366</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B89" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C89" t="s">
         <v>14</v>
@@ -2765,397 +2774,411 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B90" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="C90" t="s">
         <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B91" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C91" t="s">
         <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B92" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C92" t="s">
         <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>124</v>
+        <v>318</v>
       </c>
       <c r="B93" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C93" t="s">
         <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C94" t="s">
         <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B95" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C95" t="s">
         <v>14</v>
       </c>
       <c r="D95" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B96" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C96" t="s">
         <v>14</v>
       </c>
       <c r="D96" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B97" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="C97" t="s">
         <v>14</v>
       </c>
       <c r="D97" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>207</v>
+        <v>135</v>
       </c>
       <c r="B98" t="s">
-        <v>208</v>
+        <v>42</v>
       </c>
       <c r="C98" t="s">
         <v>14</v>
       </c>
       <c r="D98" t="s">
-        <v>209</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>330</v>
+        <v>206</v>
       </c>
       <c r="B99" t="s">
-        <v>107</v>
+        <v>207</v>
       </c>
       <c r="C99" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>116</v>
+        <v>208</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B100" t="s">
         <v>106</v>
       </c>
       <c r="C100" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D100" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B101" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C101" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D101" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B102" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C102" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D102" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B103" t="s">
         <v>110</v>
       </c>
       <c r="C103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D103" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B104" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="C104" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D104" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B105" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="C105" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D105" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B106" t="s">
+        <v>111</v>
+      </c>
+      <c r="C106" t="s">
+        <v>107</v>
+      </c>
+      <c r="D106" t="s">
         <v>113</v>
-      </c>
-      <c r="C106" t="s">
-        <v>108</v>
-      </c>
-      <c r="D106" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B107" t="s">
-        <v>339</v>
+        <v>112</v>
       </c>
       <c r="C107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D107" t="s">
-        <v>340</v>
+        <v>22</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B108" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C108" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D108" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B109" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D109" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B110" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C110" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D110" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>158</v>
+        <v>346</v>
       </c>
       <c r="B111" t="s">
-        <v>159</v>
+        <v>347</v>
       </c>
       <c r="C111" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="D111" t="s">
-        <v>161</v>
-      </c>
-      <c r="E111" t="s">
-        <v>162</v>
+        <v>348</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B112" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C112" t="s">
+        <v>159</v>
+      </c>
+      <c r="D112" t="s">
         <v>160</v>
       </c>
-      <c r="D112" t="s">
-        <v>165</v>
+      <c r="E112" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>230</v>
+        <v>162</v>
       </c>
       <c r="B113" t="s">
-        <v>231</v>
+        <v>163</v>
       </c>
       <c r="C113" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D113" t="s">
-        <v>232</v>
+        <v>164</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>274</v>
+        <v>229</v>
       </c>
       <c r="B114" t="s">
-        <v>275</v>
+        <v>230</v>
       </c>
       <c r="C114" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D114" t="s">
-        <v>276</v>
+        <v>231</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B115" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C115" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D115" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B116" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C116" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D116" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>279</v>
+      </c>
+      <c r="B117" t="s">
+        <v>280</v>
+      </c>
+      <c r="C117" t="s">
+        <v>159</v>
+      </c>
+      <c r="D117" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>307</v>
+      </c>
+      <c r="B118" t="s">
         <v>308</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C118" t="s">
+        <v>159</v>
+      </c>
+      <c r="D118" t="s">
         <v>309</v>
-      </c>
-      <c r="C117" t="s">
-        <v>160</v>
-      </c>
-      <c r="D117" t="s">
-        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor fixes and new variables
1. Fixed time anchor referent from ts_3 to ts_2
2. Added a quarter anchor variant
3. Added an other COVID-19 treatment variant
4. Fixed the diabetes derived variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC68F07-DD07-E444-9429-A8F0A5080720}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BE8F27-495A-F648-80E2-90F8D9B26355}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35940" yWindow="2600" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="3860" windowWidth="45100" windowHeight="23380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="370">
   <si>
     <t>Variable #</t>
   </si>
@@ -1116,6 +1116,15 @@
   </si>
   <si>
     <t>Steroids as COVID-19 treatment ever</t>
+  </si>
+  <si>
+    <t>T10a</t>
+  </si>
+  <si>
+    <t>Quarter and year of diagnosis, using the median of the inteval as anchor</t>
+  </si>
+  <si>
+    <t>quarter_median_dx</t>
   </si>
 </sst>
 </file>
@@ -1171,10 +1180,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E118" totalsRowShown="0">
-  <autoFilter ref="A1:E118" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E118">
-    <sortCondition ref="A1:A118"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E119" totalsRowShown="0">
+  <autoFilter ref="A1:E119" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E119">
+    <sortCondition ref="A1:A119"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1508,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2870,7 +2879,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>134</v>
       </c>
@@ -2884,7 +2893,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>135</v>
       </c>
@@ -2898,7 +2907,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>206</v>
       </c>
@@ -2912,7 +2921,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>329</v>
       </c>
@@ -2926,7 +2935,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>330</v>
       </c>
@@ -2940,7 +2949,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>331</v>
       </c>
@@ -2954,7 +2963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>332</v>
       </c>
@@ -2968,7 +2977,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>333</v>
       </c>
@@ -2982,7 +2991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>334</v>
       </c>
@@ -2996,7 +3005,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>335</v>
       </c>
@@ -3010,7 +3019,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>336</v>
       </c>
@@ -3024,7 +3033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>337</v>
       </c>
@@ -3038,7 +3047,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>340</v>
       </c>
@@ -3052,132 +3061,146 @@
         <v>342</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>343</v>
+        <v>367</v>
       </c>
       <c r="B110" t="s">
-        <v>344</v>
+        <v>369</v>
       </c>
       <c r="C110" t="s">
         <v>107</v>
       </c>
       <c r="D110" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B111" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C111" t="s">
         <v>107</v>
       </c>
       <c r="D111" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>346</v>
+      </c>
+      <c r="B112" t="s">
+        <v>347</v>
+      </c>
+      <c r="C112" t="s">
+        <v>107</v>
+      </c>
+      <c r="D112" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>157</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>158</v>
-      </c>
-      <c r="C112" t="s">
-        <v>159</v>
-      </c>
-      <c r="D112" t="s">
-        <v>160</v>
-      </c>
-      <c r="E112" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>162</v>
-      </c>
-      <c r="B113" t="s">
-        <v>163</v>
       </c>
       <c r="C113" t="s">
         <v>159</v>
       </c>
       <c r="D113" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="E113" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>229</v>
+        <v>162</v>
       </c>
       <c r="B114" t="s">
-        <v>230</v>
+        <v>163</v>
       </c>
       <c r="C114" t="s">
         <v>159</v>
       </c>
       <c r="D114" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>273</v>
+        <v>229</v>
       </c>
       <c r="B115" t="s">
-        <v>274</v>
+        <v>230</v>
       </c>
       <c r="C115" t="s">
         <v>159</v>
       </c>
       <c r="D115" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B116" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C116" t="s">
         <v>159</v>
       </c>
       <c r="D116" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B117" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C117" t="s">
         <v>159</v>
       </c>
       <c r="D117" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>307</v>
+        <v>279</v>
       </c>
       <c r="B118" t="s">
-        <v>308</v>
+        <v>280</v>
       </c>
       <c r="C118" t="s">
         <v>159</v>
       </c>
       <c r="D118" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>307</v>
+      </c>
+      <c r="B119" t="s">
+        <v>308</v>
+      </c>
+      <c r="C119" t="s">
+        <v>159</v>
+      </c>
+      <c r="D119" t="s">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rearranged comorbidites into their own section
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BE8F27-495A-F648-80E2-90F8D9B26355}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D015D4B5-515C-DB4B-8C8E-A47F7CC5052A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="3860" windowWidth="45100" windowHeight="23380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45220" yWindow="2200" windowWidth="45100" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="379">
   <si>
     <t>Variable #</t>
   </si>
@@ -434,21 +434,9 @@
     <t>obesity</t>
   </si>
   <si>
-    <t>D10</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
-    <t>D12</t>
-  </si>
-  <si>
     <t>Cardiovascular comorbidity (CAD, CHF, Afib, arrhythmia NOS, PVD, CVA, cardiac disease NOS)</t>
   </si>
   <si>
-    <t>D13</t>
-  </si>
-  <si>
     <t>D14</t>
   </si>
   <si>
@@ -461,9 +449,6 @@
     <t>US Census Division</t>
   </si>
   <si>
-    <t>D16</t>
-  </si>
-  <si>
     <t>htn</t>
   </si>
   <si>
@@ -644,9 +629,6 @@
     <t>Baseline anticoagulation, aspirin, or APA</t>
   </si>
   <si>
-    <t>D20</t>
-  </si>
-  <si>
     <t>dementia</t>
   </si>
   <si>
@@ -914,24 +896,9 @@
     <t>D04a</t>
   </si>
   <si>
-    <t>D05</t>
-  </si>
-  <si>
     <t>D06</t>
   </si>
   <si>
-    <t>D07</t>
-  </si>
-  <si>
-    <t>D08</t>
-  </si>
-  <si>
-    <t>D08b</t>
-  </si>
-  <si>
-    <t>D09</t>
-  </si>
-  <si>
     <t>Indicates severe composite outcome (no severe hosp)</t>
   </si>
   <si>
@@ -1125,6 +1092,66 @@
   </si>
   <si>
     <t>quarter_median_dx</t>
+  </si>
+  <si>
+    <t>Rx07a</t>
+  </si>
+  <si>
+    <t>other_tx_c19_v2</t>
+  </si>
+  <si>
+    <t>COVID-19 treatments other than HCQ, steroids, remdesivir</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>Derived variable including calculation of BMI from height/weight</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>C03a</t>
+  </si>
+  <si>
+    <t>C03b</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>comorbid_combined</t>
+  </si>
+  <si>
+    <t>Combined CV, pulm, renal, DM2, and 1+ of these</t>
   </si>
 </sst>
 </file>
@@ -1180,10 +1207,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E119" totalsRowShown="0">
-  <autoFilter ref="A1:E119" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E119">
-    <sortCondition ref="A1:A119"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E122" totalsRowShown="0">
+  <autoFilter ref="A1:E122" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E122">
+    <sortCondition ref="A1:A122"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1517,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1551,7 +1578,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -1565,21 +1592,21 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -1588,12 +1615,12 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -1607,7 +1634,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -1621,7 +1648,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
@@ -1635,7 +1662,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -1649,10 +1676,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -1663,133 +1690,133 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B13" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B14" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B15" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B18" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B19" t="s">
         <v>136</v>
@@ -1803,7 +1830,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B20" t="s">
         <v>46</v>
@@ -1817,7 +1844,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B21" t="s">
         <v>137</v>
@@ -1826,12 +1853,12 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
@@ -1845,21 +1872,21 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B23" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>299</v>
+        <v>362</v>
       </c>
       <c r="B24" t="s">
         <v>138</v>
@@ -1873,1116 +1900,1116 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>300</v>
+        <v>363</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>364</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>365</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>302</v>
+        <v>366</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
         <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>303</v>
+        <v>367</v>
       </c>
       <c r="B28" t="s">
-        <v>217</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>218</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>304</v>
+        <v>368</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>211</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>139</v>
+        <v>369</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>140</v>
+        <v>370</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>141</v>
+        <v>371</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>143</v>
+        <v>372</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>144</v>
+        <v>373</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>354</v>
+        <v>140</v>
       </c>
       <c r="B35" t="s">
-        <v>355</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>356</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>343</v>
       </c>
       <c r="B36" t="s">
-        <v>146</v>
+        <v>344</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>147</v>
+        <v>345</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>374</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="B40" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B41" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>261</v>
+        <v>375</v>
       </c>
       <c r="B42" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="C42" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="D42" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>262</v>
+        <v>376</v>
       </c>
       <c r="B43" t="s">
-        <v>184</v>
+        <v>377</v>
       </c>
       <c r="C43" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>185</v>
+        <v>378</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B44" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C44" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D44" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B45" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C45" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D45" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B46" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C46" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D46" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B47" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C47" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B48" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C48" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D48" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B49" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C49" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D49" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B50" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C50" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D50" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>200</v>
+        <v>262</v>
       </c>
       <c r="B51" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C51" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D51" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>240</v>
+        <v>263</v>
       </c>
       <c r="B52" t="s">
-        <v>244</v>
+        <v>193</v>
       </c>
       <c r="C52" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D52" t="s">
-        <v>245</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>246</v>
+        <v>195</v>
       </c>
       <c r="B53" t="s">
-        <v>247</v>
+        <v>196</v>
       </c>
       <c r="C53" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D53" t="s">
-        <v>248</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="B54" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="C54" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D54" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="B55" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="C55" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D55" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B56" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="C56" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D56" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="B57" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="C57" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D57" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B58" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="C58" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D58" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="B59" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="C59" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D59" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>235</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D60" t="s">
-        <v>59</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>265</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D61" t="s">
-        <v>60</v>
+        <v>266</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>351</v>
+        <v>276</v>
       </c>
       <c r="B62" t="s">
-        <v>352</v>
+        <v>4</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>353</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>285</v>
+        <v>340</v>
       </c>
       <c r="B64" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="C64" t="s">
         <v>6</v>
       </c>
       <c r="D64" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B65" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>338</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>85</v>
+        <v>339</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>228</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>305</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B69" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
       </c>
       <c r="D69" t="s">
-        <v>306</v>
+        <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>283</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="C70" t="s">
         <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>88</v>
+        <v>294</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>284</v>
       </c>
       <c r="B71" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C71" t="s">
         <v>6</v>
       </c>
       <c r="D71" t="s">
-        <v>74</v>
+        <v>295</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C72" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D72" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="C73" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D73" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B74" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C74" t="s">
         <v>35</v>
       </c>
       <c r="D74" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B75" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C75" t="s">
         <v>35</v>
       </c>
       <c r="D75" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B76" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="C76" t="s">
         <v>35</v>
       </c>
       <c r="D76" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B77" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D77" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D78" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>169</v>
+        <v>104</v>
       </c>
       <c r="B79" t="s">
-        <v>170</v>
+        <v>54</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>171</v>
+        <v>55</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="B80" t="s">
-        <v>173</v>
+        <v>23</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>174</v>
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>291</v>
+        <v>164</v>
       </c>
       <c r="B81" t="s">
-        <v>292</v>
+        <v>165</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>293</v>
+        <v>166</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>357</v>
+        <v>167</v>
       </c>
       <c r="B82" t="s">
-        <v>358</v>
+        <v>168</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>359</v>
+        <v>169</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>360</v>
+        <v>285</v>
       </c>
       <c r="B83" t="s">
-        <v>361</v>
+        <v>286</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>310</v>
+        <v>346</v>
       </c>
       <c r="B84" t="s">
-        <v>13</v>
+        <v>347</v>
       </c>
       <c r="C84" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>63</v>
+        <v>348</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>311</v>
+        <v>349</v>
       </c>
       <c r="B85" t="s">
-        <v>31</v>
+        <v>350</v>
       </c>
       <c r="C85" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>73</v>
+        <v>351</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="B86" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="C86" t="s">
         <v>14</v>
       </c>
       <c r="D86" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="B87" t="s">
-        <v>364</v>
+        <v>31</v>
       </c>
       <c r="C87" t="s">
         <v>14</v>
       </c>
       <c r="D87" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>363</v>
+        <v>301</v>
       </c>
       <c r="B88" t="s">
-        <v>365</v>
+        <v>52</v>
       </c>
       <c r="C88" t="s">
         <v>14</v>
       </c>
       <c r="D88" t="s">
-        <v>366</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="B89" t="s">
-        <v>56</v>
+        <v>353</v>
       </c>
       <c r="C89" t="s">
         <v>14</v>
       </c>
       <c r="D89" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>315</v>
+        <v>352</v>
       </c>
       <c r="B90" t="s">
-        <v>77</v>
+        <v>354</v>
       </c>
       <c r="C90" t="s">
         <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>78</v>
+        <v>355</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="B91" t="s">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="C91" t="s">
         <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="B92" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="C92" t="s">
         <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="B93" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C93" t="s">
         <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>123</v>
+        <v>359</v>
       </c>
       <c r="B94" t="s">
-        <v>124</v>
+        <v>360</v>
       </c>
       <c r="C94" t="s">
         <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>125</v>
+        <v>361</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>127</v>
+        <v>306</v>
       </c>
       <c r="B95" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C95" t="s">
         <v>14</v>
       </c>
       <c r="D95" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>130</v>
+        <v>307</v>
       </c>
       <c r="B96" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C96" t="s">
         <v>14</v>
       </c>
       <c r="D96" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B97" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C97" t="s">
         <v>14</v>
       </c>
       <c r="D97" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B98" t="s">
-        <v>42</v>
+        <v>128</v>
       </c>
       <c r="C98" t="s">
         <v>14</v>
       </c>
       <c r="D98" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>206</v>
+        <v>130</v>
       </c>
       <c r="B99" t="s">
-        <v>207</v>
+        <v>131</v>
       </c>
       <c r="C99" t="s">
         <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>208</v>
+        <v>129</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>329</v>
+        <v>134</v>
       </c>
       <c r="B100" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="C100" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="D100" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>330</v>
+        <v>135</v>
       </c>
       <c r="B101" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="C101" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="D101" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>331</v>
+        <v>201</v>
       </c>
       <c r="B102" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="C102" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>24</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="B103" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C103" t="s">
         <v>107</v>
       </c>
       <c r="D103" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="B104" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C104" t="s">
         <v>107</v>
@@ -2993,38 +3020,38 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="B105" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="C105" t="s">
         <v>107</v>
       </c>
       <c r="D105" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="B106" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C106" t="s">
         <v>107</v>
       </c>
       <c r="D106" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="B107" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C107" t="s">
         <v>107</v>
@@ -3035,173 +3062,215 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="B108" t="s">
-        <v>338</v>
+        <v>32</v>
       </c>
       <c r="C108" t="s">
         <v>107</v>
       </c>
       <c r="D108" t="s">
-        <v>339</v>
+        <v>33</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="B109" t="s">
-        <v>341</v>
+        <v>111</v>
       </c>
       <c r="C109" t="s">
         <v>107</v>
       </c>
       <c r="D109" t="s">
-        <v>342</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>367</v>
+        <v>325</v>
       </c>
       <c r="B110" t="s">
-        <v>369</v>
+        <v>112</v>
       </c>
       <c r="C110" t="s">
         <v>107</v>
       </c>
       <c r="D110" t="s">
-        <v>368</v>
+        <v>22</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="B111" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="C111" t="s">
         <v>107</v>
       </c>
       <c r="D111" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="B112" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="C112" t="s">
         <v>107</v>
       </c>
       <c r="D112" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>157</v>
+        <v>356</v>
       </c>
       <c r="B113" t="s">
-        <v>158</v>
+        <v>358</v>
       </c>
       <c r="C113" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
       <c r="D113" t="s">
-        <v>160</v>
-      </c>
-      <c r="E113" t="s">
-        <v>161</v>
+        <v>357</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>162</v>
+        <v>332</v>
       </c>
       <c r="B114" t="s">
-        <v>163</v>
+        <v>333</v>
       </c>
       <c r="C114" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
       <c r="D114" t="s">
-        <v>164</v>
+        <v>334</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>229</v>
+        <v>335</v>
       </c>
       <c r="B115" t="s">
-        <v>230</v>
+        <v>336</v>
       </c>
       <c r="C115" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
       <c r="D115" t="s">
-        <v>231</v>
+        <v>337</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>273</v>
+        <v>152</v>
       </c>
       <c r="B116" t="s">
-        <v>274</v>
+        <v>153</v>
       </c>
       <c r="C116" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D116" t="s">
-        <v>275</v>
+        <v>155</v>
+      </c>
+      <c r="E116" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>276</v>
+        <v>157</v>
       </c>
       <c r="B117" t="s">
-        <v>277</v>
+        <v>158</v>
       </c>
       <c r="C117" t="s">
+        <v>154</v>
+      </c>
+      <c r="D117" t="s">
         <v>159</v>
-      </c>
-      <c r="D117" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>279</v>
+        <v>223</v>
       </c>
       <c r="B118" t="s">
-        <v>280</v>
+        <v>224</v>
       </c>
       <c r="C118" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D118" t="s">
-        <v>281</v>
+        <v>225</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>307</v>
+        <v>267</v>
       </c>
       <c r="B119" t="s">
-        <v>308</v>
+        <v>268</v>
       </c>
       <c r="C119" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D119" t="s">
-        <v>309</v>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>270</v>
+      </c>
+      <c r="B120" t="s">
+        <v>271</v>
+      </c>
+      <c r="C120" t="s">
+        <v>154</v>
+      </c>
+      <c r="D120" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>273</v>
+      </c>
+      <c r="B121" t="s">
+        <v>274</v>
+      </c>
+      <c r="C121" t="s">
+        <v>154</v>
+      </c>
+      <c r="D121" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>296</v>
+      </c>
+      <c r="B122" t="s">
+        <v>297</v>
+      </c>
+      <c r="C122" t="s">
+        <v>154</v>
+      </c>
+      <c r="D122" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add variant of cancer status derived variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90969F22-6FC5-C544-93D8-A45EF5C6BD09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67370C04-7C83-BA4D-9145-F057293467A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-49680" yWindow="1440" windowWidth="45100" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="406">
   <si>
     <t>Variable #</t>
   </si>
@@ -1224,6 +1224,15 @@
   </si>
   <si>
     <t>T13</t>
+  </si>
+  <si>
+    <t>Ca07a</t>
+  </si>
+  <si>
+    <t>cancer_status_v2</t>
+  </si>
+  <si>
+    <t>Same as Ca07 except do not combine stable and responding</t>
   </si>
 </sst>
 </file>
@@ -1279,10 +1288,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E130" totalsRowShown="0">
-  <autoFilter ref="A1:E130" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E130">
-    <sortCondition ref="A1:A130"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E131" totalsRowShown="0">
+  <autoFilter ref="A1:E131" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E131">
+    <sortCondition ref="A1:A131"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1616,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1972,1488 +1981,1502 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>314</v>
+        <v>403</v>
       </c>
       <c r="B25" t="s">
-        <v>160</v>
+        <v>404</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>162</v>
+        <v>405</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>173</v>
+        <v>315</v>
       </c>
       <c r="B27" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>213</v>
+        <v>173</v>
       </c>
       <c r="B28" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B29" t="s">
-        <v>388</v>
+        <v>214</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>394</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B30" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>384</v>
+        <v>219</v>
       </c>
       <c r="B31" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B32" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B33" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B34" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="B35" t="s">
-        <v>217</v>
+        <v>393</v>
       </c>
       <c r="C35" t="s">
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>218</v>
+        <v>398</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B36" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>206</v>
+        <v>383</v>
       </c>
       <c r="B37" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="B38" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B39" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>402</v>
+        <v>230</v>
       </c>
       <c r="B40" t="s">
-        <v>400</v>
+        <v>231</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>401</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>286</v>
+        <v>402</v>
       </c>
       <c r="B41" t="s">
-        <v>136</v>
+        <v>400</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>48</v>
+        <v>401</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>150</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B45" t="s">
-        <v>209</v>
+        <v>17</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>210</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>209</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>67</v>
+        <v>210</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>140</v>
+        <v>291</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>341</v>
+        <v>140</v>
       </c>
       <c r="B48" t="s">
-        <v>342</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>343</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>141</v>
+        <v>341</v>
       </c>
       <c r="B49" t="s">
-        <v>142</v>
+        <v>342</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
+        <v>343</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="B51" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="C51" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B52" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>254</v>
+        <v>198</v>
       </c>
       <c r="B53" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="C53" t="s">
-        <v>171</v>
+        <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C54" t="s">
         <v>171</v>
       </c>
       <c r="D54" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B55" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C55" t="s">
         <v>171</v>
       </c>
       <c r="D55" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B56" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C56" t="s">
         <v>171</v>
       </c>
       <c r="D56" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C57" t="s">
         <v>171</v>
       </c>
       <c r="D57" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B58" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C58" t="s">
         <v>171</v>
       </c>
       <c r="D58" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B59" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C59" t="s">
         <v>171</v>
       </c>
       <c r="D59" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B60" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C60" t="s">
         <v>171</v>
       </c>
       <c r="D60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B61" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C61" t="s">
         <v>171</v>
       </c>
       <c r="D61" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>195</v>
+        <v>262</v>
       </c>
       <c r="B62" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C62" t="s">
         <v>171</v>
       </c>
       <c r="D62" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>233</v>
+        <v>195</v>
       </c>
       <c r="B63" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="C63" t="s">
         <v>171</v>
       </c>
       <c r="D63" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B64" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C64" t="s">
         <v>171</v>
       </c>
       <c r="D64" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B65" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C65" t="s">
         <v>171</v>
       </c>
       <c r="D65" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B66" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C66" t="s">
         <v>171</v>
       </c>
       <c r="D66" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B67" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C67" t="s">
         <v>171</v>
       </c>
       <c r="D67" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B68" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C68" t="s">
         <v>171</v>
       </c>
       <c r="D68" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="B69" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="C69" t="s">
         <v>171</v>
       </c>
       <c r="D69" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
       <c r="B70" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="C70" t="s">
         <v>171</v>
       </c>
       <c r="D70" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>264</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>59</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B72" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C72" t="s">
         <v>6</v>
       </c>
       <c r="D72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>338</v>
+        <v>275</v>
       </c>
       <c r="B73" t="s">
-        <v>339</v>
+        <v>11</v>
       </c>
       <c r="C73" t="s">
         <v>6</v>
       </c>
       <c r="D73" t="s">
-        <v>340</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>276</v>
+        <v>338</v>
       </c>
       <c r="B74" t="s">
-        <v>10</v>
+        <v>339</v>
       </c>
       <c r="C74" t="s">
         <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>61</v>
+        <v>340</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B75" t="s">
-        <v>336</v>
+        <v>10</v>
       </c>
       <c r="C75" t="s">
         <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>337</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
+        <v>336</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>62</v>
+        <v>337</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B77" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B78" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>222</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B79" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>292</v>
+        <v>222</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B80" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>86</v>
+        <v>282</v>
       </c>
       <c r="B81" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>88</v>
+        <v>293</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B83" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="C83" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C84" t="s">
         <v>35</v>
       </c>
       <c r="D84" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B85" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C85" t="s">
         <v>35</v>
       </c>
       <c r="D85" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B86" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C86" t="s">
         <v>35</v>
       </c>
       <c r="D86" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B87" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="C87" t="s">
         <v>35</v>
       </c>
       <c r="D87" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B88" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C88" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D88" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B89" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C89" t="s">
         <v>6</v>
       </c>
       <c r="D89" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
       <c r="B90" t="s">
-        <v>165</v>
+        <v>23</v>
       </c>
       <c r="C90" t="s">
         <v>6</v>
       </c>
       <c r="D90" t="s">
-        <v>166</v>
+        <v>68</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B91" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C91" t="s">
         <v>6</v>
       </c>
       <c r="D91" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>283</v>
+        <v>167</v>
       </c>
       <c r="B92" t="s">
-        <v>284</v>
+        <v>168</v>
       </c>
       <c r="C92" t="s">
         <v>6</v>
       </c>
       <c r="D92" t="s">
-        <v>285</v>
+        <v>169</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>344</v>
+        <v>283</v>
       </c>
       <c r="B93" t="s">
-        <v>345</v>
+        <v>284</v>
       </c>
       <c r="C93" t="s">
         <v>6</v>
       </c>
       <c r="D93" t="s">
-        <v>346</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B94" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C94" t="s">
         <v>6</v>
       </c>
       <c r="D94" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>297</v>
+        <v>347</v>
       </c>
       <c r="B95" t="s">
-        <v>13</v>
+        <v>348</v>
       </c>
       <c r="C95" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>63</v>
+        <v>349</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B96" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C96" t="s">
         <v>14</v>
       </c>
       <c r="D96" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B97" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C97" t="s">
         <v>14</v>
       </c>
       <c r="D97" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B98" t="s">
-        <v>351</v>
+        <v>52</v>
       </c>
       <c r="C98" t="s">
         <v>14</v>
       </c>
       <c r="D98" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="B99" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C99" t="s">
         <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>353</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>301</v>
+        <v>350</v>
       </c>
       <c r="B100" t="s">
-        <v>56</v>
+        <v>352</v>
       </c>
       <c r="C100" t="s">
         <v>14</v>
       </c>
       <c r="D100" t="s">
-        <v>79</v>
+        <v>353</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B101" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C101" t="s">
         <v>14</v>
       </c>
       <c r="D101" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B102" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="C102" t="s">
         <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>357</v>
+        <v>303</v>
       </c>
       <c r="B103" t="s">
-        <v>358</v>
+        <v>118</v>
       </c>
       <c r="C103" t="s">
         <v>14</v>
       </c>
       <c r="D103" t="s">
-        <v>359</v>
+        <v>82</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>304</v>
+        <v>357</v>
       </c>
       <c r="B104" t="s">
-        <v>119</v>
+        <v>358</v>
       </c>
       <c r="C104" t="s">
         <v>14</v>
       </c>
       <c r="D104" t="s">
-        <v>120</v>
+        <v>359</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B105" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C105" t="s">
         <v>14</v>
       </c>
       <c r="D105" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>123</v>
+        <v>305</v>
       </c>
       <c r="B106" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C106" t="s">
         <v>14</v>
       </c>
       <c r="D106" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B107" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C107" t="s">
         <v>14</v>
       </c>
       <c r="D107" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B108" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C108" t="s">
         <v>14</v>
       </c>
       <c r="D108" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B109" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C109" t="s">
         <v>14</v>
       </c>
       <c r="D109" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B110" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="C110" t="s">
         <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="B111" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="C111" t="s">
         <v>14</v>
       </c>
       <c r="D111" t="s">
-        <v>203</v>
+        <v>81</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>316</v>
+        <v>201</v>
       </c>
       <c r="B112" t="s">
-        <v>106</v>
+        <v>202</v>
       </c>
       <c r="C112" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="D112" t="s">
-        <v>115</v>
+        <v>203</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B113" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C113" t="s">
         <v>107</v>
       </c>
       <c r="D113" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B114" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C114" t="s">
         <v>107</v>
       </c>
       <c r="D114" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B115" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C115" t="s">
         <v>107</v>
       </c>
       <c r="D115" t="s">
-        <v>114</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B116" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C116" t="s">
         <v>107</v>
       </c>
       <c r="D116" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B117" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="C117" t="s">
         <v>107</v>
       </c>
       <c r="D117" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B118" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="C118" t="s">
         <v>107</v>
       </c>
       <c r="D118" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B119" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C119" t="s">
         <v>107</v>
       </c>
       <c r="D119" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B120" t="s">
-        <v>325</v>
+        <v>112</v>
       </c>
       <c r="C120" t="s">
         <v>107</v>
       </c>
       <c r="D120" t="s">
-        <v>326</v>
+        <v>22</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B121" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C121" t="s">
         <v>107</v>
       </c>
       <c r="D121" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="B122" t="s">
-        <v>356</v>
+        <v>328</v>
       </c>
       <c r="C122" t="s">
         <v>107</v>
       </c>
       <c r="D122" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>330</v>
+        <v>354</v>
       </c>
       <c r="B123" t="s">
-        <v>331</v>
+        <v>356</v>
       </c>
       <c r="C123" t="s">
         <v>107</v>
       </c>
       <c r="D123" t="s">
-        <v>332</v>
+        <v>355</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B124" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C124" t="s">
         <v>107</v>
       </c>
       <c r="D124" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>152</v>
+        <v>333</v>
       </c>
       <c r="B125" t="s">
-        <v>153</v>
+        <v>334</v>
       </c>
       <c r="C125" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="D125" t="s">
-        <v>155</v>
-      </c>
-      <c r="E125" t="s">
-        <v>156</v>
+        <v>335</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B126" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C126" t="s">
         <v>154</v>
       </c>
       <c r="D126" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="E126" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>223</v>
+        <v>157</v>
       </c>
       <c r="B127" t="s">
-        <v>224</v>
+        <v>158</v>
       </c>
       <c r="C127" t="s">
         <v>154</v>
       </c>
       <c r="D127" t="s">
-        <v>225</v>
+        <v>159</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="B128" t="s">
-        <v>267</v>
+        <v>224</v>
       </c>
       <c r="C128" t="s">
         <v>154</v>
       </c>
       <c r="D128" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B129" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C129" t="s">
         <v>154</v>
       </c>
       <c r="D129" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="B130" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="C130" t="s">
         <v>154</v>
       </c>
       <c r="D130" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>294</v>
+      </c>
+      <c r="B131" t="s">
+        <v>295</v>
+      </c>
+      <c r="C131" t="s">
+        <v>154</v>
+      </c>
+      <c r="D131" t="s">
         <v>296</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added local (RT or surgery) cancer tx derived variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E632FE5F-8C41-FC45-80A9-47EB2A9A6330}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09508BB8-851A-D949-86C1-B92FF46543A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-50160" yWindow="5840" windowWidth="45100" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="412">
   <si>
     <t>Variable #</t>
   </si>
@@ -1242,6 +1242,15 @@
   </si>
   <si>
     <t>Combined TnI and high-sensitivity troponin</t>
+  </si>
+  <si>
+    <t>Ca10j</t>
+  </si>
+  <si>
+    <t>any_local</t>
+  </si>
+  <si>
+    <t>Any local therapy (surgery or RT) within 3 months</t>
   </si>
 </sst>
 </file>
@@ -1297,10 +1306,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E132" totalsRowShown="0">
-  <autoFilter ref="A1:E132" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E132">
-    <sortCondition ref="A1:A132"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E133" totalsRowShown="0">
+  <autoFilter ref="A1:E133" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E133">
+    <sortCondition ref="A1:A133"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1634,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2172,1334 +2181,1348 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>206</v>
+        <v>409</v>
       </c>
       <c r="B38" t="s">
-        <v>207</v>
+        <v>410</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>208</v>
+        <v>411</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="B39" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B40" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>400</v>
+        <v>230</v>
       </c>
       <c r="B41" t="s">
-        <v>398</v>
+        <v>231</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>399</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>286</v>
+        <v>400</v>
       </c>
       <c r="B42" t="s">
-        <v>136</v>
+        <v>398</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>48</v>
+        <v>399</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>150</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B46" t="s">
-        <v>209</v>
+        <v>17</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>210</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>209</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>67</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>140</v>
+        <v>291</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>341</v>
+        <v>140</v>
       </c>
       <c r="B49" t="s">
-        <v>342</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>343</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>341</v>
       </c>
       <c r="B50" t="s">
-        <v>142</v>
+        <v>342</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>343</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B51" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B53" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C53" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>254</v>
+        <v>198</v>
       </c>
       <c r="B54" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="C54" t="s">
-        <v>171</v>
+        <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B55" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C55" t="s">
         <v>171</v>
       </c>
       <c r="D55" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B56" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
         <v>171</v>
       </c>
       <c r="D56" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B57" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C57" t="s">
         <v>171</v>
       </c>
       <c r="D57" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B58" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C58" t="s">
         <v>171</v>
       </c>
       <c r="D58" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C59" t="s">
         <v>171</v>
       </c>
       <c r="D59" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B60" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C60" t="s">
         <v>171</v>
       </c>
       <c r="D60" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B61" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C61" t="s">
         <v>171</v>
       </c>
       <c r="D61" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B62" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C62" t="s">
         <v>171</v>
       </c>
       <c r="D62" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>195</v>
+        <v>262</v>
       </c>
       <c r="B63" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C63" t="s">
         <v>171</v>
       </c>
       <c r="D63" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>233</v>
+        <v>195</v>
       </c>
       <c r="B64" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="C64" t="s">
         <v>171</v>
       </c>
       <c r="D64" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B65" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C65" t="s">
         <v>171</v>
       </c>
       <c r="D65" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B66" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C66" t="s">
         <v>171</v>
       </c>
       <c r="D66" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B67" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C67" t="s">
         <v>171</v>
       </c>
       <c r="D67" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B68" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C68" t="s">
         <v>171</v>
       </c>
       <c r="D68" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B69" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C69" t="s">
         <v>171</v>
       </c>
       <c r="D69" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="B70" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="C70" t="s">
         <v>171</v>
       </c>
       <c r="D70" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
       <c r="B71" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="C71" t="s">
         <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>406</v>
+        <v>263</v>
       </c>
       <c r="B72" t="s">
-        <v>407</v>
+        <v>264</v>
       </c>
       <c r="C72" t="s">
         <v>171</v>
       </c>
       <c r="D72" t="s">
-        <v>408</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>274</v>
+        <v>406</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>407</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D73" t="s">
-        <v>59</v>
+        <v>408</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B74" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C74" t="s">
         <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>338</v>
+        <v>275</v>
       </c>
       <c r="B75" t="s">
-        <v>339</v>
+        <v>11</v>
       </c>
       <c r="C75" t="s">
         <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>340</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>276</v>
+        <v>338</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>339</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>61</v>
+        <v>340</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B77" t="s">
-        <v>336</v>
+        <v>10</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>337</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B78" t="s">
-        <v>12</v>
+        <v>336</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>62</v>
+        <v>337</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B79" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B80" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>222</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B81" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>292</v>
+        <v>222</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B82" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>282</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>88</v>
+        <v>293</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="C84" t="s">
         <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B85" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="C85" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B86" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C86" t="s">
         <v>35</v>
       </c>
       <c r="D86" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B87" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C87" t="s">
         <v>35</v>
       </c>
       <c r="D87" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B88" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C88" t="s">
         <v>35</v>
       </c>
       <c r="D88" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B89" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="C89" t="s">
         <v>35</v>
       </c>
       <c r="D89" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B90" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C90" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D90" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B91" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C91" t="s">
         <v>6</v>
       </c>
       <c r="D91" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
       <c r="B92" t="s">
-        <v>165</v>
+        <v>23</v>
       </c>
       <c r="C92" t="s">
         <v>6</v>
       </c>
       <c r="D92" t="s">
-        <v>166</v>
+        <v>68</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B93" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C93" t="s">
         <v>6</v>
       </c>
       <c r="D93" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>283</v>
+        <v>167</v>
       </c>
       <c r="B94" t="s">
-        <v>284</v>
+        <v>168</v>
       </c>
       <c r="C94" t="s">
         <v>6</v>
       </c>
       <c r="D94" t="s">
-        <v>285</v>
+        <v>169</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>344</v>
+        <v>283</v>
       </c>
       <c r="B95" t="s">
-        <v>345</v>
+        <v>284</v>
       </c>
       <c r="C95" t="s">
         <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>346</v>
+        <v>285</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B96" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C96" t="s">
         <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>297</v>
+        <v>347</v>
       </c>
       <c r="B97" t="s">
-        <v>13</v>
+        <v>348</v>
       </c>
       <c r="C97" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>63</v>
+        <v>349</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B98" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C98" t="s">
         <v>14</v>
       </c>
       <c r="D98" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B99" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C99" t="s">
         <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B100" t="s">
-        <v>351</v>
+        <v>52</v>
       </c>
       <c r="C100" t="s">
         <v>14</v>
       </c>
       <c r="D100" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="B101" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C101" t="s">
         <v>14</v>
       </c>
       <c r="D101" t="s">
-        <v>353</v>
+        <v>117</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>301</v>
+        <v>350</v>
       </c>
       <c r="B102" t="s">
-        <v>56</v>
+        <v>352</v>
       </c>
       <c r="C102" t="s">
         <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>79</v>
+        <v>353</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B103" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C103" t="s">
         <v>14</v>
       </c>
       <c r="D103" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B104" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="C104" t="s">
         <v>14</v>
       </c>
       <c r="D104" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>355</v>
+        <v>303</v>
       </c>
       <c r="B105" t="s">
-        <v>356</v>
+        <v>118</v>
       </c>
       <c r="C105" t="s">
         <v>14</v>
       </c>
       <c r="D105" t="s">
-        <v>357</v>
+        <v>82</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>304</v>
+        <v>355</v>
       </c>
       <c r="B106" t="s">
-        <v>119</v>
+        <v>356</v>
       </c>
       <c r="C106" t="s">
         <v>14</v>
       </c>
       <c r="D106" t="s">
-        <v>120</v>
+        <v>357</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B107" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C107" t="s">
         <v>14</v>
       </c>
       <c r="D107" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>123</v>
+        <v>305</v>
       </c>
       <c r="B108" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C108" t="s">
         <v>14</v>
       </c>
       <c r="D108" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B109" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C109" t="s">
         <v>14</v>
       </c>
       <c r="D109" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B110" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C110" t="s">
         <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B111" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C111" t="s">
         <v>14</v>
       </c>
       <c r="D111" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B112" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="C112" t="s">
         <v>14</v>
       </c>
       <c r="D112" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="B113" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="C113" t="s">
         <v>14</v>
       </c>
       <c r="D113" t="s">
-        <v>203</v>
+        <v>81</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>316</v>
+        <v>201</v>
       </c>
       <c r="B114" t="s">
-        <v>106</v>
+        <v>202</v>
       </c>
       <c r="C114" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="D114" t="s">
-        <v>115</v>
+        <v>203</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B115" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C115" t="s">
         <v>107</v>
       </c>
       <c r="D115" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B116" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C116" t="s">
         <v>107</v>
       </c>
       <c r="D116" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B117" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C117" t="s">
         <v>107</v>
       </c>
       <c r="D117" t="s">
-        <v>114</v>
+        <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B118" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C118" t="s">
         <v>107</v>
       </c>
       <c r="D118" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B119" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="C119" t="s">
         <v>107</v>
       </c>
       <c r="D119" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B120" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="C120" t="s">
         <v>107</v>
       </c>
       <c r="D120" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B121" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C121" t="s">
         <v>107</v>
       </c>
       <c r="D121" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B122" t="s">
-        <v>325</v>
+        <v>112</v>
       </c>
       <c r="C122" t="s">
         <v>107</v>
       </c>
       <c r="D122" t="s">
-        <v>326</v>
+        <v>22</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B123" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C123" t="s">
         <v>107</v>
       </c>
       <c r="D123" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="B124" t="s">
-        <v>404</v>
+        <v>328</v>
       </c>
       <c r="C124" t="s">
         <v>107</v>
       </c>
       <c r="D124" t="s">
-        <v>405</v>
+        <v>329</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>330</v>
+        <v>354</v>
       </c>
       <c r="B125" t="s">
-        <v>331</v>
+        <v>404</v>
       </c>
       <c r="C125" t="s">
         <v>107</v>
       </c>
       <c r="D125" t="s">
-        <v>332</v>
+        <v>405</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B126" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C126" t="s">
         <v>107</v>
       </c>
       <c r="D126" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>152</v>
+        <v>333</v>
       </c>
       <c r="B127" t="s">
-        <v>153</v>
+        <v>334</v>
       </c>
       <c r="C127" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="D127" t="s">
-        <v>155</v>
-      </c>
-      <c r="E127" t="s">
-        <v>156</v>
+        <v>335</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B128" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C128" t="s">
         <v>154</v>
       </c>
       <c r="D128" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="E128" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>223</v>
+        <v>157</v>
       </c>
       <c r="B129" t="s">
-        <v>224</v>
+        <v>158</v>
       </c>
       <c r="C129" t="s">
         <v>154</v>
       </c>
       <c r="D129" t="s">
-        <v>225</v>
+        <v>159</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="B130" t="s">
-        <v>267</v>
+        <v>224</v>
       </c>
       <c r="C130" t="s">
         <v>154</v>
       </c>
       <c r="D130" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B131" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C131" t="s">
         <v>154</v>
       </c>
       <c r="D131" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="B132" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="C132" t="s">
         <v>154</v>
       </c>
       <c r="D132" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>294</v>
+      </c>
+      <c r="B133" t="s">
+        <v>295</v>
+      </c>
+      <c r="C133" t="s">
+        <v>154</v>
+      </c>
+      <c r="D133" t="s">
         <v>296</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add derived convalescent plasma variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09508BB8-851A-D949-86C1-B92FF46543A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1CDE66-E633-054D-BB0A-6EC9ED7999B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-50160" yWindow="5840" windowWidth="45100" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="415">
   <si>
     <t>Variable #</t>
   </si>
@@ -1251,6 +1251,15 @@
   </si>
   <si>
     <t>Any local therapy (surgery or RT) within 3 months</t>
+  </si>
+  <si>
+    <t>Rx16</t>
+  </si>
+  <si>
+    <t>plasma</t>
+  </si>
+  <si>
+    <t>Convalescent plasma as COVID-19 treatment ever</t>
   </si>
 </sst>
 </file>
@@ -1306,10 +1315,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E133" totalsRowShown="0">
-  <autoFilter ref="A1:E133" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E133">
-    <sortCondition ref="A1:A133"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E134" totalsRowShown="0">
+  <autoFilter ref="A1:E134" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E134">
+    <sortCondition ref="A1:A134"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1643,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E133"/>
+  <dimension ref="A1:E134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3229,7 +3238,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>135</v>
       </c>
@@ -3243,7 +3252,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>201</v>
       </c>
@@ -3257,272 +3266,286 @@
         <v>203</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>412</v>
+      </c>
+      <c r="B115" t="s">
+        <v>413</v>
+      </c>
+      <c r="C115" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>316</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>106</v>
-      </c>
-      <c r="C115" t="s">
-        <v>107</v>
-      </c>
-      <c r="D115" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>317</v>
-      </c>
-      <c r="B116" t="s">
-        <v>105</v>
       </c>
       <c r="C116" t="s">
         <v>107</v>
       </c>
       <c r="D116" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B117" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C117" t="s">
         <v>107</v>
       </c>
       <c r="D117" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B118" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C118" t="s">
         <v>107</v>
       </c>
       <c r="D118" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B119" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C119" t="s">
         <v>107</v>
       </c>
       <c r="D119" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B120" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="C120" t="s">
         <v>107</v>
       </c>
       <c r="D120" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B121" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="C121" t="s">
         <v>107</v>
       </c>
       <c r="D121" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B122" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C122" t="s">
         <v>107</v>
       </c>
       <c r="D122" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B123" t="s">
-        <v>325</v>
+        <v>112</v>
       </c>
       <c r="C123" t="s">
         <v>107</v>
       </c>
       <c r="D123" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B124" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C124" t="s">
         <v>107</v>
       </c>
       <c r="D124" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="B125" t="s">
-        <v>404</v>
+        <v>328</v>
       </c>
       <c r="C125" t="s">
         <v>107</v>
       </c>
       <c r="D125" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>330</v>
+        <v>354</v>
       </c>
       <c r="B126" t="s">
-        <v>331</v>
+        <v>404</v>
       </c>
       <c r="C126" t="s">
         <v>107</v>
       </c>
       <c r="D126" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B127" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C127" t="s">
         <v>107</v>
       </c>
       <c r="D127" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>333</v>
+      </c>
+      <c r="B128" t="s">
+        <v>334</v>
+      </c>
+      <c r="C128" t="s">
+        <v>107</v>
+      </c>
+      <c r="D128" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>152</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B129" t="s">
         <v>153</v>
-      </c>
-      <c r="C128" t="s">
-        <v>154</v>
-      </c>
-      <c r="D128" t="s">
-        <v>155</v>
-      </c>
-      <c r="E128" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>157</v>
-      </c>
-      <c r="B129" t="s">
-        <v>158</v>
       </c>
       <c r="C129" t="s">
         <v>154</v>
       </c>
       <c r="D129" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E129" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>223</v>
+        <v>157</v>
       </c>
       <c r="B130" t="s">
-        <v>224</v>
+        <v>158</v>
       </c>
       <c r="C130" t="s">
         <v>154</v>
       </c>
       <c r="D130" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="B131" t="s">
-        <v>267</v>
+        <v>224</v>
       </c>
       <c r="C131" t="s">
         <v>154</v>
       </c>
       <c r="D131" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B132" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C132" t="s">
         <v>154</v>
       </c>
       <c r="D132" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="B133" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="C133" t="s">
         <v>154</v>
       </c>
       <c r="D133" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>294</v>
+      </c>
+      <c r="B134" t="s">
+        <v>295</v>
+      </c>
+      <c r="C134" t="s">
+        <v>154</v>
+      </c>
+      <c r="D134" t="s">
         <v>296</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New treatment variable and dictionary mod
1. Collapsed cancer treatment timing variable
2. Added bamlanivimab
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1CDE66-E633-054D-BB0A-6EC9ED7999B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9C6B46-61C9-3746-B08A-18DDE990B332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50160" yWindow="5840" windowWidth="45100" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="418">
   <si>
     <t>Variable #</t>
   </si>
@@ -1260,6 +1260,15 @@
   </si>
   <si>
     <t>Convalescent plasma as COVID-19 treatment ever</t>
+  </si>
+  <si>
+    <t>T13a</t>
+  </si>
+  <si>
+    <t>cancer_tx_timing_v2</t>
+  </si>
+  <si>
+    <t>Timing of cancer treatment relative to COVID-19, collapsed</t>
   </si>
 </sst>
 </file>
@@ -1315,10 +1324,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E134" totalsRowShown="0">
-  <autoFilter ref="A1:E134" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E134">
-    <sortCondition ref="A1:A134"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E135" totalsRowShown="0">
+  <autoFilter ref="A1:E135" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E135">
+    <sortCondition ref="A1:A135"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1652,10 +1661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2260,1292 +2269,1306 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>286</v>
+        <v>415</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>416</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>417</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B45" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>150</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="C46" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B47" t="s">
-        <v>209</v>
+        <v>17</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>210</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>209</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>67</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>291</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>341</v>
+        <v>140</v>
       </c>
       <c r="B50" t="s">
-        <v>342</v>
+        <v>3</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>343</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>141</v>
+        <v>341</v>
       </c>
       <c r="B51" t="s">
-        <v>142</v>
+        <v>342</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>343</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="C53" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B54" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>254</v>
+        <v>198</v>
       </c>
       <c r="B55" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="C55" t="s">
-        <v>171</v>
+        <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B56" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C56" t="s">
         <v>171</v>
       </c>
       <c r="D56" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B57" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C57" t="s">
         <v>171</v>
       </c>
       <c r="D57" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B58" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C58" t="s">
         <v>171</v>
       </c>
       <c r="D58" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B59" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C59" t="s">
         <v>171</v>
       </c>
       <c r="D59" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C60" t="s">
         <v>171</v>
       </c>
       <c r="D60" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B61" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C61" t="s">
         <v>171</v>
       </c>
       <c r="D61" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B62" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C62" t="s">
         <v>171</v>
       </c>
       <c r="D62" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B63" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C63" t="s">
         <v>171</v>
       </c>
       <c r="D63" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>195</v>
+        <v>262</v>
       </c>
       <c r="B64" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C64" t="s">
         <v>171</v>
       </c>
       <c r="D64" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>233</v>
+        <v>195</v>
       </c>
       <c r="B65" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="C65" t="s">
         <v>171</v>
       </c>
       <c r="D65" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B66" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C66" t="s">
         <v>171</v>
       </c>
       <c r="D66" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B67" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C67" t="s">
         <v>171</v>
       </c>
       <c r="D67" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B68" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C68" t="s">
         <v>171</v>
       </c>
       <c r="D68" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B69" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C69" t="s">
         <v>171</v>
       </c>
       <c r="D69" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B70" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C70" t="s">
         <v>171</v>
       </c>
       <c r="D70" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="B71" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="C71" t="s">
         <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
       <c r="B72" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="C72" t="s">
         <v>171</v>
       </c>
       <c r="D72" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>406</v>
+        <v>263</v>
       </c>
       <c r="B73" t="s">
-        <v>407</v>
+        <v>264</v>
       </c>
       <c r="C73" t="s">
         <v>171</v>
       </c>
       <c r="D73" t="s">
-        <v>408</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>274</v>
+        <v>406</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>407</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D74" t="s">
-        <v>59</v>
+        <v>408</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B75" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C75" t="s">
         <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>338</v>
+        <v>275</v>
       </c>
       <c r="B76" t="s">
-        <v>339</v>
+        <v>11</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>340</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>276</v>
+        <v>338</v>
       </c>
       <c r="B77" t="s">
-        <v>10</v>
+        <v>339</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>61</v>
+        <v>340</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B78" t="s">
-        <v>336</v>
+        <v>10</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>337</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B79" t="s">
-        <v>12</v>
+        <v>336</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>62</v>
+        <v>337</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B80" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B81" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>222</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B82" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>292</v>
+        <v>222</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B83" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>282</v>
       </c>
       <c r="B84" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="C84" t="s">
         <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>88</v>
+        <v>293</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="C85" t="s">
         <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B86" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="C86" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D86" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B87" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C87" t="s">
         <v>35</v>
       </c>
       <c r="D87" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B88" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C88" t="s">
         <v>35</v>
       </c>
       <c r="D88" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B89" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C89" t="s">
         <v>35</v>
       </c>
       <c r="D89" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B90" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="C90" t="s">
         <v>35</v>
       </c>
       <c r="D90" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B91" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C91" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D91" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C92" t="s">
         <v>6</v>
       </c>
       <c r="D92" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
       <c r="B93" t="s">
-        <v>165</v>
+        <v>23</v>
       </c>
       <c r="C93" t="s">
         <v>6</v>
       </c>
       <c r="D93" t="s">
-        <v>166</v>
+        <v>68</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B94" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C94" t="s">
         <v>6</v>
       </c>
       <c r="D94" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>283</v>
+        <v>167</v>
       </c>
       <c r="B95" t="s">
-        <v>284</v>
+        <v>168</v>
       </c>
       <c r="C95" t="s">
         <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>285</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>344</v>
+        <v>283</v>
       </c>
       <c r="B96" t="s">
-        <v>345</v>
+        <v>284</v>
       </c>
       <c r="C96" t="s">
         <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>346</v>
+        <v>285</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B97" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C97" t="s">
         <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>297</v>
+        <v>347</v>
       </c>
       <c r="B98" t="s">
-        <v>13</v>
+        <v>348</v>
       </c>
       <c r="C98" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>63</v>
+        <v>349</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B99" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C99" t="s">
         <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B100" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C100" t="s">
         <v>14</v>
       </c>
       <c r="D100" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B101" t="s">
-        <v>351</v>
+        <v>52</v>
       </c>
       <c r="C101" t="s">
         <v>14</v>
       </c>
       <c r="D101" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="B102" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C102" t="s">
         <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>353</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>301</v>
+        <v>350</v>
       </c>
       <c r="B103" t="s">
-        <v>56</v>
+        <v>352</v>
       </c>
       <c r="C103" t="s">
         <v>14</v>
       </c>
       <c r="D103" t="s">
-        <v>79</v>
+        <v>353</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B104" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C104" t="s">
         <v>14</v>
       </c>
       <c r="D104" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B105" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="C105" t="s">
         <v>14</v>
       </c>
       <c r="D105" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>355</v>
+        <v>303</v>
       </c>
       <c r="B106" t="s">
-        <v>356</v>
+        <v>118</v>
       </c>
       <c r="C106" t="s">
         <v>14</v>
       </c>
       <c r="D106" t="s">
-        <v>357</v>
+        <v>82</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>304</v>
+        <v>355</v>
       </c>
       <c r="B107" t="s">
-        <v>119</v>
+        <v>356</v>
       </c>
       <c r="C107" t="s">
         <v>14</v>
       </c>
       <c r="D107" t="s">
-        <v>120</v>
+        <v>357</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B108" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C108" t="s">
         <v>14</v>
       </c>
       <c r="D108" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>123</v>
+        <v>305</v>
       </c>
       <c r="B109" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C109" t="s">
         <v>14</v>
       </c>
       <c r="D109" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B110" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C110" t="s">
         <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B111" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C111" t="s">
         <v>14</v>
       </c>
       <c r="D111" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C112" t="s">
         <v>14</v>
       </c>
       <c r="D112" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B113" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="C113" t="s">
         <v>14</v>
       </c>
       <c r="D113" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="B114" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="C114" t="s">
         <v>14</v>
       </c>
       <c r="D114" t="s">
-        <v>203</v>
+        <v>81</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>412</v>
+        <v>201</v>
       </c>
       <c r="B115" t="s">
-        <v>413</v>
+        <v>202</v>
       </c>
       <c r="C115" t="s">
         <v>14</v>
       </c>
       <c r="D115" t="s">
-        <v>414</v>
+        <v>203</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>316</v>
+        <v>412</v>
       </c>
       <c r="B116" t="s">
-        <v>106</v>
+        <v>413</v>
       </c>
       <c r="C116" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="D116" t="s">
-        <v>115</v>
+        <v>414</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B117" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C117" t="s">
         <v>107</v>
       </c>
       <c r="D117" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B118" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C118" t="s">
         <v>107</v>
       </c>
       <c r="D118" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B119" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C119" t="s">
         <v>107</v>
       </c>
       <c r="D119" t="s">
-        <v>114</v>
+        <v>24</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B120" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C120" t="s">
         <v>107</v>
       </c>
       <c r="D120" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B121" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="C121" t="s">
         <v>107</v>
       </c>
       <c r="D121" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B122" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="C122" t="s">
         <v>107</v>
       </c>
       <c r="D122" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B123" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C123" t="s">
         <v>107</v>
       </c>
       <c r="D123" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B124" t="s">
-        <v>325</v>
+        <v>112</v>
       </c>
       <c r="C124" t="s">
         <v>107</v>
       </c>
       <c r="D124" t="s">
-        <v>326</v>
+        <v>22</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B125" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C125" t="s">
         <v>107</v>
       </c>
       <c r="D125" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="B126" t="s">
-        <v>404</v>
+        <v>328</v>
       </c>
       <c r="C126" t="s">
         <v>107</v>
       </c>
       <c r="D126" t="s">
-        <v>405</v>
+        <v>329</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>330</v>
+        <v>354</v>
       </c>
       <c r="B127" t="s">
-        <v>331</v>
+        <v>404</v>
       </c>
       <c r="C127" t="s">
         <v>107</v>
       </c>
       <c r="D127" t="s">
-        <v>332</v>
+        <v>405</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B128" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C128" t="s">
         <v>107</v>
       </c>
       <c r="D128" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>152</v>
+        <v>333</v>
       </c>
       <c r="B129" t="s">
-        <v>153</v>
+        <v>334</v>
       </c>
       <c r="C129" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="D129" t="s">
-        <v>155</v>
-      </c>
-      <c r="E129" t="s">
-        <v>156</v>
+        <v>335</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B130" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C130" t="s">
         <v>154</v>
       </c>
       <c r="D130" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="E130" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>223</v>
+        <v>157</v>
       </c>
       <c r="B131" t="s">
-        <v>224</v>
+        <v>158</v>
       </c>
       <c r="C131" t="s">
         <v>154</v>
       </c>
       <c r="D131" t="s">
-        <v>225</v>
+        <v>159</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="B132" t="s">
-        <v>267</v>
+        <v>224</v>
       </c>
       <c r="C132" t="s">
         <v>154</v>
       </c>
       <c r="D132" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B133" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C133" t="s">
         <v>154</v>
       </c>
       <c r="D133" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="B134" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="C134" t="s">
         <v>154</v>
       </c>
       <c r="D134" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>294</v>
+      </c>
+      <c r="B135" t="s">
+        <v>295</v>
+      </c>
+      <c r="C135" t="s">
+        <v>154</v>
+      </c>
+      <c r="D135" t="s">
         <v>296</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New derived variables, minor fix
1. Trimester of diagnosis
2. CVD risk factor (binary Y/N)
3. Minor fix of grep patterns
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9C6B46-61C9-3746-B08A-18DDE990B332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F179CF4-DC5B-5549-9041-1ADE466AD140}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35840" yWindow="3680" windowWidth="35840" windowHeight="20720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="423">
   <si>
     <t>Variable #</t>
   </si>
@@ -1269,6 +1269,21 @@
   </si>
   <si>
     <t>Timing of cancer treatment relative to COVID-19, collapsed</t>
+  </si>
+  <si>
+    <t>tri_rt_dx</t>
+  </si>
+  <si>
+    <t>Trimester and year of diagnosis, using the most recent side of the interval as anchor</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>CVD_risk</t>
+  </si>
+  <si>
+    <t>CVD risk factor indicator</t>
   </si>
 </sst>
 </file>
@@ -1324,10 +1339,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E135" totalsRowShown="0">
-  <autoFilter ref="A1:E135" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E135">
-    <sortCondition ref="A1:A135"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E137" totalsRowShown="0">
+  <autoFilter ref="A1:E137" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E137">
+    <sortCondition ref="A1:A137"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1661,10 +1676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1883,7 +1898,7 @@
         <v>272</v>
       </c>
       <c r="C15" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
         <v>273</v>
@@ -1891,1684 +1906,1712 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>306</v>
+        <v>420</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>421</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>422</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B17" t="s">
-        <v>226</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>378</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>376</v>
+        <v>307</v>
       </c>
       <c r="B18" t="s">
-        <v>377</v>
+        <v>226</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>308</v>
+        <v>376</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>149</v>
+        <v>379</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>401</v>
+        <v>313</v>
       </c>
       <c r="B25" t="s">
-        <v>402</v>
+        <v>151</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>403</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>314</v>
+        <v>401</v>
       </c>
       <c r="B26" t="s">
-        <v>160</v>
+        <v>402</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>162</v>
+        <v>403</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>173</v>
+        <v>315</v>
       </c>
       <c r="B28" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>213</v>
+        <v>173</v>
       </c>
       <c r="B29" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B30" t="s">
-        <v>386</v>
+        <v>214</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>392</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>382</v>
+        <v>219</v>
       </c>
       <c r="B32" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B33" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B34" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B35" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C35" t="s">
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="B36" t="s">
-        <v>217</v>
+        <v>391</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>218</v>
+        <v>396</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B37" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>409</v>
+        <v>381</v>
       </c>
       <c r="B38" t="s">
-        <v>410</v>
+        <v>220</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>411</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>206</v>
+        <v>409</v>
       </c>
       <c r="B39" t="s">
-        <v>207</v>
+        <v>410</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>208</v>
+        <v>411</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="B40" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B41" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>400</v>
+        <v>230</v>
       </c>
       <c r="B42" t="s">
-        <v>398</v>
+        <v>231</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>399</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="B43" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="C43" t="s">
         <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>286</v>
+        <v>415</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>416</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>48</v>
+        <v>417</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>150</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B48" t="s">
-        <v>209</v>
+        <v>17</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>210</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>209</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>67</v>
+        <v>210</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>140</v>
+        <v>291</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>341</v>
+        <v>140</v>
       </c>
       <c r="B51" t="s">
-        <v>342</v>
+        <v>3</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>343</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>141</v>
+        <v>341</v>
       </c>
       <c r="B52" t="s">
-        <v>142</v>
+        <v>342</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>143</v>
+        <v>343</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B53" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B55" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>254</v>
+        <v>198</v>
       </c>
       <c r="B56" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="C56" t="s">
-        <v>171</v>
+        <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B57" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C57" t="s">
         <v>171</v>
       </c>
       <c r="D57" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B58" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C58" t="s">
         <v>171</v>
       </c>
       <c r="D58" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B59" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C59" t="s">
         <v>171</v>
       </c>
       <c r="D59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B60" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C60" t="s">
         <v>171</v>
       </c>
       <c r="D60" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B61" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C61" t="s">
         <v>171</v>
       </c>
       <c r="D61" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B62" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C62" t="s">
         <v>171</v>
       </c>
       <c r="D62" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B63" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C63" t="s">
         <v>171</v>
       </c>
       <c r="D63" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B64" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C64" t="s">
         <v>171</v>
       </c>
       <c r="D64" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>195</v>
+        <v>262</v>
       </c>
       <c r="B65" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C65" t="s">
         <v>171</v>
       </c>
       <c r="D65" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>233</v>
+        <v>195</v>
       </c>
       <c r="B66" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="C66" t="s">
         <v>171</v>
       </c>
       <c r="D66" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B67" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C67" t="s">
         <v>171</v>
       </c>
       <c r="D67" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B68" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C68" t="s">
         <v>171</v>
       </c>
       <c r="D68" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B69" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C69" t="s">
         <v>171</v>
       </c>
       <c r="D69" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B70" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C70" t="s">
         <v>171</v>
       </c>
       <c r="D70" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B71" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C71" t="s">
         <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="B72" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="C72" t="s">
         <v>171</v>
       </c>
       <c r="D72" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
       <c r="B73" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="C73" t="s">
         <v>171</v>
       </c>
       <c r="D73" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>406</v>
+        <v>263</v>
       </c>
       <c r="B74" t="s">
-        <v>407</v>
+        <v>264</v>
       </c>
       <c r="C74" t="s">
         <v>171</v>
       </c>
       <c r="D74" t="s">
-        <v>408</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>274</v>
+        <v>406</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
+        <v>407</v>
       </c>
       <c r="C75" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D75" t="s">
-        <v>59</v>
+        <v>408</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B76" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>338</v>
+        <v>275</v>
       </c>
       <c r="B77" t="s">
-        <v>339</v>
+        <v>11</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>340</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>276</v>
+        <v>338</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>339</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>61</v>
+        <v>340</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B79" t="s">
-        <v>336</v>
+        <v>10</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>337</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B80" t="s">
-        <v>12</v>
+        <v>336</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>62</v>
+        <v>337</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B81" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B82" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>222</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B83" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>292</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B84" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C84" t="s">
         <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>282</v>
       </c>
       <c r="B85" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="C85" t="s">
         <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>88</v>
+        <v>293</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="C86" t="s">
         <v>6</v>
       </c>
       <c r="D86" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="C87" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D87" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C88" t="s">
         <v>35</v>
       </c>
       <c r="D88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B89" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C89" t="s">
         <v>35</v>
       </c>
       <c r="D89" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B90" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C90" t="s">
         <v>35</v>
       </c>
       <c r="D90" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B91" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="C91" t="s">
         <v>35</v>
       </c>
       <c r="D91" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B92" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C92" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D92" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B93" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C93" t="s">
         <v>6</v>
       </c>
       <c r="D93" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
       <c r="B94" t="s">
-        <v>165</v>
+        <v>23</v>
       </c>
       <c r="C94" t="s">
         <v>6</v>
       </c>
       <c r="D94" t="s">
-        <v>166</v>
+        <v>68</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B95" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C95" t="s">
         <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>283</v>
+        <v>167</v>
       </c>
       <c r="B96" t="s">
-        <v>284</v>
+        <v>168</v>
       </c>
       <c r="C96" t="s">
         <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>285</v>
+        <v>169</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>344</v>
+        <v>283</v>
       </c>
       <c r="B97" t="s">
-        <v>345</v>
+        <v>284</v>
       </c>
       <c r="C97" t="s">
         <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>346</v>
+        <v>285</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B98" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C98" t="s">
         <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>297</v>
+        <v>347</v>
       </c>
       <c r="B99" t="s">
-        <v>13</v>
+        <v>348</v>
       </c>
       <c r="C99" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D99" t="s">
-        <v>63</v>
+        <v>349</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B100" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C100" t="s">
         <v>14</v>
       </c>
       <c r="D100" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B101" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C101" t="s">
         <v>14</v>
       </c>
       <c r="D101" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B102" t="s">
-        <v>351</v>
+        <v>52</v>
       </c>
       <c r="C102" t="s">
         <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="B103" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C103" t="s">
         <v>14</v>
       </c>
       <c r="D103" t="s">
-        <v>353</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>301</v>
+        <v>350</v>
       </c>
       <c r="B104" t="s">
-        <v>56</v>
+        <v>352</v>
       </c>
       <c r="C104" t="s">
         <v>14</v>
       </c>
       <c r="D104" t="s">
-        <v>79</v>
+        <v>353</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B105" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C105" t="s">
         <v>14</v>
       </c>
       <c r="D105" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B106" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="C106" t="s">
         <v>14</v>
       </c>
       <c r="D106" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>355</v>
+        <v>303</v>
       </c>
       <c r="B107" t="s">
-        <v>356</v>
+        <v>118</v>
       </c>
       <c r="C107" t="s">
         <v>14</v>
       </c>
       <c r="D107" t="s">
-        <v>357</v>
+        <v>82</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>304</v>
+        <v>355</v>
       </c>
       <c r="B108" t="s">
-        <v>119</v>
+        <v>356</v>
       </c>
       <c r="C108" t="s">
         <v>14</v>
       </c>
       <c r="D108" t="s">
-        <v>120</v>
+        <v>357</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B109" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C109" t="s">
         <v>14</v>
       </c>
       <c r="D109" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>123</v>
+        <v>305</v>
       </c>
       <c r="B110" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C110" t="s">
         <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B111" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C111" t="s">
         <v>14</v>
       </c>
       <c r="D111" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B112" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C112" t="s">
         <v>14</v>
       </c>
       <c r="D112" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B113" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C113" t="s">
         <v>14</v>
       </c>
       <c r="D113" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B114" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="C114" t="s">
         <v>14</v>
       </c>
       <c r="D114" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="B115" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="C115" t="s">
         <v>14</v>
       </c>
       <c r="D115" t="s">
-        <v>203</v>
+        <v>81</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>412</v>
+        <v>201</v>
       </c>
       <c r="B116" t="s">
-        <v>413</v>
+        <v>202</v>
       </c>
       <c r="C116" t="s">
         <v>14</v>
       </c>
       <c r="D116" t="s">
-        <v>414</v>
+        <v>203</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>316</v>
+        <v>412</v>
       </c>
       <c r="B117" t="s">
-        <v>106</v>
+        <v>413</v>
       </c>
       <c r="C117" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="D117" t="s">
-        <v>115</v>
+        <v>414</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B118" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C118" t="s">
         <v>107</v>
       </c>
       <c r="D118" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B119" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C119" t="s">
         <v>107</v>
       </c>
       <c r="D119" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B120" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C120" t="s">
         <v>107</v>
       </c>
       <c r="D120" t="s">
-        <v>114</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B121" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C121" t="s">
         <v>107</v>
       </c>
       <c r="D121" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B122" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="C122" t="s">
         <v>107</v>
       </c>
       <c r="D122" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B123" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="C123" t="s">
         <v>107</v>
       </c>
       <c r="D123" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B124" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C124" t="s">
         <v>107</v>
       </c>
       <c r="D124" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B125" t="s">
-        <v>325</v>
+        <v>112</v>
       </c>
       <c r="C125" t="s">
         <v>107</v>
       </c>
       <c r="D125" t="s">
-        <v>326</v>
+        <v>22</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B126" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C126" t="s">
         <v>107</v>
       </c>
       <c r="D126" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="B127" t="s">
-        <v>404</v>
+        <v>328</v>
       </c>
       <c r="C127" t="s">
         <v>107</v>
       </c>
       <c r="D127" t="s">
-        <v>405</v>
+        <v>329</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>330</v>
+        <v>354</v>
       </c>
       <c r="B128" t="s">
-        <v>331</v>
+        <v>404</v>
       </c>
       <c r="C128" t="s">
         <v>107</v>
       </c>
       <c r="D128" t="s">
-        <v>332</v>
+        <v>405</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B129" t="s">
-        <v>334</v>
+        <v>418</v>
       </c>
       <c r="C129" t="s">
         <v>107</v>
       </c>
       <c r="D129" t="s">
-        <v>335</v>
+        <v>419</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>152</v>
+        <v>333</v>
       </c>
       <c r="B130" t="s">
-        <v>153</v>
+        <v>331</v>
       </c>
       <c r="C130" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="D130" t="s">
-        <v>155</v>
-      </c>
-      <c r="E130" t="s">
-        <v>156</v>
+        <v>332</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>157</v>
+        <v>400</v>
       </c>
       <c r="B131" t="s">
-        <v>158</v>
+        <v>334</v>
       </c>
       <c r="C131" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="D131" t="s">
-        <v>159</v>
+        <v>335</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>223</v>
+        <v>152</v>
       </c>
       <c r="B132" t="s">
-        <v>224</v>
+        <v>153</v>
       </c>
       <c r="C132" t="s">
         <v>154</v>
       </c>
       <c r="D132" t="s">
-        <v>225</v>
+        <v>155</v>
+      </c>
+      <c r="E132" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>266</v>
+        <v>157</v>
       </c>
       <c r="B133" t="s">
-        <v>267</v>
+        <v>158</v>
       </c>
       <c r="C133" t="s">
         <v>154</v>
       </c>
       <c r="D133" t="s">
-        <v>268</v>
+        <v>159</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>269</v>
+        <v>223</v>
       </c>
       <c r="B134" t="s">
-        <v>270</v>
+        <v>224</v>
       </c>
       <c r="C134" t="s">
         <v>154</v>
       </c>
       <c r="D134" t="s">
-        <v>271</v>
+        <v>225</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>294</v>
+        <v>266</v>
       </c>
       <c r="B135" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
       <c r="C135" t="s">
         <v>154</v>
       </c>
       <c r="D135" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>269</v>
+      </c>
+      <c r="B136" t="s">
+        <v>270</v>
+      </c>
+      <c r="C136" t="s">
+        <v>154</v>
+      </c>
+      <c r="D136" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>294</v>
+      </c>
+      <c r="B137" t="s">
+        <v>295</v>
+      </c>
+      <c r="C137" t="s">
+        <v>154</v>
+      </c>
+      <c r="D137" t="s">
         <v>296</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New derived variable, files added to archive
1. New VTE derived variable that combines just PE & DVT
2. Moved some older versions of the data dictionary to the archive
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,32 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A95C45-84AC-7F4C-852F-5D996CE7105C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685E6C2E-E0DA-804C-B6A2-FF9B2B159DDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="438">
   <si>
     <t>Variable #</t>
   </si>
@@ -1331,6 +1320,15 @@
   </si>
   <si>
     <t>Modified IMWG frailty index (non-frail; prefrail; frail)</t>
+  </si>
+  <si>
+    <t>O19a</t>
+  </si>
+  <si>
+    <t>VTE_comp_v2</t>
+  </si>
+  <si>
+    <t>Combined VTE complications (excluding SVT and thrombosis NOS)</t>
   </si>
 </sst>
 </file>
@@ -1386,10 +1384,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E141" totalsRowShown="0">
-  <autoFilter ref="A1:E141" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E141">
-    <sortCondition ref="A1:A141"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E142" totalsRowShown="0">
+  <autoFilter ref="A1:E142" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E142">
+    <sortCondition ref="A1:A142"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1723,10 +1721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3073,520 +3071,520 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>165</v>
+        <v>435</v>
       </c>
       <c r="B96" t="s">
-        <v>166</v>
+        <v>436</v>
       </c>
       <c r="C96" t="s">
         <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>167</v>
+        <v>437</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>422</v>
+        <v>165</v>
       </c>
       <c r="B97" t="s">
-        <v>423</v>
+        <v>166</v>
       </c>
       <c r="C97" t="s">
         <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>424</v>
+        <v>167</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>281</v>
+        <v>422</v>
       </c>
       <c r="B98" t="s">
-        <v>282</v>
+        <v>423</v>
       </c>
       <c r="C98" t="s">
         <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>283</v>
+        <v>424</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>342</v>
+        <v>281</v>
       </c>
       <c r="B99" t="s">
-        <v>343</v>
+        <v>282</v>
       </c>
       <c r="C99" t="s">
         <v>6</v>
       </c>
       <c r="D99" t="s">
-        <v>344</v>
+        <v>283</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B100" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C100" t="s">
         <v>6</v>
       </c>
       <c r="D100" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>295</v>
+        <v>345</v>
       </c>
       <c r="B101" t="s">
-        <v>13</v>
+        <v>346</v>
       </c>
       <c r="C101" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D101" t="s">
-        <v>63</v>
+        <v>347</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B102" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C102" t="s">
         <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B103" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C103" t="s">
         <v>14</v>
       </c>
       <c r="D103" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B104" t="s">
-        <v>349</v>
+        <v>52</v>
       </c>
       <c r="C104" t="s">
         <v>14</v>
       </c>
       <c r="D104" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>348</v>
+        <v>298</v>
       </c>
       <c r="B105" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C105" t="s">
         <v>14</v>
       </c>
       <c r="D105" t="s">
-        <v>351</v>
+        <v>116</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>299</v>
+        <v>348</v>
       </c>
       <c r="B106" t="s">
-        <v>56</v>
+        <v>350</v>
       </c>
       <c r="C106" t="s">
         <v>14</v>
       </c>
       <c r="D106" t="s">
-        <v>78</v>
+        <v>351</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B107" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C107" t="s">
         <v>14</v>
       </c>
       <c r="D107" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B108" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="C108" t="s">
         <v>14</v>
       </c>
       <c r="D108" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>353</v>
+        <v>301</v>
       </c>
       <c r="B109" t="s">
-        <v>354</v>
+        <v>117</v>
       </c>
       <c r="C109" t="s">
         <v>14</v>
       </c>
       <c r="D109" t="s">
-        <v>355</v>
+        <v>81</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>302</v>
+        <v>353</v>
       </c>
       <c r="B110" t="s">
-        <v>118</v>
+        <v>354</v>
       </c>
       <c r="C110" t="s">
         <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>119</v>
+        <v>355</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B111" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C111" t="s">
         <v>14</v>
       </c>
       <c r="D111" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>122</v>
+        <v>303</v>
       </c>
       <c r="B112" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C112" t="s">
         <v>14</v>
       </c>
       <c r="D112" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B113" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C113" t="s">
         <v>14</v>
       </c>
       <c r="D113" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B114" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C114" t="s">
         <v>14</v>
       </c>
       <c r="D114" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B115" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C115" t="s">
         <v>14</v>
       </c>
       <c r="D115" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B116" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="C116" t="s">
         <v>14</v>
       </c>
       <c r="D116" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>199</v>
+        <v>134</v>
       </c>
       <c r="B117" t="s">
-        <v>200</v>
+        <v>42</v>
       </c>
       <c r="C117" t="s">
         <v>14</v>
       </c>
       <c r="D117" t="s">
-        <v>201</v>
+        <v>80</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>408</v>
+        <v>199</v>
       </c>
       <c r="B118" t="s">
-        <v>409</v>
+        <v>200</v>
       </c>
       <c r="C118" t="s">
         <v>14</v>
       </c>
       <c r="D118" t="s">
-        <v>410</v>
+        <v>201</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>314</v>
+        <v>408</v>
       </c>
       <c r="B119" t="s">
-        <v>105</v>
+        <v>409</v>
       </c>
       <c r="C119" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="D119" t="s">
-        <v>114</v>
+        <v>410</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B120" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C120" t="s">
         <v>106</v>
       </c>
       <c r="D120" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B121" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C121" t="s">
         <v>106</v>
       </c>
       <c r="D121" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B122" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C122" t="s">
         <v>106</v>
       </c>
       <c r="D122" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B123" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C123" t="s">
         <v>106</v>
       </c>
       <c r="D123" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B124" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="C124" t="s">
         <v>106</v>
       </c>
       <c r="D124" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B125" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="C125" t="s">
         <v>106</v>
       </c>
       <c r="D125" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C126" t="s">
         <v>106</v>
       </c>
       <c r="D126" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B127" t="s">
-        <v>323</v>
+        <v>111</v>
       </c>
       <c r="C127" t="s">
         <v>106</v>
       </c>
       <c r="D127" t="s">
-        <v>324</v>
+        <v>22</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B128" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C128" t="s">
         <v>106</v>
       </c>
       <c r="D128" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>352</v>
+        <v>325</v>
       </c>
       <c r="B129" t="s">
-        <v>400</v>
+        <v>326</v>
       </c>
       <c r="C129" t="s">
         <v>106</v>
       </c>
       <c r="D129" t="s">
-        <v>401</v>
+        <v>327</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>328</v>
+        <v>352</v>
       </c>
       <c r="B130" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="C130" t="s">
         <v>106</v>
       </c>
       <c r="D130" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B131" t="s">
-        <v>329</v>
+        <v>414</v>
       </c>
       <c r="C131" t="s">
         <v>106</v>
       </c>
       <c r="D131" t="s">
-        <v>330</v>
+        <v>415</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>396</v>
+        <v>331</v>
       </c>
       <c r="B132" t="s">
-        <v>394</v>
+        <v>329</v>
       </c>
       <c r="C132" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="D132" t="s">
-        <v>395</v>
+        <v>330</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -3594,127 +3592,141 @@
         <v>396</v>
       </c>
       <c r="B133" t="s">
-        <v>332</v>
+        <v>394</v>
       </c>
       <c r="C133" t="s">
-        <v>106</v>
+        <v>18</v>
       </c>
       <c r="D133" t="s">
-        <v>333</v>
+        <v>395</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="B134" t="s">
-        <v>412</v>
+        <v>332</v>
       </c>
       <c r="C134" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="D134" t="s">
-        <v>413</v>
+        <v>333</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>151</v>
+        <v>411</v>
       </c>
       <c r="B135" t="s">
-        <v>152</v>
+        <v>412</v>
       </c>
       <c r="C135" t="s">
-        <v>153</v>
+        <v>18</v>
       </c>
       <c r="D135" t="s">
-        <v>154</v>
-      </c>
-      <c r="E135" t="s">
-        <v>155</v>
+        <v>413</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B136" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C136" t="s">
         <v>153</v>
       </c>
       <c r="D136" t="s">
-        <v>431</v>
+        <v>154</v>
+      </c>
+      <c r="E136" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>432</v>
+        <v>156</v>
       </c>
       <c r="B137" t="s">
-        <v>433</v>
+        <v>157</v>
       </c>
       <c r="C137" t="s">
         <v>153</v>
       </c>
       <c r="D137" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>221</v>
+        <v>432</v>
       </c>
       <c r="B138" t="s">
-        <v>222</v>
+        <v>433</v>
       </c>
       <c r="C138" t="s">
         <v>153</v>
       </c>
       <c r="D138" t="s">
-        <v>223</v>
+        <v>434</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>264</v>
+        <v>221</v>
       </c>
       <c r="B139" t="s">
-        <v>265</v>
+        <v>222</v>
       </c>
       <c r="C139" t="s">
         <v>153</v>
       </c>
       <c r="D139" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B140" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C140" t="s">
         <v>153</v>
       </c>
       <c r="D140" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="B141" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
       <c r="C141" t="s">
         <v>153</v>
       </c>
       <c r="D141" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>292</v>
+      </c>
+      <c r="B142" t="s">
+        <v>293</v>
+      </c>
+      <c r="C142" t="s">
+        <v>153</v>
+      </c>
+      <c r="D142" t="s">
         <v>294</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Derived variables for expected due dates of f/u forms
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,32 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F457EC-C2C2-F844-8FDD-1091E53934E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02064DC9-4085-9F4C-9505-67D44CFC515C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12600" yWindow="500" windowWidth="23240" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="516">
   <si>
     <t>Variable #</t>
   </si>
@@ -1547,6 +1536,33 @@
   </si>
   <si>
     <t>Dx25</t>
+  </si>
+  <si>
+    <t>30d_due</t>
+  </si>
+  <si>
+    <t>30d follow-up is due at the latest on this date</t>
+  </si>
+  <si>
+    <t>X6b</t>
+  </si>
+  <si>
+    <t>90d_due</t>
+  </si>
+  <si>
+    <t>X6c</t>
+  </si>
+  <si>
+    <t>180d_due</t>
+  </si>
+  <si>
+    <t>X6a</t>
+  </si>
+  <si>
+    <t>90d follow-up is due at the latest on this date</t>
+  </si>
+  <si>
+    <t>180d follow-up is due at the latest on this date</t>
   </si>
 </sst>
 </file>
@@ -1602,10 +1618,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E166" totalsRowShown="0">
-  <autoFilter ref="A1:E166" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E141">
-    <sortCondition ref="A1:A141"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E169" totalsRowShown="0">
+  <autoFilter ref="A1:E169" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState ref="A2:E144">
+    <sortCondition ref="A1:A144"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1939,10 +1955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3922,305 +3938,347 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>289</v>
+        <v>513</v>
       </c>
       <c r="B141" t="s">
-        <v>290</v>
+        <v>507</v>
       </c>
       <c r="C141" t="s">
         <v>151</v>
       </c>
       <c r="D141" t="s">
-        <v>291</v>
+        <v>508</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>435</v>
+        <v>509</v>
       </c>
       <c r="B142" t="s">
-        <v>436</v>
+        <v>510</v>
       </c>
       <c r="C142" t="s">
-        <v>437</v>
+        <v>151</v>
       </c>
       <c r="D142" t="s">
-        <v>503</v>
+        <v>514</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>438</v>
+        <v>511</v>
       </c>
       <c r="B143" t="s">
-        <v>439</v>
+        <v>512</v>
       </c>
       <c r="C143" t="s">
-        <v>437</v>
+        <v>151</v>
       </c>
       <c r="D143" t="s">
-        <v>440</v>
+        <v>515</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>441</v>
+        <v>289</v>
       </c>
       <c r="B144" t="s">
-        <v>442</v>
+        <v>290</v>
       </c>
       <c r="C144" t="s">
-        <v>437</v>
+        <v>151</v>
       </c>
       <c r="D144" t="s">
-        <v>443</v>
+        <v>291</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="B145" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="C145" t="s">
         <v>437</v>
       </c>
       <c r="D145" t="s">
-        <v>446</v>
+        <v>503</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="B146" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="C146" t="s">
         <v>437</v>
       </c>
       <c r="D146" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="B147" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="C147" t="s">
         <v>437</v>
       </c>
+      <c r="D147" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="B148" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="C148" t="s">
         <v>437</v>
       </c>
       <c r="D148" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="B149" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="C149" t="s">
         <v>437</v>
       </c>
       <c r="D149" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="B150" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="C150" t="s">
         <v>437</v>
       </c>
-      <c r="D150" t="s">
-        <v>460</v>
-      </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="B151" t="s">
-        <v>462</v>
+        <v>453</v>
+      </c>
+      <c r="C151" t="s">
+        <v>437</v>
+      </c>
+      <c r="D151" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="B152" t="s">
-        <v>464</v>
+        <v>456</v>
+      </c>
+      <c r="C152" t="s">
+        <v>437</v>
       </c>
       <c r="D152" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="B153" t="s">
-        <v>467</v>
+        <v>459</v>
+      </c>
+      <c r="C153" t="s">
+        <v>437</v>
+      </c>
+      <c r="D153" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B154" t="s">
-        <v>469</v>
-      </c>
-      <c r="D154" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="B155" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="D155" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B156" t="s">
-        <v>475</v>
-      </c>
-      <c r="D156" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="B157" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="D157" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="B158" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="D158" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="B159" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="D159" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="B160" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="D160" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="B161" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="D161" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="B162" t="s">
-        <v>493</v>
+        <v>484</v>
+      </c>
+      <c r="D162" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B163" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="D163" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>504</v>
+        <v>489</v>
       </c>
       <c r="B164" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="D164" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="B165" t="s">
-        <v>499</v>
-      </c>
-      <c r="D165" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>494</v>
+      </c>
+      <c r="B166" t="s">
+        <v>495</v>
+      </c>
+      <c r="D166" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>504</v>
+      </c>
+      <c r="B167" t="s">
+        <v>497</v>
+      </c>
+      <c r="D167" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>505</v>
+      </c>
+      <c r="B168" t="s">
+        <v>499</v>
+      </c>
+      <c r="D168" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
         <v>506</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B169" t="s">
         <v>501</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D169" t="s">
         <v>502</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added several prostate-specific derived variables
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02064DC9-4085-9F4C-9505-67D44CFC515C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7685596D-82D9-2D48-9655-81571B3FB719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="500" windowWidth="23240" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="500" windowWidth="23240" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="536">
   <si>
     <t>Variable #</t>
   </si>
@@ -449,9 +449,6 @@
     <t>Hypertension</t>
   </si>
   <si>
-    <t>D17</t>
-  </si>
-  <si>
     <t>smoking2</t>
   </si>
   <si>
@@ -866,12 +863,6 @@
     <t>D02</t>
   </si>
   <si>
-    <t>D03</t>
-  </si>
-  <si>
-    <t>D04</t>
-  </si>
-  <si>
     <t>D04a</t>
   </si>
   <si>
@@ -926,21 +917,12 @@
     <t>Ca01a</t>
   </si>
   <si>
-    <t>Ca03</t>
-  </si>
-  <si>
     <t>Ca04</t>
   </si>
   <si>
-    <t>Ca05</t>
-  </si>
-  <si>
     <t>Ca06</t>
   </si>
   <si>
-    <t>Ca07</t>
-  </si>
-  <si>
     <t>Ca08</t>
   </si>
   <si>
@@ -1563,6 +1545,84 @@
   </si>
   <si>
     <t>180d follow-up is due at the latest on this date</t>
+  </si>
+  <si>
+    <t>D05</t>
+  </si>
+  <si>
+    <t>ethnicity</t>
+  </si>
+  <si>
+    <t>Ca03b</t>
+  </si>
+  <si>
+    <t>Ca03a</t>
+  </si>
+  <si>
+    <t>D03a</t>
+  </si>
+  <si>
+    <t>D03b</t>
+  </si>
+  <si>
+    <t>D04b</t>
+  </si>
+  <si>
+    <t>Ca07c</t>
+  </si>
+  <si>
+    <t>X8</t>
+  </si>
+  <si>
+    <t>gleason</t>
+  </si>
+  <si>
+    <t>Gleason score derived variable</t>
+  </si>
+  <si>
+    <t>Ca14</t>
+  </si>
+  <si>
+    <t>ARA_1st_gen</t>
+  </si>
+  <si>
+    <t>Bicalutamide Flutamide Nilutamide (1st gen ARA)</t>
+  </si>
+  <si>
+    <t>ARA_2nd_gen</t>
+  </si>
+  <si>
+    <t>Enzalutamide, Apalutamide, Darolutamide (2nd gen ARA)</t>
+  </si>
+  <si>
+    <t>Ca15</t>
+  </si>
+  <si>
+    <t>Ca16</t>
+  </si>
+  <si>
+    <t>abi</t>
+  </si>
+  <si>
+    <t>Abiraterone</t>
+  </si>
+  <si>
+    <t>Ca17</t>
+  </si>
+  <si>
+    <t>chemo_prca</t>
+  </si>
+  <si>
+    <t>Chemotherapy for prostate cancer (cabazitaxel, carboplatin, docetaxel)</t>
+  </si>
+  <si>
+    <t>Ca18</t>
+  </si>
+  <si>
+    <t>adt</t>
+  </si>
+  <si>
+    <t>ADT for prostate cancer</t>
   </si>
 </sst>
 </file>
@@ -1618,10 +1678,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E169" totalsRowShown="0">
-  <autoFilter ref="A1:E169" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState ref="A2:E144">
-    <sortCondition ref="A1:A144"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E176" totalsRowShown="0">
+  <autoFilter ref="A1:E176" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E175">
+    <sortCondition ref="A1:A175"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -1955,10 +2015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1989,21 +2049,21 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="B2" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="B3" t="s">
         <v>136</v>
@@ -2012,26 +2072,26 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="B4" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -2045,7 +2105,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
@@ -2059,21 +2119,21 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -2087,7 +2147,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B9" t="s">
         <v>40</v>
@@ -2101,7 +2161,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
@@ -2115,7 +2175,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
@@ -2129,7 +2189,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="B12" t="s">
         <v>56</v>
@@ -2143,7 +2203,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B13" t="s">
         <v>142</v>
@@ -2157,63 +2217,63 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="B15" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="B16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="B17" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -2227,35 +2287,35 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="B20" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>303</v>
+        <v>513</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
@@ -2269,35 +2329,35 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>304</v>
+        <v>512</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -2311,10 +2371,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>307</v>
+        <v>387</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -2325,1961 +2385,2056 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>393</v>
+        <v>409</v>
       </c>
       <c r="B26" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>415</v>
+        <v>517</v>
       </c>
       <c r="B27" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" t="s">
         <v>208</v>
-      </c>
-      <c r="B31" t="s">
-        <v>209</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B32" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B33" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>368</v>
+      </c>
+      <c r="B34" t="s">
         <v>374</v>
-      </c>
-      <c r="B34" t="s">
-        <v>380</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>369</v>
+      </c>
+      <c r="B35" t="s">
         <v>375</v>
-      </c>
-      <c r="B35" t="s">
-        <v>381</v>
       </c>
       <c r="C35" t="s">
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>370</v>
+      </c>
+      <c r="B36" t="s">
         <v>376</v>
-      </c>
-      <c r="B36" t="s">
-        <v>382</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>371</v>
+      </c>
+      <c r="B37" t="s">
         <v>377</v>
-      </c>
-      <c r="B37" t="s">
-        <v>383</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="B38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="B40" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41" t="s">
         <v>202</v>
-      </c>
-      <c r="B41" t="s">
-        <v>203</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>221</v>
+      </c>
+      <c r="B42" t="s">
         <v>222</v>
-      </c>
-      <c r="B42" t="s">
-        <v>223</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>224</v>
+      </c>
+      <c r="B43" t="s">
         <v>225</v>
-      </c>
-      <c r="B43" t="s">
-        <v>226</v>
       </c>
       <c r="C43" t="s">
         <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>281</v>
+        <v>521</v>
       </c>
       <c r="B44" t="s">
-        <v>134</v>
+        <v>522</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>47</v>
+        <v>523</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>282</v>
+        <v>526</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>524</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>46</v>
+        <v>525</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>283</v>
+        <v>527</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>528</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>147</v>
+        <v>529</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>284</v>
+        <v>530</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>531</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>64</v>
+        <v>532</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>285</v>
+        <v>533</v>
       </c>
       <c r="B48" t="s">
-        <v>204</v>
+        <v>534</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>205</v>
+        <v>535</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>138</v>
+        <v>281</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>335</v>
+        <v>514</v>
       </c>
       <c r="B51" t="s">
-        <v>336</v>
+        <v>135</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>337</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>139</v>
+        <v>515</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>144</v>
+        <v>282</v>
       </c>
       <c r="B53" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>146</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>170</v>
+        <v>516</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
       <c r="C54" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>172</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>194</v>
+        <v>510</v>
       </c>
       <c r="B55" t="s">
-        <v>195</v>
+        <v>511</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
       </c>
-      <c r="D55" t="s">
-        <v>196</v>
-      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>249</v>
+        <v>283</v>
       </c>
       <c r="B56" t="s">
-        <v>166</v>
+        <v>20</v>
       </c>
       <c r="C56" t="s">
-        <v>167</v>
+        <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>168</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>250</v>
+        <v>138</v>
       </c>
       <c r="B57" t="s">
-        <v>175</v>
+        <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>176</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>251</v>
+        <v>329</v>
       </c>
       <c r="B58" t="s">
-        <v>177</v>
+        <v>330</v>
       </c>
       <c r="C58" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>178</v>
+        <v>331</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>252</v>
+        <v>139</v>
       </c>
       <c r="B59" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="C59" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>253</v>
+        <v>169</v>
       </c>
       <c r="B60" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C60" t="s">
-        <v>167</v>
+        <v>15</v>
       </c>
       <c r="D60" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>254</v>
+        <v>193</v>
       </c>
       <c r="B61" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="C61" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>255</v>
+        <v>429</v>
       </c>
       <c r="B62" t="s">
-        <v>185</v>
+        <v>430</v>
       </c>
       <c r="C62" t="s">
-        <v>167</v>
+        <v>431</v>
       </c>
       <c r="D62" t="s">
-        <v>186</v>
+        <v>497</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>256</v>
+        <v>432</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>433</v>
       </c>
       <c r="C63" t="s">
-        <v>167</v>
+        <v>431</v>
       </c>
       <c r="D63" t="s">
-        <v>188</v>
+        <v>434</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>257</v>
+        <v>435</v>
       </c>
       <c r="B64" t="s">
-        <v>189</v>
+        <v>436</v>
       </c>
       <c r="C64" t="s">
-        <v>167</v>
+        <v>431</v>
       </c>
       <c r="D64" t="s">
-        <v>190</v>
+        <v>437</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>191</v>
+        <v>438</v>
       </c>
       <c r="B65" t="s">
-        <v>192</v>
+        <v>439</v>
       </c>
       <c r="C65" t="s">
-        <v>167</v>
+        <v>431</v>
       </c>
       <c r="D65" t="s">
-        <v>193</v>
+        <v>440</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>228</v>
+        <v>441</v>
       </c>
       <c r="B66" t="s">
-        <v>232</v>
+        <v>442</v>
       </c>
       <c r="C66" t="s">
-        <v>167</v>
+        <v>431</v>
       </c>
       <c r="D66" t="s">
-        <v>233</v>
+        <v>443</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>234</v>
+        <v>444</v>
       </c>
       <c r="B67" t="s">
-        <v>235</v>
+        <v>445</v>
       </c>
       <c r="C67" t="s">
-        <v>167</v>
-      </c>
-      <c r="D67" t="s">
-        <v>236</v>
+        <v>431</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>237</v>
+        <v>446</v>
       </c>
       <c r="B68" t="s">
-        <v>238</v>
+        <v>447</v>
       </c>
       <c r="C68" t="s">
-        <v>167</v>
+        <v>431</v>
       </c>
       <c r="D68" t="s">
-        <v>239</v>
+        <v>448</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>240</v>
+        <v>449</v>
       </c>
       <c r="B69" t="s">
-        <v>241</v>
+        <v>450</v>
       </c>
       <c r="C69" t="s">
-        <v>167</v>
+        <v>431</v>
       </c>
       <c r="D69" t="s">
-        <v>242</v>
+        <v>451</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>243</v>
+        <v>452</v>
       </c>
       <c r="B70" t="s">
-        <v>244</v>
+        <v>453</v>
       </c>
       <c r="C70" t="s">
-        <v>167</v>
+        <v>431</v>
       </c>
       <c r="D70" t="s">
-        <v>245</v>
+        <v>454</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>246</v>
+        <v>455</v>
       </c>
       <c r="B71" t="s">
-        <v>247</v>
-      </c>
-      <c r="C71" t="s">
-        <v>167</v>
-      </c>
-      <c r="D71" t="s">
-        <v>248</v>
+        <v>456</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>231</v>
+        <v>457</v>
       </c>
       <c r="B72" t="s">
-        <v>229</v>
-      </c>
-      <c r="C72" t="s">
-        <v>167</v>
+        <v>458</v>
       </c>
       <c r="D72" t="s">
-        <v>230</v>
+        <v>459</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>258</v>
+        <v>460</v>
       </c>
       <c r="B73" t="s">
-        <v>259</v>
-      </c>
-      <c r="C73" t="s">
-        <v>167</v>
-      </c>
-      <c r="D73" t="s">
-        <v>260</v>
+        <v>461</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>398</v>
+        <v>462</v>
       </c>
       <c r="B74" t="s">
-        <v>399</v>
-      </c>
-      <c r="C74" t="s">
-        <v>167</v>
+        <v>463</v>
       </c>
       <c r="D74" t="s">
-        <v>400</v>
+        <v>464</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>269</v>
+        <v>465</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75" t="s">
-        <v>6</v>
+        <v>466</v>
       </c>
       <c r="D75" t="s">
-        <v>58</v>
+        <v>467</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>270</v>
+        <v>468</v>
       </c>
       <c r="B76" t="s">
-        <v>11</v>
-      </c>
-      <c r="C76" t="s">
-        <v>6</v>
+        <v>469</v>
       </c>
       <c r="D76" t="s">
-        <v>59</v>
+        <v>470</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>332</v>
+        <v>471</v>
       </c>
       <c r="B77" t="s">
-        <v>333</v>
-      </c>
-      <c r="C77" t="s">
-        <v>6</v>
+        <v>472</v>
       </c>
       <c r="D77" t="s">
-        <v>334</v>
+        <v>473</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>271</v>
+        <v>474</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
-      </c>
-      <c r="C78" t="s">
-        <v>6</v>
+        <v>475</v>
       </c>
       <c r="D78" t="s">
-        <v>60</v>
+        <v>476</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>272</v>
+        <v>477</v>
       </c>
       <c r="B79" t="s">
-        <v>330</v>
-      </c>
-      <c r="C79" t="s">
-        <v>6</v>
+        <v>478</v>
       </c>
       <c r="D79" t="s">
-        <v>331</v>
+        <v>479</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>273</v>
+        <v>480</v>
       </c>
       <c r="B80" t="s">
-        <v>12</v>
-      </c>
-      <c r="C80" t="s">
-        <v>6</v>
+        <v>481</v>
       </c>
       <c r="D80" t="s">
-        <v>61</v>
+        <v>482</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>274</v>
+        <v>483</v>
       </c>
       <c r="B81" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" t="s">
-        <v>6</v>
+        <v>484</v>
       </c>
       <c r="D81" t="s">
-        <v>83</v>
+        <v>485</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>275</v>
+        <v>486</v>
       </c>
       <c r="B82" t="s">
-        <v>26</v>
-      </c>
-      <c r="C82" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" t="s">
-        <v>217</v>
+        <v>487</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>276</v>
+        <v>488</v>
       </c>
       <c r="B83" t="s">
-        <v>27</v>
-      </c>
-      <c r="C83" t="s">
-        <v>6</v>
+        <v>489</v>
       </c>
       <c r="D83" t="s">
-        <v>287</v>
+        <v>490</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>277</v>
+        <v>498</v>
       </c>
       <c r="B84" t="s">
-        <v>48</v>
-      </c>
-      <c r="C84" t="s">
-        <v>6</v>
+        <v>491</v>
       </c>
       <c r="D84" t="s">
-        <v>288</v>
+        <v>492</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>499</v>
       </c>
       <c r="B85" t="s">
-        <v>85</v>
-      </c>
-      <c r="C85" t="s">
-        <v>6</v>
+        <v>493</v>
       </c>
       <c r="D85" t="s">
-        <v>86</v>
+        <v>494</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>500</v>
       </c>
       <c r="B86" t="s">
-        <v>33</v>
-      </c>
-      <c r="C86" t="s">
-        <v>6</v>
+        <v>495</v>
       </c>
       <c r="D86" t="s">
-        <v>72</v>
+        <v>496</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>248</v>
       </c>
       <c r="B87" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="C87" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="D87" t="s">
-        <v>99</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>249</v>
       </c>
       <c r="B88" t="s">
-        <v>91</v>
+        <v>174</v>
       </c>
       <c r="C88" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="D88" t="s">
-        <v>98</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>250</v>
       </c>
       <c r="B89" t="s">
-        <v>93</v>
+        <v>176</v>
       </c>
       <c r="C89" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="D89" t="s">
-        <v>97</v>
+        <v>177</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>94</v>
+        <v>251</v>
       </c>
       <c r="B90" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="C90" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="D90" t="s">
-        <v>96</v>
+        <v>178</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>252</v>
       </c>
       <c r="B91" t="s">
-        <v>38</v>
+        <v>180</v>
       </c>
       <c r="C91" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="D91" t="s">
-        <v>101</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>102</v>
+        <v>253</v>
       </c>
       <c r="B92" t="s">
-        <v>53</v>
+        <v>182</v>
       </c>
       <c r="C92" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="D92" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="B93" t="s">
-        <v>22</v>
+        <v>184</v>
       </c>
       <c r="C93" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="D93" t="s">
-        <v>66</v>
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>160</v>
+        <v>255</v>
       </c>
       <c r="B94" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="C94" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="D94" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>431</v>
+        <v>256</v>
       </c>
       <c r="B95" t="s">
-        <v>432</v>
+        <v>188</v>
       </c>
       <c r="C95" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="D95" t="s">
-        <v>433</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>163</v>
+        <v>190</v>
       </c>
       <c r="B96" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="C96" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="D96" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>418</v>
+        <v>227</v>
       </c>
       <c r="B97" t="s">
-        <v>419</v>
+        <v>231</v>
       </c>
       <c r="C97" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="D97" t="s">
-        <v>420</v>
+        <v>232</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>278</v>
+        <v>233</v>
       </c>
       <c r="B98" t="s">
-        <v>279</v>
+        <v>234</v>
       </c>
       <c r="C98" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="D98" t="s">
-        <v>280</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>338</v>
+        <v>236</v>
       </c>
       <c r="B99" t="s">
-        <v>339</v>
+        <v>237</v>
       </c>
       <c r="C99" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="D99" t="s">
-        <v>340</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>341</v>
+        <v>239</v>
       </c>
       <c r="B100" t="s">
-        <v>342</v>
+        <v>240</v>
       </c>
       <c r="C100" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="D100" t="s">
-        <v>343</v>
+        <v>241</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B101" t="s">
-        <v>13</v>
+        <v>243</v>
       </c>
       <c r="C101" t="s">
-        <v>14</v>
+        <v>166</v>
       </c>
       <c r="D101" t="s">
-        <v>62</v>
+        <v>244</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>293</v>
+        <v>245</v>
       </c>
       <c r="B102" t="s">
-        <v>30</v>
+        <v>246</v>
       </c>
       <c r="C102" t="s">
-        <v>14</v>
+        <v>166</v>
       </c>
       <c r="D102" t="s">
-        <v>71</v>
+        <v>247</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>294</v>
+        <v>230</v>
       </c>
       <c r="B103" t="s">
-        <v>51</v>
+        <v>228</v>
       </c>
       <c r="C103" t="s">
-        <v>14</v>
+        <v>166</v>
       </c>
       <c r="D103" t="s">
-        <v>78</v>
+        <v>229</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>295</v>
+        <v>257</v>
       </c>
       <c r="B104" t="s">
-        <v>345</v>
+        <v>258</v>
       </c>
       <c r="C104" t="s">
-        <v>14</v>
+        <v>166</v>
       </c>
       <c r="D104" t="s">
-        <v>115</v>
+        <v>259</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>344</v>
+        <v>392</v>
       </c>
       <c r="B105" t="s">
-        <v>346</v>
+        <v>393</v>
       </c>
       <c r="C105" t="s">
-        <v>14</v>
+        <v>166</v>
       </c>
       <c r="D105" t="s">
-        <v>347</v>
+        <v>394</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
       <c r="B106" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="C106" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D106" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
       <c r="B107" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="C107" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D107" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="B108" t="s">
-        <v>116</v>
+        <v>327</v>
       </c>
       <c r="C108" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D108" t="s">
-        <v>80</v>
+        <v>328</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>349</v>
+        <v>270</v>
       </c>
       <c r="B109" t="s">
-        <v>350</v>
+        <v>10</v>
       </c>
       <c r="C109" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D109" t="s">
-        <v>351</v>
+        <v>60</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="B110" t="s">
-        <v>117</v>
+        <v>324</v>
       </c>
       <c r="C110" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>118</v>
+        <v>325</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>300</v>
+        <v>272</v>
       </c>
       <c r="B111" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="C111" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>121</v>
+        <v>273</v>
       </c>
       <c r="B112" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="C112" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>125</v>
+        <v>274</v>
       </c>
       <c r="B113" t="s">
-        <v>126</v>
+        <v>26</v>
       </c>
       <c r="C113" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>124</v>
+        <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>128</v>
+        <v>275</v>
       </c>
       <c r="B114" t="s">
-        <v>129</v>
+        <v>27</v>
       </c>
       <c r="C114" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>127</v>
+        <v>284</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>132</v>
+        <v>276</v>
       </c>
       <c r="B115" t="s">
-        <v>131</v>
+        <v>48</v>
       </c>
       <c r="C115" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>130</v>
+        <v>285</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
       <c r="B116" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C116" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>197</v>
+        <v>87</v>
       </c>
       <c r="B117" t="s">
-        <v>198</v>
+        <v>33</v>
       </c>
       <c r="C117" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>199</v>
+        <v>72</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>404</v>
+        <v>88</v>
       </c>
       <c r="B118" t="s">
-        <v>405</v>
+        <v>89</v>
       </c>
       <c r="C118" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D118" t="s">
-        <v>406</v>
+        <v>99</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>310</v>
+        <v>90</v>
       </c>
       <c r="B119" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C119" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="D119" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>311</v>
+        <v>92</v>
       </c>
       <c r="B120" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C120" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="D120" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>312</v>
+        <v>94</v>
       </c>
       <c r="B121" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C121" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="D121" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>313</v>
+        <v>100</v>
       </c>
       <c r="B122" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="C122" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="D122" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>314</v>
+        <v>102</v>
       </c>
       <c r="B123" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="C123" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>315</v>
+        <v>114</v>
       </c>
       <c r="B124" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C124" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>316</v>
+        <v>159</v>
       </c>
       <c r="B125" t="s">
-        <v>109</v>
+        <v>160</v>
       </c>
       <c r="C125" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>111</v>
+        <v>161</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>317</v>
+        <v>425</v>
       </c>
       <c r="B126" t="s">
-        <v>110</v>
+        <v>426</v>
       </c>
       <c r="C126" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>21</v>
+        <v>427</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>318</v>
+        <v>162</v>
       </c>
       <c r="B127" t="s">
-        <v>319</v>
+        <v>163</v>
       </c>
       <c r="C127" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>320</v>
+        <v>164</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>321</v>
+        <v>412</v>
       </c>
       <c r="B128" t="s">
-        <v>322</v>
+        <v>413</v>
       </c>
       <c r="C128" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>348</v>
+        <v>277</v>
       </c>
       <c r="B129" t="s">
-        <v>396</v>
+        <v>278</v>
       </c>
       <c r="C129" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="B130" t="s">
-        <v>410</v>
+        <v>333</v>
       </c>
       <c r="C130" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="B131" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
       <c r="C131" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>392</v>
+        <v>289</v>
       </c>
       <c r="B132" t="s">
-        <v>390</v>
+        <v>13</v>
       </c>
       <c r="C132" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D132" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>392</v>
+        <v>290</v>
       </c>
       <c r="B133" t="s">
-        <v>328</v>
+        <v>30</v>
       </c>
       <c r="C133" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="D133" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>407</v>
+        <v>291</v>
       </c>
       <c r="B134" t="s">
-        <v>408</v>
+        <v>51</v>
       </c>
       <c r="C134" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D134" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>149</v>
+        <v>292</v>
       </c>
       <c r="B135" t="s">
-        <v>150</v>
+        <v>339</v>
       </c>
       <c r="C135" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="D135" t="s">
-        <v>152</v>
-      </c>
-      <c r="E135" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>154</v>
+        <v>338</v>
       </c>
       <c r="B136" t="s">
-        <v>155</v>
+        <v>340</v>
       </c>
       <c r="C136" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="D136" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>428</v>
+        <v>293</v>
       </c>
       <c r="B137" t="s">
-        <v>429</v>
+        <v>55</v>
       </c>
       <c r="C137" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="D137" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>218</v>
+        <v>294</v>
       </c>
       <c r="B138" t="s">
-        <v>219</v>
+        <v>75</v>
       </c>
       <c r="C138" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="D138" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>261</v>
+        <v>295</v>
       </c>
       <c r="B139" t="s">
-        <v>262</v>
+        <v>116</v>
       </c>
       <c r="C139" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="D139" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>264</v>
+        <v>343</v>
       </c>
       <c r="B140" t="s">
-        <v>265</v>
+        <v>344</v>
       </c>
       <c r="C140" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="D140" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>513</v>
+        <v>296</v>
       </c>
       <c r="B141" t="s">
-        <v>507</v>
+        <v>117</v>
       </c>
       <c r="C141" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="D141" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>509</v>
+        <v>297</v>
       </c>
       <c r="B142" t="s">
-        <v>510</v>
+        <v>119</v>
       </c>
       <c r="C142" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="D142" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>511</v>
+        <v>121</v>
       </c>
       <c r="B143" t="s">
-        <v>512</v>
+        <v>122</v>
       </c>
       <c r="C143" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="D143" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>289</v>
+        <v>125</v>
       </c>
       <c r="B144" t="s">
-        <v>290</v>
+        <v>126</v>
       </c>
       <c r="C144" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="D144" t="s">
-        <v>291</v>
+        <v>124</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>435</v>
+        <v>128</v>
       </c>
       <c r="B145" t="s">
-        <v>436</v>
+        <v>129</v>
       </c>
       <c r="C145" t="s">
-        <v>437</v>
+        <v>14</v>
       </c>
       <c r="D145" t="s">
-        <v>503</v>
+        <v>127</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>438</v>
+        <v>132</v>
       </c>
       <c r="B146" t="s">
-        <v>439</v>
+        <v>131</v>
       </c>
       <c r="C146" t="s">
-        <v>437</v>
+        <v>14</v>
       </c>
       <c r="D146" t="s">
-        <v>440</v>
+        <v>130</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>441</v>
+        <v>133</v>
       </c>
       <c r="B147" t="s">
-        <v>442</v>
+        <v>41</v>
       </c>
       <c r="C147" t="s">
-        <v>437</v>
+        <v>14</v>
       </c>
       <c r="D147" t="s">
-        <v>443</v>
+        <v>79</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>444</v>
+        <v>196</v>
       </c>
       <c r="B148" t="s">
-        <v>445</v>
+        <v>197</v>
       </c>
       <c r="C148" t="s">
-        <v>437</v>
+        <v>14</v>
       </c>
       <c r="D148" t="s">
-        <v>446</v>
+        <v>198</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>447</v>
+        <v>398</v>
       </c>
       <c r="B149" t="s">
-        <v>448</v>
+        <v>399</v>
       </c>
       <c r="C149" t="s">
-        <v>437</v>
+        <v>14</v>
       </c>
       <c r="D149" t="s">
-        <v>449</v>
+        <v>400</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>450</v>
+        <v>304</v>
       </c>
       <c r="B150" t="s">
-        <v>451</v>
+        <v>104</v>
       </c>
       <c r="C150" t="s">
-        <v>437</v>
+        <v>105</v>
+      </c>
+      <c r="D150" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>452</v>
+        <v>305</v>
       </c>
       <c r="B151" t="s">
-        <v>453</v>
+        <v>103</v>
       </c>
       <c r="C151" t="s">
-        <v>437</v>
+        <v>105</v>
       </c>
       <c r="D151" t="s">
-        <v>454</v>
+        <v>21</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>455</v>
+        <v>306</v>
       </c>
       <c r="B152" t="s">
-        <v>456</v>
+        <v>106</v>
       </c>
       <c r="C152" t="s">
-        <v>437</v>
+        <v>105</v>
       </c>
       <c r="D152" t="s">
-        <v>457</v>
+        <v>23</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>458</v>
+        <v>307</v>
       </c>
       <c r="B153" t="s">
-        <v>459</v>
+        <v>108</v>
       </c>
       <c r="C153" t="s">
-        <v>437</v>
+        <v>105</v>
       </c>
       <c r="D153" t="s">
-        <v>460</v>
+        <v>112</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>461</v>
+        <v>308</v>
       </c>
       <c r="B154" t="s">
-        <v>462</v>
+        <v>107</v>
+      </c>
+      <c r="C154" t="s">
+        <v>105</v>
+      </c>
+      <c r="D154" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>463</v>
+        <v>309</v>
       </c>
       <c r="B155" t="s">
-        <v>464</v>
+        <v>31</v>
+      </c>
+      <c r="C155" t="s">
+        <v>105</v>
       </c>
       <c r="D155" t="s">
-        <v>465</v>
+        <v>32</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>466</v>
+        <v>310</v>
       </c>
       <c r="B156" t="s">
-        <v>467</v>
+        <v>109</v>
+      </c>
+      <c r="C156" t="s">
+        <v>105</v>
+      </c>
+      <c r="D156" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>468</v>
+        <v>311</v>
       </c>
       <c r="B157" t="s">
-        <v>469</v>
+        <v>110</v>
+      </c>
+      <c r="C157" t="s">
+        <v>105</v>
       </c>
       <c r="D157" t="s">
-        <v>470</v>
+        <v>21</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>471</v>
+        <v>312</v>
       </c>
       <c r="B158" t="s">
-        <v>472</v>
+        <v>313</v>
+      </c>
+      <c r="C158" t="s">
+        <v>105</v>
       </c>
       <c r="D158" t="s">
-        <v>473</v>
+        <v>314</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>474</v>
+        <v>315</v>
       </c>
       <c r="B159" t="s">
-        <v>475</v>
+        <v>316</v>
+      </c>
+      <c r="C159" t="s">
+        <v>105</v>
       </c>
       <c r="D159" t="s">
-        <v>476</v>
+        <v>317</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>477</v>
+        <v>342</v>
       </c>
       <c r="B160" t="s">
-        <v>478</v>
+        <v>390</v>
+      </c>
+      <c r="C160" t="s">
+        <v>105</v>
       </c>
       <c r="D160" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>480</v>
+        <v>318</v>
       </c>
       <c r="B161" t="s">
-        <v>481</v>
+        <v>404</v>
+      </c>
+      <c r="C161" t="s">
+        <v>105</v>
       </c>
       <c r="D161" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>483</v>
+        <v>321</v>
       </c>
       <c r="B162" t="s">
-        <v>484</v>
+        <v>319</v>
+      </c>
+      <c r="C162" t="s">
+        <v>105</v>
       </c>
       <c r="D162" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>486</v>
+        <v>386</v>
       </c>
       <c r="B163" t="s">
-        <v>487</v>
+        <v>384</v>
+      </c>
+      <c r="C163" t="s">
+        <v>18</v>
       </c>
       <c r="D163" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>489</v>
+        <v>386</v>
       </c>
       <c r="B164" t="s">
-        <v>490</v>
+        <v>322</v>
+      </c>
+      <c r="C164" t="s">
+        <v>105</v>
       </c>
       <c r="D164" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>492</v>
+        <v>401</v>
       </c>
       <c r="B165" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+      <c r="C165" t="s">
+        <v>18</v>
+      </c>
+      <c r="D165" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>494</v>
+        <v>148</v>
       </c>
       <c r="B166" t="s">
-        <v>495</v>
+        <v>149</v>
+      </c>
+      <c r="C166" t="s">
+        <v>150</v>
       </c>
       <c r="D166" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="E166" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>153</v>
+      </c>
+      <c r="B167" t="s">
+        <v>154</v>
+      </c>
+      <c r="C167" t="s">
+        <v>150</v>
+      </c>
+      <c r="D167" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>422</v>
+      </c>
+      <c r="B168" t="s">
+        <v>423</v>
+      </c>
+      <c r="C168" t="s">
+        <v>150</v>
+      </c>
+      <c r="D168" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>217</v>
+      </c>
+      <c r="B169" t="s">
+        <v>218</v>
+      </c>
+      <c r="C169" t="s">
+        <v>150</v>
+      </c>
+      <c r="D169" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>260</v>
+      </c>
+      <c r="B170" t="s">
+        <v>261</v>
+      </c>
+      <c r="C170" t="s">
+        <v>150</v>
+      </c>
+      <c r="D170" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>263</v>
+      </c>
+      <c r="B171" t="s">
+        <v>264</v>
+      </c>
+      <c r="C171" t="s">
+        <v>150</v>
+      </c>
+      <c r="D171" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>507</v>
+      </c>
+      <c r="B172" t="s">
+        <v>501</v>
+      </c>
+      <c r="C172" t="s">
+        <v>150</v>
+      </c>
+      <c r="D172" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>503</v>
+      </c>
+      <c r="B173" t="s">
         <v>504</v>
       </c>
-      <c r="B167" t="s">
-        <v>497</v>
-      </c>
-      <c r="D167" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
+      <c r="C173" t="s">
+        <v>150</v>
+      </c>
+      <c r="D173" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
         <v>505</v>
       </c>
-      <c r="B168" t="s">
-        <v>499</v>
-      </c>
-      <c r="D168" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
+      <c r="B174" t="s">
         <v>506</v>
       </c>
-      <c r="B169" t="s">
-        <v>501</v>
-      </c>
-      <c r="D169" t="s">
-        <v>502</v>
+      <c r="C174" t="s">
+        <v>150</v>
+      </c>
+      <c r="D174" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>286</v>
+      </c>
+      <c r="B175" t="s">
+        <v>287</v>
+      </c>
+      <c r="C175" t="s">
+        <v>150</v>
+      </c>
+      <c r="D175" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>518</v>
+      </c>
+      <c r="B176" t="s">
+        <v>519</v>
+      </c>
+      <c r="C176" t="s">
+        <v>150</v>
+      </c>
+      <c r="D176" t="s">
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new ordinal with death ever
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7685596D-82D9-2D48-9655-81571B3FB719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFE199A-52AF-B54E-9938-64CD018057A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="500" windowWidth="23240" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="500" windowWidth="32960" windowHeight="21680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="539">
   <si>
     <t>Variable #</t>
   </si>
@@ -1019,9 +1030,6 @@
     <t>ordinal_v1</t>
   </si>
   <si>
-    <t>Custom ordinal outcome ignoring oxygen requirement</t>
-  </si>
-  <si>
     <t>O23</t>
   </si>
   <si>
@@ -1623,6 +1631,18 @@
   </si>
   <si>
     <t>ADT for prostate cancer</t>
+  </si>
+  <si>
+    <t>O22a</t>
+  </si>
+  <si>
+    <t>ordinal_v1a</t>
+  </si>
+  <si>
+    <t>Custom ordinal outcome with death at any time</t>
+  </si>
+  <si>
+    <t>Custom ordinal outcome with death within 30 days</t>
   </si>
 </sst>
 </file>
@@ -1678,10 +1698,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E176" totalsRowShown="0">
-  <autoFilter ref="A1:E176" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E175">
-    <sortCondition ref="A1:A175"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E177" totalsRowShown="0">
+  <autoFilter ref="A1:E177" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E176">
+    <sortCondition ref="A1:A176"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -2015,10 +2035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E176"/>
+  <dimension ref="A1:E177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2049,21 +2069,21 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B3" t="s">
         <v>136</v>
@@ -2072,26 +2092,26 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B4" t="s">
         <v>416</v>
-      </c>
-      <c r="B4" t="s">
-        <v>417</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -2105,7 +2125,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
@@ -2119,7 +2139,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B7" t="s">
         <v>205</v>
@@ -2133,7 +2153,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -2147,7 +2167,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B9" t="s">
         <v>40</v>
@@ -2161,7 +2181,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
@@ -2175,7 +2195,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
@@ -2189,7 +2209,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B12" t="s">
         <v>56</v>
@@ -2203,7 +2223,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B13" t="s">
         <v>142</v>
@@ -2217,7 +2237,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B14" t="s">
         <v>199</v>
@@ -2231,21 +2251,21 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>357</v>
+      </c>
+      <c r="B15" t="s">
         <v>358</v>
-      </c>
-      <c r="B15" t="s">
-        <v>359</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B16" t="s">
         <v>266</v>
@@ -2259,16 +2279,16 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>405</v>
+      </c>
+      <c r="B17" t="s">
         <v>406</v>
-      </c>
-      <c r="B17" t="s">
-        <v>407</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2296,26 +2316,26 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>361</v>
+      </c>
+      <c r="B20" t="s">
         <v>362</v>
-      </c>
-      <c r="B20" t="s">
-        <v>363</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
@@ -2329,7 +2349,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B22" t="s">
         <v>73</v>
@@ -2371,7 +2391,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B25" t="s">
         <v>147</v>
@@ -2385,30 +2405,30 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B27" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -2472,13 +2492,13 @@
         <v>210</v>
       </c>
       <c r="B32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2486,74 +2506,74 @@
         <v>213</v>
       </c>
       <c r="B33" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B34" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B35" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C35" t="s">
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B36" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B37" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B38" t="s">
         <v>211</v>
@@ -2567,7 +2587,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B39" t="s">
         <v>214</v>
@@ -2581,16 +2601,16 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>394</v>
+      </c>
+      <c r="B40" t="s">
         <v>395</v>
-      </c>
-      <c r="B40" t="s">
-        <v>396</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -2604,7 +2624,7 @@
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -2637,72 +2657,72 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>520</v>
+      </c>
+      <c r="B44" t="s">
         <v>521</v>
-      </c>
-      <c r="B44" t="s">
-        <v>522</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B45" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C45" t="s">
         <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>526</v>
+      </c>
+      <c r="B46" t="s">
         <v>527</v>
-      </c>
-      <c r="B46" t="s">
-        <v>528</v>
       </c>
       <c r="C46" t="s">
         <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>529</v>
+      </c>
+      <c r="B47" t="s">
         <v>530</v>
-      </c>
-      <c r="B47" t="s">
-        <v>531</v>
       </c>
       <c r="C47" t="s">
         <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>532</v>
+      </c>
+      <c r="B48" t="s">
         <v>533</v>
-      </c>
-      <c r="B48" t="s">
-        <v>534</v>
       </c>
       <c r="C48" t="s">
         <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -2735,7 +2755,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B51" t="s">
         <v>135</v>
@@ -2749,7 +2769,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B52" t="s">
         <v>144</v>
@@ -2777,7 +2797,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B54" t="s">
         <v>203</v>
@@ -2791,10 +2811,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>509</v>
+      </c>
+      <c r="B55" t="s">
         <v>510</v>
-      </c>
-      <c r="B55" t="s">
-        <v>511</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -2886,292 +2906,292 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>428</v>
+      </c>
+      <c r="B62" t="s">
         <v>429</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>430</v>
       </c>
-      <c r="C62" t="s">
-        <v>431</v>
-      </c>
       <c r="D62" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>431</v>
+      </c>
+      <c r="B63" t="s">
         <v>432</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
+        <v>430</v>
+      </c>
+      <c r="D63" t="s">
         <v>433</v>
-      </c>
-      <c r="C63" t="s">
-        <v>431</v>
-      </c>
-      <c r="D63" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>434</v>
+      </c>
+      <c r="B64" t="s">
         <v>435</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
+        <v>430</v>
+      </c>
+      <c r="D64" t="s">
         <v>436</v>
-      </c>
-      <c r="C64" t="s">
-        <v>431</v>
-      </c>
-      <c r="D64" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>437</v>
+      </c>
+      <c r="B65" t="s">
         <v>438</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
+        <v>430</v>
+      </c>
+      <c r="D65" t="s">
         <v>439</v>
-      </c>
-      <c r="C65" t="s">
-        <v>431</v>
-      </c>
-      <c r="D65" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>440</v>
+      </c>
+      <c r="B66" t="s">
         <v>441</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>430</v>
+      </c>
+      <c r="D66" t="s">
         <v>442</v>
-      </c>
-      <c r="C66" t="s">
-        <v>431</v>
-      </c>
-      <c r="D66" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>443</v>
+      </c>
+      <c r="B67" t="s">
         <v>444</v>
       </c>
-      <c r="B67" t="s">
-        <v>445</v>
-      </c>
       <c r="C67" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>445</v>
+      </c>
+      <c r="B68" t="s">
         <v>446</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
+        <v>430</v>
+      </c>
+      <c r="D68" t="s">
         <v>447</v>
-      </c>
-      <c r="C68" t="s">
-        <v>431</v>
-      </c>
-      <c r="D68" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>448</v>
+      </c>
+      <c r="B69" t="s">
         <v>449</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
+        <v>430</v>
+      </c>
+      <c r="D69" t="s">
         <v>450</v>
-      </c>
-      <c r="C69" t="s">
-        <v>431</v>
-      </c>
-      <c r="D69" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>451</v>
+      </c>
+      <c r="B70" t="s">
         <v>452</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>430</v>
+      </c>
+      <c r="D70" t="s">
         <v>453</v>
-      </c>
-      <c r="C70" t="s">
-        <v>431</v>
-      </c>
-      <c r="D70" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>454</v>
+      </c>
+      <c r="B71" t="s">
         <v>455</v>
-      </c>
-      <c r="B71" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>456</v>
+      </c>
+      <c r="B72" t="s">
         <v>457</v>
       </c>
-      <c r="B72" t="s">
+      <c r="D72" t="s">
         <v>458</v>
-      </c>
-      <c r="D72" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>459</v>
+      </c>
+      <c r="B73" t="s">
         <v>460</v>
-      </c>
-      <c r="B73" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>461</v>
+      </c>
+      <c r="B74" t="s">
         <v>462</v>
       </c>
-      <c r="B74" t="s">
+      <c r="D74" t="s">
         <v>463</v>
-      </c>
-      <c r="D74" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>464</v>
+      </c>
+      <c r="B75" t="s">
         <v>465</v>
       </c>
-      <c r="B75" t="s">
+      <c r="D75" t="s">
         <v>466</v>
-      </c>
-      <c r="D75" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>467</v>
+      </c>
+      <c r="B76" t="s">
         <v>468</v>
       </c>
-      <c r="B76" t="s">
+      <c r="D76" t="s">
         <v>469</v>
-      </c>
-      <c r="D76" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>470</v>
+      </c>
+      <c r="B77" t="s">
         <v>471</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D77" t="s">
         <v>472</v>
-      </c>
-      <c r="D77" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>473</v>
+      </c>
+      <c r="B78" t="s">
         <v>474</v>
       </c>
-      <c r="B78" t="s">
+      <c r="D78" t="s">
         <v>475</v>
-      </c>
-      <c r="D78" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>476</v>
+      </c>
+      <c r="B79" t="s">
         <v>477</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
         <v>478</v>
-      </c>
-      <c r="D79" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>479</v>
+      </c>
+      <c r="B80" t="s">
         <v>480</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>481</v>
-      </c>
-      <c r="D80" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>482</v>
+      </c>
+      <c r="B81" t="s">
         <v>483</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>484</v>
-      </c>
-      <c r="D81" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>485</v>
+      </c>
+      <c r="B82" t="s">
         <v>486</v>
-      </c>
-      <c r="B82" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>487</v>
+      </c>
+      <c r="B83" t="s">
         <v>488</v>
       </c>
-      <c r="B83" t="s">
+      <c r="D83" t="s">
         <v>489</v>
-      </c>
-      <c r="D83" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B84" t="s">
+        <v>490</v>
+      </c>
+      <c r="D84" t="s">
         <v>491</v>
-      </c>
-      <c r="D84" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B85" t="s">
+        <v>492</v>
+      </c>
+      <c r="D85" t="s">
         <v>493</v>
-      </c>
-      <c r="D85" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B86" t="s">
+        <v>494</v>
+      </c>
+      <c r="D86" t="s">
         <v>495</v>
-      </c>
-      <c r="D86" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -3428,16 +3448,16 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>391</v>
+      </c>
+      <c r="B105" t="s">
         <v>392</v>
-      </c>
-      <c r="B105" t="s">
-        <v>393</v>
       </c>
       <c r="C105" t="s">
         <v>166</v>
       </c>
       <c r="D105" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -3722,16 +3742,16 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>424</v>
+      </c>
+      <c r="B126" t="s">
         <v>425</v>
-      </c>
-      <c r="B126" t="s">
-        <v>426</v>
       </c>
       <c r="C126" t="s">
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -3750,16 +3770,16 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>411</v>
+      </c>
+      <c r="B128" t="s">
         <v>412</v>
-      </c>
-      <c r="B128" t="s">
-        <v>413</v>
       </c>
       <c r="C128" t="s">
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -3787,654 +3807,668 @@
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>334</v>
+        <v>538</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>335</v>
+        <v>535</v>
       </c>
       <c r="B131" t="s">
-        <v>336</v>
+        <v>536</v>
       </c>
       <c r="C131" t="s">
         <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>337</v>
+        <v>537</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>289</v>
+        <v>334</v>
       </c>
       <c r="B132" t="s">
-        <v>13</v>
+        <v>335</v>
       </c>
       <c r="C132" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>62</v>
+        <v>336</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B133" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C133" t="s">
         <v>14</v>
       </c>
       <c r="D133" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B134" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C134" t="s">
         <v>14</v>
       </c>
       <c r="D134" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B135" t="s">
-        <v>339</v>
+        <v>51</v>
       </c>
       <c r="C135" t="s">
         <v>14</v>
       </c>
       <c r="D135" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>292</v>
+      </c>
+      <c r="B136" t="s">
         <v>338</v>
-      </c>
-      <c r="B136" t="s">
-        <v>340</v>
       </c>
       <c r="C136" t="s">
         <v>14</v>
       </c>
       <c r="D136" t="s">
-        <v>341</v>
+        <v>115</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>293</v>
+        <v>337</v>
       </c>
       <c r="B137" t="s">
-        <v>55</v>
+        <v>339</v>
       </c>
       <c r="C137" t="s">
         <v>14</v>
       </c>
       <c r="D137" t="s">
-        <v>77</v>
+        <v>340</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B138" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C138" t="s">
         <v>14</v>
       </c>
       <c r="D138" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B139" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="C139" t="s">
         <v>14</v>
       </c>
       <c r="D139" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>343</v>
+        <v>295</v>
       </c>
       <c r="B140" t="s">
-        <v>344</v>
+        <v>116</v>
       </c>
       <c r="C140" t="s">
         <v>14</v>
       </c>
       <c r="D140" t="s">
-        <v>345</v>
+        <v>80</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>296</v>
+        <v>342</v>
       </c>
       <c r="B141" t="s">
-        <v>117</v>
+        <v>343</v>
       </c>
       <c r="C141" t="s">
         <v>14</v>
       </c>
       <c r="D141" t="s">
-        <v>118</v>
+        <v>344</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B142" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C142" t="s">
         <v>14</v>
       </c>
       <c r="D142" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>121</v>
+        <v>297</v>
       </c>
       <c r="B143" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C143" t="s">
         <v>14</v>
       </c>
       <c r="D143" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B144" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C144" t="s">
         <v>14</v>
       </c>
       <c r="D144" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B145" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C145" t="s">
         <v>14</v>
       </c>
       <c r="D145" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B146" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C146" t="s">
         <v>14</v>
       </c>
       <c r="D146" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B147" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="C147" t="s">
         <v>14</v>
       </c>
       <c r="D147" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>196</v>
+        <v>133</v>
       </c>
       <c r="B148" t="s">
-        <v>197</v>
+        <v>41</v>
       </c>
       <c r="C148" t="s">
         <v>14</v>
       </c>
       <c r="D148" t="s">
-        <v>198</v>
+        <v>79</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>398</v>
+        <v>196</v>
       </c>
       <c r="B149" t="s">
-        <v>399</v>
+        <v>197</v>
       </c>
       <c r="C149" t="s">
         <v>14</v>
       </c>
       <c r="D149" t="s">
-        <v>400</v>
+        <v>198</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>304</v>
+        <v>397</v>
       </c>
       <c r="B150" t="s">
-        <v>104</v>
+        <v>398</v>
       </c>
       <c r="C150" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="D150" t="s">
-        <v>113</v>
+        <v>399</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B151" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C151" t="s">
         <v>105</v>
       </c>
       <c r="D151" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B152" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C152" t="s">
         <v>105</v>
       </c>
       <c r="D152" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B153" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C153" t="s">
         <v>105</v>
       </c>
       <c r="D153" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B154" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C154" t="s">
         <v>105</v>
       </c>
       <c r="D154" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B155" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="C155" t="s">
         <v>105</v>
       </c>
       <c r="D155" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B156" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="C156" t="s">
         <v>105</v>
       </c>
       <c r="D156" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B157" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C157" t="s">
         <v>105</v>
       </c>
       <c r="D157" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B158" t="s">
-        <v>313</v>
+        <v>110</v>
       </c>
       <c r="C158" t="s">
         <v>105</v>
       </c>
       <c r="D158" t="s">
-        <v>314</v>
+        <v>21</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B159" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C159" t="s">
         <v>105</v>
       </c>
       <c r="D159" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="B160" t="s">
-        <v>390</v>
+        <v>316</v>
       </c>
       <c r="C160" t="s">
         <v>105</v>
       </c>
       <c r="D160" t="s">
-        <v>391</v>
+        <v>317</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>318</v>
+        <v>341</v>
       </c>
       <c r="B161" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C161" t="s">
         <v>105</v>
       </c>
       <c r="D161" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B162" t="s">
-        <v>319</v>
+        <v>403</v>
       </c>
       <c r="C162" t="s">
         <v>105</v>
       </c>
       <c r="D162" t="s">
-        <v>320</v>
+        <v>404</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>386</v>
+        <v>321</v>
       </c>
       <c r="B163" t="s">
-        <v>384</v>
+        <v>319</v>
       </c>
       <c r="C163" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="D163" t="s">
-        <v>385</v>
+        <v>320</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B164" t="s">
-        <v>322</v>
+        <v>383</v>
       </c>
       <c r="C164" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="D164" t="s">
-        <v>323</v>
+        <v>384</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="B165" t="s">
-        <v>402</v>
+        <v>322</v>
       </c>
       <c r="C165" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="D165" t="s">
-        <v>403</v>
+        <v>323</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>148</v>
+        <v>400</v>
       </c>
       <c r="B166" t="s">
-        <v>149</v>
+        <v>401</v>
       </c>
       <c r="C166" t="s">
-        <v>150</v>
+        <v>18</v>
       </c>
       <c r="D166" t="s">
-        <v>151</v>
-      </c>
-      <c r="E166" t="s">
-        <v>152</v>
+        <v>402</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B167" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C167" t="s">
         <v>150</v>
       </c>
       <c r="D167" t="s">
-        <v>421</v>
+        <v>151</v>
+      </c>
+      <c r="E167" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>422</v>
+        <v>153</v>
       </c>
       <c r="B168" t="s">
-        <v>423</v>
+        <v>154</v>
       </c>
       <c r="C168" t="s">
         <v>150</v>
       </c>
       <c r="D168" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>217</v>
+        <v>421</v>
       </c>
       <c r="B169" t="s">
-        <v>218</v>
+        <v>422</v>
       </c>
       <c r="C169" t="s">
         <v>150</v>
       </c>
       <c r="D169" t="s">
-        <v>219</v>
+        <v>423</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="B170" t="s">
-        <v>261</v>
+        <v>218</v>
       </c>
       <c r="C170" t="s">
         <v>150</v>
       </c>
       <c r="D170" t="s">
-        <v>262</v>
+        <v>219</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B171" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C171" t="s">
         <v>150</v>
       </c>
       <c r="D171" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>507</v>
+        <v>263</v>
       </c>
       <c r="B172" t="s">
-        <v>501</v>
+        <v>264</v>
       </c>
       <c r="C172" t="s">
         <v>150</v>
       </c>
       <c r="D172" t="s">
-        <v>502</v>
+        <v>265</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B173" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C173" t="s">
         <v>150</v>
       </c>
       <c r="D173" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B174" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C174" t="s">
         <v>150</v>
       </c>
       <c r="D174" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>286</v>
+        <v>504</v>
       </c>
       <c r="B175" t="s">
-        <v>287</v>
+        <v>505</v>
       </c>
       <c r="C175" t="s">
         <v>150</v>
       </c>
       <c r="D175" t="s">
-        <v>288</v>
+        <v>508</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>518</v>
+        <v>286</v>
       </c>
       <c r="B176" t="s">
-        <v>519</v>
+        <v>287</v>
       </c>
       <c r="C176" t="s">
         <v>150</v>
       </c>
       <c r="D176" t="s">
-        <v>520</v>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>517</v>
+      </c>
+      <c r="B177" t="s">
+        <v>518</v>
+      </c>
+      <c r="C177" t="s">
+        <v>150</v>
+      </c>
+      <c r="D177" t="s">
+        <v>519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Metastatic status derived variable added
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFE199A-52AF-B54E-9938-64CD018057A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5779106E-E2D7-034D-93B4-F8C69E7C5BB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="500" windowWidth="32960" windowHeight="21680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="542">
   <si>
     <t>Variable #</t>
   </si>
@@ -1643,6 +1643,15 @@
   </si>
   <si>
     <t>Custom ordinal outcome with death within 30 days</t>
+  </si>
+  <si>
+    <t>Ca19</t>
+  </si>
+  <si>
+    <t>metastatic</t>
+  </si>
+  <si>
+    <t>Metastatic cancer status</t>
   </si>
 </sst>
 </file>
@@ -1698,10 +1707,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E177" totalsRowShown="0">
-  <autoFilter ref="A1:E177" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E176">
-    <sortCondition ref="A1:A176"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E178" totalsRowShown="0">
+  <autoFilter ref="A1:E178" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E177">
+    <sortCondition ref="A1:A177"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -2035,10 +2044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E177"/>
+  <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2727,1563 +2736,1563 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>280</v>
+        <v>539</v>
       </c>
       <c r="B49" t="s">
-        <v>134</v>
+        <v>540</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>47</v>
+        <v>541</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>134</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>513</v>
+        <v>281</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>146</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B52" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>282</v>
+        <v>514</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>64</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>515</v>
+        <v>282</v>
       </c>
       <c r="B54" t="s">
-        <v>203</v>
+        <v>17</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>204</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="B55" t="s">
-        <v>510</v>
+        <v>203</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
       </c>
+      <c r="D55" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>283</v>
+        <v>509</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
+        <v>510</v>
       </c>
       <c r="C56" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>138</v>
+        <v>283</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>329</v>
+        <v>138</v>
       </c>
       <c r="B58" t="s">
-        <v>330</v>
+        <v>3</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>331</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>139</v>
+        <v>329</v>
       </c>
       <c r="B59" t="s">
-        <v>140</v>
+        <v>330</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>141</v>
+        <v>331</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="B60" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="C60" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="B61" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>428</v>
+        <v>193</v>
       </c>
       <c r="B62" t="s">
-        <v>429</v>
+        <v>194</v>
       </c>
       <c r="C62" t="s">
-        <v>430</v>
+        <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>496</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B63" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C63" t="s">
         <v>430</v>
       </c>
       <c r="D63" t="s">
-        <v>433</v>
+        <v>496</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B64" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C64" t="s">
         <v>430</v>
       </c>
       <c r="D64" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B65" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C65" t="s">
         <v>430</v>
       </c>
       <c r="D65" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B66" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C66" t="s">
         <v>430</v>
       </c>
       <c r="D66" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B67" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C67" t="s">
         <v>430</v>
       </c>
+      <c r="D67" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B68" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C68" t="s">
         <v>430</v>
       </c>
-      <c r="D68" t="s">
-        <v>447</v>
-      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B69" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C69" t="s">
         <v>430</v>
       </c>
       <c r="D69" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B70" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C70" t="s">
         <v>430</v>
       </c>
       <c r="D70" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B71" t="s">
-        <v>455</v>
+        <v>452</v>
+      </c>
+      <c r="C71" t="s">
+        <v>430</v>
+      </c>
+      <c r="D71" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B72" t="s">
-        <v>457</v>
-      </c>
-      <c r="D72" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B73" t="s">
-        <v>460</v>
+        <v>457</v>
+      </c>
+      <c r="D73" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B74" t="s">
-        <v>462</v>
-      </c>
-      <c r="D74" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B75" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D75" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B76" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D76" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B77" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D77" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B78" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D78" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B79" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D79" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B80" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D80" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B81" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D81" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B82" t="s">
-        <v>486</v>
+        <v>483</v>
+      </c>
+      <c r="D82" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B83" t="s">
-        <v>488</v>
-      </c>
-      <c r="D83" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="B84" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D84" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B85" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D85" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B86" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D86" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>248</v>
+        <v>499</v>
       </c>
       <c r="B87" t="s">
-        <v>165</v>
-      </c>
-      <c r="C87" t="s">
-        <v>166</v>
+        <v>494</v>
       </c>
       <c r="D87" t="s">
-        <v>167</v>
+        <v>495</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B88" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C88" t="s">
         <v>166</v>
       </c>
       <c r="D88" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C89" t="s">
         <v>166</v>
       </c>
       <c r="D89" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B90" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C90" t="s">
         <v>166</v>
       </c>
       <c r="D90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C91" t="s">
         <v>166</v>
       </c>
       <c r="D91" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B92" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C92" t="s">
         <v>166</v>
       </c>
       <c r="D92" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C93" t="s">
         <v>166</v>
       </c>
       <c r="D93" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C94" t="s">
         <v>166</v>
       </c>
       <c r="D94" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B95" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C95" t="s">
         <v>166</v>
       </c>
       <c r="D95" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>190</v>
+        <v>256</v>
       </c>
       <c r="B96" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C96" t="s">
         <v>166</v>
       </c>
       <c r="D96" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="B97" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
       <c r="C97" t="s">
         <v>166</v>
       </c>
       <c r="D97" t="s">
-        <v>232</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B98" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C98" t="s">
         <v>166</v>
       </c>
       <c r="D98" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B99" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C99" t="s">
         <v>166</v>
       </c>
       <c r="D99" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B100" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C100" t="s">
         <v>166</v>
       </c>
       <c r="D100" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B101" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C101" t="s">
         <v>166</v>
       </c>
       <c r="D101" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B102" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C102" t="s">
         <v>166</v>
       </c>
       <c r="D102" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="B103" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="C103" t="s">
         <v>166</v>
       </c>
       <c r="D103" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>257</v>
+        <v>230</v>
       </c>
       <c r="B104" t="s">
-        <v>258</v>
+        <v>228</v>
       </c>
       <c r="C104" t="s">
         <v>166</v>
       </c>
       <c r="D104" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>391</v>
+        <v>257</v>
       </c>
       <c r="B105" t="s">
-        <v>392</v>
+        <v>258</v>
       </c>
       <c r="C105" t="s">
         <v>166</v>
       </c>
       <c r="D105" t="s">
-        <v>393</v>
+        <v>259</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>268</v>
+        <v>391</v>
       </c>
       <c r="B106" t="s">
-        <v>4</v>
+        <v>392</v>
       </c>
       <c r="C106" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="D106" t="s">
-        <v>58</v>
+        <v>393</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B107" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C107" t="s">
         <v>6</v>
       </c>
       <c r="D107" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>326</v>
+        <v>269</v>
       </c>
       <c r="B108" t="s">
-        <v>327</v>
+        <v>11</v>
       </c>
       <c r="C108" t="s">
         <v>6</v>
       </c>
       <c r="D108" t="s">
-        <v>328</v>
+        <v>59</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>270</v>
+        <v>326</v>
       </c>
       <c r="B109" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="C109" t="s">
         <v>6</v>
       </c>
       <c r="D109" t="s">
-        <v>60</v>
+        <v>328</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B110" t="s">
-        <v>324</v>
+        <v>10</v>
       </c>
       <c r="C110" t="s">
         <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>325</v>
+        <v>60</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B111" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>61</v>
+        <v>325</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B112" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="C112" t="s">
         <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B113" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="C113" t="s">
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>216</v>
+        <v>83</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B114" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C114" t="s">
         <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>284</v>
+        <v>216</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B115" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C115" t="s">
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>84</v>
+        <v>276</v>
       </c>
       <c r="B116" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="C116" t="s">
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>86</v>
+        <v>285</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B117" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C117" t="s">
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B118" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="C118" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B119" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C119" t="s">
         <v>34</v>
       </c>
       <c r="D119" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B120" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C120" t="s">
         <v>34</v>
       </c>
       <c r="D120" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B121" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C121" t="s">
         <v>34</v>
       </c>
       <c r="D121" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B122" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C122" t="s">
         <v>34</v>
       </c>
       <c r="D122" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B123" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C123" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D123" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B124" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C124" t="s">
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
       <c r="B125" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="C125" t="s">
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>161</v>
+        <v>66</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>424</v>
+        <v>159</v>
       </c>
       <c r="B126" t="s">
-        <v>425</v>
+        <v>160</v>
       </c>
       <c r="C126" t="s">
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>426</v>
+        <v>161</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>162</v>
+        <v>424</v>
       </c>
       <c r="B127" t="s">
-        <v>163</v>
+        <v>425</v>
       </c>
       <c r="C127" t="s">
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>164</v>
+        <v>426</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>411</v>
+        <v>162</v>
       </c>
       <c r="B128" t="s">
-        <v>412</v>
+        <v>163</v>
       </c>
       <c r="C128" t="s">
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>413</v>
+        <v>164</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>277</v>
+        <v>411</v>
       </c>
       <c r="B129" t="s">
-        <v>278</v>
+        <v>412</v>
       </c>
       <c r="C129" t="s">
         <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>279</v>
+        <v>413</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>332</v>
+        <v>277</v>
       </c>
       <c r="B130" t="s">
-        <v>333</v>
+        <v>278</v>
       </c>
       <c r="C130" t="s">
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>538</v>
+        <v>279</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>535</v>
+        <v>332</v>
       </c>
       <c r="B131" t="s">
-        <v>536</v>
+        <v>333</v>
       </c>
       <c r="C131" t="s">
         <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>334</v>
+        <v>535</v>
       </c>
       <c r="B132" t="s">
-        <v>335</v>
+        <v>536</v>
       </c>
       <c r="C132" t="s">
         <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>336</v>
+        <v>537</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>289</v>
+        <v>334</v>
       </c>
       <c r="B133" t="s">
-        <v>13</v>
+        <v>335</v>
       </c>
       <c r="C133" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D133" t="s">
-        <v>62</v>
+        <v>336</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B134" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C134" t="s">
         <v>14</v>
       </c>
       <c r="D134" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B135" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C135" t="s">
         <v>14</v>
       </c>
       <c r="D135" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B136" t="s">
-        <v>338</v>
+        <v>51</v>
       </c>
       <c r="C136" t="s">
         <v>14</v>
       </c>
       <c r="D136" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>337</v>
+        <v>292</v>
       </c>
       <c r="B137" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C137" t="s">
         <v>14</v>
       </c>
       <c r="D137" t="s">
-        <v>340</v>
+        <v>115</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>293</v>
+        <v>337</v>
       </c>
       <c r="B138" t="s">
-        <v>55</v>
+        <v>339</v>
       </c>
       <c r="C138" t="s">
         <v>14</v>
       </c>
       <c r="D138" t="s">
-        <v>77</v>
+        <v>340</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B139" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C139" t="s">
         <v>14</v>
       </c>
       <c r="D139" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B140" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="C140" t="s">
         <v>14</v>
       </c>
       <c r="D140" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>342</v>
+        <v>295</v>
       </c>
       <c r="B141" t="s">
-        <v>343</v>
+        <v>116</v>
       </c>
       <c r="C141" t="s">
         <v>14</v>
       </c>
       <c r="D141" t="s">
-        <v>344</v>
+        <v>80</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>296</v>
+        <v>342</v>
       </c>
       <c r="B142" t="s">
-        <v>117</v>
+        <v>343</v>
       </c>
       <c r="C142" t="s">
         <v>14</v>
       </c>
       <c r="D142" t="s">
-        <v>118</v>
+        <v>344</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B143" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C143" t="s">
         <v>14</v>
       </c>
       <c r="D143" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>121</v>
+        <v>297</v>
       </c>
       <c r="B144" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C144" t="s">
         <v>14</v>
       </c>
       <c r="D144" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B145" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C145" t="s">
         <v>14</v>
       </c>
       <c r="D145" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B146" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C146" t="s">
         <v>14</v>
       </c>
       <c r="D146" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B147" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C147" t="s">
         <v>14</v>
       </c>
       <c r="D147" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B148" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="C148" t="s">
         <v>14</v>
       </c>
       <c r="D148" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>196</v>
+        <v>133</v>
       </c>
       <c r="B149" t="s">
-        <v>197</v>
+        <v>41</v>
       </c>
       <c r="C149" t="s">
         <v>14</v>
       </c>
       <c r="D149" t="s">
-        <v>198</v>
+        <v>79</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>397</v>
+        <v>196</v>
       </c>
       <c r="B150" t="s">
-        <v>398</v>
+        <v>197</v>
       </c>
       <c r="C150" t="s">
         <v>14</v>
       </c>
       <c r="D150" t="s">
-        <v>399</v>
+        <v>198</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>304</v>
+        <v>397</v>
       </c>
       <c r="B151" t="s">
-        <v>104</v>
+        <v>398</v>
       </c>
       <c r="C151" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="D151" t="s">
-        <v>113</v>
+        <v>399</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B152" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C152" t="s">
         <v>105</v>
       </c>
       <c r="D152" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B153" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C153" t="s">
         <v>105</v>
       </c>
       <c r="D153" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B154" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C154" t="s">
         <v>105</v>
       </c>
       <c r="D154" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B155" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C155" t="s">
         <v>105</v>
       </c>
       <c r="D155" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B156" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="C156" t="s">
         <v>105</v>
       </c>
       <c r="D156" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B157" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="C157" t="s">
         <v>105</v>
       </c>
       <c r="D157" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B158" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C158" t="s">
         <v>105</v>
       </c>
       <c r="D158" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B159" t="s">
-        <v>313</v>
+        <v>110</v>
       </c>
       <c r="C159" t="s">
         <v>105</v>
       </c>
       <c r="D159" t="s">
-        <v>314</v>
+        <v>21</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B160" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C160" t="s">
         <v>105</v>
       </c>
       <c r="D160" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>341</v>
+        <v>315</v>
       </c>
       <c r="B161" t="s">
-        <v>389</v>
+        <v>316</v>
       </c>
       <c r="C161" t="s">
         <v>105</v>
       </c>
       <c r="D161" t="s">
-        <v>390</v>
+        <v>317</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>318</v>
+        <v>341</v>
       </c>
       <c r="B162" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="C162" t="s">
         <v>105</v>
       </c>
       <c r="D162" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B163" t="s">
-        <v>319</v>
+        <v>403</v>
       </c>
       <c r="C163" t="s">
         <v>105</v>
       </c>
       <c r="D163" t="s">
-        <v>320</v>
+        <v>404</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>385</v>
+        <v>321</v>
       </c>
       <c r="B164" t="s">
-        <v>383</v>
+        <v>319</v>
       </c>
       <c r="C164" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="D164" t="s">
-        <v>384</v>
+        <v>320</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -4291,183 +4300,197 @@
         <v>385</v>
       </c>
       <c r="B165" t="s">
-        <v>322</v>
+        <v>383</v>
       </c>
       <c r="C165" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="D165" t="s">
-        <v>323</v>
+        <v>384</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="B166" t="s">
-        <v>401</v>
+        <v>322</v>
       </c>
       <c r="C166" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="D166" t="s">
-        <v>402</v>
+        <v>323</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>148</v>
+        <v>400</v>
       </c>
       <c r="B167" t="s">
-        <v>149</v>
+        <v>401</v>
       </c>
       <c r="C167" t="s">
-        <v>150</v>
+        <v>18</v>
       </c>
       <c r="D167" t="s">
-        <v>151</v>
-      </c>
-      <c r="E167" t="s">
-        <v>152</v>
+        <v>402</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B168" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C168" t="s">
         <v>150</v>
       </c>
       <c r="D168" t="s">
-        <v>420</v>
+        <v>151</v>
+      </c>
+      <c r="E168" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>421</v>
+        <v>153</v>
       </c>
       <c r="B169" t="s">
-        <v>422</v>
+        <v>154</v>
       </c>
       <c r="C169" t="s">
         <v>150</v>
       </c>
       <c r="D169" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>217</v>
+        <v>421</v>
       </c>
       <c r="B170" t="s">
-        <v>218</v>
+        <v>422</v>
       </c>
       <c r="C170" t="s">
         <v>150</v>
       </c>
       <c r="D170" t="s">
-        <v>219</v>
+        <v>423</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="B171" t="s">
-        <v>261</v>
+        <v>218</v>
       </c>
       <c r="C171" t="s">
         <v>150</v>
       </c>
       <c r="D171" t="s">
-        <v>262</v>
+        <v>219</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B172" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C172" t="s">
         <v>150</v>
       </c>
       <c r="D172" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>506</v>
+        <v>263</v>
       </c>
       <c r="B173" t="s">
-        <v>500</v>
+        <v>264</v>
       </c>
       <c r="C173" t="s">
         <v>150</v>
       </c>
       <c r="D173" t="s">
-        <v>501</v>
+        <v>265</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="B174" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C174" t="s">
         <v>150</v>
       </c>
       <c r="D174" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B175" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C175" t="s">
         <v>150</v>
       </c>
       <c r="D175" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>286</v>
+        <v>504</v>
       </c>
       <c r="B176" t="s">
-        <v>287</v>
+        <v>505</v>
       </c>
       <c r="C176" t="s">
         <v>150</v>
       </c>
       <c r="D176" t="s">
-        <v>288</v>
+        <v>508</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>517</v>
+        <v>286</v>
       </c>
       <c r="B177" t="s">
-        <v>518</v>
+        <v>287</v>
       </c>
       <c r="C177" t="s">
         <v>150</v>
       </c>
       <c r="D177" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>517</v>
+      </c>
+      <c r="B178" t="s">
+        <v>518</v>
+      </c>
+      <c r="C178" t="s">
+        <v>150</v>
+      </c>
+      <c r="D178" t="s">
         <v>519</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a new ordinal outcome
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5779106E-E2D7-034D-93B4-F8C69E7C5BB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A7850C-3C45-5748-9CEB-49AD76CB7509}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="500" windowWidth="32960" windowHeight="21680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="500" windowWidth="32960" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="545">
   <si>
     <t>Variable #</t>
   </si>
@@ -1652,6 +1652,15 @@
   </si>
   <si>
     <t>Metastatic cancer status</t>
+  </si>
+  <si>
+    <t>O23a</t>
+  </si>
+  <si>
+    <t>ordinal_v2a</t>
+  </si>
+  <si>
+    <t>Custom ordinal including need for oxygen in the hospital</t>
   </si>
 </sst>
 </file>
@@ -1707,10 +1716,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E178" totalsRowShown="0">
-  <autoFilter ref="A1:E178" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E177">
-    <sortCondition ref="A1:A177"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E179" totalsRowShown="0">
+  <autoFilter ref="A1:E179" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E178">
+    <sortCondition ref="A1:A178"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -2044,10 +2053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E178"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3863,450 +3872,450 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>289</v>
+        <v>542</v>
       </c>
       <c r="B134" t="s">
-        <v>13</v>
+        <v>543</v>
       </c>
       <c r="C134" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D134" t="s">
-        <v>62</v>
+        <v>544</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B135" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C135" t="s">
         <v>14</v>
       </c>
       <c r="D135" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B136" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C136" t="s">
         <v>14</v>
       </c>
       <c r="D136" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B137" t="s">
-        <v>338</v>
+        <v>51</v>
       </c>
       <c r="C137" t="s">
         <v>14</v>
       </c>
       <c r="D137" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>337</v>
+        <v>292</v>
       </c>
       <c r="B138" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C138" t="s">
         <v>14</v>
       </c>
       <c r="D138" t="s">
-        <v>340</v>
+        <v>115</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>293</v>
+        <v>337</v>
       </c>
       <c r="B139" t="s">
-        <v>55</v>
+        <v>339</v>
       </c>
       <c r="C139" t="s">
         <v>14</v>
       </c>
       <c r="D139" t="s">
-        <v>77</v>
+        <v>340</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B140" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C140" t="s">
         <v>14</v>
       </c>
       <c r="D140" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B141" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="C141" t="s">
         <v>14</v>
       </c>
       <c r="D141" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>342</v>
+        <v>295</v>
       </c>
       <c r="B142" t="s">
-        <v>343</v>
+        <v>116</v>
       </c>
       <c r="C142" t="s">
         <v>14</v>
       </c>
       <c r="D142" t="s">
-        <v>344</v>
+        <v>80</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>296</v>
+        <v>342</v>
       </c>
       <c r="B143" t="s">
-        <v>117</v>
+        <v>343</v>
       </c>
       <c r="C143" t="s">
         <v>14</v>
       </c>
       <c r="D143" t="s">
-        <v>118</v>
+        <v>344</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B144" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C144" t="s">
         <v>14</v>
       </c>
       <c r="D144" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>121</v>
+        <v>297</v>
       </c>
       <c r="B145" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C145" t="s">
         <v>14</v>
       </c>
       <c r="D145" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B146" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C146" t="s">
         <v>14</v>
       </c>
       <c r="D146" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B147" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C147" t="s">
         <v>14</v>
       </c>
       <c r="D147" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B148" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C148" t="s">
         <v>14</v>
       </c>
       <c r="D148" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B149" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="C149" t="s">
         <v>14</v>
       </c>
       <c r="D149" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>196</v>
+        <v>133</v>
       </c>
       <c r="B150" t="s">
-        <v>197</v>
+        <v>41</v>
       </c>
       <c r="C150" t="s">
         <v>14</v>
       </c>
       <c r="D150" t="s">
-        <v>198</v>
+        <v>79</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>397</v>
+        <v>196</v>
       </c>
       <c r="B151" t="s">
-        <v>398</v>
+        <v>197</v>
       </c>
       <c r="C151" t="s">
         <v>14</v>
       </c>
       <c r="D151" t="s">
-        <v>399</v>
+        <v>198</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>304</v>
+        <v>397</v>
       </c>
       <c r="B152" t="s">
-        <v>104</v>
+        <v>398</v>
       </c>
       <c r="C152" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="D152" t="s">
-        <v>113</v>
+        <v>399</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B153" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C153" t="s">
         <v>105</v>
       </c>
       <c r="D153" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B154" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C154" t="s">
         <v>105</v>
       </c>
       <c r="D154" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B155" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C155" t="s">
         <v>105</v>
       </c>
       <c r="D155" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B156" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C156" t="s">
         <v>105</v>
       </c>
       <c r="D156" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B157" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="C157" t="s">
         <v>105</v>
       </c>
       <c r="D157" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B158" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="C158" t="s">
         <v>105</v>
       </c>
       <c r="D158" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B159" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C159" t="s">
         <v>105</v>
       </c>
       <c r="D159" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B160" t="s">
-        <v>313</v>
+        <v>110</v>
       </c>
       <c r="C160" t="s">
         <v>105</v>
       </c>
       <c r="D160" t="s">
-        <v>314</v>
+        <v>21</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B161" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C161" t="s">
         <v>105</v>
       </c>
       <c r="D161" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>341</v>
+        <v>315</v>
       </c>
       <c r="B162" t="s">
-        <v>389</v>
+        <v>316</v>
       </c>
       <c r="C162" t="s">
         <v>105</v>
       </c>
       <c r="D162" t="s">
-        <v>390</v>
+        <v>317</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>318</v>
+        <v>341</v>
       </c>
       <c r="B163" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="C163" t="s">
         <v>105</v>
       </c>
       <c r="D163" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B164" t="s">
-        <v>319</v>
+        <v>403</v>
       </c>
       <c r="C164" t="s">
         <v>105</v>
       </c>
       <c r="D164" t="s">
-        <v>320</v>
+        <v>404</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>385</v>
+        <v>321</v>
       </c>
       <c r="B165" t="s">
-        <v>383</v>
+        <v>319</v>
       </c>
       <c r="C165" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="D165" t="s">
-        <v>384</v>
+        <v>320</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -4314,183 +4323,197 @@
         <v>385</v>
       </c>
       <c r="B166" t="s">
-        <v>322</v>
+        <v>383</v>
       </c>
       <c r="C166" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="D166" t="s">
-        <v>323</v>
+        <v>384</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="B167" t="s">
-        <v>401</v>
+        <v>322</v>
       </c>
       <c r="C167" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="D167" t="s">
-        <v>402</v>
+        <v>323</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>148</v>
+        <v>400</v>
       </c>
       <c r="B168" t="s">
-        <v>149</v>
+        <v>401</v>
       </c>
       <c r="C168" t="s">
-        <v>150</v>
+        <v>18</v>
       </c>
       <c r="D168" t="s">
-        <v>151</v>
-      </c>
-      <c r="E168" t="s">
-        <v>152</v>
+        <v>402</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B169" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C169" t="s">
         <v>150</v>
       </c>
       <c r="D169" t="s">
-        <v>420</v>
+        <v>151</v>
+      </c>
+      <c r="E169" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>421</v>
+        <v>153</v>
       </c>
       <c r="B170" t="s">
-        <v>422</v>
+        <v>154</v>
       </c>
       <c r="C170" t="s">
         <v>150</v>
       </c>
       <c r="D170" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>217</v>
+        <v>421</v>
       </c>
       <c r="B171" t="s">
-        <v>218</v>
+        <v>422</v>
       </c>
       <c r="C171" t="s">
         <v>150</v>
       </c>
       <c r="D171" t="s">
-        <v>219</v>
+        <v>423</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="B172" t="s">
-        <v>261</v>
+        <v>218</v>
       </c>
       <c r="C172" t="s">
         <v>150</v>
       </c>
       <c r="D172" t="s">
-        <v>262</v>
+        <v>219</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B173" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C173" t="s">
         <v>150</v>
       </c>
       <c r="D173" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>506</v>
+        <v>263</v>
       </c>
       <c r="B174" t="s">
-        <v>500</v>
+        <v>264</v>
       </c>
       <c r="C174" t="s">
         <v>150</v>
       </c>
       <c r="D174" t="s">
-        <v>501</v>
+        <v>265</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="B175" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C175" t="s">
         <v>150</v>
       </c>
       <c r="D175" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B176" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C176" t="s">
         <v>150</v>
       </c>
       <c r="D176" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>286</v>
+        <v>504</v>
       </c>
       <c r="B177" t="s">
-        <v>287</v>
+        <v>505</v>
       </c>
       <c r="C177" t="s">
         <v>150</v>
       </c>
       <c r="D177" t="s">
-        <v>288</v>
+        <v>508</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>517</v>
+        <v>286</v>
       </c>
       <c r="B178" t="s">
-        <v>518</v>
+        <v>287</v>
       </c>
       <c r="C178" t="s">
         <v>150</v>
       </c>
       <c r="D178" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>517</v>
+      </c>
+      <c r="B179" t="s">
+        <v>518</v>
+      </c>
+      <c r="C179" t="s">
+        <v>150</v>
+      </c>
+      <c r="D179" t="s">
         <v>519</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New fixed outcome variables (90d mortality, 180d mortality)
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A7850C-3C45-5748-9CEB-49AD76CB7509}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC21BF6D-821C-C64D-BF68-CF2E432C83AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="500" windowWidth="32960" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="551">
   <si>
     <t>Variable #</t>
   </si>
@@ -226,9 +226,6 @@
     <t>Derived variable indicating if there has been surgery within 4 weeks</t>
   </si>
   <si>
-    <t>Derived variable indicating whether patient has died within 30 days of COVID-19 diagnosis</t>
-  </si>
-  <si>
     <t>Derived variable indicating cancer status</t>
   </si>
   <si>
@@ -1661,6 +1658,27 @@
   </si>
   <si>
     <t>Custom ordinal including need for oxygen in the hospital</t>
+  </si>
+  <si>
+    <t>O24</t>
+  </si>
+  <si>
+    <t>O25</t>
+  </si>
+  <si>
+    <t>dead90</t>
+  </si>
+  <si>
+    <t>Derived variable indicating whether patient has died within 90 days of COVID-19 diagnosis (default = No)</t>
+  </si>
+  <si>
+    <t>Derived variable indicating whether patient has died within 30 days of COVID-19 diagnosis (default = No)</t>
+  </si>
+  <si>
+    <t>dead180</t>
+  </si>
+  <si>
+    <t>Derived variable indicating whether patient has died within 180 days of COVID-19 diagnosis (default = No)</t>
   </si>
 </sst>
 </file>
@@ -1716,10 +1734,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E179" totalsRowShown="0">
-  <autoFilter ref="A1:E179" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E178">
-    <sortCondition ref="A1:A178"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E181" totalsRowShown="0">
+  <autoFilter ref="A1:E181" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E180">
+    <sortCondition ref="A1:A180"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -2053,10 +2071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2073,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2087,49 +2105,49 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B4" t="s">
         <v>415</v>
-      </c>
-      <c r="B4" t="s">
-        <v>416</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -2143,7 +2161,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
@@ -2157,21 +2175,21 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -2180,12 +2198,12 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B9" t="s">
         <v>40</v>
@@ -2194,12 +2212,12 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
@@ -2208,12 +2226,12 @@
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
@@ -2222,12 +2240,12 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B12" t="s">
         <v>56</v>
@@ -2241,77 +2259,77 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>356</v>
+      </c>
+      <c r="B15" t="s">
         <v>357</v>
-      </c>
-      <c r="B15" t="s">
-        <v>358</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>404</v>
+      </c>
+      <c r="B17" t="s">
         <v>405</v>
-      </c>
-      <c r="B17" t="s">
-        <v>406</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -2325,35 +2343,35 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>360</v>
+      </c>
+      <c r="B20" t="s">
         <v>361</v>
-      </c>
-      <c r="B20" t="s">
-        <v>362</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
@@ -2367,21 +2385,21 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
         <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B23" t="s">
         <v>35</v>
@@ -2395,7 +2413,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -2409,360 +2427,360 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B26" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B27" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>206</v>
+      </c>
+      <c r="B31" t="s">
         <v>207</v>
-      </c>
-      <c r="B31" t="s">
-        <v>208</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B32" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B34" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B35" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C35" t="s">
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B37" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>393</v>
+      </c>
+      <c r="B40" t="s">
         <v>394</v>
-      </c>
-      <c r="B40" t="s">
-        <v>395</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" t="s">
         <v>201</v>
-      </c>
-      <c r="B41" t="s">
-        <v>202</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>220</v>
+      </c>
+      <c r="B42" t="s">
         <v>221</v>
-      </c>
-      <c r="B42" t="s">
-        <v>222</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>223</v>
+      </c>
+      <c r="B43" t="s">
         <v>224</v>
-      </c>
-      <c r="B43" t="s">
-        <v>225</v>
       </c>
       <c r="C43" t="s">
         <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>519</v>
+      </c>
+      <c r="B44" t="s">
         <v>520</v>
-      </c>
-      <c r="B44" t="s">
-        <v>521</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B45" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C45" t="s">
         <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>525</v>
+      </c>
+      <c r="B46" t="s">
         <v>526</v>
-      </c>
-      <c r="B46" t="s">
-        <v>527</v>
       </c>
       <c r="C46" t="s">
         <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>528</v>
+      </c>
+      <c r="B47" t="s">
         <v>529</v>
-      </c>
-      <c r="B47" t="s">
-        <v>530</v>
       </c>
       <c r="C47" t="s">
         <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>531</v>
+      </c>
+      <c r="B48" t="s">
         <v>532</v>
-      </c>
-      <c r="B48" t="s">
-        <v>533</v>
       </c>
       <c r="C48" t="s">
         <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>538</v>
+      </c>
+      <c r="B49" t="s">
         <v>539</v>
-      </c>
-      <c r="B49" t="s">
-        <v>540</v>
       </c>
       <c r="C49" t="s">
         <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -2773,7 +2791,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B51" t="s">
         <v>45</v>
@@ -2787,35 +2805,35 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B54" t="s">
         <v>17</v>
@@ -2829,24 +2847,24 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B55" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>508</v>
+      </c>
+      <c r="B56" t="s">
         <v>509</v>
-      </c>
-      <c r="B56" t="s">
-        <v>510</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -2854,7 +2872,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B57" t="s">
         <v>20</v>
@@ -2868,7 +2886,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B58" t="s">
         <v>3</v>
@@ -2882,619 +2900,619 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>328</v>
+      </c>
+      <c r="B59" t="s">
         <v>329</v>
-      </c>
-      <c r="B59" t="s">
-        <v>330</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>138</v>
+      </c>
+      <c r="B60" t="s">
         <v>139</v>
-      </c>
-      <c r="B60" t="s">
-        <v>140</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>168</v>
+      </c>
+      <c r="B61" t="s">
         <v>169</v>
-      </c>
-      <c r="B61" t="s">
-        <v>170</v>
       </c>
       <c r="C61" t="s">
         <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" t="s">
         <v>193</v>
-      </c>
-      <c r="B62" t="s">
-        <v>194</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>427</v>
+      </c>
+      <c r="B63" t="s">
         <v>428</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>429</v>
       </c>
-      <c r="C63" t="s">
-        <v>430</v>
-      </c>
       <c r="D63" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>430</v>
+      </c>
+      <c r="B64" t="s">
         <v>431</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
+        <v>429</v>
+      </c>
+      <c r="D64" t="s">
         <v>432</v>
-      </c>
-      <c r="C64" t="s">
-        <v>430</v>
-      </c>
-      <c r="D64" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>433</v>
+      </c>
+      <c r="B65" t="s">
         <v>434</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
+        <v>429</v>
+      </c>
+      <c r="D65" t="s">
         <v>435</v>
-      </c>
-      <c r="C65" t="s">
-        <v>430</v>
-      </c>
-      <c r="D65" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>436</v>
+      </c>
+      <c r="B66" t="s">
         <v>437</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>429</v>
+      </c>
+      <c r="D66" t="s">
         <v>438</v>
-      </c>
-      <c r="C66" t="s">
-        <v>430</v>
-      </c>
-      <c r="D66" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>439</v>
+      </c>
+      <c r="B67" t="s">
         <v>440</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>429</v>
+      </c>
+      <c r="D67" t="s">
         <v>441</v>
-      </c>
-      <c r="C67" t="s">
-        <v>430</v>
-      </c>
-      <c r="D67" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>442</v>
+      </c>
+      <c r="B68" t="s">
         <v>443</v>
       </c>
-      <c r="B68" t="s">
-        <v>444</v>
-      </c>
       <c r="C68" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>444</v>
+      </c>
+      <c r="B69" t="s">
         <v>445</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
+        <v>429</v>
+      </c>
+      <c r="D69" t="s">
         <v>446</v>
-      </c>
-      <c r="C69" t="s">
-        <v>430</v>
-      </c>
-      <c r="D69" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>447</v>
+      </c>
+      <c r="B70" t="s">
         <v>448</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>429</v>
+      </c>
+      <c r="D70" t="s">
         <v>449</v>
-      </c>
-      <c r="C70" t="s">
-        <v>430</v>
-      </c>
-      <c r="D70" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>450</v>
+      </c>
+      <c r="B71" t="s">
         <v>451</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
+        <v>429</v>
+      </c>
+      <c r="D71" t="s">
         <v>452</v>
-      </c>
-      <c r="C71" t="s">
-        <v>430</v>
-      </c>
-      <c r="D71" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>453</v>
+      </c>
+      <c r="B72" t="s">
         <v>454</v>
-      </c>
-      <c r="B72" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>455</v>
+      </c>
+      <c r="B73" t="s">
         <v>456</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D73" t="s">
         <v>457</v>
-      </c>
-      <c r="D73" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>458</v>
+      </c>
+      <c r="B74" t="s">
         <v>459</v>
-      </c>
-      <c r="B74" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>460</v>
+      </c>
+      <c r="B75" t="s">
         <v>461</v>
       </c>
-      <c r="B75" t="s">
+      <c r="D75" t="s">
         <v>462</v>
-      </c>
-      <c r="D75" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>463</v>
+      </c>
+      <c r="B76" t="s">
         <v>464</v>
       </c>
-      <c r="B76" t="s">
+      <c r="D76" t="s">
         <v>465</v>
-      </c>
-      <c r="D76" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>466</v>
+      </c>
+      <c r="B77" t="s">
         <v>467</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D77" t="s">
         <v>468</v>
-      </c>
-      <c r="D77" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>469</v>
+      </c>
+      <c r="B78" t="s">
         <v>470</v>
       </c>
-      <c r="B78" t="s">
+      <c r="D78" t="s">
         <v>471</v>
-      </c>
-      <c r="D78" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>472</v>
+      </c>
+      <c r="B79" t="s">
         <v>473</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
         <v>474</v>
-      </c>
-      <c r="D79" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>475</v>
+      </c>
+      <c r="B80" t="s">
         <v>476</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>477</v>
-      </c>
-      <c r="D80" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>478</v>
+      </c>
+      <c r="B81" t="s">
         <v>479</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>480</v>
-      </c>
-      <c r="D81" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>481</v>
+      </c>
+      <c r="B82" t="s">
         <v>482</v>
       </c>
-      <c r="B82" t="s">
+      <c r="D82" t="s">
         <v>483</v>
-      </c>
-      <c r="D82" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>484</v>
+      </c>
+      <c r="B83" t="s">
         <v>485</v>
-      </c>
-      <c r="B83" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>486</v>
+      </c>
+      <c r="B84" t="s">
         <v>487</v>
       </c>
-      <c r="B84" t="s">
+      <c r="D84" t="s">
         <v>488</v>
-      </c>
-      <c r="D84" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B85" t="s">
+        <v>489</v>
+      </c>
+      <c r="D85" t="s">
         <v>490</v>
-      </c>
-      <c r="D85" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B86" t="s">
+        <v>491</v>
+      </c>
+      <c r="D86" t="s">
         <v>492</v>
-      </c>
-      <c r="D86" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B87" t="s">
+        <v>493</v>
+      </c>
+      <c r="D87" t="s">
         <v>494</v>
-      </c>
-      <c r="D87" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B88" t="s">
+        <v>164</v>
+      </c>
+      <c r="C88" t="s">
         <v>165</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>166</v>
-      </c>
-      <c r="D88" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B89" t="s">
+        <v>173</v>
+      </c>
+      <c r="C89" t="s">
+        <v>165</v>
+      </c>
+      <c r="D89" t="s">
         <v>174</v>
-      </c>
-      <c r="C89" t="s">
-        <v>166</v>
-      </c>
-      <c r="D89" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B90" t="s">
+        <v>175</v>
+      </c>
+      <c r="C90" t="s">
+        <v>165</v>
+      </c>
+      <c r="D90" t="s">
         <v>176</v>
-      </c>
-      <c r="C90" t="s">
-        <v>166</v>
-      </c>
-      <c r="D90" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B91" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C91" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D91" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B92" t="s">
+        <v>179</v>
+      </c>
+      <c r="C92" t="s">
+        <v>165</v>
+      </c>
+      <c r="D92" t="s">
         <v>180</v>
-      </c>
-      <c r="C92" t="s">
-        <v>166</v>
-      </c>
-      <c r="D92" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B93" t="s">
+        <v>181</v>
+      </c>
+      <c r="C93" t="s">
+        <v>165</v>
+      </c>
+      <c r="D93" t="s">
         <v>182</v>
-      </c>
-      <c r="C93" t="s">
-        <v>166</v>
-      </c>
-      <c r="D93" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B94" t="s">
+        <v>183</v>
+      </c>
+      <c r="C94" t="s">
+        <v>165</v>
+      </c>
+      <c r="D94" t="s">
         <v>184</v>
-      </c>
-      <c r="C94" t="s">
-        <v>166</v>
-      </c>
-      <c r="D94" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B95" t="s">
+        <v>185</v>
+      </c>
+      <c r="C95" t="s">
+        <v>165</v>
+      </c>
+      <c r="D95" t="s">
         <v>186</v>
-      </c>
-      <c r="C95" t="s">
-        <v>166</v>
-      </c>
-      <c r="D95" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B96" t="s">
+        <v>187</v>
+      </c>
+      <c r="C96" t="s">
+        <v>165</v>
+      </c>
+      <c r="D96" t="s">
         <v>188</v>
-      </c>
-      <c r="C96" t="s">
-        <v>166</v>
-      </c>
-      <c r="D96" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>189</v>
+      </c>
+      <c r="B97" t="s">
         <v>190</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
+        <v>165</v>
+      </c>
+      <c r="D97" t="s">
         <v>191</v>
-      </c>
-      <c r="C97" t="s">
-        <v>166</v>
-      </c>
-      <c r="D97" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B98" t="s">
+        <v>230</v>
+      </c>
+      <c r="C98" t="s">
+        <v>165</v>
+      </c>
+      <c r="D98" t="s">
         <v>231</v>
-      </c>
-      <c r="C98" t="s">
-        <v>166</v>
-      </c>
-      <c r="D98" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>232</v>
+      </c>
+      <c r="B99" t="s">
         <v>233</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
+        <v>165</v>
+      </c>
+      <c r="D99" t="s">
         <v>234</v>
-      </c>
-      <c r="C99" t="s">
-        <v>166</v>
-      </c>
-      <c r="D99" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>235</v>
+      </c>
+      <c r="B100" t="s">
         <v>236</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
+        <v>165</v>
+      </c>
+      <c r="D100" t="s">
         <v>237</v>
-      </c>
-      <c r="C100" t="s">
-        <v>166</v>
-      </c>
-      <c r="D100" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>238</v>
+      </c>
+      <c r="B101" t="s">
         <v>239</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
+        <v>165</v>
+      </c>
+      <c r="D101" t="s">
         <v>240</v>
-      </c>
-      <c r="C101" t="s">
-        <v>166</v>
-      </c>
-      <c r="D101" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>241</v>
+      </c>
+      <c r="B102" t="s">
         <v>242</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
+        <v>165</v>
+      </c>
+      <c r="D102" t="s">
         <v>243</v>
-      </c>
-      <c r="C102" t="s">
-        <v>166</v>
-      </c>
-      <c r="D102" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>244</v>
+      </c>
+      <c r="B103" t="s">
         <v>245</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
+        <v>165</v>
+      </c>
+      <c r="D103" t="s">
         <v>246</v>
-      </c>
-      <c r="C103" t="s">
-        <v>166</v>
-      </c>
-      <c r="D103" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B104" t="s">
+        <v>227</v>
+      </c>
+      <c r="C104" t="s">
+        <v>165</v>
+      </c>
+      <c r="D104" t="s">
         <v>228</v>
-      </c>
-      <c r="C104" t="s">
-        <v>166</v>
-      </c>
-      <c r="D104" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>256</v>
+      </c>
+      <c r="B105" t="s">
         <v>257</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
+        <v>165</v>
+      </c>
+      <c r="D105" t="s">
         <v>258</v>
-      </c>
-      <c r="C105" t="s">
-        <v>166</v>
-      </c>
-      <c r="D105" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>390</v>
+      </c>
+      <c r="B106" t="s">
         <v>391</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
+        <v>165</v>
+      </c>
+      <c r="D106" t="s">
         <v>392</v>
-      </c>
-      <c r="C106" t="s">
-        <v>166</v>
-      </c>
-      <c r="D106" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B107" t="s">
         <v>4</v>
@@ -3508,7 +3526,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B108" t="s">
         <v>11</v>
@@ -3522,21 +3540,21 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>325</v>
+      </c>
+      <c r="B109" t="s">
         <v>326</v>
-      </c>
-      <c r="B109" t="s">
-        <v>327</v>
       </c>
       <c r="C109" t="s">
         <v>6</v>
       </c>
       <c r="D109" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B110" t="s">
         <v>10</v>
@@ -3550,21 +3568,21 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B111" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B112" t="s">
         <v>12</v>
@@ -3578,21 +3596,21 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B113" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C113" t="s">
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B114" t="s">
         <v>26</v>
@@ -3601,12 +3619,12 @@
         <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B115" t="s">
         <v>27</v>
@@ -3615,12 +3633,12 @@
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B116" t="s">
         <v>48</v>
@@ -3629,26 +3647,26 @@
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>83</v>
+      </c>
+      <c r="B117" t="s">
         <v>84</v>
-      </c>
-      <c r="B117" t="s">
-        <v>85</v>
       </c>
       <c r="C117" t="s">
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B118" t="s">
         <v>33</v>
@@ -3657,68 +3675,68 @@
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>87</v>
+      </c>
+      <c r="B119" t="s">
         <v>88</v>
-      </c>
-      <c r="B119" t="s">
-        <v>89</v>
       </c>
       <c r="C119" t="s">
         <v>34</v>
       </c>
       <c r="D119" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
+        <v>89</v>
+      </c>
+      <c r="B120" t="s">
         <v>90</v>
-      </c>
-      <c r="B120" t="s">
-        <v>91</v>
       </c>
       <c r="C120" t="s">
         <v>34</v>
       </c>
       <c r="D120" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>91</v>
+      </c>
+      <c r="B121" t="s">
         <v>92</v>
-      </c>
-      <c r="B121" t="s">
-        <v>93</v>
       </c>
       <c r="C121" t="s">
         <v>34</v>
       </c>
       <c r="D121" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>93</v>
+      </c>
+      <c r="B122" t="s">
         <v>94</v>
-      </c>
-      <c r="B122" t="s">
-        <v>95</v>
       </c>
       <c r="C122" t="s">
         <v>34</v>
       </c>
       <c r="D122" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B123" t="s">
         <v>38</v>
@@ -3727,12 +3745,12 @@
         <v>34</v>
       </c>
       <c r="D123" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B124" t="s">
         <v>53</v>
@@ -3746,7 +3764,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B125" t="s">
         <v>22</v>
@@ -3755,766 +3773,794 @@
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>66</v>
+        <v>548</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>158</v>
+      </c>
+      <c r="B126" t="s">
         <v>159</v>
-      </c>
-      <c r="B126" t="s">
-        <v>160</v>
       </c>
       <c r="C126" t="s">
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>423</v>
+      </c>
+      <c r="B127" t="s">
         <v>424</v>
-      </c>
-      <c r="B127" t="s">
-        <v>425</v>
       </c>
       <c r="C127" t="s">
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>161</v>
+      </c>
+      <c r="B128" t="s">
         <v>162</v>
-      </c>
-      <c r="B128" t="s">
-        <v>163</v>
       </c>
       <c r="C128" t="s">
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>410</v>
+      </c>
+      <c r="B129" t="s">
         <v>411</v>
-      </c>
-      <c r="B129" t="s">
-        <v>412</v>
       </c>
       <c r="C129" t="s">
         <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>276</v>
+      </c>
+      <c r="B130" t="s">
         <v>277</v>
-      </c>
-      <c r="B130" t="s">
-        <v>278</v>
       </c>
       <c r="C130" t="s">
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>331</v>
+      </c>
+      <c r="B131" t="s">
         <v>332</v>
-      </c>
-      <c r="B131" t="s">
-        <v>333</v>
       </c>
       <c r="C131" t="s">
         <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>534</v>
+      </c>
+      <c r="B132" t="s">
         <v>535</v>
-      </c>
-      <c r="B132" t="s">
-        <v>536</v>
       </c>
       <c r="C132" t="s">
         <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>333</v>
+      </c>
+      <c r="B133" t="s">
         <v>334</v>
-      </c>
-      <c r="B133" t="s">
-        <v>335</v>
       </c>
       <c r="C133" t="s">
         <v>6</v>
       </c>
       <c r="D133" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>541</v>
+      </c>
+      <c r="B134" t="s">
         <v>542</v>
-      </c>
-      <c r="B134" t="s">
-        <v>543</v>
       </c>
       <c r="C134" t="s">
         <v>6</v>
       </c>
       <c r="D134" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>289</v>
+        <v>544</v>
       </c>
       <c r="B135" t="s">
-        <v>13</v>
+        <v>546</v>
       </c>
       <c r="C135" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D135" t="s">
-        <v>62</v>
+        <v>547</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>290</v>
+        <v>545</v>
       </c>
       <c r="B136" t="s">
-        <v>30</v>
+        <v>549</v>
       </c>
       <c r="C136" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D136" t="s">
-        <v>71</v>
+        <v>550</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B137" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="C137" t="s">
         <v>14</v>
       </c>
       <c r="D137" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B138" t="s">
-        <v>338</v>
+        <v>30</v>
       </c>
       <c r="C138" t="s">
         <v>14</v>
       </c>
       <c r="D138" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>337</v>
+        <v>290</v>
       </c>
       <c r="B139" t="s">
-        <v>339</v>
+        <v>51</v>
       </c>
       <c r="C139" t="s">
         <v>14</v>
       </c>
       <c r="D139" t="s">
-        <v>340</v>
+        <v>77</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B140" t="s">
-        <v>55</v>
+        <v>337</v>
       </c>
       <c r="C140" t="s">
         <v>14</v>
       </c>
       <c r="D140" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>294</v>
+        <v>336</v>
       </c>
       <c r="B141" t="s">
-        <v>75</v>
+        <v>338</v>
       </c>
       <c r="C141" t="s">
         <v>14</v>
       </c>
       <c r="D141" t="s">
-        <v>76</v>
+        <v>339</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B142" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="C142" t="s">
         <v>14</v>
       </c>
       <c r="D142" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>342</v>
+        <v>293</v>
       </c>
       <c r="B143" t="s">
-        <v>343</v>
+        <v>74</v>
       </c>
       <c r="C143" t="s">
         <v>14</v>
       </c>
       <c r="D143" t="s">
-        <v>344</v>
+        <v>75</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B144" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C144" t="s">
         <v>14</v>
       </c>
       <c r="D144" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>297</v>
+        <v>341</v>
       </c>
       <c r="B145" t="s">
-        <v>119</v>
+        <v>342</v>
       </c>
       <c r="C145" t="s">
         <v>14</v>
       </c>
       <c r="D145" t="s">
-        <v>120</v>
+        <v>343</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>121</v>
+        <v>295</v>
       </c>
       <c r="B146" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C146" t="s">
         <v>14</v>
       </c>
       <c r="D146" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>125</v>
+        <v>296</v>
       </c>
       <c r="B147" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C147" t="s">
         <v>14</v>
       </c>
       <c r="D147" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B148" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C148" t="s">
         <v>14</v>
       </c>
       <c r="D148" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B149" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C149" t="s">
         <v>14</v>
       </c>
       <c r="D149" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B150" t="s">
-        <v>41</v>
+        <v>128</v>
       </c>
       <c r="C150" t="s">
         <v>14</v>
       </c>
       <c r="D150" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>196</v>
+        <v>131</v>
       </c>
       <c r="B151" t="s">
-        <v>197</v>
+        <v>130</v>
       </c>
       <c r="C151" t="s">
         <v>14</v>
       </c>
       <c r="D151" t="s">
-        <v>198</v>
+        <v>129</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>397</v>
+        <v>132</v>
       </c>
       <c r="B152" t="s">
-        <v>398</v>
+        <v>41</v>
       </c>
       <c r="C152" t="s">
         <v>14</v>
       </c>
       <c r="D152" t="s">
-        <v>399</v>
+        <v>78</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>304</v>
+        <v>195</v>
       </c>
       <c r="B153" t="s">
-        <v>104</v>
+        <v>196</v>
       </c>
       <c r="C153" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="D153" t="s">
-        <v>113</v>
+        <v>197</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>305</v>
+        <v>396</v>
       </c>
       <c r="B154" t="s">
-        <v>103</v>
+        <v>397</v>
       </c>
       <c r="C154" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="D154" t="s">
-        <v>21</v>
+        <v>398</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B155" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C155" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D155" t="s">
-        <v>23</v>
+        <v>112</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B156" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C156" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D156" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B157" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C157" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D157" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B158" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="C158" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D158" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B159" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C159" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D159" t="s">
-        <v>111</v>
+        <v>21</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B160" t="s">
-        <v>110</v>
+        <v>31</v>
       </c>
       <c r="C160" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D160" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B161" t="s">
-        <v>313</v>
+        <v>108</v>
       </c>
       <c r="C161" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D161" t="s">
-        <v>314</v>
+        <v>110</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B162" t="s">
-        <v>316</v>
+        <v>109</v>
       </c>
       <c r="C162" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D162" t="s">
-        <v>317</v>
+        <v>21</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>341</v>
+        <v>311</v>
       </c>
       <c r="B163" t="s">
-        <v>389</v>
+        <v>312</v>
       </c>
       <c r="C163" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D163" t="s">
-        <v>390</v>
+        <v>313</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B164" t="s">
-        <v>403</v>
+        <v>315</v>
       </c>
       <c r="C164" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D164" t="s">
-        <v>404</v>
+        <v>316</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>321</v>
+        <v>340</v>
       </c>
       <c r="B165" t="s">
-        <v>319</v>
+        <v>388</v>
       </c>
       <c r="C165" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D165" t="s">
-        <v>320</v>
+        <v>389</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>385</v>
+        <v>317</v>
       </c>
       <c r="B166" t="s">
-        <v>383</v>
+        <v>402</v>
       </c>
       <c r="C166" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="D166" t="s">
-        <v>384</v>
+        <v>403</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>385</v>
+        <v>320</v>
       </c>
       <c r="B167" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C167" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D167" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="B168" t="s">
-        <v>401</v>
+        <v>382</v>
       </c>
       <c r="C168" t="s">
         <v>18</v>
       </c>
       <c r="D168" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>148</v>
+        <v>384</v>
       </c>
       <c r="B169" t="s">
-        <v>149</v>
+        <v>321</v>
       </c>
       <c r="C169" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
       <c r="D169" t="s">
-        <v>151</v>
-      </c>
-      <c r="E169" t="s">
-        <v>152</v>
+        <v>322</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>153</v>
+        <v>399</v>
       </c>
       <c r="B170" t="s">
-        <v>154</v>
+        <v>400</v>
       </c>
       <c r="C170" t="s">
-        <v>150</v>
+        <v>18</v>
       </c>
       <c r="D170" t="s">
-        <v>420</v>
+        <v>401</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>421</v>
+        <v>147</v>
       </c>
       <c r="B171" t="s">
-        <v>422</v>
+        <v>148</v>
       </c>
       <c r="C171" t="s">
+        <v>149</v>
+      </c>
+      <c r="D171" t="s">
         <v>150</v>
       </c>
-      <c r="D171" t="s">
-        <v>423</v>
+      <c r="E171" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>217</v>
+        <v>152</v>
       </c>
       <c r="B172" t="s">
-        <v>218</v>
+        <v>153</v>
       </c>
       <c r="C172" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D172" t="s">
-        <v>219</v>
+        <v>419</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>260</v>
+        <v>420</v>
       </c>
       <c r="B173" t="s">
-        <v>261</v>
+        <v>421</v>
       </c>
       <c r="C173" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D173" t="s">
-        <v>262</v>
+        <v>422</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>263</v>
+        <v>216</v>
       </c>
       <c r="B174" t="s">
-        <v>264</v>
+        <v>217</v>
       </c>
       <c r="C174" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D174" t="s">
-        <v>265</v>
+        <v>218</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>506</v>
+        <v>259</v>
       </c>
       <c r="B175" t="s">
-        <v>500</v>
+        <v>260</v>
       </c>
       <c r="C175" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D175" t="s">
-        <v>501</v>
+        <v>261</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>502</v>
+        <v>262</v>
       </c>
       <c r="B176" t="s">
-        <v>503</v>
+        <v>263</v>
       </c>
       <c r="C176" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D176" t="s">
-        <v>507</v>
+        <v>264</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B177" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="C177" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D177" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>286</v>
+        <v>501</v>
       </c>
       <c r="B178" t="s">
-        <v>287</v>
+        <v>502</v>
       </c>
       <c r="C178" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D178" t="s">
-        <v>288</v>
+        <v>506</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
+        <v>503</v>
+      </c>
+      <c r="B179" t="s">
+        <v>504</v>
+      </c>
+      <c r="C179" t="s">
+        <v>149</v>
+      </c>
+      <c r="D179" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>285</v>
+      </c>
+      <c r="B180" t="s">
+        <v>286</v>
+      </c>
+      <c r="C180" t="s">
+        <v>149</v>
+      </c>
+      <c r="D180" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>516</v>
+      </c>
+      <c r="B181" t="s">
         <v>517</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C181" t="s">
+        <v>149</v>
+      </c>
+      <c r="D181" t="s">
         <v>518</v>
-      </c>
-      <c r="C179" t="s">
-        <v>150</v>
-      </c>
-      <c r="D179" t="s">
-        <v>519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New "active cancer" variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F7FE1A-B1C8-DE4B-AFB7-FB181DBE9FB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E06D0E-B438-9045-8FC4-1B47F27BD1AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33960" yWindow="3660" windowWidth="32960" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="560">
   <si>
     <t>Variable #</t>
   </si>
@@ -1697,6 +1697,15 @@
   </si>
   <si>
     <t>Derived stage (two levels: localized or disseminated)</t>
+  </si>
+  <si>
+    <t>Ca21</t>
+  </si>
+  <si>
+    <t>cancer_active</t>
+  </si>
+  <si>
+    <t>Active cancer/treatment vs inactive</t>
   </si>
 </sst>
 </file>
@@ -1752,10 +1761,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E183" totalsRowShown="0">
-  <autoFilter ref="A1:E183" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E182">
-    <sortCondition ref="A1:A182"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E184" totalsRowShown="0">
+  <autoFilter ref="A1:E184" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E183">
+    <sortCondition ref="A1:A183"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -2089,9 +2098,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E183"/>
+  <dimension ref="A1:E184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -2809,1619 +2818,1619 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>279</v>
+        <v>557</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>558</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>46</v>
+        <v>559</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>133</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>512</v>
+        <v>280</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
       <c r="C53" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>281</v>
+        <v>513</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>514</v>
+        <v>281</v>
       </c>
       <c r="B56" t="s">
-        <v>202</v>
+        <v>17</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>203</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="B57" t="s">
-        <v>509</v>
+        <v>202</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
       </c>
+      <c r="D57" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>282</v>
+        <v>508</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>509</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>137</v>
+        <v>282</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>328</v>
+        <v>137</v>
       </c>
       <c r="B60" t="s">
-        <v>329</v>
+        <v>3</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>330</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>138</v>
+        <v>328</v>
       </c>
       <c r="B61" t="s">
-        <v>139</v>
+        <v>329</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>140</v>
+        <v>330</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="B62" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="C62" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="B63" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="C63" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D63" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>427</v>
+        <v>192</v>
       </c>
       <c r="B64" t="s">
-        <v>428</v>
+        <v>193</v>
       </c>
       <c r="C64" t="s">
-        <v>429</v>
+        <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>495</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B65" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C65" t="s">
         <v>429</v>
       </c>
       <c r="D65" t="s">
-        <v>432</v>
+        <v>495</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B66" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C66" t="s">
         <v>429</v>
       </c>
       <c r="D66" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B67" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C67" t="s">
         <v>429</v>
       </c>
       <c r="D67" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B68" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C68" t="s">
         <v>429</v>
       </c>
       <c r="D68" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B69" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C69" t="s">
         <v>429</v>
       </c>
+      <c r="D69" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B70" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C70" t="s">
         <v>429</v>
       </c>
-      <c r="D70" t="s">
-        <v>446</v>
-      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B71" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C71" t="s">
         <v>429</v>
       </c>
       <c r="D71" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B72" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C72" t="s">
         <v>429</v>
       </c>
       <c r="D72" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B73" t="s">
-        <v>454</v>
+        <v>451</v>
+      </c>
+      <c r="C73" t="s">
+        <v>429</v>
+      </c>
+      <c r="D73" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B74" t="s">
-        <v>456</v>
-      </c>
-      <c r="D74" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B75" t="s">
-        <v>459</v>
+        <v>456</v>
+      </c>
+      <c r="D75" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B76" t="s">
-        <v>461</v>
-      </c>
-      <c r="D76" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B77" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D77" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B78" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D78" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B79" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D79" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B80" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D80" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B81" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D81" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B82" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D82" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B83" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D83" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B84" t="s">
-        <v>485</v>
+        <v>482</v>
+      </c>
+      <c r="D84" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B85" t="s">
-        <v>487</v>
-      </c>
-      <c r="D85" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="B86" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D86" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B87" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D87" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B88" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D88" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>247</v>
+        <v>498</v>
       </c>
       <c r="B89" t="s">
-        <v>164</v>
-      </c>
-      <c r="C89" t="s">
-        <v>165</v>
+        <v>493</v>
       </c>
       <c r="D89" t="s">
-        <v>166</v>
+        <v>494</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B90" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C90" t="s">
         <v>165</v>
       </c>
       <c r="D90" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B91" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C91" t="s">
         <v>165</v>
       </c>
       <c r="D91" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B92" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C92" t="s">
         <v>165</v>
       </c>
       <c r="D92" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B93" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C93" t="s">
         <v>165</v>
       </c>
       <c r="D93" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B94" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C94" t="s">
         <v>165</v>
       </c>
       <c r="D94" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B95" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C95" t="s">
         <v>165</v>
       </c>
       <c r="D95" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B96" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C96" t="s">
         <v>165</v>
       </c>
       <c r="D96" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B97" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C97" t="s">
         <v>165</v>
       </c>
       <c r="D97" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>189</v>
+        <v>255</v>
       </c>
       <c r="B98" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C98" t="s">
         <v>165</v>
       </c>
       <c r="D98" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>226</v>
+        <v>189</v>
       </c>
       <c r="B99" t="s">
-        <v>230</v>
+        <v>190</v>
       </c>
       <c r="C99" t="s">
         <v>165</v>
       </c>
       <c r="D99" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B100" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C100" t="s">
         <v>165</v>
       </c>
       <c r="D100" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B101" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C101" t="s">
         <v>165</v>
       </c>
       <c r="D101" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B102" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C102" t="s">
         <v>165</v>
       </c>
       <c r="D102" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B103" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C103" t="s">
         <v>165</v>
       </c>
       <c r="D103" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B104" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C104" t="s">
         <v>165</v>
       </c>
       <c r="D104" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="B105" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="C105" t="s">
         <v>165</v>
       </c>
       <c r="D105" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>256</v>
+        <v>229</v>
       </c>
       <c r="B106" t="s">
-        <v>257</v>
+        <v>227</v>
       </c>
       <c r="C106" t="s">
         <v>165</v>
       </c>
       <c r="D106" t="s">
-        <v>258</v>
+        <v>228</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>390</v>
+        <v>256</v>
       </c>
       <c r="B107" t="s">
-        <v>391</v>
+        <v>257</v>
       </c>
       <c r="C107" t="s">
         <v>165</v>
       </c>
       <c r="D107" t="s">
-        <v>392</v>
+        <v>258</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>267</v>
+        <v>390</v>
       </c>
       <c r="B108" t="s">
-        <v>4</v>
+        <v>391</v>
       </c>
       <c r="C108" t="s">
-        <v>6</v>
+        <v>165</v>
       </c>
       <c r="D108" t="s">
-        <v>57</v>
+        <v>392</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B109" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C109" t="s">
         <v>6</v>
       </c>
       <c r="D109" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>325</v>
+        <v>268</v>
       </c>
       <c r="B110" t="s">
-        <v>326</v>
+        <v>11</v>
       </c>
       <c r="C110" t="s">
         <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>327</v>
+        <v>58</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>269</v>
+        <v>325</v>
       </c>
       <c r="B111" t="s">
-        <v>10</v>
+        <v>326</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>59</v>
+        <v>327</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B112" t="s">
-        <v>323</v>
+        <v>10</v>
       </c>
       <c r="C112" t="s">
         <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>324</v>
+        <v>59</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B113" t="s">
-        <v>12</v>
+        <v>323</v>
       </c>
       <c r="C113" t="s">
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>60</v>
+        <v>324</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B114" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="C114" t="s">
         <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B115" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C115" t="s">
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>215</v>
+        <v>82</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B116" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C116" t="s">
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B117" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="C117" t="s">
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>83</v>
+        <v>275</v>
       </c>
       <c r="B118" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="C118" t="s">
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>85</v>
+        <v>284</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B119" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="C119" t="s">
         <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B120" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="C120" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B121" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C121" t="s">
         <v>34</v>
       </c>
       <c r="D121" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B122" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C122" t="s">
         <v>34</v>
       </c>
       <c r="D122" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B123" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C123" t="s">
         <v>34</v>
       </c>
       <c r="D123" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B124" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="C124" t="s">
         <v>34</v>
       </c>
       <c r="D124" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B125" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C125" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D125" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B126" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C126" t="s">
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>548</v>
+        <v>53</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>551</v>
+        <v>113</v>
       </c>
       <c r="B127" t="s">
-        <v>552</v>
+        <v>22</v>
       </c>
       <c r="C127" t="s">
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>65</v>
+        <v>548</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>158</v>
+        <v>551</v>
       </c>
       <c r="B128" t="s">
-        <v>159</v>
+        <v>552</v>
       </c>
       <c r="C128" t="s">
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>160</v>
+        <v>65</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>423</v>
+        <v>158</v>
       </c>
       <c r="B129" t="s">
-        <v>424</v>
+        <v>159</v>
       </c>
       <c r="C129" t="s">
         <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>425</v>
+        <v>160</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>161</v>
+        <v>423</v>
       </c>
       <c r="B130" t="s">
-        <v>162</v>
+        <v>424</v>
       </c>
       <c r="C130" t="s">
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>163</v>
+        <v>425</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>410</v>
+        <v>161</v>
       </c>
       <c r="B131" t="s">
-        <v>411</v>
+        <v>162</v>
       </c>
       <c r="C131" t="s">
         <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>412</v>
+        <v>163</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>276</v>
+        <v>410</v>
       </c>
       <c r="B132" t="s">
-        <v>277</v>
+        <v>411</v>
       </c>
       <c r="C132" t="s">
         <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>278</v>
+        <v>412</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>331</v>
+        <v>276</v>
       </c>
       <c r="B133" t="s">
-        <v>332</v>
+        <v>277</v>
       </c>
       <c r="C133" t="s">
         <v>6</v>
       </c>
       <c r="D133" t="s">
-        <v>537</v>
+        <v>278</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>534</v>
+        <v>331</v>
       </c>
       <c r="B134" t="s">
-        <v>535</v>
+        <v>332</v>
       </c>
       <c r="C134" t="s">
         <v>6</v>
       </c>
       <c r="D134" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>333</v>
+        <v>534</v>
       </c>
       <c r="B135" t="s">
-        <v>334</v>
+        <v>535</v>
       </c>
       <c r="C135" t="s">
         <v>6</v>
       </c>
       <c r="D135" t="s">
-        <v>335</v>
+        <v>536</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>541</v>
+        <v>333</v>
       </c>
       <c r="B136" t="s">
-        <v>542</v>
+        <v>334</v>
       </c>
       <c r="C136" t="s">
         <v>6</v>
       </c>
       <c r="D136" t="s">
-        <v>543</v>
+        <v>335</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B137" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C137" t="s">
         <v>6</v>
       </c>
       <c r="D137" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B138" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C138" t="s">
         <v>6</v>
       </c>
       <c r="D138" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>288</v>
+        <v>545</v>
       </c>
       <c r="B139" t="s">
-        <v>13</v>
+        <v>549</v>
       </c>
       <c r="C139" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D139" t="s">
-        <v>61</v>
+        <v>550</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B140" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C140" t="s">
         <v>14</v>
       </c>
       <c r="D140" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B141" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C141" t="s">
         <v>14</v>
       </c>
       <c r="D141" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B142" t="s">
-        <v>337</v>
+        <v>50</v>
       </c>
       <c r="C142" t="s">
         <v>14</v>
       </c>
       <c r="D142" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>336</v>
+        <v>291</v>
       </c>
       <c r="B143" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C143" t="s">
         <v>14</v>
       </c>
       <c r="D143" t="s">
-        <v>339</v>
+        <v>114</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>292</v>
+        <v>336</v>
       </c>
       <c r="B144" t="s">
-        <v>54</v>
+        <v>338</v>
       </c>
       <c r="C144" t="s">
         <v>14</v>
       </c>
       <c r="D144" t="s">
-        <v>76</v>
+        <v>339</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B145" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C145" t="s">
         <v>14</v>
       </c>
       <c r="D145" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B146" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="C146" t="s">
         <v>14</v>
       </c>
       <c r="D146" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>341</v>
+        <v>294</v>
       </c>
       <c r="B147" t="s">
-        <v>342</v>
+        <v>115</v>
       </c>
       <c r="C147" t="s">
         <v>14</v>
       </c>
       <c r="D147" t="s">
-        <v>343</v>
+        <v>79</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>295</v>
+        <v>341</v>
       </c>
       <c r="B148" t="s">
-        <v>116</v>
+        <v>342</v>
       </c>
       <c r="C148" t="s">
         <v>14</v>
       </c>
       <c r="D148" t="s">
-        <v>117</v>
+        <v>343</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B149" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C149" t="s">
         <v>14</v>
       </c>
       <c r="D149" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>120</v>
+        <v>296</v>
       </c>
       <c r="B150" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C150" t="s">
         <v>14</v>
       </c>
       <c r="D150" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B151" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C151" t="s">
         <v>14</v>
       </c>
       <c r="D151" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B152" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C152" t="s">
         <v>14</v>
       </c>
       <c r="D152" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B153" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C153" t="s">
         <v>14</v>
       </c>
       <c r="D153" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B154" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C154" t="s">
         <v>14</v>
       </c>
       <c r="D154" t="s">
-        <v>78</v>
+        <v>129</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>195</v>
+        <v>132</v>
       </c>
       <c r="B155" t="s">
-        <v>196</v>
+        <v>40</v>
       </c>
       <c r="C155" t="s">
         <v>14</v>
       </c>
       <c r="D155" t="s">
-        <v>197</v>
+        <v>78</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>396</v>
+        <v>195</v>
       </c>
       <c r="B156" t="s">
-        <v>397</v>
+        <v>196</v>
       </c>
       <c r="C156" t="s">
         <v>14</v>
       </c>
       <c r="D156" t="s">
-        <v>398</v>
+        <v>197</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>303</v>
+        <v>396</v>
       </c>
       <c r="B157" t="s">
-        <v>103</v>
+        <v>397</v>
       </c>
       <c r="C157" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="D157" t="s">
-        <v>112</v>
+        <v>398</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B158" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C158" t="s">
         <v>104</v>
       </c>
       <c r="D158" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B159" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C159" t="s">
         <v>104</v>
       </c>
       <c r="D159" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B160" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C160" t="s">
         <v>104</v>
       </c>
       <c r="D160" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B161" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C161" t="s">
         <v>104</v>
       </c>
       <c r="D161" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B162" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="C162" t="s">
         <v>104</v>
       </c>
       <c r="D162" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B163" t="s">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="C163" t="s">
         <v>104</v>
       </c>
       <c r="D163" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B164" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C164" t="s">
         <v>104</v>
       </c>
       <c r="D164" t="s">
-        <v>21</v>
+        <v>110</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B165" t="s">
-        <v>312</v>
+        <v>109</v>
       </c>
       <c r="C165" t="s">
         <v>104</v>
       </c>
       <c r="D165" t="s">
-        <v>313</v>
+        <v>21</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B166" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C166" t="s">
         <v>104</v>
       </c>
       <c r="D166" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
       <c r="B167" t="s">
-        <v>388</v>
+        <v>315</v>
       </c>
       <c r="C167" t="s">
         <v>104</v>
       </c>
       <c r="D167" t="s">
-        <v>389</v>
+        <v>316</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>317</v>
+        <v>340</v>
       </c>
       <c r="B168" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="C168" t="s">
         <v>104</v>
       </c>
       <c r="D168" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B169" t="s">
-        <v>318</v>
+        <v>402</v>
       </c>
       <c r="C169" t="s">
         <v>104</v>
       </c>
       <c r="D169" t="s">
-        <v>319</v>
+        <v>403</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>384</v>
+        <v>320</v>
       </c>
       <c r="B170" t="s">
-        <v>382</v>
+        <v>318</v>
       </c>
       <c r="C170" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="D170" t="s">
-        <v>383</v>
+        <v>319</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -4429,183 +4438,197 @@
         <v>384</v>
       </c>
       <c r="B171" t="s">
-        <v>321</v>
+        <v>382</v>
       </c>
       <c r="C171" t="s">
-        <v>104</v>
+        <v>18</v>
       </c>
       <c r="D171" t="s">
-        <v>322</v>
+        <v>383</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="B172" t="s">
-        <v>400</v>
+        <v>321</v>
       </c>
       <c r="C172" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="D172" t="s">
-        <v>401</v>
+        <v>322</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>147</v>
+        <v>399</v>
       </c>
       <c r="B173" t="s">
-        <v>148</v>
+        <v>400</v>
       </c>
       <c r="C173" t="s">
-        <v>149</v>
+        <v>18</v>
       </c>
       <c r="D173" t="s">
-        <v>150</v>
-      </c>
-      <c r="E173" t="s">
-        <v>151</v>
+        <v>401</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B174" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C174" t="s">
         <v>149</v>
       </c>
       <c r="D174" t="s">
-        <v>419</v>
+        <v>150</v>
+      </c>
+      <c r="E174" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>420</v>
+        <v>152</v>
       </c>
       <c r="B175" t="s">
-        <v>421</v>
+        <v>153</v>
       </c>
       <c r="C175" t="s">
         <v>149</v>
       </c>
       <c r="D175" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>216</v>
+        <v>420</v>
       </c>
       <c r="B176" t="s">
-        <v>217</v>
+        <v>421</v>
       </c>
       <c r="C176" t="s">
         <v>149</v>
       </c>
       <c r="D176" t="s">
-        <v>218</v>
+        <v>422</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>259</v>
+        <v>216</v>
       </c>
       <c r="B177" t="s">
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="C177" t="s">
         <v>149</v>
       </c>
       <c r="D177" t="s">
-        <v>261</v>
+        <v>218</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B178" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C178" t="s">
         <v>149</v>
       </c>
       <c r="D178" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>505</v>
+        <v>262</v>
       </c>
       <c r="B179" t="s">
-        <v>499</v>
+        <v>263</v>
       </c>
       <c r="C179" t="s">
         <v>149</v>
       </c>
       <c r="D179" t="s">
-        <v>500</v>
+        <v>264</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B180" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C180" t="s">
         <v>149</v>
       </c>
       <c r="D180" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B181" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C181" t="s">
         <v>149</v>
       </c>
       <c r="D181" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>285</v>
+        <v>503</v>
       </c>
       <c r="B182" t="s">
-        <v>286</v>
+        <v>504</v>
       </c>
       <c r="C182" t="s">
         <v>149</v>
       </c>
       <c r="D182" t="s">
-        <v>287</v>
+        <v>507</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>516</v>
+        <v>285</v>
       </c>
       <c r="B183" t="s">
-        <v>517</v>
+        <v>286</v>
       </c>
       <c r="C183" t="s">
         <v>149</v>
       </c>
       <c r="D183" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>516</v>
+      </c>
+      <c r="B184" t="s">
+        <v>517</v>
+      </c>
+      <c r="C184" t="s">
+        <v>149</v>
+      </c>
+      <c r="D184" t="s">
         <v>518</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Time dependent thrombosis variables added
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E06D0E-B438-9045-8FC4-1B47F27BD1AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9943DC71-9860-6240-8718-D58029DCE56B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="578">
   <si>
     <t>Variable #</t>
   </si>
@@ -310,9 +310,6 @@
     <t>O15</t>
   </si>
   <si>
-    <t>thrombosis_NOS</t>
-  </si>
-  <si>
     <t>Thrombosis NOS complications</t>
   </si>
   <si>
@@ -1706,6 +1703,63 @@
   </si>
   <si>
     <t>Active cancer/treatment vs inactive</t>
+  </si>
+  <si>
+    <t>O12a</t>
+  </si>
+  <si>
+    <t>PE_comp_within_3mo</t>
+  </si>
+  <si>
+    <t>PE complications within 3 months of COVID-19 diagnosis</t>
+  </si>
+  <si>
+    <t>O14a</t>
+  </si>
+  <si>
+    <t>DVT_comp_within_3mo</t>
+  </si>
+  <si>
+    <t>DVT complications within 3 months of COVID-19 diagnosis</t>
+  </si>
+  <si>
+    <t>thrombosis_NOS_comp</t>
+  </si>
+  <si>
+    <t>O15a</t>
+  </si>
+  <si>
+    <t>thrombosis_NOS_comp_within_3mo</t>
+  </si>
+  <si>
+    <t>Thrombosis NOS complications within 3 months of COVID-19 diagnosis</t>
+  </si>
+  <si>
+    <t>O19b</t>
+  </si>
+  <si>
+    <t>VTE_comp_within_3mo</t>
+  </si>
+  <si>
+    <t>Combined VTE complications within 3 months of COVID-19 diagnosis</t>
+  </si>
+  <si>
+    <t>O26</t>
+  </si>
+  <si>
+    <t>ATE_comp_within_3mo</t>
+  </si>
+  <si>
+    <t>Combined ATE complications within 3 months of COVID-19 diagnosis</t>
+  </si>
+  <si>
+    <t>O26a</t>
+  </si>
+  <si>
+    <t>stroke_comp_within_3mo</t>
+  </si>
+  <si>
+    <t>CVA as a complication within 3 months of COVID-19 diagnosis</t>
   </si>
 </sst>
 </file>
@@ -1761,10 +1815,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E184" totalsRowShown="0">
-  <autoFilter ref="A1:E184" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E183">
-    <sortCondition ref="A1:A183"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E190" totalsRowShown="0">
+  <autoFilter ref="A1:E190" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E189">
+    <sortCondition ref="A1:A189"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -2098,10 +2152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E184"/>
+  <dimension ref="A1:E190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2132,49 +2186,49 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B4" t="s">
         <v>414</v>
-      </c>
-      <c r="B4" t="s">
-        <v>415</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -2188,7 +2242,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
@@ -2202,21 +2256,21 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B8" t="s">
         <v>38</v>
@@ -2230,7 +2284,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
@@ -2244,7 +2298,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
@@ -2258,7 +2312,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B11" t="s">
         <v>42</v>
@@ -2267,12 +2321,12 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B12" t="s">
         <v>55</v>
@@ -2286,83 +2340,83 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>355</v>
+      </c>
+      <c r="B15" t="s">
         <v>356</v>
-      </c>
-      <c r="B15" t="s">
-        <v>357</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>403</v>
+      </c>
+      <c r="B17" t="s">
         <v>404</v>
-      </c>
-      <c r="B17" t="s">
-        <v>405</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D18" t="s">
         <v>62</v>
@@ -2370,35 +2424,35 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C19" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>359</v>
+      </c>
+      <c r="B20" t="s">
         <v>360</v>
       </c>
-      <c r="B20" t="s">
-        <v>361</v>
-      </c>
       <c r="C20" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
@@ -2412,7 +2466,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B22" t="s">
         <v>72</v>
@@ -2426,13 +2480,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B23" t="s">
         <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D23" t="s">
         <v>36</v>
@@ -2440,7 +2494,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -2454,10 +2508,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -2468,374 +2522,374 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B26" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B27" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" t="s">
         <v>206</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>552</v>
+      </c>
+      <c r="D31" t="s">
         <v>207</v>
-      </c>
-      <c r="C31" t="s">
-        <v>553</v>
-      </c>
-      <c r="D31" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B32" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C32" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D32" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C33" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B34" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C34" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D34" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B35" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C35" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C36" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D36" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B37" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C37" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D37" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B38" t="s">
+        <v>209</v>
+      </c>
+      <c r="C38" t="s">
+        <v>552</v>
+      </c>
+      <c r="D38" t="s">
         <v>210</v>
-      </c>
-      <c r="C38" t="s">
-        <v>553</v>
-      </c>
-      <c r="D38" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B39" t="s">
+        <v>212</v>
+      </c>
+      <c r="C39" t="s">
+        <v>552</v>
+      </c>
+      <c r="D39" t="s">
         <v>213</v>
-      </c>
-      <c r="C39" t="s">
-        <v>553</v>
-      </c>
-      <c r="D39" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>392</v>
+      </c>
+      <c r="B40" t="s">
         <v>393</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>552</v>
+      </c>
+      <c r="D40" t="s">
         <v>394</v>
-      </c>
-      <c r="C40" t="s">
-        <v>553</v>
-      </c>
-      <c r="D40" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>199</v>
+      </c>
+      <c r="B41" t="s">
         <v>200</v>
-      </c>
-      <c r="B41" t="s">
-        <v>201</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>219</v>
+      </c>
+      <c r="B42" t="s">
         <v>220</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
+        <v>552</v>
+      </c>
+      <c r="D42" t="s">
         <v>221</v>
-      </c>
-      <c r="C42" t="s">
-        <v>553</v>
-      </c>
-      <c r="D42" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>222</v>
+      </c>
+      <c r="B43" t="s">
         <v>223</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
+        <v>552</v>
+      </c>
+      <c r="D43" t="s">
         <v>224</v>
-      </c>
-      <c r="C43" t="s">
-        <v>553</v>
-      </c>
-      <c r="D43" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>518</v>
+      </c>
+      <c r="B44" t="s">
         <v>519</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
+        <v>552</v>
+      </c>
+      <c r="D44" t="s">
         <v>520</v>
-      </c>
-      <c r="C44" t="s">
-        <v>553</v>
-      </c>
-      <c r="D44" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B45" t="s">
+        <v>521</v>
+      </c>
+      <c r="C45" t="s">
+        <v>552</v>
+      </c>
+      <c r="D45" t="s">
         <v>522</v>
-      </c>
-      <c r="C45" t="s">
-        <v>553</v>
-      </c>
-      <c r="D45" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>524</v>
+      </c>
+      <c r="B46" t="s">
         <v>525</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
+        <v>552</v>
+      </c>
+      <c r="D46" t="s">
         <v>526</v>
-      </c>
-      <c r="C46" t="s">
-        <v>553</v>
-      </c>
-      <c r="D46" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>527</v>
+      </c>
+      <c r="B47" t="s">
         <v>528</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
+        <v>552</v>
+      </c>
+      <c r="D47" t="s">
         <v>529</v>
-      </c>
-      <c r="C47" t="s">
-        <v>553</v>
-      </c>
-      <c r="D47" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>530</v>
+      </c>
+      <c r="B48" t="s">
         <v>531</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
+        <v>552</v>
+      </c>
+      <c r="D48" t="s">
         <v>532</v>
-      </c>
-      <c r="C48" t="s">
-        <v>553</v>
-      </c>
-      <c r="D48" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>537</v>
+      </c>
+      <c r="B49" t="s">
         <v>538</v>
-      </c>
-      <c r="B49" t="s">
-        <v>539</v>
       </c>
       <c r="C49" t="s">
         <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>553</v>
+      </c>
+      <c r="B50" t="s">
         <v>554</v>
-      </c>
-      <c r="B50" t="s">
-        <v>555</v>
       </c>
       <c r="C50" t="s">
         <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>556</v>
+      </c>
+      <c r="B51" t="s">
         <v>557</v>
-      </c>
-      <c r="B51" t="s">
-        <v>558</v>
       </c>
       <c r="C51" t="s">
         <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -2846,7 +2900,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B53" t="s">
         <v>44</v>
@@ -2860,35 +2914,35 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C54" t="s">
         <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B56" t="s">
         <v>17</v>
@@ -2902,24 +2956,24 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B57" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>507</v>
+      </c>
+      <c r="B58" t="s">
         <v>508</v>
-      </c>
-      <c r="B58" t="s">
-        <v>509</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -2927,7 +2981,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B59" t="s">
         <v>20</v>
@@ -2941,7 +2995,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
@@ -2955,619 +3009,619 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>327</v>
+      </c>
+      <c r="B61" t="s">
         <v>328</v>
-      </c>
-      <c r="B61" t="s">
-        <v>329</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>137</v>
+      </c>
+      <c r="B62" t="s">
         <v>138</v>
-      </c>
-      <c r="B62" t="s">
-        <v>139</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>167</v>
+      </c>
+      <c r="B63" t="s">
         <v>168</v>
-      </c>
-      <c r="B63" t="s">
-        <v>169</v>
       </c>
       <c r="C63" t="s">
         <v>15</v>
       </c>
       <c r="D63" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>191</v>
+      </c>
+      <c r="B64" t="s">
         <v>192</v>
-      </c>
-      <c r="B64" t="s">
-        <v>193</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>426</v>
+      </c>
+      <c r="B65" t="s">
         <v>427</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>428</v>
       </c>
-      <c r="C65" t="s">
-        <v>429</v>
-      </c>
       <c r="D65" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>429</v>
+      </c>
+      <c r="B66" t="s">
         <v>430</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>428</v>
+      </c>
+      <c r="D66" t="s">
         <v>431</v>
-      </c>
-      <c r="C66" t="s">
-        <v>429</v>
-      </c>
-      <c r="D66" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>432</v>
+      </c>
+      <c r="B67" t="s">
         <v>433</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>428</v>
+      </c>
+      <c r="D67" t="s">
         <v>434</v>
-      </c>
-      <c r="C67" t="s">
-        <v>429</v>
-      </c>
-      <c r="D67" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>435</v>
+      </c>
+      <c r="B68" t="s">
         <v>436</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
+        <v>428</v>
+      </c>
+      <c r="D68" t="s">
         <v>437</v>
-      </c>
-      <c r="C68" t="s">
-        <v>429</v>
-      </c>
-      <c r="D68" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>438</v>
+      </c>
+      <c r="B69" t="s">
         <v>439</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
+        <v>428</v>
+      </c>
+      <c r="D69" t="s">
         <v>440</v>
-      </c>
-      <c r="C69" t="s">
-        <v>429</v>
-      </c>
-      <c r="D69" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>441</v>
+      </c>
+      <c r="B70" t="s">
         <v>442</v>
       </c>
-      <c r="B70" t="s">
-        <v>443</v>
-      </c>
       <c r="C70" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>443</v>
+      </c>
+      <c r="B71" t="s">
         <v>444</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
+        <v>428</v>
+      </c>
+      <c r="D71" t="s">
         <v>445</v>
-      </c>
-      <c r="C71" t="s">
-        <v>429</v>
-      </c>
-      <c r="D71" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>446</v>
+      </c>
+      <c r="B72" t="s">
         <v>447</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
+        <v>428</v>
+      </c>
+      <c r="D72" t="s">
         <v>448</v>
-      </c>
-      <c r="C72" t="s">
-        <v>429</v>
-      </c>
-      <c r="D72" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>449</v>
+      </c>
+      <c r="B73" t="s">
         <v>450</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
+        <v>428</v>
+      </c>
+      <c r="D73" t="s">
         <v>451</v>
-      </c>
-      <c r="C73" t="s">
-        <v>429</v>
-      </c>
-      <c r="D73" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>452</v>
+      </c>
+      <c r="B74" t="s">
         <v>453</v>
-      </c>
-      <c r="B74" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>454</v>
+      </c>
+      <c r="B75" t="s">
         <v>455</v>
       </c>
-      <c r="B75" t="s">
+      <c r="D75" t="s">
         <v>456</v>
-      </c>
-      <c r="D75" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>457</v>
+      </c>
+      <c r="B76" t="s">
         <v>458</v>
-      </c>
-      <c r="B76" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>459</v>
+      </c>
+      <c r="B77" t="s">
         <v>460</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D77" t="s">
         <v>461</v>
-      </c>
-      <c r="D77" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>462</v>
+      </c>
+      <c r="B78" t="s">
         <v>463</v>
       </c>
-      <c r="B78" t="s">
+      <c r="D78" t="s">
         <v>464</v>
-      </c>
-      <c r="D78" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>465</v>
+      </c>
+      <c r="B79" t="s">
         <v>466</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
         <v>467</v>
-      </c>
-      <c r="D79" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>468</v>
+      </c>
+      <c r="B80" t="s">
         <v>469</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>470</v>
-      </c>
-      <c r="D80" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>471</v>
+      </c>
+      <c r="B81" t="s">
         <v>472</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>473</v>
-      </c>
-      <c r="D81" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>474</v>
+      </c>
+      <c r="B82" t="s">
         <v>475</v>
       </c>
-      <c r="B82" t="s">
+      <c r="D82" t="s">
         <v>476</v>
-      </c>
-      <c r="D82" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>477</v>
+      </c>
+      <c r="B83" t="s">
         <v>478</v>
       </c>
-      <c r="B83" t="s">
+      <c r="D83" t="s">
         <v>479</v>
-      </c>
-      <c r="D83" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>480</v>
+      </c>
+      <c r="B84" t="s">
         <v>481</v>
       </c>
-      <c r="B84" t="s">
+      <c r="D84" t="s">
         <v>482</v>
-      </c>
-      <c r="D84" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>483</v>
+      </c>
+      <c r="B85" t="s">
         <v>484</v>
-      </c>
-      <c r="B85" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>485</v>
+      </c>
+      <c r="B86" t="s">
         <v>486</v>
       </c>
-      <c r="B86" t="s">
+      <c r="D86" t="s">
         <v>487</v>
-      </c>
-      <c r="D86" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B87" t="s">
+        <v>488</v>
+      </c>
+      <c r="D87" t="s">
         <v>489</v>
-      </c>
-      <c r="D87" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B88" t="s">
+        <v>490</v>
+      </c>
+      <c r="D88" t="s">
         <v>491</v>
-      </c>
-      <c r="D88" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B89" t="s">
+        <v>492</v>
+      </c>
+      <c r="D89" t="s">
         <v>493</v>
-      </c>
-      <c r="D89" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B90" t="s">
+        <v>163</v>
+      </c>
+      <c r="C90" t="s">
         <v>164</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>165</v>
-      </c>
-      <c r="D90" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B91" t="s">
+        <v>172</v>
+      </c>
+      <c r="C91" t="s">
+        <v>164</v>
+      </c>
+      <c r="D91" t="s">
         <v>173</v>
-      </c>
-      <c r="C91" t="s">
-        <v>165</v>
-      </c>
-      <c r="D91" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B92" t="s">
+        <v>174</v>
+      </c>
+      <c r="C92" t="s">
+        <v>164</v>
+      </c>
+      <c r="D92" t="s">
         <v>175</v>
-      </c>
-      <c r="C92" t="s">
-        <v>165</v>
-      </c>
-      <c r="D92" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B93" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C93" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D93" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B94" t="s">
+        <v>178</v>
+      </c>
+      <c r="C94" t="s">
+        <v>164</v>
+      </c>
+      <c r="D94" t="s">
         <v>179</v>
-      </c>
-      <c r="C94" t="s">
-        <v>165</v>
-      </c>
-      <c r="D94" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B95" t="s">
+        <v>180</v>
+      </c>
+      <c r="C95" t="s">
+        <v>164</v>
+      </c>
+      <c r="D95" t="s">
         <v>181</v>
-      </c>
-      <c r="C95" t="s">
-        <v>165</v>
-      </c>
-      <c r="D95" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B96" t="s">
+        <v>182</v>
+      </c>
+      <c r="C96" t="s">
+        <v>164</v>
+      </c>
+      <c r="D96" t="s">
         <v>183</v>
-      </c>
-      <c r="C96" t="s">
-        <v>165</v>
-      </c>
-      <c r="D96" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B97" t="s">
+        <v>184</v>
+      </c>
+      <c r="C97" t="s">
+        <v>164</v>
+      </c>
+      <c r="D97" t="s">
         <v>185</v>
-      </c>
-      <c r="C97" t="s">
-        <v>165</v>
-      </c>
-      <c r="D97" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B98" t="s">
+        <v>186</v>
+      </c>
+      <c r="C98" t="s">
+        <v>164</v>
+      </c>
+      <c r="D98" t="s">
         <v>187</v>
-      </c>
-      <c r="C98" t="s">
-        <v>165</v>
-      </c>
-      <c r="D98" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>188</v>
+      </c>
+      <c r="B99" t="s">
         <v>189</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
+        <v>164</v>
+      </c>
+      <c r="D99" t="s">
         <v>190</v>
-      </c>
-      <c r="C99" t="s">
-        <v>165</v>
-      </c>
-      <c r="D99" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B100" t="s">
+        <v>229</v>
+      </c>
+      <c r="C100" t="s">
+        <v>164</v>
+      </c>
+      <c r="D100" t="s">
         <v>230</v>
-      </c>
-      <c r="C100" t="s">
-        <v>165</v>
-      </c>
-      <c r="D100" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>231</v>
+      </c>
+      <c r="B101" t="s">
         <v>232</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
+        <v>164</v>
+      </c>
+      <c r="D101" t="s">
         <v>233</v>
-      </c>
-      <c r="C101" t="s">
-        <v>165</v>
-      </c>
-      <c r="D101" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>234</v>
+      </c>
+      <c r="B102" t="s">
         <v>235</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
+        <v>164</v>
+      </c>
+      <c r="D102" t="s">
         <v>236</v>
-      </c>
-      <c r="C102" t="s">
-        <v>165</v>
-      </c>
-      <c r="D102" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>237</v>
+      </c>
+      <c r="B103" t="s">
         <v>238</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
+        <v>164</v>
+      </c>
+      <c r="D103" t="s">
         <v>239</v>
-      </c>
-      <c r="C103" t="s">
-        <v>165</v>
-      </c>
-      <c r="D103" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>240</v>
+      </c>
+      <c r="B104" t="s">
         <v>241</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
+        <v>164</v>
+      </c>
+      <c r="D104" t="s">
         <v>242</v>
-      </c>
-      <c r="C104" t="s">
-        <v>165</v>
-      </c>
-      <c r="D104" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>243</v>
+      </c>
+      <c r="B105" t="s">
         <v>244</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
+        <v>164</v>
+      </c>
+      <c r="D105" t="s">
         <v>245</v>
-      </c>
-      <c r="C105" t="s">
-        <v>165</v>
-      </c>
-      <c r="D105" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B106" t="s">
+        <v>226</v>
+      </c>
+      <c r="C106" t="s">
+        <v>164</v>
+      </c>
+      <c r="D106" t="s">
         <v>227</v>
-      </c>
-      <c r="C106" t="s">
-        <v>165</v>
-      </c>
-      <c r="D106" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>255</v>
+      </c>
+      <c r="B107" t="s">
         <v>256</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
+        <v>164</v>
+      </c>
+      <c r="D107" t="s">
         <v>257</v>
-      </c>
-      <c r="C107" t="s">
-        <v>165</v>
-      </c>
-      <c r="D107" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>389</v>
+      </c>
+      <c r="B108" t="s">
         <v>390</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
+        <v>164</v>
+      </c>
+      <c r="D108" t="s">
         <v>391</v>
-      </c>
-      <c r="C108" t="s">
-        <v>165</v>
-      </c>
-      <c r="D108" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B109" t="s">
         <v>4</v>
@@ -3581,7 +3635,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B110" t="s">
         <v>11</v>
@@ -3595,21 +3649,21 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>324</v>
+      </c>
+      <c r="B111" t="s">
         <v>325</v>
-      </c>
-      <c r="B111" t="s">
-        <v>326</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B112" t="s">
         <v>10</v>
@@ -3623,21 +3677,21 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B113" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C113" t="s">
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B114" t="s">
         <v>12</v>
@@ -3651,7 +3705,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B115" t="s">
         <v>81</v>
@@ -3665,7 +3719,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B116" t="s">
         <v>26</v>
@@ -3674,12 +3728,12 @@
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B117" t="s">
         <v>27</v>
@@ -3688,12 +3742,12 @@
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B118" t="s">
         <v>47</v>
@@ -3702,7 +3756,7 @@
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -3744,29 +3798,29 @@
         <v>34</v>
       </c>
       <c r="D121" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>89</v>
+        <v>559</v>
       </c>
       <c r="B122" t="s">
-        <v>90</v>
+        <v>560</v>
       </c>
       <c r="C122" t="s">
         <v>34</v>
       </c>
       <c r="D122" t="s">
-        <v>97</v>
+        <v>561</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B123" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C123" t="s">
         <v>34</v>
@@ -3777,10 +3831,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B124" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C124" t="s">
         <v>34</v>
@@ -3791,845 +3845,929 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>99</v>
+        <v>562</v>
       </c>
       <c r="B125" t="s">
-        <v>37</v>
+        <v>563</v>
       </c>
       <c r="C125" t="s">
         <v>34</v>
       </c>
       <c r="D125" t="s">
-        <v>100</v>
+        <v>564</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B126" t="s">
-        <v>52</v>
+        <v>565</v>
       </c>
       <c r="C126" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D126" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>113</v>
+        <v>566</v>
       </c>
       <c r="B127" t="s">
-        <v>22</v>
+        <v>567</v>
       </c>
       <c r="C127" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D127" t="s">
-        <v>548</v>
+        <v>568</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>551</v>
+        <v>98</v>
       </c>
       <c r="B128" t="s">
-        <v>552</v>
+        <v>37</v>
       </c>
       <c r="C128" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D128" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>158</v>
+        <v>100</v>
       </c>
       <c r="B129" t="s">
-        <v>159</v>
+        <v>52</v>
       </c>
       <c r="C129" t="s">
         <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>423</v>
+        <v>112</v>
       </c>
       <c r="B130" t="s">
-        <v>424</v>
+        <v>22</v>
       </c>
       <c r="C130" t="s">
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>425</v>
+        <v>547</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>161</v>
+        <v>550</v>
       </c>
       <c r="B131" t="s">
-        <v>162</v>
+        <v>551</v>
       </c>
       <c r="C131" t="s">
         <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>163</v>
+        <v>65</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>410</v>
+        <v>157</v>
       </c>
       <c r="B132" t="s">
-        <v>411</v>
+        <v>158</v>
       </c>
       <c r="C132" t="s">
         <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>412</v>
+        <v>159</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>276</v>
+        <v>422</v>
       </c>
       <c r="B133" t="s">
-        <v>277</v>
+        <v>423</v>
       </c>
       <c r="C133" t="s">
         <v>6</v>
       </c>
       <c r="D133" t="s">
-        <v>278</v>
+        <v>424</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>331</v>
+        <v>569</v>
       </c>
       <c r="B134" t="s">
-        <v>332</v>
+        <v>570</v>
       </c>
       <c r="C134" t="s">
         <v>6</v>
       </c>
       <c r="D134" t="s">
-        <v>537</v>
+        <v>571</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>534</v>
+        <v>160</v>
       </c>
       <c r="B135" t="s">
-        <v>535</v>
+        <v>161</v>
       </c>
       <c r="C135" t="s">
         <v>6</v>
       </c>
       <c r="D135" t="s">
-        <v>536</v>
+        <v>162</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>333</v>
+        <v>409</v>
       </c>
       <c r="B136" t="s">
-        <v>334</v>
+        <v>573</v>
       </c>
       <c r="C136" t="s">
         <v>6</v>
       </c>
       <c r="D136" t="s">
-        <v>335</v>
+        <v>574</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>541</v>
+        <v>572</v>
       </c>
       <c r="B137" t="s">
-        <v>542</v>
+        <v>410</v>
       </c>
       <c r="C137" t="s">
         <v>6</v>
       </c>
       <c r="D137" t="s">
-        <v>543</v>
+        <v>411</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>544</v>
+        <v>575</v>
       </c>
       <c r="B138" t="s">
-        <v>546</v>
+        <v>576</v>
       </c>
       <c r="C138" t="s">
         <v>6</v>
       </c>
       <c r="D138" t="s">
-        <v>547</v>
+        <v>577</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>545</v>
+        <v>275</v>
       </c>
       <c r="B139" t="s">
-        <v>549</v>
+        <v>276</v>
       </c>
       <c r="C139" t="s">
         <v>6</v>
       </c>
       <c r="D139" t="s">
-        <v>550</v>
+        <v>277</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>288</v>
+        <v>330</v>
       </c>
       <c r="B140" t="s">
-        <v>13</v>
+        <v>331</v>
       </c>
       <c r="C140" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D140" t="s">
-        <v>61</v>
+        <v>536</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>289</v>
+        <v>533</v>
       </c>
       <c r="B141" t="s">
-        <v>30</v>
+        <v>534</v>
       </c>
       <c r="C141" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D141" t="s">
-        <v>70</v>
+        <v>535</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>290</v>
+        <v>332</v>
       </c>
       <c r="B142" t="s">
-        <v>50</v>
+        <v>333</v>
       </c>
       <c r="C142" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D142" t="s">
-        <v>77</v>
+        <v>334</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>291</v>
+        <v>540</v>
       </c>
       <c r="B143" t="s">
-        <v>337</v>
+        <v>541</v>
       </c>
       <c r="C143" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D143" t="s">
-        <v>114</v>
+        <v>542</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>336</v>
+        <v>543</v>
       </c>
       <c r="B144" t="s">
-        <v>338</v>
+        <v>545</v>
       </c>
       <c r="C144" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D144" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>292</v>
+        <v>544</v>
       </c>
       <c r="B145" t="s">
-        <v>54</v>
+        <v>548</v>
       </c>
       <c r="C145" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D145" t="s">
-        <v>76</v>
+        <v>549</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B146" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="C146" t="s">
         <v>14</v>
       </c>
       <c r="D146" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B147" t="s">
-        <v>115</v>
+        <v>30</v>
       </c>
       <c r="C147" t="s">
         <v>14</v>
       </c>
       <c r="D147" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>341</v>
+        <v>289</v>
       </c>
       <c r="B148" t="s">
-        <v>342</v>
+        <v>50</v>
       </c>
       <c r="C148" t="s">
         <v>14</v>
       </c>
       <c r="D148" t="s">
-        <v>343</v>
+        <v>77</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B149" t="s">
-        <v>116</v>
+        <v>336</v>
       </c>
       <c r="C149" t="s">
         <v>14</v>
       </c>
       <c r="D149" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
       <c r="B150" t="s">
-        <v>118</v>
+        <v>337</v>
       </c>
       <c r="C150" t="s">
         <v>14</v>
       </c>
       <c r="D150" t="s">
-        <v>119</v>
+        <v>338</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>120</v>
+        <v>291</v>
       </c>
       <c r="B151" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="C151" t="s">
         <v>14</v>
       </c>
       <c r="D151" t="s">
-        <v>122</v>
+        <v>76</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>124</v>
+        <v>292</v>
       </c>
       <c r="B152" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="C152" t="s">
         <v>14</v>
       </c>
       <c r="D152" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>127</v>
+        <v>293</v>
       </c>
       <c r="B153" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C153" t="s">
         <v>14</v>
       </c>
       <c r="D153" t="s">
-        <v>126</v>
+        <v>79</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>131</v>
+        <v>340</v>
       </c>
       <c r="B154" t="s">
-        <v>130</v>
+        <v>341</v>
       </c>
       <c r="C154" t="s">
         <v>14</v>
       </c>
       <c r="D154" t="s">
-        <v>129</v>
+        <v>342</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>132</v>
+        <v>294</v>
       </c>
       <c r="B155" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="C155" t="s">
         <v>14</v>
       </c>
       <c r="D155" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>195</v>
+        <v>295</v>
       </c>
       <c r="B156" t="s">
-        <v>196</v>
+        <v>117</v>
       </c>
       <c r="C156" t="s">
         <v>14</v>
       </c>
       <c r="D156" t="s">
-        <v>197</v>
+        <v>118</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>396</v>
+        <v>119</v>
       </c>
       <c r="B157" t="s">
-        <v>397</v>
+        <v>120</v>
       </c>
       <c r="C157" t="s">
         <v>14</v>
       </c>
       <c r="D157" t="s">
-        <v>398</v>
+        <v>121</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>303</v>
+        <v>123</v>
       </c>
       <c r="B158" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="C158" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="D158" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>304</v>
+        <v>126</v>
       </c>
       <c r="B159" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="C159" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="D159" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>305</v>
+        <v>130</v>
       </c>
       <c r="B160" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C160" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="D160" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>306</v>
+        <v>131</v>
       </c>
       <c r="B161" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="C161" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="D161" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>194</v>
+      </c>
+      <c r="B162" t="s">
+        <v>195</v>
+      </c>
+      <c r="C162" t="s">
+        <v>14</v>
+      </c>
+      <c r="D162" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>395</v>
+      </c>
+      <c r="B163" t="s">
+        <v>396</v>
+      </c>
+      <c r="C163" t="s">
+        <v>14</v>
+      </c>
+      <c r="D163" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>302</v>
+      </c>
+      <c r="B164" t="s">
+        <v>102</v>
+      </c>
+      <c r="C164" t="s">
+        <v>103</v>
+      </c>
+      <c r="D164" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>307</v>
-      </c>
-      <c r="B162" t="s">
-        <v>106</v>
-      </c>
-      <c r="C162" t="s">
-        <v>104</v>
-      </c>
-      <c r="D162" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>308</v>
-      </c>
-      <c r="B163" t="s">
-        <v>31</v>
-      </c>
-      <c r="C163" t="s">
-        <v>104</v>
-      </c>
-      <c r="D163" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>309</v>
-      </c>
-      <c r="B164" t="s">
-        <v>108</v>
-      </c>
-      <c r="C164" t="s">
-        <v>104</v>
-      </c>
-      <c r="D164" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="B165" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C165" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D165" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>304</v>
+      </c>
+      <c r="B166" t="s">
+        <v>104</v>
+      </c>
+      <c r="C166" t="s">
+        <v>103</v>
+      </c>
+      <c r="D166" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>305</v>
+      </c>
+      <c r="B167" t="s">
+        <v>106</v>
+      </c>
+      <c r="C167" t="s">
+        <v>103</v>
+      </c>
+      <c r="D167" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>306</v>
+      </c>
+      <c r="B168" t="s">
+        <v>105</v>
+      </c>
+      <c r="C168" t="s">
+        <v>103</v>
+      </c>
+      <c r="D168" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>307</v>
+      </c>
+      <c r="B169" t="s">
+        <v>31</v>
+      </c>
+      <c r="C169" t="s">
+        <v>103</v>
+      </c>
+      <c r="D169" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>308</v>
+      </c>
+      <c r="B170" t="s">
+        <v>107</v>
+      </c>
+      <c r="C170" t="s">
+        <v>103</v>
+      </c>
+      <c r="D170" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>309</v>
+      </c>
+      <c r="B171" t="s">
+        <v>108</v>
+      </c>
+      <c r="C171" t="s">
+        <v>103</v>
+      </c>
+      <c r="D171" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>310</v>
+      </c>
+      <c r="B172" t="s">
         <v>311</v>
       </c>
-      <c r="B166" t="s">
+      <c r="C172" t="s">
+        <v>103</v>
+      </c>
+      <c r="D172" t="s">
         <v>312</v>
       </c>
-      <c r="C166" t="s">
-        <v>104</v>
-      </c>
-      <c r="D166" t="s">
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
+      <c r="B173" t="s">
         <v>314</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C173" t="s">
+        <v>103</v>
+      </c>
+      <c r="D173" t="s">
         <v>315</v>
       </c>
-      <c r="C167" t="s">
-        <v>104</v>
-      </c>
-      <c r="D167" t="s">
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>339</v>
+      </c>
+      <c r="B174" t="s">
+        <v>387</v>
+      </c>
+      <c r="C174" t="s">
+        <v>103</v>
+      </c>
+      <c r="D174" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>340</v>
-      </c>
-      <c r="B168" t="s">
-        <v>388</v>
-      </c>
-      <c r="C168" t="s">
-        <v>104</v>
-      </c>
-      <c r="D168" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
+      <c r="B175" t="s">
+        <v>401</v>
+      </c>
+      <c r="C175" t="s">
+        <v>103</v>
+      </c>
+      <c r="D175" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>319</v>
+      </c>
+      <c r="B176" t="s">
         <v>317</v>
       </c>
-      <c r="B169" t="s">
-        <v>402</v>
-      </c>
-      <c r="C169" t="s">
-        <v>104</v>
-      </c>
-      <c r="D169" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
+      <c r="C176" t="s">
+        <v>103</v>
+      </c>
+      <c r="D176" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>383</v>
+      </c>
+      <c r="B177" t="s">
+        <v>381</v>
+      </c>
+      <c r="C177" t="s">
+        <v>18</v>
+      </c>
+      <c r="D177" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>383</v>
+      </c>
+      <c r="B178" t="s">
         <v>320</v>
       </c>
-      <c r="B170" t="s">
-        <v>318</v>
-      </c>
-      <c r="C170" t="s">
-        <v>104</v>
-      </c>
-      <c r="D170" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>384</v>
-      </c>
-      <c r="B171" t="s">
-        <v>382</v>
-      </c>
-      <c r="C171" t="s">
+      <c r="C178" t="s">
+        <v>103</v>
+      </c>
+      <c r="D178" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>398</v>
+      </c>
+      <c r="B179" t="s">
+        <v>399</v>
+      </c>
+      <c r="C179" t="s">
         <v>18</v>
       </c>
-      <c r="D171" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
-        <v>384</v>
-      </c>
-      <c r="B172" t="s">
-        <v>321</v>
-      </c>
-      <c r="C172" t="s">
-        <v>104</v>
-      </c>
-      <c r="D172" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>399</v>
-      </c>
-      <c r="B173" t="s">
+      <c r="D179" t="s">
         <v>400</v>
       </c>
-      <c r="C173" t="s">
-        <v>18</v>
-      </c>
-      <c r="D173" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A174" t="s">
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>146</v>
+      </c>
+      <c r="B180" t="s">
         <v>147</v>
       </c>
-      <c r="B174" t="s">
+      <c r="C180" t="s">
         <v>148</v>
       </c>
-      <c r="C174" t="s">
+      <c r="D180" t="s">
         <v>149</v>
       </c>
-      <c r="D174" t="s">
+      <c r="E180" t="s">
         <v>150</v>
       </c>
-      <c r="E174" t="s">
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
+      <c r="B181" t="s">
         <v>152</v>
       </c>
-      <c r="B175" t="s">
-        <v>153</v>
-      </c>
-      <c r="C175" t="s">
-        <v>149</v>
-      </c>
-      <c r="D175" t="s">
+      <c r="C181" t="s">
+        <v>148</v>
+      </c>
+      <c r="D181" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
+      <c r="B182" t="s">
         <v>420</v>
       </c>
-      <c r="B176" t="s">
+      <c r="C182" t="s">
+        <v>148</v>
+      </c>
+      <c r="D182" t="s">
         <v>421</v>
       </c>
-      <c r="C176" t="s">
-        <v>149</v>
-      </c>
-      <c r="D176" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>215</v>
+      </c>
+      <c r="B183" t="s">
         <v>216</v>
       </c>
-      <c r="B177" t="s">
+      <c r="C183" t="s">
+        <v>148</v>
+      </c>
+      <c r="D183" t="s">
         <v>217</v>
       </c>
-      <c r="C177" t="s">
-        <v>149</v>
-      </c>
-      <c r="D177" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>258</v>
+      </c>
+      <c r="B184" t="s">
         <v>259</v>
       </c>
-      <c r="B178" t="s">
+      <c r="C184" t="s">
+        <v>148</v>
+      </c>
+      <c r="D184" t="s">
         <v>260</v>
       </c>
-      <c r="C178" t="s">
-        <v>149</v>
-      </c>
-      <c r="D178" t="s">
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
+      <c r="B185" t="s">
         <v>262</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C185" t="s">
+        <v>148</v>
+      </c>
+      <c r="D185" t="s">
         <v>263</v>
       </c>
-      <c r="C179" t="s">
-        <v>149</v>
-      </c>
-      <c r="D179" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>504</v>
+      </c>
+      <c r="B186" t="s">
+        <v>498</v>
+      </c>
+      <c r="C186" t="s">
+        <v>148</v>
+      </c>
+      <c r="D186" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>500</v>
+      </c>
+      <c r="B187" t="s">
+        <v>501</v>
+      </c>
+      <c r="C187" t="s">
+        <v>148</v>
+      </c>
+      <c r="D187" t="s">
         <v>505</v>
       </c>
-      <c r="B180" t="s">
-        <v>499</v>
-      </c>
-      <c r="C180" t="s">
-        <v>149</v>
-      </c>
-      <c r="D180" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>501</v>
-      </c>
-      <c r="B181" t="s">
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
         <v>502</v>
       </c>
-      <c r="C181" t="s">
-        <v>149</v>
-      </c>
-      <c r="D181" t="s">
+      <c r="B188" t="s">
+        <v>503</v>
+      </c>
+      <c r="C188" t="s">
+        <v>148</v>
+      </c>
+      <c r="D188" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
-        <v>503</v>
-      </c>
-      <c r="B182" t="s">
-        <v>504</v>
-      </c>
-      <c r="C182" t="s">
-        <v>149</v>
-      </c>
-      <c r="D182" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>284</v>
+      </c>
+      <c r="B189" t="s">
         <v>285</v>
       </c>
-      <c r="B183" t="s">
+      <c r="C189" t="s">
+        <v>148</v>
+      </c>
+      <c r="D189" t="s">
         <v>286</v>
       </c>
-      <c r="C183" t="s">
-        <v>149</v>
-      </c>
-      <c r="D183" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>515</v>
+      </c>
+      <c r="B190" t="s">
         <v>516</v>
       </c>
-      <c r="B184" t="s">
+      <c r="C190" t="s">
+        <v>148</v>
+      </c>
+      <c r="D190" t="s">
         <v>517</v>
-      </c>
-      <c r="C184" t="s">
-        <v>149</v>
-      </c>
-      <c r="D184" t="s">
-        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 20+ derived complication variables
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D907080D-4F66-234C-ADBF-A5A820026EC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1464D50E-6CAC-CB48-BF83-7C2C1605846C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37880" yWindow="2540" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35860" yWindow="2900" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="671">
   <si>
     <t>Variable #</t>
   </si>
@@ -289,27 +289,15 @@
     <t>O11</t>
   </si>
   <si>
-    <t>O12</t>
-  </si>
-  <si>
     <t>PE_comp</t>
   </si>
   <si>
-    <t>O13</t>
-  </si>
-  <si>
     <t>SVT_comp</t>
   </si>
   <si>
-    <t>O14</t>
-  </si>
-  <si>
     <t>DVT_comp</t>
   </si>
   <si>
-    <t>O15</t>
-  </si>
-  <si>
     <t>Thrombosis NOS complications</t>
   </si>
   <si>
@@ -322,15 +310,6 @@
     <t>PE complications</t>
   </si>
   <si>
-    <t>O16</t>
-  </si>
-  <si>
-    <t>Arrhythmia complications</t>
-  </si>
-  <si>
-    <t>O17</t>
-  </si>
-  <si>
     <t>righttime</t>
   </si>
   <si>
@@ -499,18 +478,12 @@
     <t>Solid tumor indicator</t>
   </si>
   <si>
-    <t>O19</t>
-  </si>
-  <si>
     <t>VTE_comp</t>
   </si>
   <si>
     <t>Combined VTE complications (excluding SVT)</t>
   </si>
   <si>
-    <t>O20</t>
-  </si>
-  <si>
     <t>ATE_comp</t>
   </si>
   <si>
@@ -847,9 +820,6 @@
     <t>O09</t>
   </si>
   <si>
-    <t>O21</t>
-  </si>
-  <si>
     <t>CV_event</t>
   </si>
   <si>
@@ -1231,9 +1201,6 @@
     <t>Same as Ca07 except do not combine active unknown and unknown</t>
   </si>
   <si>
-    <t>O20a</t>
-  </si>
-  <si>
     <t>stroke_comp</t>
   </si>
   <si>
@@ -1270,9 +1237,6 @@
     <t>Modified IMWG frailty index (non-frail; prefrail; frail)</t>
   </si>
   <si>
-    <t>O19a</t>
-  </si>
-  <si>
     <t>VTE_comp_v2</t>
   </si>
   <si>
@@ -1681,18 +1645,12 @@
     <t>Active cancer/treatment vs inactive</t>
   </si>
   <si>
-    <t>O12a</t>
-  </si>
-  <si>
     <t>PE_comp_within_3mo</t>
   </si>
   <si>
     <t>PE complications within 3 months of COVID-19 diagnosis</t>
   </si>
   <si>
-    <t>O14a</t>
-  </si>
-  <si>
     <t>DVT_comp_within_3mo</t>
   </si>
   <si>
@@ -1702,36 +1660,24 @@
     <t>thrombosis_NOS_comp</t>
   </si>
   <si>
-    <t>O15a</t>
-  </si>
-  <si>
     <t>thrombosis_NOS_comp_within_3mo</t>
   </si>
   <si>
     <t>Thrombosis NOS complications within 3 months of COVID-19 diagnosis</t>
   </si>
   <si>
-    <t>O19b</t>
-  </si>
-  <si>
     <t>VTE_comp_within_3mo</t>
   </si>
   <si>
     <t>Combined VTE complications within 3 months of COVID-19 diagnosis</t>
   </si>
   <si>
-    <t>O26</t>
-  </si>
-  <si>
     <t>ATE_comp_within_3mo</t>
   </si>
   <si>
     <t>Combined ATE complications within 3 months of COVID-19 diagnosis</t>
   </si>
   <si>
-    <t>O26a</t>
-  </si>
-  <si>
     <t>stroke_comp_within_3mo</t>
   </si>
   <si>
@@ -1805,6 +1751,294 @@
   </si>
   <si>
     <t>Timing of cytotoxic chemotherapy</t>
+  </si>
+  <si>
+    <t>Comp01</t>
+  </si>
+  <si>
+    <t>Comp01a</t>
+  </si>
+  <si>
+    <t>Comp02</t>
+  </si>
+  <si>
+    <t>Comp03</t>
+  </si>
+  <si>
+    <t>Comp03a</t>
+  </si>
+  <si>
+    <t>Comp04</t>
+  </si>
+  <si>
+    <t>Comp04a</t>
+  </si>
+  <si>
+    <t>Comp05</t>
+  </si>
+  <si>
+    <t>Comp05a</t>
+  </si>
+  <si>
+    <t>Comp05b</t>
+  </si>
+  <si>
+    <t>Comp06</t>
+  </si>
+  <si>
+    <t>Comp06a</t>
+  </si>
+  <si>
+    <t>Comp07</t>
+  </si>
+  <si>
+    <t>Comp07a</t>
+  </si>
+  <si>
+    <t>Comp08</t>
+  </si>
+  <si>
+    <t>Comp09</t>
+  </si>
+  <si>
+    <t>Comp10</t>
+  </si>
+  <si>
+    <t>Comp11</t>
+  </si>
+  <si>
+    <t>MOF_comp</t>
+  </si>
+  <si>
+    <t>Multisystem organ failure</t>
+  </si>
+  <si>
+    <t>Comp12</t>
+  </si>
+  <si>
+    <t>sepsis_comp</t>
+  </si>
+  <si>
+    <t>Sepsis</t>
+  </si>
+  <si>
+    <t>Comp13</t>
+  </si>
+  <si>
+    <t>bleeding_comp</t>
+  </si>
+  <si>
+    <t>Bleeding</t>
+  </si>
+  <si>
+    <t>Comp14</t>
+  </si>
+  <si>
+    <t>DIC_comp</t>
+  </si>
+  <si>
+    <t>DIC (without modifier of definite/probable/possible)</t>
+  </si>
+  <si>
+    <t>Comp15</t>
+  </si>
+  <si>
+    <t>resp_failure</t>
+  </si>
+  <si>
+    <t>Respiratory failure (checkbox only)</t>
+  </si>
+  <si>
+    <t>Comp16</t>
+  </si>
+  <si>
+    <t>pneumonitis_comp</t>
+  </si>
+  <si>
+    <t>Pneumonitis</t>
+  </si>
+  <si>
+    <t>Comp17</t>
+  </si>
+  <si>
+    <t>pneumonia_comp</t>
+  </si>
+  <si>
+    <t>Pneumonia</t>
+  </si>
+  <si>
+    <t>Comp18</t>
+  </si>
+  <si>
+    <t>pneumo_comp</t>
+  </si>
+  <si>
+    <t>Combined pneumonitis/pneumonia</t>
+  </si>
+  <si>
+    <t>Comp19</t>
+  </si>
+  <si>
+    <t>ARDS_comp</t>
+  </si>
+  <si>
+    <t>ARDS</t>
+  </si>
+  <si>
+    <t>Comp20</t>
+  </si>
+  <si>
+    <t>pleural_eff</t>
+  </si>
+  <si>
+    <t>Pleural effusion</t>
+  </si>
+  <si>
+    <t>Comp21</t>
+  </si>
+  <si>
+    <t>empyema_comp</t>
+  </si>
+  <si>
+    <t>Empyema</t>
+  </si>
+  <si>
+    <t>Comp22</t>
+  </si>
+  <si>
+    <t>hotn_comp</t>
+  </si>
+  <si>
+    <t>Hypotension</t>
+  </si>
+  <si>
+    <t>Comp23</t>
+  </si>
+  <si>
+    <t>MI_comp</t>
+  </si>
+  <si>
+    <t>Myocardial infarction</t>
+  </si>
+  <si>
+    <t>Comp24</t>
+  </si>
+  <si>
+    <t>card_isch_comp</t>
+  </si>
+  <si>
+    <t>Other cardiac ischemia</t>
+  </si>
+  <si>
+    <t>Comp25</t>
+  </si>
+  <si>
+    <t>AFib_comp</t>
+  </si>
+  <si>
+    <t>Atrial fibrillation</t>
+  </si>
+  <si>
+    <t>Comp26</t>
+  </si>
+  <si>
+    <t>VF_comp</t>
+  </si>
+  <si>
+    <t>Ventricular fibrillation</t>
+  </si>
+  <si>
+    <t>Arrhythmia complications (partial derived)</t>
+  </si>
+  <si>
+    <t>Comp27</t>
+  </si>
+  <si>
+    <t>Other cardiac arrhythmia</t>
+  </si>
+  <si>
+    <t>Comp28</t>
+  </si>
+  <si>
+    <t>CMY_comp</t>
+  </si>
+  <si>
+    <t>arry_oth_comp</t>
+  </si>
+  <si>
+    <t>Cardiomyopathy</t>
+  </si>
+  <si>
+    <t>Comp29</t>
+  </si>
+  <si>
+    <t>CHF_comp</t>
+  </si>
+  <si>
+    <t>Congestive heart failure</t>
+  </si>
+  <si>
+    <t>Comp30</t>
+  </si>
+  <si>
+    <t>AHI_comp</t>
+  </si>
+  <si>
+    <t>Acute hepatic injury</t>
+  </si>
+  <si>
+    <t>Comp31</t>
+  </si>
+  <si>
+    <t>ascites_comp</t>
+  </si>
+  <si>
+    <t>Ascites</t>
+  </si>
+  <si>
+    <t>Comp32</t>
+  </si>
+  <si>
+    <t>BO_comp</t>
+  </si>
+  <si>
+    <t>Bowel obstruction</t>
+  </si>
+  <si>
+    <t>Comp33</t>
+  </si>
+  <si>
+    <t>bowelPerf_comp</t>
+  </si>
+  <si>
+    <t>Bowel perforation</t>
+  </si>
+  <si>
+    <t>Comp34</t>
+  </si>
+  <si>
+    <t>ileus_comp</t>
+  </si>
+  <si>
+    <t>Ileus</t>
+  </si>
+  <si>
+    <t>Comp35</t>
+  </si>
+  <si>
+    <t>peritonitis</t>
+  </si>
+  <si>
+    <t>Peritonitis</t>
+  </si>
+  <si>
+    <t>Comp36</t>
+  </si>
+  <si>
+    <t>AKI_comp</t>
+  </si>
+  <si>
+    <t>Acute kidney injury (checkbox only)</t>
   </si>
 </sst>
 </file>
@@ -1860,10 +2094,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E195" totalsRowShown="0">
-  <autoFilter ref="A1:E195" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E194">
-    <sortCondition ref="A1:A194"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E221" totalsRowShown="0">
+  <autoFilter ref="A1:E221" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E221">
+    <sortCondition ref="A1:A221"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
@@ -2197,10 +2431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A222" sqref="A222:XFD222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2231,63 +2465,63 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B2" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="B4" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>584</v>
+        <v>566</v>
       </c>
       <c r="B5" t="s">
-        <v>585</v>
+        <v>567</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>586</v>
+        <v>568</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
@@ -2301,7 +2535,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
@@ -2315,21 +2549,21 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="B9" t="s">
         <v>38</v>
@@ -2343,7 +2577,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
@@ -2357,7 +2591,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
@@ -2371,7 +2605,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="B12" t="s">
         <v>42</v>
@@ -2380,12 +2614,12 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B13" t="s">
         <v>55</v>
@@ -2399,83 +2633,83 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B16" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B17" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="B18" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D19" t="s">
         <v>62</v>
@@ -2483,49 +2717,49 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="B20" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C20" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D20" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B21" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="C21" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D21" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>587</v>
+        <v>569</v>
       </c>
       <c r="B22" t="s">
-        <v>588</v>
+        <v>570</v>
       </c>
       <c r="C22" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D22" t="s">
-        <v>589</v>
+        <v>571</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -2539,7 +2773,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="B24" t="s">
         <v>72</v>
@@ -2553,13 +2787,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="B25" t="s">
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D25" t="s">
         <v>36</v>
@@ -2567,7 +2801,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -2581,10 +2815,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="B27" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -2595,2294 +2829,2658 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="B28" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>506</v>
+        <v>494</v>
       </c>
       <c r="B29" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="B30" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B31" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B32" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>576</v>
+        <v>558</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B33" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C33" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D33" t="s">
-        <v>577</v>
+        <v>559</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="C34" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D34" t="s">
-        <v>578</v>
+        <v>560</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B35" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="C35" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D35" t="s">
-        <v>579</v>
+        <v>561</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B36" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="C36" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D36" t="s">
-        <v>580</v>
+        <v>562</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="B37" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="C37" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D37" t="s">
-        <v>581</v>
+        <v>563</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B38" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="C38" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D38" t="s">
-        <v>582</v>
+        <v>564</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="B39" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="C39" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D39" t="s">
-        <v>583</v>
+        <v>565</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="B40" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C40" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D40" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B41" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C41" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D41" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="B42" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="C42" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D42" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>573</v>
+        <v>555</v>
       </c>
       <c r="B43" t="s">
-        <v>574</v>
+        <v>556</v>
       </c>
       <c r="C43" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D43" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B44" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B45" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C45" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D45" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B46" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C46" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D46" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>510</v>
+        <v>498</v>
       </c>
       <c r="B47" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
       <c r="C47" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D47" t="s">
-        <v>512</v>
+        <v>500</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="B48" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="C48" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D48" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>516</v>
+        <v>504</v>
       </c>
       <c r="B49" t="s">
-        <v>517</v>
+        <v>505</v>
       </c>
       <c r="C49" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D49" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="B50" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="C50" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D50" t="s">
-        <v>521</v>
+        <v>509</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>522</v>
+        <v>510</v>
       </c>
       <c r="B51" t="s">
-        <v>523</v>
+        <v>511</v>
       </c>
       <c r="C51" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D51" t="s">
-        <v>524</v>
+        <v>512</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="B52" t="s">
-        <v>530</v>
+        <v>518</v>
       </c>
       <c r="C52" t="s">
         <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>531</v>
+        <v>519</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="B53" t="s">
-        <v>546</v>
+        <v>534</v>
       </c>
       <c r="C53" t="s">
         <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>547</v>
+        <v>535</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="B54" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="C54" t="s">
         <v>18</v>
       </c>
       <c r="D54" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
       <c r="B55" t="s">
-        <v>591</v>
+        <v>573</v>
       </c>
       <c r="C55" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="D55" t="s">
-        <v>592</v>
+        <v>574</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>276</v>
+        <v>575</v>
       </c>
       <c r="B56" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="C56" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D56" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>277</v>
+        <v>576</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>539</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D57" t="s">
-        <v>45</v>
+        <v>540</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>503</v>
+        <v>577</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D58" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>504</v>
+        <v>578</v>
       </c>
       <c r="B59" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>278</v>
+        <v>579</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>541</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D60" t="s">
-        <v>63</v>
+        <v>542</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>505</v>
+        <v>580</v>
       </c>
       <c r="B61" t="s">
-        <v>200</v>
+        <v>543</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D61" t="s">
-        <v>201</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>499</v>
+        <v>581</v>
       </c>
       <c r="B62" t="s">
-        <v>500</v>
+        <v>544</v>
       </c>
       <c r="C62" t="s">
-        <v>5</v>
+        <v>34</v>
+      </c>
+      <c r="D62" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>279</v>
+        <v>582</v>
       </c>
       <c r="B63" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="C63" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D63" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>136</v>
+        <v>583</v>
       </c>
       <c r="B64" t="s">
-        <v>3</v>
+        <v>403</v>
       </c>
       <c r="C64" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D64" t="s">
-        <v>7</v>
+        <v>404</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>325</v>
+        <v>584</v>
       </c>
       <c r="B65" t="s">
-        <v>326</v>
+        <v>546</v>
       </c>
       <c r="C65" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D65" t="s">
-        <v>327</v>
+        <v>547</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>137</v>
+        <v>585</v>
       </c>
       <c r="B66" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="C66" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D66" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>167</v>
+        <v>586</v>
       </c>
       <c r="B67" t="s">
-        <v>168</v>
+        <v>548</v>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D67" t="s">
-        <v>169</v>
+        <v>549</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>190</v>
+        <v>587</v>
       </c>
       <c r="B68" t="s">
-        <v>191</v>
+        <v>391</v>
       </c>
       <c r="C68" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D68" t="s">
-        <v>192</v>
+        <v>392</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>418</v>
+        <v>588</v>
       </c>
       <c r="B69" t="s">
-        <v>419</v>
+        <v>550</v>
       </c>
       <c r="C69" t="s">
-        <v>420</v>
+        <v>34</v>
       </c>
       <c r="D69" t="s">
-        <v>486</v>
+        <v>551</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>421</v>
+        <v>589</v>
       </c>
       <c r="B70" t="s">
-        <v>422</v>
+        <v>37</v>
       </c>
       <c r="C70" t="s">
-        <v>420</v>
+        <v>34</v>
       </c>
       <c r="D70" t="s">
-        <v>423</v>
+        <v>640</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>424</v>
+        <v>590</v>
       </c>
       <c r="B71" t="s">
-        <v>425</v>
+        <v>264</v>
       </c>
       <c r="C71" t="s">
-        <v>420</v>
+        <v>34</v>
       </c>
       <c r="D71" t="s">
-        <v>426</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>427</v>
+        <v>591</v>
       </c>
       <c r="B72" t="s">
-        <v>428</v>
+        <v>52</v>
       </c>
       <c r="C72" t="s">
-        <v>420</v>
+        <v>34</v>
       </c>
       <c r="D72" t="s">
-        <v>429</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>430</v>
+        <v>592</v>
       </c>
       <c r="B73" t="s">
-        <v>431</v>
+        <v>593</v>
       </c>
       <c r="C73" t="s">
-        <v>420</v>
+        <v>34</v>
       </c>
       <c r="D73" t="s">
-        <v>432</v>
+        <v>594</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>433</v>
+        <v>595</v>
       </c>
       <c r="B74" t="s">
-        <v>434</v>
+        <v>596</v>
       </c>
       <c r="C74" t="s">
-        <v>420</v>
+        <v>34</v>
+      </c>
+      <c r="D74" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>435</v>
+        <v>598</v>
       </c>
       <c r="B75" t="s">
-        <v>436</v>
+        <v>599</v>
       </c>
       <c r="C75" t="s">
-        <v>420</v>
+        <v>34</v>
       </c>
       <c r="D75" t="s">
-        <v>437</v>
+        <v>600</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>438</v>
+        <v>601</v>
       </c>
       <c r="B76" t="s">
-        <v>439</v>
+        <v>602</v>
       </c>
       <c r="C76" t="s">
-        <v>420</v>
+        <v>34</v>
       </c>
       <c r="D76" t="s">
-        <v>440</v>
+        <v>603</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>441</v>
+        <v>604</v>
       </c>
       <c r="B77" t="s">
-        <v>442</v>
+        <v>605</v>
       </c>
       <c r="C77" t="s">
-        <v>420</v>
+        <v>34</v>
       </c>
       <c r="D77" t="s">
-        <v>443</v>
+        <v>606</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>444</v>
+        <v>607</v>
       </c>
       <c r="B78" t="s">
-        <v>445</v>
+        <v>608</v>
+      </c>
+      <c r="C78" t="s">
+        <v>34</v>
+      </c>
+      <c r="D78" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>446</v>
+        <v>610</v>
       </c>
       <c r="B79" t="s">
-        <v>447</v>
+        <v>611</v>
+      </c>
+      <c r="C79" t="s">
+        <v>34</v>
       </c>
       <c r="D79" t="s">
-        <v>448</v>
+        <v>612</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>449</v>
+        <v>613</v>
       </c>
       <c r="B80" t="s">
-        <v>450</v>
+        <v>614</v>
+      </c>
+      <c r="C80" t="s">
+        <v>34</v>
+      </c>
+      <c r="D80" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>451</v>
+        <v>616</v>
       </c>
       <c r="B81" t="s">
-        <v>452</v>
+        <v>617</v>
+      </c>
+      <c r="C81" t="s">
+        <v>34</v>
       </c>
       <c r="D81" t="s">
-        <v>453</v>
+        <v>618</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>454</v>
+        <v>619</v>
       </c>
       <c r="B82" t="s">
-        <v>455</v>
+        <v>620</v>
+      </c>
+      <c r="C82" t="s">
+        <v>34</v>
       </c>
       <c r="D82" t="s">
-        <v>456</v>
+        <v>621</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>457</v>
+        <v>622</v>
       </c>
       <c r="B83" t="s">
-        <v>458</v>
+        <v>623</v>
+      </c>
+      <c r="C83" t="s">
+        <v>34</v>
       </c>
       <c r="D83" t="s">
-        <v>459</v>
+        <v>624</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>460</v>
+        <v>625</v>
       </c>
       <c r="B84" t="s">
-        <v>461</v>
+        <v>626</v>
+      </c>
+      <c r="C84" t="s">
+        <v>34</v>
       </c>
       <c r="D84" t="s">
-        <v>462</v>
+        <v>627</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>463</v>
+        <v>628</v>
       </c>
       <c r="B85" t="s">
-        <v>464</v>
+        <v>629</v>
+      </c>
+      <c r="C85" t="s">
+        <v>34</v>
       </c>
       <c r="D85" t="s">
-        <v>465</v>
+        <v>630</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>466</v>
+        <v>631</v>
       </c>
       <c r="B86" t="s">
-        <v>467</v>
+        <v>632</v>
+      </c>
+      <c r="C86" t="s">
+        <v>34</v>
       </c>
       <c r="D86" t="s">
-        <v>468</v>
+        <v>633</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>469</v>
+        <v>634</v>
       </c>
       <c r="B87" t="s">
-        <v>470</v>
+        <v>635</v>
+      </c>
+      <c r="C87" t="s">
+        <v>34</v>
       </c>
       <c r="D87" t="s">
-        <v>471</v>
+        <v>636</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>472</v>
+        <v>637</v>
       </c>
       <c r="B88" t="s">
-        <v>473</v>
+        <v>638</v>
+      </c>
+      <c r="C88" t="s">
+        <v>34</v>
       </c>
       <c r="D88" t="s">
-        <v>474</v>
+        <v>639</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>475</v>
+        <v>641</v>
       </c>
       <c r="B89" t="s">
-        <v>476</v>
+        <v>645</v>
+      </c>
+      <c r="C89" t="s">
+        <v>34</v>
+      </c>
+      <c r="D89" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>477</v>
+        <v>643</v>
       </c>
       <c r="B90" t="s">
-        <v>478</v>
+        <v>644</v>
+      </c>
+      <c r="C90" t="s">
+        <v>34</v>
       </c>
       <c r="D90" t="s">
-        <v>479</v>
+        <v>646</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>487</v>
+        <v>647</v>
       </c>
       <c r="B91" t="s">
-        <v>480</v>
+        <v>648</v>
+      </c>
+      <c r="C91" t="s">
+        <v>34</v>
       </c>
       <c r="D91" t="s">
-        <v>481</v>
+        <v>649</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>488</v>
+        <v>650</v>
       </c>
       <c r="B92" t="s">
-        <v>482</v>
+        <v>651</v>
+      </c>
+      <c r="C92" t="s">
+        <v>34</v>
       </c>
       <c r="D92" t="s">
-        <v>483</v>
+        <v>652</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>489</v>
+        <v>653</v>
       </c>
       <c r="B93" t="s">
-        <v>484</v>
+        <v>654</v>
+      </c>
+      <c r="C93" t="s">
+        <v>34</v>
       </c>
       <c r="D93" t="s">
-        <v>485</v>
+        <v>655</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>244</v>
+        <v>656</v>
       </c>
       <c r="B94" t="s">
-        <v>163</v>
+        <v>657</v>
       </c>
       <c r="C94" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
       <c r="D94" t="s">
-        <v>165</v>
+        <v>658</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>245</v>
+        <v>659</v>
       </c>
       <c r="B95" t="s">
-        <v>171</v>
+        <v>660</v>
       </c>
       <c r="C95" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
       <c r="D95" t="s">
-        <v>172</v>
+        <v>661</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>246</v>
+        <v>662</v>
       </c>
       <c r="B96" t="s">
-        <v>173</v>
+        <v>663</v>
       </c>
       <c r="C96" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
       <c r="D96" t="s">
-        <v>174</v>
+        <v>664</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>247</v>
+        <v>665</v>
       </c>
       <c r="B97" t="s">
-        <v>176</v>
+        <v>666</v>
       </c>
       <c r="C97" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
       <c r="D97" t="s">
-        <v>175</v>
+        <v>667</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>248</v>
+        <v>668</v>
       </c>
       <c r="B98" t="s">
-        <v>177</v>
+        <v>669</v>
       </c>
       <c r="C98" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
       <c r="D98" t="s">
-        <v>178</v>
+        <v>670</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="B99" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="C99" t="s">
-        <v>164</v>
+        <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>180</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="B100" t="s">
-        <v>181</v>
+        <v>44</v>
       </c>
       <c r="C100" t="s">
-        <v>164</v>
+        <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>182</v>
+        <v>45</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>251</v>
+        <v>491</v>
       </c>
       <c r="B101" t="s">
-        <v>183</v>
+        <v>126</v>
       </c>
       <c r="C101" t="s">
-        <v>164</v>
+        <v>15</v>
       </c>
       <c r="D101" t="s">
-        <v>184</v>
+        <v>137</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>252</v>
+        <v>492</v>
       </c>
       <c r="B102" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="C102" t="s">
-        <v>164</v>
+        <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>187</v>
+        <v>268</v>
       </c>
       <c r="B103" t="s">
-        <v>188</v>
+        <v>17</v>
       </c>
       <c r="C103" t="s">
-        <v>164</v>
+        <v>5</v>
       </c>
       <c r="D103" t="s">
-        <v>189</v>
+        <v>63</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>223</v>
+        <v>493</v>
       </c>
       <c r="B104" t="s">
-        <v>227</v>
+        <v>191</v>
       </c>
       <c r="C104" t="s">
-        <v>164</v>
+        <v>5</v>
       </c>
       <c r="D104" t="s">
-        <v>228</v>
+        <v>192</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>229</v>
+        <v>487</v>
       </c>
       <c r="B105" t="s">
-        <v>230</v>
+        <v>488</v>
       </c>
       <c r="C105" t="s">
-        <v>164</v>
-      </c>
-      <c r="D105" t="s">
-        <v>231</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>232</v>
+        <v>269</v>
       </c>
       <c r="B106" t="s">
-        <v>233</v>
+        <v>20</v>
       </c>
       <c r="C106" t="s">
-        <v>164</v>
+        <v>15</v>
       </c>
       <c r="D106" t="s">
-        <v>234</v>
+        <v>64</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>235</v>
+        <v>129</v>
       </c>
       <c r="B107" t="s">
-        <v>236</v>
+        <v>3</v>
       </c>
       <c r="C107" t="s">
-        <v>164</v>
+        <v>5</v>
       </c>
       <c r="D107" t="s">
-        <v>237</v>
+        <v>7</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>238</v>
+        <v>315</v>
       </c>
       <c r="B108" t="s">
-        <v>239</v>
+        <v>316</v>
       </c>
       <c r="C108" t="s">
-        <v>164</v>
+        <v>5</v>
       </c>
       <c r="D108" t="s">
-        <v>240</v>
+        <v>317</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>241</v>
+        <v>130</v>
       </c>
       <c r="B109" t="s">
-        <v>242</v>
+        <v>131</v>
       </c>
       <c r="C109" t="s">
-        <v>164</v>
+        <v>5</v>
       </c>
       <c r="D109" t="s">
-        <v>243</v>
+        <v>132</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>226</v>
+        <v>158</v>
       </c>
       <c r="B110" t="s">
-        <v>224</v>
+        <v>159</v>
       </c>
       <c r="C110" t="s">
-        <v>164</v>
+        <v>15</v>
       </c>
       <c r="D110" t="s">
-        <v>225</v>
+        <v>160</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>253</v>
+        <v>181</v>
       </c>
       <c r="B111" t="s">
-        <v>254</v>
+        <v>182</v>
       </c>
       <c r="C111" t="s">
-        <v>164</v>
+        <v>5</v>
       </c>
       <c r="D111" t="s">
-        <v>255</v>
+        <v>183</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>381</v>
+        <v>406</v>
       </c>
       <c r="B112" t="s">
-        <v>382</v>
+        <v>407</v>
       </c>
       <c r="C112" t="s">
-        <v>164</v>
+        <v>408</v>
       </c>
       <c r="D112" t="s">
-        <v>383</v>
+        <v>474</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>264</v>
+        <v>409</v>
       </c>
       <c r="B113" t="s">
-        <v>4</v>
+        <v>410</v>
       </c>
       <c r="C113" t="s">
-        <v>6</v>
+        <v>408</v>
       </c>
       <c r="D113" t="s">
-        <v>57</v>
+        <v>411</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>265</v>
+        <v>412</v>
       </c>
       <c r="B114" t="s">
-        <v>11</v>
+        <v>413</v>
       </c>
       <c r="C114" t="s">
-        <v>6</v>
+        <v>408</v>
       </c>
       <c r="D114" t="s">
-        <v>58</v>
+        <v>414</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>322</v>
+        <v>415</v>
       </c>
       <c r="B115" t="s">
-        <v>323</v>
+        <v>416</v>
       </c>
       <c r="C115" t="s">
-        <v>6</v>
+        <v>408</v>
       </c>
       <c r="D115" t="s">
-        <v>324</v>
+        <v>417</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>266</v>
+        <v>418</v>
       </c>
       <c r="B116" t="s">
-        <v>10</v>
+        <v>419</v>
       </c>
       <c r="C116" t="s">
-        <v>6</v>
+        <v>408</v>
       </c>
       <c r="D116" t="s">
-        <v>59</v>
+        <v>420</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>570</v>
+        <v>421</v>
       </c>
       <c r="B117" t="s">
-        <v>571</v>
+        <v>422</v>
       </c>
       <c r="C117" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" t="s">
-        <v>572</v>
+        <v>408</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>267</v>
+        <v>423</v>
       </c>
       <c r="B118" t="s">
-        <v>320</v>
+        <v>424</v>
       </c>
       <c r="C118" t="s">
-        <v>6</v>
+        <v>408</v>
       </c>
       <c r="D118" t="s">
-        <v>321</v>
+        <v>425</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>268</v>
+        <v>426</v>
       </c>
       <c r="B119" t="s">
-        <v>12</v>
+        <v>427</v>
       </c>
       <c r="C119" t="s">
-        <v>6</v>
+        <v>408</v>
       </c>
       <c r="D119" t="s">
-        <v>60</v>
+        <v>428</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>269</v>
+        <v>429</v>
       </c>
       <c r="B120" t="s">
-        <v>81</v>
+        <v>430</v>
       </c>
       <c r="C120" t="s">
-        <v>6</v>
+        <v>408</v>
       </c>
       <c r="D120" t="s">
-        <v>82</v>
+        <v>431</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>270</v>
+        <v>432</v>
       </c>
       <c r="B121" t="s">
-        <v>26</v>
-      </c>
-      <c r="C121" t="s">
-        <v>6</v>
-      </c>
-      <c r="D121" t="s">
-        <v>212</v>
+        <v>433</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>271</v>
+        <v>434</v>
       </c>
       <c r="B122" t="s">
-        <v>27</v>
-      </c>
-      <c r="C122" t="s">
-        <v>6</v>
+        <v>435</v>
       </c>
       <c r="D122" t="s">
-        <v>280</v>
+        <v>436</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>272</v>
+        <v>437</v>
       </c>
       <c r="B123" t="s">
-        <v>47</v>
-      </c>
-      <c r="C123" t="s">
-        <v>6</v>
-      </c>
-      <c r="D123" t="s">
-        <v>281</v>
+        <v>438</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>83</v>
+        <v>439</v>
       </c>
       <c r="B124" t="s">
-        <v>84</v>
-      </c>
-      <c r="C124" t="s">
-        <v>6</v>
+        <v>440</v>
       </c>
       <c r="D124" t="s">
-        <v>85</v>
+        <v>441</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>86</v>
+        <v>442</v>
       </c>
       <c r="B125" t="s">
-        <v>33</v>
-      </c>
-      <c r="C125" t="s">
-        <v>6</v>
+        <v>443</v>
       </c>
       <c r="D125" t="s">
-        <v>71</v>
+        <v>444</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>87</v>
+        <v>445</v>
       </c>
       <c r="B126" t="s">
-        <v>88</v>
-      </c>
-      <c r="C126" t="s">
-        <v>34</v>
+        <v>446</v>
       </c>
       <c r="D126" t="s">
-        <v>97</v>
+        <v>447</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>551</v>
+        <v>448</v>
       </c>
       <c r="B127" t="s">
-        <v>552</v>
-      </c>
-      <c r="C127" t="s">
-        <v>34</v>
+        <v>449</v>
       </c>
       <c r="D127" t="s">
-        <v>553</v>
+        <v>450</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>89</v>
+        <v>451</v>
       </c>
       <c r="B128" t="s">
-        <v>90</v>
-      </c>
-      <c r="C128" t="s">
-        <v>34</v>
+        <v>452</v>
       </c>
       <c r="D128" t="s">
-        <v>96</v>
+        <v>453</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>91</v>
+        <v>454</v>
       </c>
       <c r="B129" t="s">
-        <v>92</v>
-      </c>
-      <c r="C129" t="s">
-        <v>34</v>
+        <v>455</v>
       </c>
       <c r="D129" t="s">
-        <v>95</v>
+        <v>456</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>554</v>
+        <v>457</v>
       </c>
       <c r="B130" t="s">
-        <v>555</v>
-      </c>
-      <c r="C130" t="s">
-        <v>34</v>
+        <v>458</v>
       </c>
       <c r="D130" t="s">
-        <v>556</v>
+        <v>459</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>93</v>
+        <v>460</v>
       </c>
       <c r="B131" t="s">
-        <v>557</v>
-      </c>
-      <c r="C131" t="s">
-        <v>34</v>
+        <v>461</v>
       </c>
       <c r="D131" t="s">
-        <v>94</v>
+        <v>462</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>558</v>
+        <v>463</v>
       </c>
       <c r="B132" t="s">
-        <v>559</v>
-      </c>
-      <c r="C132" t="s">
-        <v>34</v>
-      </c>
-      <c r="D132" t="s">
-        <v>560</v>
+        <v>464</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>98</v>
+        <v>465</v>
       </c>
       <c r="B133" t="s">
-        <v>37</v>
-      </c>
-      <c r="C133" t="s">
-        <v>34</v>
+        <v>466</v>
       </c>
       <c r="D133" t="s">
-        <v>99</v>
+        <v>467</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>100</v>
+        <v>475</v>
       </c>
       <c r="B134" t="s">
-        <v>52</v>
-      </c>
-      <c r="C134" t="s">
-        <v>6</v>
+        <v>468</v>
       </c>
       <c r="D134" t="s">
-        <v>53</v>
+        <v>469</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>112</v>
+        <v>476</v>
       </c>
       <c r="B135" t="s">
-        <v>22</v>
-      </c>
-      <c r="C135" t="s">
-        <v>6</v>
+        <v>470</v>
       </c>
       <c r="D135" t="s">
-        <v>539</v>
+        <v>471</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>542</v>
+        <v>477</v>
       </c>
       <c r="B136" t="s">
-        <v>543</v>
-      </c>
-      <c r="C136" t="s">
-        <v>6</v>
+        <v>472</v>
       </c>
       <c r="D136" t="s">
-        <v>65</v>
+        <v>473</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>157</v>
+        <v>235</v>
       </c>
       <c r="B137" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C137" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D137" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>414</v>
+        <v>236</v>
       </c>
       <c r="B138" t="s">
-        <v>415</v>
+        <v>162</v>
       </c>
       <c r="C138" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D138" t="s">
-        <v>416</v>
+        <v>163</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>561</v>
+        <v>237</v>
       </c>
       <c r="B139" t="s">
-        <v>562</v>
+        <v>164</v>
       </c>
       <c r="C139" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D139" t="s">
-        <v>563</v>
+        <v>165</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="B140" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C140" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D140" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>401</v>
+        <v>239</v>
       </c>
       <c r="B141" t="s">
-        <v>565</v>
+        <v>168</v>
       </c>
       <c r="C141" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D141" t="s">
-        <v>566</v>
+        <v>169</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>564</v>
+        <v>240</v>
       </c>
       <c r="B142" t="s">
-        <v>402</v>
+        <v>170</v>
       </c>
       <c r="C142" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D142" t="s">
-        <v>403</v>
+        <v>171</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>567</v>
+        <v>241</v>
       </c>
       <c r="B143" t="s">
-        <v>568</v>
+        <v>172</v>
       </c>
       <c r="C143" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D143" t="s">
-        <v>569</v>
+        <v>173</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>273</v>
+        <v>242</v>
       </c>
       <c r="B144" t="s">
-        <v>274</v>
+        <v>174</v>
       </c>
       <c r="C144" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D144" t="s">
-        <v>275</v>
+        <v>175</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>328</v>
+        <v>243</v>
       </c>
       <c r="B145" t="s">
-        <v>329</v>
+        <v>176</v>
       </c>
       <c r="C145" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D145" t="s">
-        <v>528</v>
+        <v>177</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>525</v>
+        <v>178</v>
       </c>
       <c r="B146" t="s">
-        <v>526</v>
+        <v>179</v>
       </c>
       <c r="C146" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D146" t="s">
-        <v>527</v>
+        <v>180</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>330</v>
+        <v>214</v>
       </c>
       <c r="B147" t="s">
-        <v>331</v>
+        <v>218</v>
       </c>
       <c r="C147" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D147" t="s">
-        <v>332</v>
+        <v>219</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>532</v>
+        <v>220</v>
       </c>
       <c r="B148" t="s">
-        <v>533</v>
+        <v>221</v>
       </c>
       <c r="C148" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D148" t="s">
-        <v>534</v>
+        <v>222</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>535</v>
+        <v>223</v>
       </c>
       <c r="B149" t="s">
-        <v>537</v>
+        <v>224</v>
       </c>
       <c r="C149" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D149" t="s">
-        <v>538</v>
+        <v>225</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>536</v>
+        <v>226</v>
       </c>
       <c r="B150" t="s">
-        <v>540</v>
+        <v>227</v>
       </c>
       <c r="C150" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D150" t="s">
-        <v>541</v>
+        <v>228</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>285</v>
+        <v>229</v>
       </c>
       <c r="B151" t="s">
-        <v>13</v>
+        <v>230</v>
       </c>
       <c r="C151" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="D151" t="s">
-        <v>61</v>
+        <v>231</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>286</v>
+        <v>232</v>
       </c>
       <c r="B152" t="s">
-        <v>30</v>
+        <v>233</v>
       </c>
       <c r="C152" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="D152" t="s">
-        <v>70</v>
+        <v>234</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>287</v>
+        <v>217</v>
       </c>
       <c r="B153" t="s">
-        <v>50</v>
+        <v>215</v>
       </c>
       <c r="C153" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="D153" t="s">
-        <v>77</v>
+        <v>216</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>288</v>
+        <v>244</v>
       </c>
       <c r="B154" t="s">
-        <v>334</v>
+        <v>245</v>
       </c>
       <c r="C154" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="D154" t="s">
-        <v>113</v>
+        <v>246</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>333</v>
+        <v>371</v>
       </c>
       <c r="B155" t="s">
-        <v>335</v>
+        <v>372</v>
       </c>
       <c r="C155" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="D155" t="s">
-        <v>336</v>
+        <v>373</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="B156" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="C156" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D156" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="B157" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="C157" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D157" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="B158" t="s">
-        <v>114</v>
+        <v>313</v>
       </c>
       <c r="C158" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D158" t="s">
-        <v>79</v>
+        <v>314</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>338</v>
+        <v>257</v>
       </c>
       <c r="B159" t="s">
-        <v>339</v>
+        <v>10</v>
       </c>
       <c r="C159" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D159" t="s">
-        <v>340</v>
+        <v>59</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>292</v>
+        <v>552</v>
       </c>
       <c r="B160" t="s">
-        <v>115</v>
+        <v>553</v>
       </c>
       <c r="C160" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D160" t="s">
-        <v>116</v>
+        <v>554</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="B161" t="s">
-        <v>117</v>
+        <v>310</v>
       </c>
       <c r="C161" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D161" t="s">
-        <v>118</v>
+        <v>311</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>119</v>
+        <v>259</v>
       </c>
       <c r="B162" t="s">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="C162" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D162" t="s">
-        <v>121</v>
+        <v>60</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>123</v>
+        <v>260</v>
       </c>
       <c r="B163" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="C163" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D163" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>126</v>
+        <v>261</v>
       </c>
       <c r="B164" t="s">
-        <v>127</v>
+        <v>26</v>
       </c>
       <c r="C164" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D164" t="s">
-        <v>125</v>
+        <v>203</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>130</v>
+        <v>262</v>
       </c>
       <c r="B165" t="s">
-        <v>129</v>
+        <v>27</v>
       </c>
       <c r="C165" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D165" t="s">
-        <v>128</v>
+        <v>270</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>131</v>
+        <v>263</v>
       </c>
       <c r="B166" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C166" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D166" t="s">
-        <v>78</v>
+        <v>271</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>193</v>
+        <v>83</v>
       </c>
       <c r="B167" t="s">
-        <v>194</v>
+        <v>84</v>
       </c>
       <c r="C167" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D167" t="s">
-        <v>195</v>
+        <v>85</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>387</v>
+        <v>86</v>
       </c>
       <c r="B168" t="s">
-        <v>388</v>
+        <v>33</v>
       </c>
       <c r="C168" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D168" t="s">
-        <v>389</v>
+        <v>71</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>300</v>
+        <v>105</v>
       </c>
       <c r="B169" t="s">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="C169" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="D169" t="s">
-        <v>111</v>
+        <v>527</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>301</v>
+        <v>530</v>
       </c>
       <c r="B170" t="s">
-        <v>101</v>
+        <v>531</v>
       </c>
       <c r="C170" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="D170" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="B171" t="s">
-        <v>104</v>
+        <v>319</v>
       </c>
       <c r="C171" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="D171" t="s">
-        <v>23</v>
+        <v>516</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>303</v>
+        <v>513</v>
       </c>
       <c r="B172" t="s">
-        <v>106</v>
+        <v>514</v>
       </c>
       <c r="C172" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="D172" t="s">
-        <v>110</v>
+        <v>515</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>304</v>
+        <v>320</v>
       </c>
       <c r="B173" t="s">
-        <v>105</v>
+        <v>321</v>
       </c>
       <c r="C173" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="D173" t="s">
-        <v>21</v>
+        <v>322</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>305</v>
+        <v>520</v>
       </c>
       <c r="B174" t="s">
-        <v>31</v>
+        <v>521</v>
       </c>
       <c r="C174" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="D174" t="s">
-        <v>32</v>
+        <v>522</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>306</v>
+        <v>523</v>
       </c>
       <c r="B175" t="s">
-        <v>107</v>
+        <v>525</v>
       </c>
       <c r="C175" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="D175" t="s">
-        <v>109</v>
+        <v>526</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>307</v>
+        <v>524</v>
       </c>
       <c r="B176" t="s">
+        <v>528</v>
+      </c>
+      <c r="C176" t="s">
+        <v>6</v>
+      </c>
+      <c r="D176" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>275</v>
+      </c>
+      <c r="B177" t="s">
+        <v>13</v>
+      </c>
+      <c r="C177" t="s">
+        <v>14</v>
+      </c>
+      <c r="D177" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>276</v>
+      </c>
+      <c r="B178" t="s">
+        <v>30</v>
+      </c>
+      <c r="C178" t="s">
+        <v>14</v>
+      </c>
+      <c r="D178" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>277</v>
+      </c>
+      <c r="B179" t="s">
+        <v>50</v>
+      </c>
+      <c r="C179" t="s">
+        <v>14</v>
+      </c>
+      <c r="D179" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>278</v>
+      </c>
+      <c r="B180" t="s">
+        <v>324</v>
+      </c>
+      <c r="C180" t="s">
+        <v>14</v>
+      </c>
+      <c r="D180" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>323</v>
+      </c>
+      <c r="B181" t="s">
+        <v>325</v>
+      </c>
+      <c r="C181" t="s">
+        <v>14</v>
+      </c>
+      <c r="D181" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>279</v>
+      </c>
+      <c r="B182" t="s">
+        <v>54</v>
+      </c>
+      <c r="C182" t="s">
+        <v>14</v>
+      </c>
+      <c r="D182" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>280</v>
+      </c>
+      <c r="B183" t="s">
+        <v>74</v>
+      </c>
+      <c r="C183" t="s">
+        <v>14</v>
+      </c>
+      <c r="D183" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>281</v>
+      </c>
+      <c r="B184" t="s">
+        <v>107</v>
+      </c>
+      <c r="C184" t="s">
+        <v>14</v>
+      </c>
+      <c r="D184" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>328</v>
+      </c>
+      <c r="B185" t="s">
+        <v>329</v>
+      </c>
+      <c r="C185" t="s">
+        <v>14</v>
+      </c>
+      <c r="D185" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>282</v>
+      </c>
+      <c r="B186" t="s">
         <v>108</v>
       </c>
-      <c r="C176" t="s">
-        <v>103</v>
-      </c>
-      <c r="D176" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
-        <v>308</v>
-      </c>
-      <c r="B177" t="s">
-        <v>309</v>
-      </c>
-      <c r="C177" t="s">
-        <v>103</v>
-      </c>
-      <c r="D177" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>311</v>
-      </c>
-      <c r="B178" t="s">
-        <v>312</v>
-      </c>
-      <c r="C178" t="s">
-        <v>103</v>
-      </c>
-      <c r="D178" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>337</v>
-      </c>
-      <c r="B179" t="s">
-        <v>379</v>
-      </c>
-      <c r="C179" t="s">
-        <v>103</v>
-      </c>
-      <c r="D179" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
-        <v>314</v>
-      </c>
-      <c r="B180" t="s">
-        <v>393</v>
-      </c>
-      <c r="C180" t="s">
-        <v>103</v>
-      </c>
-      <c r="D180" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>317</v>
-      </c>
-      <c r="B181" t="s">
-        <v>315</v>
-      </c>
-      <c r="C181" t="s">
-        <v>103</v>
-      </c>
-      <c r="D181" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
-        <v>375</v>
-      </c>
-      <c r="B182" t="s">
-        <v>373</v>
-      </c>
-      <c r="C182" t="s">
-        <v>18</v>
-      </c>
-      <c r="D182" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
-        <v>375</v>
-      </c>
-      <c r="B183" t="s">
-        <v>318</v>
-      </c>
-      <c r="C183" t="s">
-        <v>103</v>
-      </c>
-      <c r="D183" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
-        <v>390</v>
-      </c>
-      <c r="B184" t="s">
-        <v>391</v>
-      </c>
-      <c r="C184" t="s">
-        <v>18</v>
-      </c>
-      <c r="D184" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A185" t="s">
-        <v>146</v>
-      </c>
-      <c r="B185" t="s">
-        <v>147</v>
-      </c>
-      <c r="C185" t="s">
-        <v>148</v>
-      </c>
-      <c r="D185" t="s">
-        <v>149</v>
-      </c>
-      <c r="E185" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A186" t="s">
-        <v>151</v>
-      </c>
-      <c r="B186" t="s">
-        <v>152</v>
-      </c>
       <c r="C186" t="s">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="D186" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>411</v>
+        <v>283</v>
       </c>
       <c r="B187" t="s">
-        <v>412</v>
+        <v>110</v>
       </c>
       <c r="C187" t="s">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="D187" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>213</v>
+        <v>112</v>
       </c>
       <c r="B188" t="s">
-        <v>214</v>
+        <v>113</v>
       </c>
       <c r="C188" t="s">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="D188" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>256</v>
+        <v>116</v>
       </c>
       <c r="B189" t="s">
-        <v>257</v>
+        <v>117</v>
       </c>
       <c r="C189" t="s">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="D189" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>259</v>
+        <v>119</v>
       </c>
       <c r="B190" t="s">
-        <v>260</v>
+        <v>120</v>
       </c>
       <c r="C190" t="s">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="D190" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>496</v>
+        <v>123</v>
       </c>
       <c r="B191" t="s">
-        <v>490</v>
+        <v>122</v>
       </c>
       <c r="C191" t="s">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="D191" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>492</v>
+        <v>124</v>
       </c>
       <c r="B192" t="s">
-        <v>493</v>
+        <v>40</v>
       </c>
       <c r="C192" t="s">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="D192" t="s">
-        <v>497</v>
+        <v>78</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>494</v>
+        <v>184</v>
       </c>
       <c r="B193" t="s">
-        <v>495</v>
+        <v>185</v>
       </c>
       <c r="C193" t="s">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="D193" t="s">
-        <v>498</v>
+        <v>186</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>282</v>
+        <v>377</v>
       </c>
       <c r="B194" t="s">
-        <v>283</v>
+        <v>378</v>
       </c>
       <c r="C194" t="s">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="D194" t="s">
-        <v>284</v>
+        <v>379</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>507</v>
+        <v>290</v>
       </c>
       <c r="B195" t="s">
-        <v>508</v>
+        <v>95</v>
       </c>
       <c r="C195" t="s">
-        <v>148</v>
+        <v>96</v>
       </c>
       <c r="D195" t="s">
-        <v>509</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>291</v>
+      </c>
+      <c r="B196" t="s">
+        <v>94</v>
+      </c>
+      <c r="C196" t="s">
+        <v>96</v>
+      </c>
+      <c r="D196" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>292</v>
+      </c>
+      <c r="B197" t="s">
+        <v>97</v>
+      </c>
+      <c r="C197" t="s">
+        <v>96</v>
+      </c>
+      <c r="D197" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>293</v>
+      </c>
+      <c r="B198" t="s">
+        <v>99</v>
+      </c>
+      <c r="C198" t="s">
+        <v>96</v>
+      </c>
+      <c r="D198" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>294</v>
+      </c>
+      <c r="B199" t="s">
+        <v>98</v>
+      </c>
+      <c r="C199" t="s">
+        <v>96</v>
+      </c>
+      <c r="D199" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>295</v>
+      </c>
+      <c r="B200" t="s">
+        <v>31</v>
+      </c>
+      <c r="C200" t="s">
+        <v>96</v>
+      </c>
+      <c r="D200" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>296</v>
+      </c>
+      <c r="B201" t="s">
+        <v>100</v>
+      </c>
+      <c r="C201" t="s">
+        <v>96</v>
+      </c>
+      <c r="D201" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>297</v>
+      </c>
+      <c r="B202" t="s">
+        <v>101</v>
+      </c>
+      <c r="C202" t="s">
+        <v>96</v>
+      </c>
+      <c r="D202" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>298</v>
+      </c>
+      <c r="B203" t="s">
+        <v>299</v>
+      </c>
+      <c r="C203" t="s">
+        <v>96</v>
+      </c>
+      <c r="D203" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>301</v>
+      </c>
+      <c r="B204" t="s">
+        <v>302</v>
+      </c>
+      <c r="C204" t="s">
+        <v>96</v>
+      </c>
+      <c r="D204" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>327</v>
+      </c>
+      <c r="B205" t="s">
+        <v>369</v>
+      </c>
+      <c r="C205" t="s">
+        <v>96</v>
+      </c>
+      <c r="D205" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>304</v>
+      </c>
+      <c r="B206" t="s">
+        <v>383</v>
+      </c>
+      <c r="C206" t="s">
+        <v>96</v>
+      </c>
+      <c r="D206" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>307</v>
+      </c>
+      <c r="B207" t="s">
+        <v>305</v>
+      </c>
+      <c r="C207" t="s">
+        <v>96</v>
+      </c>
+      <c r="D207" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>365</v>
+      </c>
+      <c r="B208" t="s">
+        <v>363</v>
+      </c>
+      <c r="C208" t="s">
+        <v>18</v>
+      </c>
+      <c r="D208" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>365</v>
+      </c>
+      <c r="B209" t="s">
+        <v>308</v>
+      </c>
+      <c r="C209" t="s">
+        <v>96</v>
+      </c>
+      <c r="D209" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>380</v>
+      </c>
+      <c r="B210" t="s">
+        <v>381</v>
+      </c>
+      <c r="C210" t="s">
+        <v>18</v>
+      </c>
+      <c r="D210" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>139</v>
+      </c>
+      <c r="B211" t="s">
+        <v>140</v>
+      </c>
+      <c r="C211" t="s">
+        <v>141</v>
+      </c>
+      <c r="D211" t="s">
+        <v>142</v>
+      </c>
+      <c r="E211" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>144</v>
+      </c>
+      <c r="B212" t="s">
+        <v>145</v>
+      </c>
+      <c r="C212" t="s">
+        <v>141</v>
+      </c>
+      <c r="D212" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>400</v>
+      </c>
+      <c r="B213" t="s">
+        <v>401</v>
+      </c>
+      <c r="C213" t="s">
+        <v>141</v>
+      </c>
+      <c r="D213" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>204</v>
+      </c>
+      <c r="B214" t="s">
+        <v>205</v>
+      </c>
+      <c r="C214" t="s">
+        <v>141</v>
+      </c>
+      <c r="D214" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>247</v>
+      </c>
+      <c r="B215" t="s">
+        <v>248</v>
+      </c>
+      <c r="C215" t="s">
+        <v>141</v>
+      </c>
+      <c r="D215" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>250</v>
+      </c>
+      <c r="B216" t="s">
+        <v>251</v>
+      </c>
+      <c r="C216" t="s">
+        <v>141</v>
+      </c>
+      <c r="D216" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>484</v>
+      </c>
+      <c r="B217" t="s">
+        <v>478</v>
+      </c>
+      <c r="C217" t="s">
+        <v>141</v>
+      </c>
+      <c r="D217" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>480</v>
+      </c>
+      <c r="B218" t="s">
+        <v>481</v>
+      </c>
+      <c r="C218" t="s">
+        <v>141</v>
+      </c>
+      <c r="D218" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>482</v>
+      </c>
+      <c r="B219" t="s">
+        <v>483</v>
+      </c>
+      <c r="C219" t="s">
+        <v>141</v>
+      </c>
+      <c r="D219" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>272</v>
+      </c>
+      <c r="B220" t="s">
+        <v>273</v>
+      </c>
+      <c r="C220" t="s">
+        <v>141</v>
+      </c>
+      <c r="D220" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>495</v>
+      </c>
+      <c r="B221" t="s">
+        <v>496</v>
+      </c>
+      <c r="C221" t="s">
+        <v>141</v>
+      </c>
+      <c r="D221" t="s">
+        <v>497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Two new variables, added values column to spreadsheet
1. Immunosuppressed v2
2. BCG ever
3. Added a values column to spreadsheet and began to populate
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5A52B9-5FE8-8749-B8B6-DA8A54C123AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B363AF-9694-B64E-B9D9-6D7DCF8A1120}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35860" yWindow="2900" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="680">
   <si>
     <t>Variable #</t>
   </si>
@@ -157,9 +157,6 @@
     <t>card</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
@@ -2045,6 +2042,30 @@
   </si>
   <si>
     <t>Bladder</t>
+  </si>
+  <si>
+    <t>Ca10l</t>
+  </si>
+  <si>
+    <t>Any intravesicular BCG</t>
+  </si>
+  <si>
+    <t>any_intravesicular_bcg</t>
+  </si>
+  <si>
+    <t>C05a</t>
+  </si>
+  <si>
+    <t>immunosuppressed_v2</t>
+  </si>
+  <si>
+    <t>Derived variable indicating whether patient has any immunosuppression including cytotoxic chemo within 3 mo</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>0-No; 1-Yes; 99-Unknown</t>
   </si>
 </sst>
 </file>
@@ -2100,17 +2121,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E222" totalsRowShown="0">
-  <autoFilter ref="A1:E222" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E222">
-    <sortCondition ref="A1:A222"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E224" totalsRowShown="0">
+  <autoFilter ref="A1:E224" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E224">
+    <sortCondition ref="A1:A224"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
     <tableColumn id="2" xr3:uid="{9AFC5F6C-2B2C-E541-A77F-830B0EABC78C}" name="Variable Name (der_name)"/>
     <tableColumn id="3" xr3:uid="{800F9FDD-F033-7A4B-A634-744A5D9FEFE2}" name="Category"/>
     <tableColumn id="4" xr3:uid="{827F03E0-E9CB-BF47-915C-D34395E5A6F4}" name="Description"/>
-    <tableColumn id="5" xr3:uid="{F9BBFA6E-9630-224E-B86A-31602DCDBEE5}" name="Notes"/>
+    <tableColumn id="5" xr3:uid="{F9BBFA6E-9630-224E-B86A-31602DCDBEE5}" name="Values"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2437,10 +2458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E222"/>
+  <dimension ref="A1:E224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2457,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2466,68 +2487,68 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>678</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B4" t="s">
         <v>394</v>
-      </c>
-      <c r="B4" t="s">
-        <v>395</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>565</v>
+      </c>
+      <c r="B5" t="s">
         <v>566</v>
-      </c>
-      <c r="B5" t="s">
-        <v>567</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
@@ -2541,35 +2562,35 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B9" t="s">
         <v>38</v>
@@ -2578,12 +2599,12 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
@@ -2592,189 +2613,195 @@
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="E10" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>338</v>
+        <v>675</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>676</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>677</v>
+      </c>
+      <c r="E11" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>134</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B15" t="s">
-        <v>187</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>188</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B16" t="s">
-        <v>344</v>
+        <v>186</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>345</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B17" t="s">
-        <v>253</v>
+        <v>343</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>254</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>385</v>
+        <v>345</v>
       </c>
       <c r="B18" t="s">
-        <v>386</v>
+        <v>252</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>387</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>284</v>
+        <v>384</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>385</v>
       </c>
       <c r="C19" t="s">
-        <v>532</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>386</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B20" t="s">
-        <v>207</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D20" t="s">
-        <v>349</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>347</v>
+        <v>284</v>
       </c>
       <c r="B21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" t="s">
+        <v>531</v>
+      </c>
+      <c r="D21" t="s">
         <v>348</v>
-      </c>
-      <c r="C21" t="s">
-        <v>532</v>
-      </c>
-      <c r="D21" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>569</v>
+        <v>346</v>
       </c>
       <c r="B22" t="s">
-        <v>570</v>
+        <v>347</v>
       </c>
       <c r="C22" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D22" t="s">
-        <v>571</v>
+        <v>349</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>490</v>
+        <v>568</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>569</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>531</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>570</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2782,483 +2809,483 @@
         <v>489</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>286</v>
+        <v>488</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>532</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>531</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>366</v>
+        <v>286</v>
       </c>
       <c r="B27" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
       <c r="B28" t="s">
-        <v>367</v>
+        <v>137</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>368</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>494</v>
+        <v>387</v>
       </c>
       <c r="B29" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>288</v>
+        <v>493</v>
       </c>
       <c r="B30" t="s">
-        <v>146</v>
+        <v>388</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>148</v>
+        <v>389</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>157</v>
+        <v>288</v>
       </c>
       <c r="B32" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>558</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="B33" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="C33" t="s">
-        <v>532</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B34" t="s">
-        <v>357</v>
+        <v>195</v>
       </c>
       <c r="C34" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D34" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B35" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C35" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D35" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>353</v>
+        <v>199</v>
       </c>
       <c r="B36" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C36" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D36" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B37" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C37" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D37" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B38" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C38" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D38" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B39" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C39" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D39" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B40" t="s">
-        <v>198</v>
+        <v>361</v>
       </c>
       <c r="C40" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D40" t="s">
-        <v>199</v>
+        <v>564</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B41" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C41" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D41" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>374</v>
+        <v>351</v>
       </c>
       <c r="B42" t="s">
-        <v>375</v>
+        <v>200</v>
       </c>
       <c r="C42" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D42" t="s">
-        <v>376</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>555</v>
+        <v>373</v>
       </c>
       <c r="B43" t="s">
-        <v>556</v>
+        <v>374</v>
       </c>
       <c r="C43" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D43" t="s">
-        <v>557</v>
+        <v>375</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>189</v>
+        <v>554</v>
       </c>
       <c r="B44" t="s">
-        <v>190</v>
+        <v>555</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>531</v>
       </c>
       <c r="D44" t="s">
-        <v>405</v>
+        <v>556</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>208</v>
+        <v>672</v>
       </c>
       <c r="B45" t="s">
-        <v>209</v>
+        <v>674</v>
       </c>
       <c r="C45" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D45" t="s">
-        <v>210</v>
+        <v>673</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="B46" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="C46" t="s">
-        <v>532</v>
+        <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>213</v>
+        <v>404</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>498</v>
+        <v>207</v>
       </c>
       <c r="B47" t="s">
-        <v>499</v>
+        <v>208</v>
       </c>
       <c r="C47" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D47" t="s">
-        <v>500</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>503</v>
+        <v>210</v>
       </c>
       <c r="B48" t="s">
-        <v>501</v>
+        <v>211</v>
       </c>
       <c r="C48" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D48" t="s">
-        <v>502</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="B49" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="C49" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D49" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="B50" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="C50" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D50" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="B51" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="C51" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D51" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="B52" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>531</v>
       </c>
       <c r="D52" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>533</v>
+        <v>509</v>
       </c>
       <c r="B53" t="s">
-        <v>534</v>
+        <v>510</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>531</v>
       </c>
       <c r="D53" t="s">
-        <v>535</v>
+        <v>511</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>536</v>
+        <v>516</v>
       </c>
       <c r="B54" t="s">
-        <v>537</v>
+        <v>517</v>
       </c>
       <c r="C54" t="s">
         <v>18</v>
       </c>
       <c r="D54" t="s">
-        <v>538</v>
+        <v>518</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>572</v>
+        <v>532</v>
       </c>
       <c r="B55" t="s">
-        <v>573</v>
+        <v>533</v>
       </c>
       <c r="C55" t="s">
-        <v>532</v>
+        <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>574</v>
+        <v>534</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>575</v>
+        <v>535</v>
       </c>
       <c r="B56" t="s">
-        <v>87</v>
+        <v>536</v>
       </c>
       <c r="C56" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D56" t="s">
-        <v>93</v>
+        <v>537</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="B57" t="s">
-        <v>539</v>
+        <v>572</v>
       </c>
       <c r="C57" t="s">
-        <v>34</v>
+        <v>531</v>
       </c>
       <c r="D57" t="s">
-        <v>540</v>
+        <v>573</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C58" t="s">
         <v>34</v>
@@ -3269,38 +3296,38 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>538</v>
       </c>
       <c r="C59" t="s">
         <v>34</v>
       </c>
       <c r="D59" t="s">
-        <v>91</v>
+        <v>539</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B60" t="s">
-        <v>541</v>
+        <v>87</v>
       </c>
       <c r="C60" t="s">
         <v>34</v>
       </c>
       <c r="D60" t="s">
-        <v>542</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B61" t="s">
-        <v>543</v>
+        <v>88</v>
       </c>
       <c r="C61" t="s">
         <v>34</v>
@@ -3311,2190 +3338,2218 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B62" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C62" t="s">
         <v>34</v>
       </c>
       <c r="D62" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B63" t="s">
-        <v>150</v>
+        <v>542</v>
       </c>
       <c r="C63" t="s">
         <v>34</v>
       </c>
       <c r="D63" t="s">
-        <v>151</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B64" t="s">
-        <v>403</v>
+        <v>543</v>
       </c>
       <c r="C64" t="s">
         <v>34</v>
       </c>
       <c r="D64" t="s">
-        <v>404</v>
+        <v>544</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B65" t="s">
-        <v>546</v>
+        <v>149</v>
       </c>
       <c r="C65" t="s">
         <v>34</v>
       </c>
       <c r="D65" t="s">
-        <v>547</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B66" t="s">
-        <v>152</v>
+        <v>402</v>
       </c>
       <c r="C66" t="s">
         <v>34</v>
       </c>
       <c r="D66" t="s">
-        <v>153</v>
+        <v>403</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B67" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C67" t="s">
         <v>34</v>
       </c>
       <c r="D67" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B68" t="s">
-        <v>391</v>
+        <v>151</v>
       </c>
       <c r="C68" t="s">
         <v>34</v>
       </c>
       <c r="D68" t="s">
-        <v>392</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B69" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C69" t="s">
         <v>34</v>
       </c>
       <c r="D69" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B70" t="s">
-        <v>37</v>
+        <v>390</v>
       </c>
       <c r="C70" t="s">
         <v>34</v>
       </c>
       <c r="D70" t="s">
-        <v>640</v>
+        <v>391</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B71" t="s">
-        <v>264</v>
+        <v>549</v>
       </c>
       <c r="C71" t="s">
         <v>34</v>
       </c>
       <c r="D71" t="s">
-        <v>265</v>
+        <v>550</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B72" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C72" t="s">
         <v>34</v>
       </c>
       <c r="D72" t="s">
-        <v>53</v>
+        <v>639</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B73" t="s">
-        <v>593</v>
+        <v>263</v>
       </c>
       <c r="C73" t="s">
         <v>34</v>
       </c>
       <c r="D73" t="s">
-        <v>594</v>
+        <v>264</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="B74" t="s">
-        <v>596</v>
+        <v>51</v>
       </c>
       <c r="C74" t="s">
         <v>34</v>
       </c>
       <c r="D74" t="s">
-        <v>597</v>
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="B75" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="C75" t="s">
         <v>34</v>
       </c>
       <c r="D75" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="B76" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="C76" t="s">
         <v>34</v>
       </c>
       <c r="D76" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="B77" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="C77" t="s">
         <v>34</v>
       </c>
       <c r="D77" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="B78" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="C78" t="s">
         <v>34</v>
       </c>
       <c r="D78" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
       <c r="B79" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="C79" t="s">
         <v>34</v>
       </c>
       <c r="D79" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="B80" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="C80" t="s">
         <v>34</v>
       </c>
       <c r="D80" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="B81" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="C81" t="s">
         <v>34</v>
       </c>
       <c r="D81" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="B82" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="C82" t="s">
         <v>34</v>
       </c>
       <c r="D82" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="B83" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="C83" t="s">
         <v>34</v>
       </c>
       <c r="D83" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="B84" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="C84" t="s">
         <v>34</v>
       </c>
       <c r="D84" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="B85" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="C85" t="s">
         <v>34</v>
       </c>
       <c r="D85" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="B86" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="C86" t="s">
         <v>34</v>
       </c>
       <c r="D86" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="B87" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="C87" t="s">
         <v>34</v>
       </c>
       <c r="D87" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="B88" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="C88" t="s">
         <v>34</v>
       </c>
       <c r="D88" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="B89" t="s">
-        <v>645</v>
+        <v>634</v>
       </c>
       <c r="C89" t="s">
         <v>34</v>
       </c>
       <c r="D89" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
       <c r="B90" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="C90" t="s">
         <v>34</v>
       </c>
       <c r="D90" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="B91" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="C91" t="s">
         <v>34</v>
       </c>
       <c r="D91" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="B92" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="C92" t="s">
         <v>34</v>
       </c>
       <c r="D92" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="B93" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="C93" t="s">
         <v>34</v>
       </c>
       <c r="D93" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="B94" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="C94" t="s">
         <v>34</v>
       </c>
       <c r="D94" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="B95" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="C95" t="s">
         <v>34</v>
       </c>
       <c r="D95" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="B96" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="C96" t="s">
         <v>34</v>
       </c>
       <c r="D96" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="B97" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="C97" t="s">
         <v>34</v>
       </c>
       <c r="D97" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="B98" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="C98" t="s">
         <v>34</v>
       </c>
       <c r="D98" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>266</v>
+        <v>664</v>
       </c>
       <c r="B99" t="s">
-        <v>125</v>
+        <v>665</v>
       </c>
       <c r="C99" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D99" t="s">
-        <v>46</v>
+        <v>666</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>267</v>
+        <v>667</v>
       </c>
       <c r="B100" t="s">
-        <v>44</v>
+        <v>668</v>
       </c>
       <c r="C100" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D100" t="s">
-        <v>45</v>
+        <v>669</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>491</v>
+        <v>265</v>
       </c>
       <c r="B101" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C101" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D101" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>492</v>
+        <v>266</v>
       </c>
       <c r="B102" t="s">
-        <v>135</v>
+        <v>43</v>
       </c>
       <c r="C102" t="s">
         <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>136</v>
+        <v>44</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>268</v>
+        <v>490</v>
       </c>
       <c r="B103" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="C103" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D103" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B104" t="s">
-        <v>191</v>
+        <v>134</v>
       </c>
       <c r="C104" t="s">
         <v>5</v>
       </c>
       <c r="D104" t="s">
-        <v>192</v>
+        <v>135</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>487</v>
+        <v>267</v>
       </c>
       <c r="B105" t="s">
-        <v>488</v>
+        <v>17</v>
       </c>
       <c r="C105" t="s">
         <v>5</v>
       </c>
+      <c r="D105" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>269</v>
+        <v>492</v>
       </c>
       <c r="B106" t="s">
-        <v>20</v>
+        <v>190</v>
       </c>
       <c r="C106" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D106" t="s">
-        <v>64</v>
+        <v>191</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>129</v>
+        <v>486</v>
       </c>
       <c r="B107" t="s">
-        <v>3</v>
+        <v>487</v>
       </c>
       <c r="C107" t="s">
         <v>5</v>
       </c>
-      <c r="D107" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>315</v>
+        <v>268</v>
       </c>
       <c r="B108" t="s">
-        <v>316</v>
+        <v>20</v>
       </c>
       <c r="C108" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D108" t="s">
-        <v>317</v>
+        <v>63</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B109" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C109" t="s">
         <v>5</v>
       </c>
       <c r="D109" t="s">
-        <v>132</v>
+        <v>7</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>158</v>
+        <v>314</v>
       </c>
       <c r="B110" t="s">
-        <v>159</v>
+        <v>315</v>
       </c>
       <c r="C110" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D110" t="s">
-        <v>160</v>
+        <v>316</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>181</v>
+        <v>129</v>
       </c>
       <c r="B111" t="s">
-        <v>182</v>
+        <v>130</v>
       </c>
       <c r="C111" t="s">
         <v>5</v>
       </c>
       <c r="D111" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>406</v>
+        <v>157</v>
       </c>
       <c r="B112" t="s">
-        <v>407</v>
+        <v>158</v>
       </c>
       <c r="C112" t="s">
-        <v>408</v>
+        <v>15</v>
       </c>
       <c r="D112" t="s">
-        <v>474</v>
+        <v>159</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>409</v>
+        <v>180</v>
       </c>
       <c r="B113" t="s">
-        <v>410</v>
+        <v>181</v>
       </c>
       <c r="C113" t="s">
-        <v>408</v>
+        <v>5</v>
       </c>
       <c r="D113" t="s">
-        <v>411</v>
+        <v>182</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B114" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C114" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D114" t="s">
-        <v>414</v>
+        <v>473</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="B115" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C115" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D115" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="B116" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="C116" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D116" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="B117" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="C117" t="s">
-        <v>408</v>
+        <v>407</v>
+      </c>
+      <c r="D117" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="B118" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C118" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D118" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="B119" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="C119" t="s">
-        <v>408</v>
-      </c>
-      <c r="D119" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="B120" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="C120" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D120" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B121" t="s">
-        <v>433</v>
+        <v>426</v>
+      </c>
+      <c r="C121" t="s">
+        <v>407</v>
+      </c>
+      <c r="D121" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="B122" t="s">
-        <v>435</v>
+        <v>429</v>
+      </c>
+      <c r="C122" t="s">
+        <v>407</v>
       </c>
       <c r="D122" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="B123" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="B124" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="D124" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="B125" t="s">
-        <v>443</v>
-      </c>
-      <c r="D125" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="B126" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="D126" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="B127" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="D127" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B128" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="D128" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B129" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="D129" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="B130" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="D130" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="B131" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="D131" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="B132" t="s">
-        <v>464</v>
+        <v>457</v>
+      </c>
+      <c r="D132" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B133" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="D133" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="B134" t="s">
-        <v>468</v>
-      </c>
-      <c r="D134" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="B135" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D135" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B136" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D136" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>671</v>
+        <v>475</v>
       </c>
       <c r="B137" t="s">
-        <v>672</v>
+        <v>469</v>
+      </c>
+      <c r="D137" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>235</v>
+        <v>476</v>
       </c>
       <c r="B138" t="s">
-        <v>154</v>
-      </c>
-      <c r="C138" t="s">
-        <v>155</v>
+        <v>471</v>
       </c>
       <c r="D138" t="s">
-        <v>156</v>
+        <v>472</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>236</v>
+        <v>670</v>
       </c>
       <c r="B139" t="s">
-        <v>162</v>
-      </c>
-      <c r="C139" t="s">
-        <v>155</v>
-      </c>
-      <c r="D139" t="s">
-        <v>163</v>
+        <v>671</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B140" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C140" t="s">
+        <v>154</v>
+      </c>
+      <c r="D140" t="s">
         <v>155</v>
-      </c>
-      <c r="D140" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B141" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C141" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D141" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B142" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C142" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D142" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B143" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C143" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D143" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B144" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C144" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D144" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B145" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C145" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D145" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B146" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C146" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D146" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>178</v>
+        <v>241</v>
       </c>
       <c r="B147" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C147" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D147" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="B148" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C148" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D148" t="s">
-        <v>219</v>
+        <v>176</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="B149" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="C149" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D149" t="s">
-        <v>222</v>
+        <v>179</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B150" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C150" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D150" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B151" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C151" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D151" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B152" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C152" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D152" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B153" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C153" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D153" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="B154" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="C154" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D154" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="B155" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="C155" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D155" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>371</v>
+        <v>216</v>
       </c>
       <c r="B156" t="s">
-        <v>372</v>
+        <v>214</v>
       </c>
       <c r="C156" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D156" t="s">
-        <v>373</v>
+        <v>215</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B157" t="s">
-        <v>4</v>
+        <v>244</v>
       </c>
       <c r="C157" t="s">
-        <v>6</v>
+        <v>154</v>
       </c>
       <c r="D157" t="s">
-        <v>57</v>
+        <v>245</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>256</v>
+        <v>370</v>
       </c>
       <c r="B158" t="s">
-        <v>11</v>
+        <v>371</v>
       </c>
       <c r="C158" t="s">
-        <v>6</v>
+        <v>154</v>
       </c>
       <c r="D158" t="s">
-        <v>58</v>
+        <v>372</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>312</v>
+        <v>254</v>
       </c>
       <c r="B159" t="s">
-        <v>313</v>
+        <v>4</v>
       </c>
       <c r="C159" t="s">
         <v>6</v>
       </c>
       <c r="D159" t="s">
-        <v>314</v>
+        <v>56</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B160" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C160" t="s">
         <v>6</v>
       </c>
       <c r="D160" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>552</v>
+        <v>311</v>
       </c>
       <c r="B161" t="s">
-        <v>553</v>
+        <v>312</v>
       </c>
       <c r="C161" t="s">
         <v>6</v>
       </c>
       <c r="D161" t="s">
-        <v>554</v>
+        <v>313</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B162" t="s">
-        <v>310</v>
+        <v>10</v>
       </c>
       <c r="C162" t="s">
         <v>6</v>
       </c>
       <c r="D162" t="s">
-        <v>311</v>
+        <v>58</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>259</v>
+        <v>551</v>
       </c>
       <c r="B163" t="s">
-        <v>12</v>
+        <v>552</v>
       </c>
       <c r="C163" t="s">
         <v>6</v>
       </c>
       <c r="D163" t="s">
-        <v>60</v>
+        <v>553</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B164" t="s">
-        <v>81</v>
+        <v>309</v>
       </c>
       <c r="C164" t="s">
         <v>6</v>
       </c>
       <c r="D164" t="s">
-        <v>82</v>
+        <v>310</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B165" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C165" t="s">
         <v>6</v>
       </c>
       <c r="D165" t="s">
-        <v>203</v>
+        <v>59</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B166" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="C166" t="s">
         <v>6</v>
       </c>
       <c r="D166" t="s">
-        <v>270</v>
+        <v>81</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B167" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C167" t="s">
         <v>6</v>
       </c>
       <c r="D167" t="s">
-        <v>271</v>
+        <v>202</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>83</v>
+        <v>261</v>
       </c>
       <c r="B168" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="C168" t="s">
         <v>6</v>
       </c>
       <c r="D168" t="s">
-        <v>85</v>
+        <v>269</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>86</v>
+        <v>262</v>
       </c>
       <c r="B169" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C169" t="s">
         <v>6</v>
       </c>
       <c r="D169" t="s">
-        <v>71</v>
+        <v>270</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B170" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="C170" t="s">
         <v>6</v>
       </c>
       <c r="D170" t="s">
-        <v>527</v>
+        <v>84</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>530</v>
+        <v>85</v>
       </c>
       <c r="B171" t="s">
-        <v>531</v>
+        <v>33</v>
       </c>
       <c r="C171" t="s">
         <v>6</v>
       </c>
       <c r="D171" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>318</v>
+        <v>104</v>
       </c>
       <c r="B172" t="s">
-        <v>319</v>
+        <v>22</v>
       </c>
       <c r="C172" t="s">
         <v>6</v>
       </c>
       <c r="D172" t="s">
-        <v>516</v>
+        <v>526</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>513</v>
+        <v>529</v>
       </c>
       <c r="B173" t="s">
-        <v>514</v>
+        <v>530</v>
       </c>
       <c r="C173" t="s">
         <v>6</v>
       </c>
       <c r="D173" t="s">
-        <v>515</v>
+        <v>64</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B174" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C174" t="s">
         <v>6</v>
       </c>
       <c r="D174" t="s">
-        <v>322</v>
+        <v>515</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="B175" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="C175" t="s">
         <v>6</v>
       </c>
       <c r="D175" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>523</v>
+        <v>319</v>
       </c>
       <c r="B176" t="s">
-        <v>525</v>
+        <v>320</v>
       </c>
       <c r="C176" t="s">
         <v>6</v>
       </c>
       <c r="D176" t="s">
-        <v>526</v>
+        <v>321</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="B177" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="C177" t="s">
         <v>6</v>
       </c>
       <c r="D177" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>275</v>
+        <v>522</v>
       </c>
       <c r="B178" t="s">
-        <v>13</v>
+        <v>524</v>
       </c>
       <c r="C178" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D178" t="s">
-        <v>61</v>
+        <v>525</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>276</v>
+        <v>523</v>
       </c>
       <c r="B179" t="s">
-        <v>30</v>
+        <v>527</v>
       </c>
       <c r="C179" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D179" t="s">
-        <v>70</v>
+        <v>528</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B180" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C180" t="s">
         <v>14</v>
       </c>
       <c r="D180" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B181" t="s">
-        <v>324</v>
+        <v>30</v>
       </c>
       <c r="C181" t="s">
         <v>14</v>
       </c>
       <c r="D181" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>323</v>
+        <v>276</v>
       </c>
       <c r="B182" t="s">
-        <v>325</v>
+        <v>49</v>
       </c>
       <c r="C182" t="s">
         <v>14</v>
       </c>
       <c r="D182" t="s">
-        <v>326</v>
+        <v>76</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B183" t="s">
-        <v>54</v>
+        <v>323</v>
       </c>
       <c r="C183" t="s">
         <v>14</v>
       </c>
       <c r="D183" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>280</v>
+        <v>322</v>
       </c>
       <c r="B184" t="s">
-        <v>74</v>
+        <v>324</v>
       </c>
       <c r="C184" t="s">
         <v>14</v>
       </c>
       <c r="D184" t="s">
-        <v>75</v>
+        <v>325</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B185" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="C185" t="s">
         <v>14</v>
       </c>
       <c r="D185" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>328</v>
+        <v>279</v>
       </c>
       <c r="B186" t="s">
-        <v>329</v>
+        <v>73</v>
       </c>
       <c r="C186" t="s">
         <v>14</v>
       </c>
       <c r="D186" t="s">
-        <v>330</v>
+        <v>74</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B187" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C187" t="s">
         <v>14</v>
       </c>
       <c r="D187" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>283</v>
+        <v>327</v>
       </c>
       <c r="B188" t="s">
-        <v>110</v>
+        <v>328</v>
       </c>
       <c r="C188" t="s">
         <v>14</v>
       </c>
       <c r="D188" t="s">
-        <v>111</v>
+        <v>329</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>112</v>
+        <v>281</v>
       </c>
       <c r="B189" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C189" t="s">
         <v>14</v>
       </c>
       <c r="D189" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>116</v>
+        <v>282</v>
       </c>
       <c r="B190" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C190" t="s">
         <v>14</v>
       </c>
       <c r="D190" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B191" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C191" t="s">
         <v>14</v>
       </c>
       <c r="D191" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B192" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C192" t="s">
         <v>14</v>
       </c>
       <c r="D192" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B193" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="C193" t="s">
         <v>14</v>
       </c>
       <c r="D193" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>184</v>
+        <v>122</v>
       </c>
       <c r="B194" t="s">
-        <v>185</v>
+        <v>121</v>
       </c>
       <c r="C194" t="s">
         <v>14</v>
       </c>
       <c r="D194" t="s">
-        <v>186</v>
+        <v>120</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>377</v>
+        <v>123</v>
       </c>
       <c r="B195" t="s">
-        <v>378</v>
+        <v>40</v>
       </c>
       <c r="C195" t="s">
         <v>14</v>
       </c>
       <c r="D195" t="s">
-        <v>379</v>
+        <v>77</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>290</v>
+        <v>183</v>
       </c>
       <c r="B196" t="s">
-        <v>95</v>
+        <v>184</v>
       </c>
       <c r="C196" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="D196" t="s">
-        <v>104</v>
+        <v>185</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>291</v>
+        <v>376</v>
       </c>
       <c r="B197" t="s">
-        <v>94</v>
+        <v>377</v>
       </c>
       <c r="C197" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="D197" t="s">
-        <v>21</v>
+        <v>378</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B198" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C198" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D198" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B199" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C199" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D199" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B200" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C200" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D200" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B201" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="C201" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D201" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B202" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C202" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D202" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B203" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="C203" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D203" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B204" t="s">
-        <v>299</v>
+        <v>99</v>
       </c>
       <c r="C204" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D204" t="s">
-        <v>300</v>
+        <v>101</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B205" t="s">
-        <v>302</v>
+        <v>100</v>
       </c>
       <c r="C205" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D205" t="s">
-        <v>303</v>
+        <v>21</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>327</v>
+        <v>297</v>
       </c>
       <c r="B206" t="s">
-        <v>369</v>
+        <v>298</v>
       </c>
       <c r="C206" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D206" t="s">
-        <v>370</v>
+        <v>299</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B207" t="s">
-        <v>383</v>
+        <v>301</v>
       </c>
       <c r="C207" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D207" t="s">
-        <v>384</v>
+        <v>302</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>307</v>
+        <v>326</v>
       </c>
       <c r="B208" t="s">
-        <v>305</v>
+        <v>368</v>
       </c>
       <c r="C208" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D208" t="s">
-        <v>306</v>
+        <v>369</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>365</v>
+        <v>303</v>
       </c>
       <c r="B209" t="s">
-        <v>363</v>
+        <v>382</v>
       </c>
       <c r="C209" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="D209" t="s">
-        <v>364</v>
+        <v>383</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>365</v>
+        <v>306</v>
       </c>
       <c r="B210" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C210" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D210" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="B211" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="C211" t="s">
         <v>18</v>
       </c>
       <c r="D211" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>139</v>
+        <v>364</v>
       </c>
       <c r="B212" t="s">
-        <v>140</v>
+        <v>307</v>
       </c>
       <c r="C212" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="D212" t="s">
-        <v>142</v>
-      </c>
-      <c r="E212" t="s">
-        <v>143</v>
+        <v>308</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>144</v>
+        <v>379</v>
       </c>
       <c r="B213" t="s">
-        <v>145</v>
+        <v>380</v>
       </c>
       <c r="C213" t="s">
-        <v>141</v>
+        <v>18</v>
       </c>
       <c r="D213" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>400</v>
+        <v>138</v>
       </c>
       <c r="B214" t="s">
-        <v>401</v>
+        <v>139</v>
       </c>
       <c r="C214" t="s">
+        <v>140</v>
+      </c>
+      <c r="D214" t="s">
         <v>141</v>
       </c>
-      <c r="D214" t="s">
-        <v>402</v>
+      <c r="E214" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
       <c r="B215" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C215" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D215" t="s">
-        <v>206</v>
+        <v>398</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>247</v>
+        <v>399</v>
       </c>
       <c r="B216" t="s">
-        <v>248</v>
+        <v>400</v>
       </c>
       <c r="C216" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D216" t="s">
-        <v>249</v>
+        <v>401</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>250</v>
+        <v>203</v>
       </c>
       <c r="B217" t="s">
-        <v>251</v>
+        <v>204</v>
       </c>
       <c r="C217" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D217" t="s">
-        <v>252</v>
+        <v>205</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>484</v>
+        <v>246</v>
       </c>
       <c r="B218" t="s">
-        <v>478</v>
+        <v>247</v>
       </c>
       <c r="C218" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D218" t="s">
-        <v>479</v>
+        <v>248</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>480</v>
+        <v>249</v>
       </c>
       <c r="B219" t="s">
-        <v>481</v>
+        <v>250</v>
       </c>
       <c r="C219" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D219" t="s">
-        <v>485</v>
+        <v>251</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B220" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="C220" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D220" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>272</v>
+        <v>479</v>
       </c>
       <c r="B221" t="s">
-        <v>273</v>
+        <v>480</v>
       </c>
       <c r="C221" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D221" t="s">
-        <v>274</v>
+        <v>484</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
+        <v>481</v>
+      </c>
+      <c r="B222" t="s">
+        <v>482</v>
+      </c>
+      <c r="C222" t="s">
+        <v>140</v>
+      </c>
+      <c r="D222" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>271</v>
+      </c>
+      <c r="B223" t="s">
+        <v>272</v>
+      </c>
+      <c r="C223" t="s">
+        <v>140</v>
+      </c>
+      <c r="D223" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>494</v>
+      </c>
+      <c r="B224" t="s">
         <v>495</v>
       </c>
-      <c r="B222" t="s">
+      <c r="C224" t="s">
+        <v>140</v>
+      </c>
+      <c r="D224" t="s">
         <v>496</v>
-      </c>
-      <c r="C222" t="s">
-        <v>141</v>
-      </c>
-      <c r="D222" t="s">
-        <v>497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding values to the derived variables, in progress
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B363AF-9694-B64E-B9D9-6D7DCF8A1120}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC341A4-C3B5-4442-8AB1-85156C80F4A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35860" yWindow="2900" windowWidth="35840" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-47660" yWindow="2900" windowWidth="47640" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="691">
   <si>
     <t>Variable #</t>
   </si>
@@ -2066,19 +2066,58 @@
   </si>
   <si>
     <t>0-No; 1-Yes; 99-Unknown</t>
+  </si>
+  <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>Years (continuous 18-89; patients noted to be greater than 89 are set to be age = 90)</t>
+  </si>
+  <si>
+    <t>Normal; High; Low; Not drawn/Not available; Unknown</t>
+  </si>
+  <si>
+    <t>0 = No; 1 = Yes; 99 = Unknown</t>
+  </si>
+  <si>
+    <t>Never; Current or Former; Unknown</t>
+  </si>
+  <si>
+    <t>0; 1; 2+; Unknown</t>
+  </si>
+  <si>
+    <t>Non-US; Other; Undesignated US; US Midwest; US Northeast; US South; US West</t>
+  </si>
+  <si>
+    <t>D14b</t>
+  </si>
+  <si>
+    <t>region_v3</t>
+  </si>
+  <si>
+    <t>Region of patient residence with US and ex-US collapsed</t>
+  </si>
+  <si>
+    <t>Non-US; Other; US</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2101,13 +2140,99 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2121,17 +2246,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E224" totalsRowShown="0">
-  <autoFilter ref="A1:E224" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E224">
-    <sortCondition ref="A1:A224"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E225" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:E225" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E225">
+    <sortCondition ref="A1:A225"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #"/>
-    <tableColumn id="2" xr3:uid="{9AFC5F6C-2B2C-E541-A77F-830B0EABC78C}" name="Variable Name (der_name)"/>
-    <tableColumn id="3" xr3:uid="{800F9FDD-F033-7A4B-A634-744A5D9FEFE2}" name="Category"/>
-    <tableColumn id="4" xr3:uid="{827F03E0-E9CB-BF47-915C-D34395E5A6F4}" name="Description"/>
-    <tableColumn id="5" xr3:uid="{F9BBFA6E-9630-224E-B86A-31602DCDBEE5}" name="Values"/>
+    <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9AFC5F6C-2B2C-E541-A77F-830B0EABC78C}" name="Variable Name (der_name)" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{800F9FDD-F033-7A4B-A634-744A5D9FEFE2}" name="Category" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{827F03E0-E9CB-BF47-915C-D34395E5A6F4}" name="Description" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{F9BBFA6E-9630-224E-B86A-31602DCDBEE5}" name="Values" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2458,10 +2583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E224"/>
+  <dimension ref="A1:E225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2470,7 +2595,7 @@
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="48.83203125" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -2491,3066 +2616,3370 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>331</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>396</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>395</v>
       </c>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>567</v>
       </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>193</v>
       </c>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>677</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="E12" s="1" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="E25" s="1" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="E34" s="1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="E35" s="1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="E36" s="1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="E37" s="1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="1" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="1" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="1" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="1" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="1" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="1" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="1" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="1" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="1" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="1" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="1" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="1" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="1" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="1" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="1" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>583</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="1" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="1" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="1" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="1" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="1" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="1" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="1" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="1" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="1" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="1" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="E79" s="1"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="1" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="E80" s="1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="1" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="E81" s="1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="1" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="E82" s="1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="1" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="1" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="1" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="1" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="1" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="1" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="1" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="1" t="s">
         <v>637</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="1" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="1" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="1" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="1" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>649</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="1" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="1" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
         <v>655</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="1" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="1" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="E97" s="1"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="1" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+      <c r="E98" s="1"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="1" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="E99" s="1"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="1" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="E100" s="1"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="E101" s="1" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="E102" s="1"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="E103" s="1"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="E104" s="1" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="E105" s="1"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="E106" s="1"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="E108" s="1"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+      <c r="E109" s="1"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="E110" s="1" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D112" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="E112" s="1"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C113" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D113" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="E113" s="1"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D114" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="E114" s="1"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C115" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D115" s="1" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C116" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D116" s="1" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="E116" s="1"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B117" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C117" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D117" s="1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="E117" s="1"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B118" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C118" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D118" s="1" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+      <c r="E118" s="1"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B119" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C119" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D119" s="1" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+      <c r="E119" s="1"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B120" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C120" s="1" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B121" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C121" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D121" s="1" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+      <c r="E121" s="1"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B122" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C122" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D122" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+      <c r="E122" s="1"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C123" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D123" s="1" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+      <c r="E123" s="1"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B124" s="1" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B125" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="D124" t="s">
+      <c r="C125" s="1"/>
+      <c r="D125" s="1" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+      <c r="E125" s="1"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B126" s="1" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B127" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="D126" t="s">
+      <c r="C127" s="1"/>
+      <c r="D127" s="1" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
+      <c r="E127" s="1"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B128" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="D127" t="s">
+      <c r="C128" s="1"/>
+      <c r="D128" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+      <c r="E128" s="1"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B129" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="D128" t="s">
+      <c r="C129" s="1"/>
+      <c r="D129" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+      <c r="E129" s="1"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B130" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="D129" t="s">
+      <c r="C130" s="1"/>
+      <c r="D130" s="1" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+      <c r="E130" s="1"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B131" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="D130" t="s">
+      <c r="C131" s="1"/>
+      <c r="D131" s="1" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="E131" s="1"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B132" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="D131" t="s">
+      <c r="C132" s="1"/>
+      <c r="D132" s="1" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+      <c r="E132" s="1"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B133" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="D132" t="s">
+      <c r="C133" s="1"/>
+      <c r="D133" s="1" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
+      <c r="E133" s="1"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B134" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="D133" t="s">
+      <c r="C134" s="1"/>
+      <c r="D134" s="1" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+      <c r="E134" s="1"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B135" s="1" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B136" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="D135" t="s">
+      <c r="C136" s="1"/>
+      <c r="D136" s="1" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+      <c r="E136" s="1"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B137" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D136" t="s">
+      <c r="C137" s="1"/>
+      <c r="D137" s="1" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
+      <c r="E137" s="1"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B138" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="D137" t="s">
+      <c r="C138" s="1"/>
+      <c r="D138" s="1" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+      <c r="E138" s="1"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B139" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D138" t="s">
+      <c r="C139" s="1"/>
+      <c r="D139" s="1" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
+      <c r="E139" s="1"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
         <v>670</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B140" s="1" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B141" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C141" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D141" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+      <c r="E141" s="1"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B142" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C142" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D142" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+      <c r="E142" s="1"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B143" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C143" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D143" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+      <c r="E143" s="1"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B144" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C144" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D144" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
+      <c r="E144" s="1"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B145" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C145" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D145" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+      <c r="E145" s="1"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B146" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C146" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D146" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+      <c r="E146" s="1"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B147" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C147" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D147" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+      <c r="E147" s="1"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B148" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C148" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D148" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="E148" s="1"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B149" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C149" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D149" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="E149" s="1"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B150" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C150" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D150" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="E150" s="1"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B151" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C151" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D151" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+      <c r="E151" s="1"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B152" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C152" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D152" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+      <c r="E152" s="1" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B153" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C153" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D153" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+      <c r="E153" s="1"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B154" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C154" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D154" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+      <c r="E154" s="1" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B155" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C155" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D155" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
+      <c r="E155" s="1" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B156" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C156" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D156" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
+      <c r="E156" s="1" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B157" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C157" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D157" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+      <c r="E157" s="1"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B158" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C158" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D158" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+      <c r="E158" s="1"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B159" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C159" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D159" s="1" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+      <c r="E159" s="1"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B160" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C160" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D160" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
+      <c r="E160" s="1"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B161" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C161" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D161" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
+      <c r="E161" s="1"/>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B162" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C162" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D162" s="1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
+      <c r="E162" s="1"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B163" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C163" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D163" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
+      <c r="E163" s="1"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B164" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C164" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D164" s="1" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
+      <c r="E164" s="1"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B165" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C165" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D165" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
+      <c r="E165" s="1"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B166" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C166" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D166" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
+      <c r="E166" s="1"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B167" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C167" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D167" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
+      <c r="E167" s="1"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B168" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C168" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D168" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
+      <c r="E168" s="1"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B169" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C169" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D169" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
+      <c r="E169" s="1"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B170" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C170" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D170" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
+      <c r="E170" s="1"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B171" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C171" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D171" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
+      <c r="E171" s="1"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B172" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C172" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D172" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
+      <c r="E172" s="1"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B173" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C173" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D173" s="1" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
+      <c r="E173" s="1"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B174" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C174" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D174" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A174" t="s">
+      <c r="E174" s="1"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B175" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C175" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D175" s="1" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
+      <c r="E175" s="1"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B176" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C176" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D176" s="1" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
+      <c r="E176" s="1"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B177" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C177" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D177" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
+      <c r="E177" s="1"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B178" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C178" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D178" s="1" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
+      <c r="E178" s="1"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B179" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C179" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D179" s="1" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
+      <c r="E179" s="1"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B180" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C180" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D180" s="1" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
+      <c r="E180" s="1"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B181" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C181" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D181" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
+      <c r="E181" s="1"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B182" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C182" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D182" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
+      <c r="E182" s="1"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B183" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C183" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D183" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
+      <c r="E183" s="1"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B184" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C184" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D184" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
+      <c r="E184" s="1"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B185" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C185" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D185" s="1" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A185" t="s">
+      <c r="E185" s="1"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B186" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C186" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D186" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A186" t="s">
+      <c r="E186" s="1"/>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B187" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C187" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D187" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
+      <c r="E187" s="1"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B188" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C188" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D188" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
+      <c r="E188" s="1"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B189" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C189" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D189" s="1" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
+      <c r="E189" s="1"/>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B190" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C190" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D190" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A190" t="s">
+      <c r="E190" s="1"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B191" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C191" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D191" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A191" t="s">
+      <c r="E191" s="1"/>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B192" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C192" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D192" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A192" t="s">
+      <c r="E192" s="1"/>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B193" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C193" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D193" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A193" t="s">
+      <c r="E193" s="1"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B194" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C194" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D194" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A194" t="s">
+      <c r="E194" s="1"/>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B195" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C195" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D195" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A195" t="s">
+      <c r="E195" s="1"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B196" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C196" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D196" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
+      <c r="E196" s="1"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B197" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C197" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D197" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A197" t="s">
+      <c r="E197" s="1"/>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B198" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C198" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D198" s="1" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A198" t="s">
+      <c r="E198" s="1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B199" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C199" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D199" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A199" t="s">
+      <c r="E199" s="1"/>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B200" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C200" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D200" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A200" t="s">
+      <c r="E200" s="1"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B201" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C201" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D201" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A201" t="s">
+      <c r="E201" s="1"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B202" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C202" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D202" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A202" t="s">
+      <c r="E202" s="1"/>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B203" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C203" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D203" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
+      <c r="E203" s="1"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B204" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C204" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D204" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
+      <c r="E204" s="1"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B205" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C205" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D205" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A205" t="s">
+      <c r="E205" s="1"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B206" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C206" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D206" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A206" t="s">
+      <c r="E206" s="1"/>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B207" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C207" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D207" s="1" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A207" t="s">
+      <c r="E207" s="1"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B208" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C208" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D208" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
+      <c r="E208" s="1"/>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B209" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C209" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D209" s="1" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A209" t="s">
+      <c r="E209" s="1"/>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B210" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C210" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D210" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A210" t="s">
+      <c r="E210" s="1"/>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B211" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C211" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D211" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A211" t="s">
+      <c r="E211" s="1"/>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B212" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C212" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D212" s="1" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A212" t="s">
+      <c r="E212" s="1"/>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B213" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C213" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D213" s="1" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
+      <c r="E213" s="1"/>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B214" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C214" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D214" s="1" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
+      <c r="E214" s="1"/>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B215" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C215" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D214" t="s">
+      <c r="D215" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E214" t="s">
+      <c r="E215" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A215" t="s">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B216" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C216" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D216" s="1" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
+      <c r="E216" s="1"/>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B217" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C217" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D217" s="1" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A217" t="s">
+      <c r="E217" s="1"/>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B218" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C218" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D218" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
+      <c r="E218" s="1"/>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B219" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C219" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D219" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A219" t="s">
+      <c r="E219" s="1"/>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B220" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C220" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D220" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A220" t="s">
+      <c r="E220" s="1"/>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B221" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C221" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D220" t="s">
+      <c r="D221" s="1" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A221" t="s">
+      <c r="E221" s="1"/>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B222" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C222" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D222" s="1" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A222" t="s">
+      <c r="E222" s="1"/>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B223" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="C222" t="s">
+      <c r="C223" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D223" s="1" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A223" t="s">
+      <c r="E223" s="1"/>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B224" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C224" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D224" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A224" t="s">
+      <c r="E224" s="1"/>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B225" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C225" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D225" s="1" t="s">
         <v>496</v>
       </c>
+      <c r="E225" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New combined sepsis variable, minor fixes
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC341A4-C3B5-4442-8AB1-85156C80F4A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBE0EC7-D971-DC4A-B2FB-BEB6858380DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47660" yWindow="2900" windowWidth="47640" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2920" windowWidth="47640" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="690">
   <si>
     <t>Variable #</t>
   </si>
@@ -2063,9 +2063,6 @@
   </si>
   <si>
     <t>Values</t>
-  </si>
-  <si>
-    <t>0-No; 1-Yes; 99-Unknown</t>
   </si>
   <si>
     <t>Continuous</t>
@@ -2246,17 +2243,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E225" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E225" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A1:E225" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E225">
     <sortCondition ref="A1:A225"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{9AFC5F6C-2B2C-E541-A77F-830B0EABC78C}" name="Variable Name (der_name)" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{800F9FDD-F033-7A4B-A634-744A5D9FEFE2}" name="Category" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{827F03E0-E9CB-BF47-915C-D34395E5A6F4}" name="Description" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{F9BBFA6E-9630-224E-B86A-31602DCDBEE5}" name="Values" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{9AFC5F6C-2B2C-E541-A77F-830B0EABC78C}" name="Variable Name (der_name)" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{800F9FDD-F033-7A4B-A634-744A5D9FEFE2}" name="Category" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{827F03E0-E9CB-BF47-915C-D34395E5A6F4}" name="Description" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{F9BBFA6E-9630-224E-B86A-31602DCDBEE5}" name="Values" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2585,8 +2582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2629,7 +2626,7 @@
         <v>331</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2646,7 +2643,7 @@
         <v>396</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2738,7 +2735,7 @@
         <v>66</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2755,7 +2752,7 @@
         <v>67</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2772,7 +2769,7 @@
         <v>677</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2789,7 +2786,7 @@
         <v>68</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2821,7 +2818,7 @@
         <v>55</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2838,7 +2835,7 @@
         <v>133</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2990,7 +2987,7 @@
         <v>72</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -3127,7 +3124,7 @@
         <v>558</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -3144,7 +3141,7 @@
         <v>559</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -3161,7 +3158,7 @@
         <v>560</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -3178,7 +3175,7 @@
         <v>561</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -3825,7 +3822,7 @@
         <v>608</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -3842,7 +3839,7 @@
         <v>611</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -3859,7 +3856,7 @@
         <v>614</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -4146,7 +4143,7 @@
         <v>45</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -4193,7 +4190,7 @@
         <v>135</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -4283,24 +4280,24 @@
         <v>316</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>687</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>688</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="E111" s="1" t="s">
         <v>689</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -4873,7 +4870,7 @@
         <v>221</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -4905,7 +4902,7 @@
         <v>227</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -4922,7 +4919,7 @@
         <v>230</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -4939,7 +4936,7 @@
         <v>233</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -5571,7 +5568,7 @@
         <v>378</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Housekeeping, two treatment variables added
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B0896A-DAB6-0940-9935-B14FD2271B41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EDDC96-8A51-BE42-87AC-955E4065F8E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-47980" yWindow="2280" windowWidth="47640" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="726">
   <si>
     <t>Variable #</t>
   </si>
@@ -2186,6 +2186,24 @@
   </si>
   <si>
     <t>Most recent line of therapy includes anti-CD20 antibody</t>
+  </si>
+  <si>
+    <t>Ca04b</t>
+  </si>
+  <si>
+    <t>Ca04c</t>
+  </si>
+  <si>
+    <t>btki</t>
+  </si>
+  <si>
+    <t>venet</t>
+  </si>
+  <si>
+    <t>Most recent line of therapy includes BTK inhibitor</t>
+  </si>
+  <si>
+    <t>Most recent line of therapy includes venetoclax</t>
   </si>
 </sst>
 </file>
@@ -2333,10 +2351,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E231" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E231" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E230">
-    <sortCondition ref="A1:A230"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E233" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E233" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E232">
+    <sortCondition ref="A1:A232"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #" dataDxfId="4"/>
@@ -2670,10 +2688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E231"/>
+  <dimension ref="A1:E233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3130,150 +3148,150 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>285</v>
+        <v>720</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>8</v>
+        <v>722</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>5</v>
+        <v>530</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>724</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>364</v>
+        <v>721</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>136</v>
+        <v>723</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>18</v>
+        <v>530</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>64</v>
+        <v>725</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>386</v>
+        <v>285</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>365</v>
+        <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>704</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>492</v>
+        <v>364</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>387</v>
+        <v>136</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>388</v>
+        <v>64</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>286</v>
+        <v>386</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>144</v>
+        <v>365</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>146</v>
+        <v>366</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>287</v>
+        <v>492</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>145</v>
+        <v>387</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>147</v>
+        <v>388</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>155</v>
+        <v>286</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>556</v>
+        <v>146</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>681</v>
+        <v>707</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>193</v>
+        <v>287</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>194</v>
+        <v>145</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>530</v>
+        <v>18</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>557</v>
+        <v>147</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>681</v>
+        <v>707</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>355</v>
+        <v>159</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>530</v>
+        <v>18</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>681</v>
@@ -3281,16 +3299,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>356</v>
+        <v>194</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>681</v>
@@ -3298,16 +3316,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>351</v>
+        <v>195</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>681</v>
@@ -3315,16 +3333,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>352</v>
+        <v>198</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>681</v>
@@ -3332,16 +3350,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>681</v>
@@ -3349,16 +3367,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>681</v>
@@ -3366,16 +3384,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>196</v>
+        <v>359</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>197</v>
+        <v>562</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>681</v>
@@ -3383,16 +3401,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>199</v>
+        <v>360</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>200</v>
+        <v>563</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>681</v>
@@ -3400,16 +3418,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>372</v>
+        <v>349</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>373</v>
+        <v>196</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>374</v>
+        <v>197</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>681</v>
@@ -3417,16 +3435,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>553</v>
+        <v>350</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>554</v>
+        <v>199</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>555</v>
+        <v>200</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>681</v>
@@ -3434,16 +3452,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>671</v>
+        <v>372</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>673</v>
+        <v>373</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>672</v>
+        <v>374</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>681</v>
@@ -3451,581 +3469,581 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>187</v>
+        <v>553</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>188</v>
+        <v>554</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>18</v>
+        <v>530</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>403</v>
+        <v>555</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>692</v>
+        <v>681</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>689</v>
+        <v>671</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>690</v>
+        <v>673</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>18</v>
+        <v>530</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>691</v>
+        <v>672</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>692</v>
+        <v>681</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>530</v>
+        <v>18</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E49" s="1"/>
+        <v>403</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>209</v>
+        <v>689</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>210</v>
+        <v>690</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>530</v>
+        <v>18</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E50" s="1"/>
+        <v>691</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>496</v>
+        <v>206</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>497</v>
+        <v>207</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>498</v>
+        <v>208</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>501</v>
+        <v>209</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>499</v>
+        <v>210</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>500</v>
+        <v>211</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>18</v>
+        <v>530</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>531</v>
+        <v>508</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>532</v>
+        <v>509</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>18</v>
+        <v>530</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>533</v>
+        <v>510</v>
       </c>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>534</v>
+        <v>515</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>535</v>
+        <v>516</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>536</v>
+        <v>517</v>
       </c>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>570</v>
+        <v>531</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>571</v>
+        <v>532</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>530</v>
+        <v>18</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>706</v>
-      </c>
+        <v>533</v>
+      </c>
+      <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>573</v>
+        <v>534</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>85</v>
+        <v>535</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>91</v>
+        <v>536</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>537</v>
+        <v>571</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>33</v>
+        <v>530</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="E61" s="1"/>
+        <v>572</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>87</v>
+        <v>537</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>89</v>
+        <v>538</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>539</v>
+        <v>86</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>540</v>
+        <v>90</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>541</v>
+        <v>87</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>148</v>
+        <v>541</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>149</v>
+        <v>88</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>401</v>
+        <v>542</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>402</v>
+        <v>543</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>544</v>
+        <v>148</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>545</v>
+        <v>149</v>
       </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>150</v>
+        <v>401</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>151</v>
+        <v>402</v>
       </c>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>389</v>
+        <v>150</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>390</v>
+        <v>151</v>
       </c>
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E73" s="1"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>36</v>
+        <v>389</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>638</v>
+        <v>390</v>
       </c>
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>262</v>
+        <v>548</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>263</v>
+        <v>549</v>
       </c>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>51</v>
+        <v>638</v>
       </c>
       <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>591</v>
+        <v>262</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>592</v>
+        <v>263</v>
       </c>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>594</v>
+        <v>50</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>595</v>
+        <v>51</v>
       </c>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>681</v>
-      </c>
+        <v>601</v>
+      </c>
+      <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>681</v>
-      </c>
+        <v>604</v>
+      </c>
+      <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>681</v>
@@ -4033,16 +4051,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>681</v>
@@ -4050,16 +4068,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>681</v>
@@ -4067,16 +4085,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>681</v>
@@ -4084,16 +4102,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>681</v>
@@ -4101,16 +4119,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>681</v>
@@ -4118,16 +4136,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>681</v>
@@ -4135,16 +4153,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>681</v>
@@ -4152,16 +4170,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>681</v>
@@ -4169,16 +4187,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>681</v>
@@ -4186,16 +4204,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>681</v>
@@ -4203,16 +4221,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>681</v>
@@ -4220,16 +4238,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>681</v>
@@ -4237,16 +4255,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>681</v>
@@ -4254,16 +4272,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>681</v>
@@ -4271,16 +4289,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>681</v>
@@ -4288,16 +4306,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>681</v>
@@ -4305,16 +4323,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>681</v>
@@ -4322,16 +4340,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>681</v>
@@ -4339,16 +4357,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>708</v>
+        <v>663</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>709</v>
+        <v>664</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>713</v>
+        <v>665</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>681</v>
@@ -4356,16 +4374,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>710</v>
+        <v>666</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>711</v>
+        <v>667</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>712</v>
+        <v>668</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>681</v>
@@ -4373,16 +4391,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>681</v>
@@ -4390,385 +4408,395 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>264</v>
+        <v>710</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>123</v>
+        <v>711</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>44</v>
+        <v>712</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>265</v>
+        <v>714</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>42</v>
+        <v>715</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E107" s="1"/>
+        <v>716</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>489</v>
+        <v>264</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>135</v>
+        <v>44</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>697</v>
+        <v>679</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>490</v>
+        <v>265</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>682</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E109" s="1"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>266</v>
+        <v>489</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>17</v>
+        <v>124</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E110" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>189</v>
+        <v>133</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E111" s="1"/>
+        <v>134</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>485</v>
+        <v>266</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>486</v>
+        <v>17</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D112" s="1"/>
+      <c r="D112" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>267</v>
+        <v>491</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>20</v>
+        <v>189</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>62</v>
+        <v>190</v>
       </c>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>127</v>
+        <v>485</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>3</v>
+        <v>486</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D114" s="1"/>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>313</v>
+        <v>267</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>314</v>
+        <v>20</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>684</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E115" s="1"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>685</v>
+        <v>127</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>686</v>
+        <v>3</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>688</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E116" s="1"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>128</v>
+        <v>313</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>129</v>
+        <v>314</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E117" s="1"/>
+        <v>315</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>156</v>
+        <v>685</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>157</v>
+        <v>686</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E118" s="1"/>
+        <v>687</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>180</v>
+        <v>129</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
       <c r="E119" s="1"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>404</v>
+        <v>156</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>405</v>
+        <v>157</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>406</v>
+        <v>15</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>472</v>
+        <v>158</v>
       </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>407</v>
+        <v>179</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>408</v>
+        <v>180</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>406</v>
+        <v>5</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>409</v>
+        <v>181</v>
       </c>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>412</v>
+        <v>472</v>
       </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D125" s="1"/>
+      <c r="D125" s="1" t="s">
+        <v>415</v>
+      </c>
       <c r="E125" s="1"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D127" s="1" t="s">
-        <v>426</v>
-      </c>
+      <c r="D127" s="1"/>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C129" s="1"/>
-      <c r="D129" s="1"/>
+        <v>425</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>426</v>
+      </c>
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C130" s="1"/>
+        <v>428</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>406</v>
+      </c>
       <c r="D130" s="1" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="E130" s="1"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
@@ -4776,333 +4804,325 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="C132" s="1"/>
       <c r="D132" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E132" s="1"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="C133" s="1"/>
-      <c r="D133" s="1" t="s">
-        <v>442</v>
-      </c>
+      <c r="D133" s="1"/>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C134" s="1"/>
       <c r="D134" s="1" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="E134" s="1"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="E135" s="1"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="E136" s="1"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="E137" s="1"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="C140" s="1"/>
-      <c r="D140" s="1"/>
+      <c r="D140" s="1" t="s">
+        <v>457</v>
+      </c>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C142" s="1"/>
-      <c r="D142" s="1" t="s">
-        <v>467</v>
-      </c>
+      <c r="D142" s="1"/>
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="E143" s="1"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="E144" s="1"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>669</v>
+        <v>474</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>670</v>
+        <v>468</v>
       </c>
       <c r="C145" s="1"/>
-      <c r="D145" s="1"/>
+      <c r="D145" s="1" t="s">
+        <v>469</v>
+      </c>
       <c r="E145" s="1"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>233</v>
+        <v>475</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>153</v>
-      </c>
+        <v>470</v>
+      </c>
+      <c r="C146" s="1"/>
       <c r="D146" s="1" t="s">
-        <v>154</v>
+        <v>471</v>
       </c>
       <c r="E146" s="1"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>234</v>
+        <v>669</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>696</v>
-      </c>
+        <v>670</v>
+      </c>
+      <c r="C147" s="1"/>
+      <c r="D147" s="1"/>
+      <c r="E147" s="1"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E148" s="1"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E149" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E150" s="1"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E151" s="1"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E152" s="1"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>696</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="E153" s="1"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E154" s="1"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>696</v>
@@ -5110,65 +5130,65 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>216</v>
+        <v>174</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>696</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="E156" s="1"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>218</v>
+        <v>176</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>219</v>
+        <v>177</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>220</v>
+        <v>178</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>680</v>
+        <v>696</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E158" s="1"/>
+        <v>217</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>680</v>
@@ -5176,33 +5196,31 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>680</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="E160" s="1"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>680</v>
@@ -5210,1057 +5228,1091 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E162" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E163" s="1"/>
+        <v>232</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>369</v>
+        <v>215</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>370</v>
+        <v>213</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>371</v>
+        <v>214</v>
       </c>
       <c r="E164" s="1"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>4</v>
+        <v>243</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>55</v>
+        <v>244</v>
       </c>
       <c r="E165" s="1"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>254</v>
+        <v>369</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>11</v>
+        <v>370</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>56</v>
+        <v>371</v>
       </c>
       <c r="E166" s="1"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>310</v>
+        <v>253</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>311</v>
+        <v>4</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>312</v>
+        <v>55</v>
       </c>
       <c r="E167" s="1"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E168" s="1"/>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>550</v>
+        <v>310</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>551</v>
+        <v>311</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>552</v>
+        <v>312</v>
       </c>
       <c r="E169" s="1"/>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>308</v>
+        <v>10</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>309</v>
+        <v>57</v>
       </c>
       <c r="E170" s="1"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>257</v>
+        <v>550</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>12</v>
+        <v>551</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>58</v>
+        <v>552</v>
       </c>
       <c r="E171" s="1"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>79</v>
+        <v>308</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>80</v>
+        <v>309</v>
       </c>
       <c r="E172" s="1"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>201</v>
+        <v>58</v>
       </c>
       <c r="E173" s="1"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>268</v>
+        <v>80</v>
       </c>
       <c r="E174" s="1"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>269</v>
+        <v>201</v>
       </c>
       <c r="E175" s="1"/>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>81</v>
+        <v>260</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>83</v>
+        <v>268</v>
       </c>
       <c r="E176" s="1"/>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>84</v>
+        <v>261</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>69</v>
+        <v>269</v>
       </c>
       <c r="E177" s="1"/>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>525</v>
+        <v>83</v>
       </c>
       <c r="E178" s="1"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>528</v>
+        <v>84</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>529</v>
+        <v>32</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E179" s="1"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>316</v>
+        <v>103</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>317</v>
+        <v>22</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>514</v>
+        <v>525</v>
       </c>
       <c r="E180" s="1"/>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>511</v>
+        <v>528</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>512</v>
+        <v>529</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>513</v>
+        <v>63</v>
       </c>
       <c r="E181" s="1"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>320</v>
+        <v>514</v>
       </c>
       <c r="E182" s="1"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="E183" s="1"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>521</v>
+        <v>318</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>523</v>
+        <v>319</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>524</v>
+        <v>320</v>
       </c>
       <c r="E184" s="1"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="E185" s="1"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>273</v>
+        <v>521</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>13</v>
+        <v>523</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>59</v>
+        <v>524</v>
       </c>
       <c r="E186" s="1"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>274</v>
+        <v>522</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>29</v>
+        <v>526</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>68</v>
+        <v>527</v>
       </c>
       <c r="E187" s="1"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E188" s="1"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>322</v>
+        <v>29</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="E189" s="1"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>321</v>
+        <v>275</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>323</v>
+        <v>48</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>324</v>
+        <v>75</v>
       </c>
       <c r="E190" s="1"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>52</v>
+        <v>322</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="E191" s="1"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>278</v>
+        <v>321</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>72</v>
+        <v>323</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>73</v>
+        <v>324</v>
       </c>
       <c r="E192" s="1"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>105</v>
+        <v>52</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E193" s="1"/>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>326</v>
+        <v>278</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>327</v>
+        <v>72</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>328</v>
+        <v>73</v>
       </c>
       <c r="E194" s="1"/>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="E195" s="1"/>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>281</v>
+        <v>326</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>108</v>
+        <v>327</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>109</v>
+        <v>328</v>
       </c>
       <c r="E196" s="1"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>110</v>
+        <v>280</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E197" s="1"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>114</v>
+        <v>281</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E198" s="1"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E199" s="1"/>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E200" s="1"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="E201" s="1"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>182</v>
+        <v>121</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>183</v>
+        <v>120</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>184</v>
+        <v>119</v>
       </c>
       <c r="E202" s="1"/>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>375</v>
+        <v>122</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>376</v>
+        <v>39</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="E203" s="1" t="s">
-        <v>681</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E203" s="1"/>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>288</v>
+        <v>182</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>93</v>
+        <v>183</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>102</v>
+        <v>184</v>
       </c>
       <c r="E204" s="1"/>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>289</v>
+        <v>375</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>92</v>
+        <v>376</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E205" s="1"/>
+        <v>377</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="E206" s="1"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>101</v>
+        <v>21</v>
       </c>
       <c r="E207" s="1"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E208" s="1"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="E209" s="1"/>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="E210" s="1"/>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E211" s="1"/>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>297</v>
+        <v>98</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>298</v>
+        <v>100</v>
       </c>
       <c r="E212" s="1"/>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>300</v>
+        <v>99</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>301</v>
+        <v>21</v>
       </c>
       <c r="E213" s="1"/>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>325</v>
+        <v>296</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>367</v>
+        <v>297</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>368</v>
+        <v>298</v>
       </c>
       <c r="E214" s="1"/>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>381</v>
+        <v>300</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>382</v>
+        <v>301</v>
       </c>
       <c r="E215" s="1"/>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>303</v>
+        <v>367</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>304</v>
+        <v>368</v>
       </c>
       <c r="E216" s="1"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>363</v>
+        <v>302</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>361</v>
+        <v>381</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>362</v>
+        <v>382</v>
       </c>
       <c r="E217" s="1"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E218" s="1"/>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="E219" s="1"/>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>137</v>
+        <v>363</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>138</v>
+        <v>306</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>139</v>
+        <v>94</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>141</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="E220" s="1"/>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>142</v>
+        <v>378</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>143</v>
+        <v>379</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
       <c r="E221" s="1"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>398</v>
+        <v>137</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>399</v>
+        <v>138</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="E222" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>202</v>
+        <v>142</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>204</v>
+        <v>397</v>
       </c>
       <c r="E223" s="1"/>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>245</v>
+        <v>398</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>246</v>
+        <v>399</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>247</v>
+        <v>400</v>
       </c>
       <c r="E224" s="1"/>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>248</v>
+        <v>202</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>249</v>
+        <v>203</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>250</v>
+        <v>204</v>
       </c>
       <c r="E225" s="1"/>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>482</v>
+        <v>245</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>476</v>
+        <v>246</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>477</v>
+        <v>247</v>
       </c>
       <c r="E226" s="1"/>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>478</v>
+        <v>248</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>479</v>
+        <v>249</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>483</v>
+        <v>250</v>
       </c>
       <c r="E227" s="1"/>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="E228" s="1"/>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>270</v>
+        <v>478</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>271</v>
+        <v>479</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>272</v>
+        <v>483</v>
       </c>
       <c r="E229" s="1"/>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="E230" s="1"/>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>693</v>
+        <v>270</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>694</v>
+        <v>271</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D231" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E231" s="1"/>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="E232" s="1"/>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A233" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D233" s="1" t="s">
         <v>695</v>
       </c>
-      <c r="E231" s="1" t="s">
+      <c r="E233" s="1" t="s">
         <v>681</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Gram pos and neg bacteria derived variables
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9A6B8B-29AD-DC40-9DCA-131FDC7B7321}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942204D7-254D-0949-B0AA-7D13703EF2F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="4060" windowWidth="47640" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="735">
   <si>
     <t>Variable #</t>
   </si>
@@ -2213,6 +2213,24 @@
   </si>
   <si>
     <t>Chronic lymphocytic leukemia</t>
+  </si>
+  <si>
+    <t>Comp38a</t>
+  </si>
+  <si>
+    <t>coinfection_bact_gram_pos</t>
+  </si>
+  <si>
+    <t>Coinfection with Gram positive bacteria</t>
+  </si>
+  <si>
+    <t>Comp38b</t>
+  </si>
+  <si>
+    <t>coinfection_bact_gram_neg</t>
+  </si>
+  <si>
+    <t>Coinfection with Gram negative bacteria</t>
   </si>
 </sst>
 </file>
@@ -2360,8 +2378,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E234" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E234" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E236" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E236" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E233">
     <sortCondition ref="A1:A233"/>
   </sortState>
@@ -2697,10 +2715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E234"/>
+  <dimension ref="A1:E236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D148" sqref="D148"/>
+    <sheetView tabSelected="1" topLeftCell="A220" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A236" sqref="A236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6338,6 +6356,40 @@
         <v>681</v>
       </c>
     </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A235" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>681</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Categorical age variable added
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942204D7-254D-0949-B0AA-7D13703EF2F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1206E07-3014-6548-902B-DF4BD395194A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="4060" windowWidth="47640" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="739">
   <si>
     <t>Variable #</t>
   </si>
@@ -2231,6 +2231,18 @@
   </si>
   <si>
     <t>Coinfection with Gram negative bacteria</t>
+  </si>
+  <si>
+    <t>D01a</t>
+  </si>
+  <si>
+    <t>age_cat</t>
+  </si>
+  <si>
+    <t>Categorical age variable</t>
+  </si>
+  <si>
+    <t>18-39 years; 40-59 years; 60-69 years; 70-79 years; 80+ years</t>
   </si>
 </sst>
 </file>
@@ -2378,10 +2390,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E236" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E236" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E233">
-    <sortCondition ref="A1:A233"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E237" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E237" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E234">
+    <sortCondition ref="A1:A234"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #" dataDxfId="4"/>
@@ -2715,10 +2727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E236"/>
+  <dimension ref="A1:E237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A236" sqref="A236"/>
+    <sheetView tabSelected="1" topLeftCell="B39" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4486,732 +4498,732 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>265</v>
+        <v>735</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>42</v>
+        <v>736</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E109" s="1"/>
+        <v>737</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>489</v>
+        <v>265</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>697</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E110" s="1"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>682</v>
+        <v>697</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>266</v>
+        <v>490</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E112" s="1"/>
+        <v>134</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>491</v>
+        <v>266</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>189</v>
+        <v>17</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>190</v>
+        <v>61</v>
       </c>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>486</v>
+        <v>189</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D114" s="1"/>
+      <c r="D114" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>267</v>
+        <v>485</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>20</v>
+        <v>486</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D115" s="1"/>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>127</v>
+        <v>267</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>313</v>
+        <v>127</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>314</v>
+        <v>3</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>684</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E117" s="1"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>685</v>
+        <v>313</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>686</v>
+        <v>314</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>687</v>
+        <v>315</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>128</v>
+        <v>685</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>129</v>
+        <v>686</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E119" s="1"/>
+        <v>687</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>404</v>
+        <v>179</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>405</v>
+        <v>180</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>406</v>
+        <v>5</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>472</v>
+        <v>181</v>
       </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>409</v>
+        <v>472</v>
       </c>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E125" s="1"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D127" s="1"/>
+      <c r="D127" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>423</v>
-      </c>
+      <c r="D128" s="1"/>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E130" s="1"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C131" s="1"/>
-      <c r="D131" s="1"/>
+        <v>428</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>429</v>
+      </c>
       <c r="E131" s="1"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C132" s="1"/>
-      <c r="D132" s="1" t="s">
-        <v>434</v>
-      </c>
+      <c r="D132" s="1"/>
       <c r="E132" s="1"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C133" s="1"/>
-      <c r="D133" s="1"/>
+      <c r="D133" s="1" t="s">
+        <v>434</v>
+      </c>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C134" s="1"/>
-      <c r="D134" s="1" t="s">
-        <v>439</v>
-      </c>
+      <c r="D134" s="1"/>
       <c r="E134" s="1"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="E135" s="1"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E136" s="1"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="E137" s="1"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C142" s="1"/>
-      <c r="D142" s="1"/>
+      <c r="D142" s="1" t="s">
+        <v>460</v>
+      </c>
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C143" s="1"/>
-      <c r="D143" s="1" t="s">
-        <v>465</v>
-      </c>
+      <c r="D143" s="1"/>
       <c r="E143" s="1"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E144" s="1"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E145" s="1"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E146" s="1"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>669</v>
+        <v>475</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>670</v>
+        <v>470</v>
       </c>
       <c r="C147" s="1"/>
-      <c r="D147" s="1"/>
+      <c r="D147" s="1" t="s">
+        <v>471</v>
+      </c>
       <c r="E147" s="1"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>726</v>
+        <v>669</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>727</v>
+        <v>670</v>
       </c>
       <c r="C148" s="1"/>
-      <c r="D148" s="1" t="s">
-        <v>728</v>
-      </c>
+      <c r="D148" s="1"/>
       <c r="E148" s="1"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>233</v>
+        <v>726</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>153</v>
-      </c>
+        <v>727</v>
+      </c>
+      <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>154</v>
+        <v>728</v>
       </c>
       <c r="E149" s="1"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>696</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="E150" s="1"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E151" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E152" s="1"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E153" s="1"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E154" s="1"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E155" s="1"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>696</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="E156" s="1"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E157" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>696</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="E158" s="1"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>217</v>
+        <v>178</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>696</v>
@@ -5219,65 +5231,65 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>680</v>
+        <v>696</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E161" s="1"/>
+        <v>220</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>680</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="E162" s="1"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>680</v>
@@ -5285,16 +5297,16 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>680</v>
@@ -5302,843 +5314,845 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E165" s="1"/>
+        <v>232</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>244</v>
+        <v>214</v>
       </c>
       <c r="E166" s="1"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>369</v>
+        <v>242</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>370</v>
+        <v>243</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>371</v>
+        <v>244</v>
       </c>
       <c r="E167" s="1"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>253</v>
+        <v>369</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>4</v>
+        <v>370</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>55</v>
+        <v>371</v>
       </c>
       <c r="E168" s="1"/>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E169" s="1"/>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>310</v>
+        <v>254</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>311</v>
+        <v>11</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>312</v>
+        <v>56</v>
       </c>
       <c r="E170" s="1"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>255</v>
+        <v>310</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>10</v>
+        <v>311</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>57</v>
+        <v>312</v>
       </c>
       <c r="E171" s="1"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>550</v>
+        <v>255</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>551</v>
+        <v>10</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>552</v>
+        <v>57</v>
       </c>
       <c r="E172" s="1"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>256</v>
+        <v>550</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>308</v>
+        <v>551</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>309</v>
+        <v>552</v>
       </c>
       <c r="E173" s="1"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>12</v>
+        <v>308</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>58</v>
+        <v>309</v>
       </c>
       <c r="E174" s="1"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E175" s="1"/>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>201</v>
+        <v>80</v>
       </c>
       <c r="E176" s="1"/>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>268</v>
+        <v>201</v>
       </c>
       <c r="E177" s="1"/>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E178" s="1"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>81</v>
+        <v>261</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>83</v>
+        <v>269</v>
       </c>
       <c r="E179" s="1"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="E180" s="1"/>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>525</v>
+        <v>69</v>
       </c>
       <c r="E181" s="1"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>528</v>
+        <v>103</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>529</v>
+        <v>22</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>63</v>
+        <v>525</v>
       </c>
       <c r="E182" s="1"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>316</v>
+        <v>528</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>317</v>
+        <v>529</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>514</v>
+        <v>63</v>
       </c>
       <c r="E183" s="1"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>511</v>
+        <v>316</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>512</v>
+        <v>317</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E184" s="1"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>318</v>
+        <v>511</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>319</v>
+        <v>512</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>320</v>
+        <v>513</v>
       </c>
       <c r="E185" s="1"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>518</v>
+        <v>318</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>519</v>
+        <v>319</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>520</v>
+        <v>320</v>
       </c>
       <c r="E186" s="1"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="E187" s="1"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="E188" s="1"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>273</v>
+        <v>522</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>13</v>
+        <v>526</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>59</v>
+        <v>527</v>
       </c>
       <c r="E189" s="1"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E190" s="1"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E191" s="1"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>322</v>
+        <v>48</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="E192" s="1"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>321</v>
+        <v>276</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>324</v>
+        <v>104</v>
       </c>
       <c r="E193" s="1"/>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>277</v>
+        <v>321</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>52</v>
+        <v>323</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>74</v>
+        <v>324</v>
       </c>
       <c r="E194" s="1"/>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E195" s="1"/>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E196" s="1"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>326</v>
+        <v>279</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>327</v>
+        <v>105</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>328</v>
+        <v>77</v>
       </c>
       <c r="E197" s="1"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>280</v>
+        <v>326</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>106</v>
+        <v>327</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>107</v>
+        <v>328</v>
       </c>
       <c r="E198" s="1"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E199" s="1"/>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>110</v>
+        <v>281</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E200" s="1"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E201" s="1"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E202" s="1"/>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E203" s="1"/>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="E204" s="1"/>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>182</v>
+        <v>122</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>183</v>
+        <v>39</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>184</v>
+        <v>76</v>
       </c>
       <c r="E205" s="1"/>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>375</v>
+        <v>182</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>376</v>
+        <v>183</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>681</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="E206" s="1"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>288</v>
+        <v>375</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>93</v>
+        <v>376</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E207" s="1"/>
+        <v>377</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="E208" s="1"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E209" s="1"/>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E210" s="1"/>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="E211" s="1"/>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E212" s="1"/>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="E213" s="1"/>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E214" s="1"/>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>297</v>
+        <v>99</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
       </c>
       <c r="E215" s="1"/>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E216" s="1"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>325</v>
+        <v>299</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>367</v>
+        <v>300</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>368</v>
+        <v>301</v>
       </c>
       <c r="E217" s="1"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="E218" s="1"/>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>303</v>
+        <v>381</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>304</v>
+        <v>382</v>
       </c>
       <c r="E219" s="1"/>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>361</v>
+        <v>303</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>362</v>
+        <v>304</v>
       </c>
       <c r="E220" s="1"/>
     </row>
@@ -6147,227 +6161,225 @@
         <v>363</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>306</v>
+        <v>361</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>307</v>
+        <v>362</v>
       </c>
       <c r="E221" s="1"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>379</v>
+        <v>306</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>380</v>
+        <v>307</v>
       </c>
       <c r="E222" s="1"/>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>137</v>
+        <v>378</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>138</v>
+        <v>379</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>141</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="E223" s="1"/>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E224" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>398</v>
+        <v>142</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>399</v>
+        <v>143</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="E225" s="1"/>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>202</v>
+        <v>398</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>203</v>
+        <v>399</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>204</v>
+        <v>400</v>
       </c>
       <c r="E226" s="1"/>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>245</v>
+        <v>202</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>246</v>
+        <v>203</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>247</v>
+        <v>204</v>
       </c>
       <c r="E227" s="1"/>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E228" s="1"/>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>482</v>
+        <v>248</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>476</v>
+        <v>249</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>477</v>
+        <v>250</v>
       </c>
       <c r="E229" s="1"/>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="E230" s="1"/>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E231" s="1"/>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>270</v>
+        <v>480</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>271</v>
+        <v>481</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>272</v>
+        <v>484</v>
       </c>
       <c r="E232" s="1"/>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>493</v>
+        <v>270</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>494</v>
+        <v>271</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>495</v>
+        <v>272</v>
       </c>
       <c r="E233" s="1"/>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>693</v>
+        <v>493</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>694</v>
+        <v>494</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>681</v>
-      </c>
+        <v>495</v>
+      </c>
+      <c r="E234" s="1"/>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>729</v>
+        <v>693</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>730</v>
+        <v>694</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>731</v>
+        <v>695</v>
       </c>
       <c r="E235" s="1" t="s">
         <v>681</v>
@@ -6375,18 +6387,35 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D236" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A237" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D237" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="E236" s="1" t="s">
+      <c r="E237" s="1" t="s">
         <v>681</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New and tweaked derived variables
1. new "any co-infection" variable
2. very minor tweaks to the lymphoid and myeloid indicator variables
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1206E07-3014-6548-902B-DF4BD395194A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC3214E-C08C-9047-A1E7-96A2B321EA5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="4060" windowWidth="47640" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="742">
   <si>
     <t>Variable #</t>
   </si>
@@ -2243,6 +2243,15 @@
   </si>
   <si>
     <t>18-39 years; 40-59 years; 60-69 years; 70-79 years; 80+ years</t>
+  </si>
+  <si>
+    <t>Comp40</t>
+  </si>
+  <si>
+    <t>coinfection_any</t>
+  </si>
+  <si>
+    <t>Any co-infection within +/- 2 weeks of COVID-19 dx</t>
   </si>
 </sst>
 </file>
@@ -2390,10 +2399,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E237" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E237" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E234">
-    <sortCondition ref="A1:A234"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E238" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E238" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E238">
+    <sortCondition ref="A1:A238"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #" dataDxfId="4"/>
@@ -2727,10 +2736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E237"/>
+  <dimension ref="A1:E238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4464,16 +4473,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>714</v>
+        <v>729</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>715</v>
+        <v>730</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>716</v>
+        <v>731</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>681</v>
@@ -4481,766 +4490,768 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>264</v>
+        <v>732</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>123</v>
+        <v>733</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>44</v>
+        <v>734</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>735</v>
+        <v>714</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>736</v>
+        <v>715</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>737</v>
+        <v>716</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>738</v>
+        <v>681</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>265</v>
+        <v>739</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>42</v>
+        <v>740</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E110" s="1"/>
+        <v>741</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>489</v>
+        <v>264</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>135</v>
+        <v>44</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>697</v>
+        <v>679</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>490</v>
+        <v>735</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>133</v>
+        <v>736</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>134</v>
+        <v>737</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>682</v>
+        <v>738</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>189</v>
+        <v>124</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E114" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>486</v>
+        <v>133</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
+      <c r="D115" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>127</v>
+        <v>491</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>3</v>
+        <v>189</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>7</v>
+        <v>190</v>
       </c>
       <c r="E117" s="1"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>313</v>
+        <v>485</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>314</v>
+        <v>486</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>684</v>
-      </c>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>685</v>
+        <v>267</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>686</v>
+        <v>20</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>688</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E119" s="1"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>156</v>
+        <v>313</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>157</v>
+        <v>314</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E121" s="1"/>
+        <v>315</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>179</v>
+        <v>685</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>180</v>
+        <v>686</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E122" s="1"/>
+        <v>687</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>404</v>
+        <v>128</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>405</v>
+        <v>129</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>406</v>
+        <v>5</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>472</v>
+        <v>130</v>
       </c>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>407</v>
+        <v>156</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>408</v>
+        <v>157</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>406</v>
+        <v>15</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>409</v>
+        <v>158</v>
       </c>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>410</v>
+        <v>179</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>411</v>
+        <v>180</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>406</v>
+        <v>5</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>412</v>
+        <v>181</v>
       </c>
       <c r="E125" s="1"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>415</v>
+        <v>472</v>
       </c>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D128" s="1"/>
+      <c r="D128" s="1" t="s">
+        <v>412</v>
+      </c>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="E130" s="1"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D131" s="1" t="s">
-        <v>429</v>
-      </c>
+      <c r="D131" s="1"/>
       <c r="E131" s="1"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C132" s="1"/>
-      <c r="D132" s="1"/>
+        <v>422</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>423</v>
+      </c>
       <c r="E132" s="1"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C133" s="1"/>
+        <v>425</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>406</v>
+      </c>
       <c r="D133" s="1" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="C134" s="1"/>
-      <c r="D134" s="1"/>
+        <v>428</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>429</v>
+      </c>
       <c r="E134" s="1"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="C135" s="1"/>
-      <c r="D135" s="1" t="s">
-        <v>439</v>
-      </c>
+      <c r="D135" s="1"/>
       <c r="E135" s="1"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="E136" s="1"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="C137" s="1"/>
-      <c r="D137" s="1" t="s">
-        <v>445</v>
-      </c>
+      <c r="D137" s="1"/>
       <c r="E137" s="1"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="C143" s="1"/>
-      <c r="D143" s="1"/>
+      <c r="D143" s="1" t="s">
+        <v>454</v>
+      </c>
       <c r="E143" s="1"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="E144" s="1"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="E145" s="1"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="C146" s="1"/>
-      <c r="D146" s="1" t="s">
-        <v>469</v>
-      </c>
+      <c r="D146" s="1"/>
       <c r="E146" s="1"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="1" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="E147" s="1"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>669</v>
+        <v>473</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>670</v>
+        <v>466</v>
       </c>
       <c r="C148" s="1"/>
-      <c r="D148" s="1"/>
+      <c r="D148" s="1" t="s">
+        <v>467</v>
+      </c>
       <c r="E148" s="1"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>726</v>
+        <v>474</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>727</v>
+        <v>468</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>728</v>
+        <v>469</v>
       </c>
       <c r="E149" s="1"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>233</v>
+        <v>475</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>153</v>
-      </c>
+        <v>470</v>
+      </c>
+      <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
-        <v>154</v>
+        <v>471</v>
       </c>
       <c r="E150" s="1"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>234</v>
+        <v>669</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>696</v>
-      </c>
+        <v>670</v>
+      </c>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>235</v>
+        <v>726</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>153</v>
-      </c>
+        <v>727</v>
+      </c>
+      <c r="C152" s="1"/>
       <c r="D152" s="1" t="s">
-        <v>163</v>
+        <v>728</v>
       </c>
       <c r="E152" s="1"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E153" s="1"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E154" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E155" s="1"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E156" s="1"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>696</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="E157" s="1"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E158" s="1"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>176</v>
+        <v>239</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>696</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="E159" s="1"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>216</v>
+        <v>172</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>696</v>
@@ -5248,65 +5259,65 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>218</v>
+        <v>241</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>219</v>
+        <v>174</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>680</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="E161" s="1"/>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>222</v>
+        <v>177</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E162" s="1"/>
+        <v>178</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>680</v>
+        <v>696</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>680</v>
@@ -5314,719 +5325,723 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>680</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="E165" s="1"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E166" s="1"/>
+        <v>226</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E167" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>369</v>
+        <v>230</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>370</v>
+        <v>231</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="E168" s="1"/>
+        <v>232</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>4</v>
+        <v>213</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>55</v>
+        <v>214</v>
       </c>
       <c r="E169" s="1"/>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>11</v>
+        <v>243</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>56</v>
+        <v>244</v>
       </c>
       <c r="E170" s="1"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>310</v>
+        <v>369</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>311</v>
+        <v>370</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>312</v>
+        <v>371</v>
       </c>
       <c r="E171" s="1"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E172" s="1"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>550</v>
+        <v>254</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>551</v>
+        <v>11</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>552</v>
+        <v>56</v>
       </c>
       <c r="E173" s="1"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>256</v>
+        <v>310</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="E174" s="1"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E175" s="1"/>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>258</v>
+        <v>550</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>79</v>
+        <v>551</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>80</v>
+        <v>552</v>
       </c>
       <c r="E176" s="1"/>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>25</v>
+        <v>308</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>201</v>
+        <v>309</v>
       </c>
       <c r="E177" s="1"/>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>268</v>
+        <v>58</v>
       </c>
       <c r="E178" s="1"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>269</v>
+        <v>80</v>
       </c>
       <c r="E179" s="1"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>81</v>
+        <v>259</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>83</v>
+        <v>201</v>
       </c>
       <c r="E180" s="1"/>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>84</v>
+        <v>260</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>69</v>
+        <v>268</v>
       </c>
       <c r="E181" s="1"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>103</v>
+        <v>261</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>525</v>
+        <v>269</v>
       </c>
       <c r="E182" s="1"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>528</v>
+        <v>81</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>529</v>
+        <v>82</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="E183" s="1"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>316</v>
+        <v>84</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>317</v>
+        <v>32</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>514</v>
+        <v>69</v>
       </c>
       <c r="E184" s="1"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>511</v>
+        <v>103</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>512</v>
+        <v>22</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="E185" s="1"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>318</v>
+        <v>528</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>319</v>
+        <v>529</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>320</v>
+        <v>63</v>
       </c>
       <c r="E186" s="1"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>518</v>
+        <v>316</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>519</v>
+        <v>317</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="E187" s="1"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
       <c r="E188" s="1"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>522</v>
+        <v>318</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>526</v>
+        <v>319</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>527</v>
+        <v>320</v>
       </c>
       <c r="E189" s="1"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>273</v>
+        <v>518</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>13</v>
+        <v>519</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>59</v>
+        <v>520</v>
       </c>
       <c r="E190" s="1"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>274</v>
+        <v>521</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>29</v>
+        <v>523</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>68</v>
+        <v>524</v>
       </c>
       <c r="E191" s="1"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>275</v>
+        <v>522</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>48</v>
+        <v>526</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>75</v>
+        <v>527</v>
       </c>
       <c r="E192" s="1"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>322</v>
+        <v>13</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="E193" s="1"/>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>321</v>
+        <v>274</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>323</v>
+        <v>29</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>324</v>
+        <v>68</v>
       </c>
       <c r="E194" s="1"/>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E195" s="1"/>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>72</v>
+        <v>322</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="E196" s="1"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>279</v>
+        <v>321</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>105</v>
+        <v>323</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>77</v>
+        <v>324</v>
       </c>
       <c r="E197" s="1"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>326</v>
+        <v>277</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>327</v>
+        <v>52</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>328</v>
+        <v>74</v>
       </c>
       <c r="E198" s="1"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="E199" s="1"/>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="E200" s="1"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>110</v>
+        <v>326</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>111</v>
+        <v>327</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>112</v>
+        <v>328</v>
       </c>
       <c r="E201" s="1"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>114</v>
+        <v>280</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E202" s="1"/>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>117</v>
+        <v>281</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E203" s="1"/>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E204" s="1"/>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="E205" s="1"/>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>182</v>
+        <v>117</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>183</v>
+        <v>118</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>184</v>
+        <v>116</v>
       </c>
       <c r="E206" s="1"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>375</v>
+        <v>121</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>376</v>
+        <v>120</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>681</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E207" s="1"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>288</v>
+        <v>122</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="E208" s="1"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>289</v>
+        <v>182</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>92</v>
+        <v>183</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>21</v>
+        <v>184</v>
       </c>
       <c r="E209" s="1"/>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>290</v>
+        <v>375</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>95</v>
+        <v>376</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E210" s="1"/>
+        <v>377</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E211" s="1"/>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>94</v>
@@ -6038,40 +6053,40 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E213" s="1"/>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E214" s="1"/>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>94</v>
@@ -6083,341 +6098,352 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>297</v>
+        <v>30</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>298</v>
+        <v>31</v>
       </c>
       <c r="E216" s="1"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>300</v>
+        <v>98</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>301</v>
+        <v>100</v>
       </c>
       <c r="E217" s="1"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>367</v>
+        <v>99</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>368</v>
+        <v>21</v>
       </c>
       <c r="E218" s="1"/>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>381</v>
+        <v>297</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>382</v>
+        <v>298</v>
       </c>
       <c r="E219" s="1"/>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E220" s="1"/>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>363</v>
+        <v>325</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="E221" s="1"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>363</v>
+        <v>302</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>306</v>
+        <v>381</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>307</v>
+        <v>382</v>
       </c>
       <c r="E222" s="1"/>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>378</v>
+        <v>305</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>379</v>
+        <v>303</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>380</v>
+        <v>304</v>
       </c>
       <c r="E223" s="1"/>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>137</v>
+        <v>363</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>138</v>
+        <v>361</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>141</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="E224" s="1"/>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>142</v>
+        <v>363</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>143</v>
+        <v>306</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>139</v>
+        <v>94</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>397</v>
+        <v>307</v>
       </c>
       <c r="E225" s="1"/>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="E226" s="1"/>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>202</v>
+        <v>693</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>203</v>
+        <v>694</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E227" s="1"/>
+        <v>695</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>245</v>
+        <v>137</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>246</v>
+        <v>138</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E228" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>248</v>
+        <v>142</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>249</v>
+        <v>143</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>250</v>
+        <v>397</v>
       </c>
       <c r="E229" s="1"/>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>482</v>
+        <v>398</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>476</v>
+        <v>399</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>477</v>
+        <v>400</v>
       </c>
       <c r="E230" s="1"/>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>478</v>
+        <v>202</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>479</v>
+        <v>203</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>483</v>
+        <v>204</v>
       </c>
       <c r="E231" s="1"/>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>480</v>
+        <v>245</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>481</v>
+        <v>246</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>484</v>
+        <v>247</v>
       </c>
       <c r="E232" s="1"/>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="E233" s="1"/>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>495</v>
+        <v>477</v>
       </c>
       <c r="E234" s="1"/>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>693</v>
+        <v>478</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>694</v>
+        <v>479</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>681</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="E235" s="1"/>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>729</v>
+        <v>480</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>730</v>
+        <v>481</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>681</v>
-      </c>
+        <v>484</v>
+      </c>
+      <c r="E236" s="1"/>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>732</v>
+        <v>270</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>733</v>
+        <v>271</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>681</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="E237" s="1"/>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A238" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="E238" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Moved order of der_heme
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC3214E-C08C-9047-A1E7-96A2B321EA5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93851124-5BC6-7147-B107-510C9A278AD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="4060" windowWidth="47640" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="743">
   <si>
     <t>Variable #</t>
   </si>
@@ -2252,6 +2252,9 @@
   </si>
   <si>
     <t>Any co-infection within +/- 2 weeks of COVID-19 dx</t>
+  </si>
+  <si>
+    <t>Canada; Other; Spain; US Midwest; US Northeast; US South; US West</t>
   </si>
 </sst>
 </file>
@@ -2738,8 +2741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4693,7 +4696,9 @@
       <c r="D120" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E120" s="1"/>
+      <c r="E120" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">

</xml_diff>

<commit_message>
New cancer treatment timing derived variables
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93851124-5BC6-7147-B107-510C9A278AD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EE7D41-4883-FB4A-A41E-D13572FE8B05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="4060" windowWidth="47640" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48380" yWindow="2880" windowWidth="47640" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="752">
   <si>
     <t>Variable #</t>
   </si>
@@ -2255,6 +2256,33 @@
   </si>
   <si>
     <t>Canada; Other; Spain; US Midwest; US Northeast; US South; US West</t>
+  </si>
+  <si>
+    <t>0 = more than 3 months; 1 = less than 2 weeks; 2 = 2-4 weeks; 3 = 1-3 months (*); 88 = never or after COVID-19 diagnosis; 99 = unknown</t>
+  </si>
+  <si>
+    <t>0 = more than 3 months; 1 = 0-4 weeks; 2 = 1-3 months (*); 88 = never or after COVID-19 diagnosis; 99 = unknown</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>T13b</t>
+  </si>
+  <si>
+    <t>cancer_tx_timing_v3</t>
+  </si>
+  <si>
+    <t>0 = more than 3 months; 1 = 0-3 months; 88 = never or after COVID-19 diagnosis; 99 = unknown</t>
+  </si>
+  <si>
+    <t>Ca10k1</t>
+  </si>
+  <si>
+    <t>any_systemic_v2</t>
+  </si>
+  <si>
+    <t>Any cytotoxic, endocrine, immunotherapy, or targeted therapy in the 12 months prior to COVID-19</t>
   </si>
 </sst>
 </file>
@@ -2296,9 +2324,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2317,6 +2351,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2402,10 +2438,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E238" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E238" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E238">
-    <sortCondition ref="A1:A238"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E240" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E240" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E240">
+    <sortCondition ref="A1:A240"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #" dataDxfId="4"/>
@@ -2739,10 +2775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E238"/>
+  <dimension ref="A1:E240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2751,10 +2787,10 @@
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="48.83203125" customWidth="1"/>
-    <col min="5" max="5" width="70.6640625" customWidth="1"/>
+    <col min="5" max="5" width="70.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2767,11 +2803,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>329</v>
       </c>
@@ -2784,11 +2820,11 @@
       <c r="D2" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>391</v>
       </c>
@@ -2801,11 +2837,11 @@
       <c r="D3" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>392</v>
       </c>
@@ -2818,11 +2854,11 @@
       <c r="D4" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>564</v>
       </c>
@@ -2835,11 +2871,11 @@
       <c r="D5" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>331</v>
       </c>
@@ -2852,11 +2888,11 @@
       <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>332</v>
       </c>
@@ -2869,11 +2905,11 @@
       <c r="D7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>333</v>
       </c>
@@ -2886,11 +2922,11 @@
       <c r="D8" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>334</v>
       </c>
@@ -2903,11 +2939,11 @@
       <c r="D9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>335</v>
       </c>
@@ -2920,11 +2956,11 @@
       <c r="D10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>674</v>
       </c>
@@ -2937,11 +2973,11 @@
       <c r="D11" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>336</v>
       </c>
@@ -2954,11 +2990,11 @@
       <c r="D12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>337</v>
       </c>
@@ -2971,11 +3007,11 @@
       <c r="D13" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>338</v>
       </c>
@@ -2988,11 +3024,11 @@
       <c r="D14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>339</v>
       </c>
@@ -3005,11 +3041,11 @@
       <c r="D15" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>340</v>
       </c>
@@ -3022,7 +3058,7 @@
       <c r="D16" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="3" t="s">
         <v>681</v>
       </c>
     </row>
@@ -3039,7 +3075,7 @@
       <c r="D17" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -3054,7 +3090,7 @@
       <c r="D18" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -3069,7 +3105,7 @@
       <c r="D19" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -3084,7 +3120,7 @@
       <c r="D20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -3099,7 +3135,7 @@
       <c r="D21" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -3114,7 +3150,7 @@
       <c r="D22" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -3129,9 +3165,9 @@
       <c r="D23" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>488</v>
       </c>
@@ -3144,11 +3180,11 @@
       <c r="D24" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="3" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>487</v>
       </c>
@@ -3161,7 +3197,7 @@
       <c r="D25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="3" t="s">
         <v>683</v>
       </c>
     </row>
@@ -3178,9 +3214,9 @@
       <c r="D26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>717</v>
       </c>
@@ -3193,11 +3229,11 @@
       <c r="D27" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="3" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>720</v>
       </c>
@@ -3210,11 +3246,11 @@
       <c r="D28" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="3" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>721</v>
       </c>
@@ -3227,7 +3263,7 @@
       <c r="D29" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="3" t="s">
         <v>707</v>
       </c>
     </row>
@@ -3244,9 +3280,9 @@
       <c r="D30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>364</v>
       </c>
@@ -3259,11 +3295,11 @@
       <c r="D31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="3" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>386</v>
       </c>
@@ -3276,11 +3312,11 @@
       <c r="D32" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="3" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>492</v>
       </c>
@@ -3293,11 +3329,11 @@
       <c r="D33" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="3" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>286</v>
       </c>
@@ -3310,11 +3346,11 @@
       <c r="D34" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="3" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>287</v>
       </c>
@@ -3327,11 +3363,11 @@
       <c r="D35" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="3" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>155</v>
       </c>
@@ -3344,11 +3380,11 @@
       <c r="D36" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>193</v>
       </c>
@@ -3361,11 +3397,11 @@
       <c r="D37" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>195</v>
       </c>
@@ -3378,11 +3414,11 @@
       <c r="D38" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>198</v>
       </c>
@@ -3395,11 +3431,11 @@
       <c r="D39" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>351</v>
       </c>
@@ -3412,11 +3448,11 @@
       <c r="D40" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>352</v>
       </c>
@@ -3429,11 +3465,11 @@
       <c r="D41" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>353</v>
       </c>
@@ -3446,11 +3482,11 @@
       <c r="D42" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>354</v>
       </c>
@@ -3463,11 +3499,11 @@
       <c r="D43" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>349</v>
       </c>
@@ -3480,11 +3516,11 @@
       <c r="D44" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>350</v>
       </c>
@@ -3497,11 +3533,11 @@
       <c r="D45" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>372</v>
       </c>
@@ -3514,11 +3550,11 @@
       <c r="D46" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>553</v>
       </c>
@@ -3531,2727 +3567,2731 @@
       <c r="D47" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>671</v>
+        <v>749</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>673</v>
+        <v>750</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E49" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>690</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="3" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E52" s="1"/>
+        <v>208</v>
+      </c>
+      <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>496</v>
+        <v>209</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>497</v>
+        <v>210</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="E53" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="E53" s="3"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="E54" s="1"/>
+        <v>498</v>
+      </c>
+      <c r="E54" s="3"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="E55" s="1"/>
+        <v>500</v>
+      </c>
+      <c r="E55" s="3"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="E56" s="1"/>
+        <v>504</v>
+      </c>
+      <c r="E56" s="3"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>530</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="E57" s="1"/>
+        <v>507</v>
+      </c>
+      <c r="E57" s="3"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>18</v>
+        <v>530</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="E58" s="1"/>
+        <v>510</v>
+      </c>
+      <c r="E58" s="3"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>531</v>
+        <v>515</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="E59" s="1"/>
+        <v>517</v>
+      </c>
+      <c r="E59" s="3"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="E60" s="1"/>
+        <v>533</v>
+      </c>
+      <c r="E60" s="3"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" ht="46" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E62" s="3" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>537</v>
+        <v>85</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="E63" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="E63" s="3"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>86</v>
+        <v>537</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E64" s="1"/>
+        <v>538</v>
+      </c>
+      <c r="E64" s="3"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E65" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>539</v>
+        <v>87</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="E66" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="E66" s="3"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E67" s="1"/>
+        <v>540</v>
+      </c>
+      <c r="E67" s="3"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="E68" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="E68" s="3"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>148</v>
+        <v>542</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E69" s="1"/>
+        <v>543</v>
+      </c>
+      <c r="E69" s="3"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>401</v>
+        <v>148</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="E70" s="1"/>
+        <v>149</v>
+      </c>
+      <c r="E70" s="3"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>544</v>
+        <v>401</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="E71" s="1"/>
+        <v>402</v>
+      </c>
+      <c r="E71" s="3"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>150</v>
+        <v>544</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E72" s="1"/>
+        <v>545</v>
+      </c>
+      <c r="E72" s="3"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>546</v>
+        <v>150</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="E73" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="E73" s="3"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>389</v>
+        <v>546</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="E74" s="1"/>
+        <v>547</v>
+      </c>
+      <c r="E74" s="3"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>548</v>
+        <v>389</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="E75" s="1"/>
+        <v>390</v>
+      </c>
+      <c r="E75" s="3"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>36</v>
+        <v>548</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="E76" s="1"/>
+        <v>549</v>
+      </c>
+      <c r="E76" s="3"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>262</v>
+        <v>36</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E77" s="1"/>
+        <v>638</v>
+      </c>
+      <c r="E77" s="3"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>50</v>
+        <v>262</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E78" s="1"/>
+        <v>263</v>
+      </c>
+      <c r="E78" s="3"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>591</v>
+        <v>50</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>592</v>
-      </c>
-      <c r="E79" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="E79" s="3"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="E80" s="1"/>
+        <v>592</v>
+      </c>
+      <c r="E80" s="3"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="E81" s="1"/>
+        <v>595</v>
+      </c>
+      <c r="E81" s="3"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="E82" s="1"/>
+        <v>598</v>
+      </c>
+      <c r="E82" s="3"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>604</v>
-      </c>
-      <c r="E83" s="1"/>
+        <v>601</v>
+      </c>
+      <c r="E83" s="3"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+        <v>604</v>
+      </c>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="E85" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="E86" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="E86" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>616</v>
-      </c>
-      <c r="E87" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="E87" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>619</v>
-      </c>
-      <c r="E88" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="E88" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="E89" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="E89" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="E90" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="E90" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="E91" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="E91" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="E92" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="E92" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="E93" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="E93" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>637</v>
-      </c>
-      <c r="E94" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="E94" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="E95" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="E95" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="E96" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="E96" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>647</v>
-      </c>
-      <c r="E97" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="E97" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="E98" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="E98" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="E99" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="E100" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="E100" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E101" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="E101" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="E102" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E102" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="E103" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="E103" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>668</v>
-      </c>
-      <c r="E104" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>708</v>
+        <v>666</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>709</v>
+        <v>667</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="E105" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="E105" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="E106" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="E106" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>729</v>
+        <v>710</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>730</v>
+        <v>711</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="E107" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="E107" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="E108" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="E108" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>714</v>
+        <v>732</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>715</v>
+        <v>733</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="E109" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="E109" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>739</v>
+        <v>714</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>740</v>
+        <v>715</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D110" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="E110" s="1" t="s">
+      <c r="E111" s="3" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
+    <row r="112" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>736</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>265</v>
+        <v>735</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>42</v>
+        <v>736</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E113" s="1"/>
+        <v>737</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E114" s="3"/>
+    </row>
+    <row r="115" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E114" s="1" t="s">
+      <c r="E115" s="3" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B116" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E116" s="1"/>
+        <v>134</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>491</v>
+        <v>266</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>189</v>
+        <v>17</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E117" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="E117" s="3"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>486</v>
+        <v>189</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
+      <c r="D118" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E118" s="3"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>267</v>
+        <v>485</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>20</v>
+        <v>486</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E119" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D119" s="1"/>
+      <c r="E119" s="3"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E120" s="3"/>
+    </row>
+    <row r="121" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>314</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>685</v>
+        <v>313</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>686</v>
+        <v>314</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>128</v>
+        <v>685</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>129</v>
+        <v>686</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E123" s="1"/>
+        <v>687</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E124" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="E124" s="3"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E125" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>404</v>
+        <v>179</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>405</v>
+        <v>180</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>406</v>
+        <v>5</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="E126" s="1"/>
+        <v>181</v>
+      </c>
+      <c r="E126" s="3"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="E127" s="1"/>
+        <v>472</v>
+      </c>
+      <c r="E127" s="3"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="E128" s="1"/>
+        <v>409</v>
+      </c>
+      <c r="E128" s="3"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="E129" s="1"/>
+        <v>412</v>
+      </c>
+      <c r="E129" s="3"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="E130" s="1"/>
+        <v>415</v>
+      </c>
+      <c r="E130" s="3"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D131" s="1"/>
-      <c r="E131" s="1"/>
+      <c r="D131" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E131" s="3"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D132" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="E132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="3"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="E133" s="1"/>
+        <v>423</v>
+      </c>
+      <c r="E133" s="3"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="E134" s="1"/>
+        <v>426</v>
+      </c>
+      <c r="E134" s="3"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C135" s="1"/>
-      <c r="D135" s="1"/>
-      <c r="E135" s="1"/>
+        <v>428</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="E135" s="3"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C136" s="1"/>
-      <c r="D136" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="E136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="3"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C137" s="1"/>
-      <c r="D137" s="1"/>
-      <c r="E137" s="1"/>
+      <c r="D137" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E137" s="3"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C138" s="1"/>
-      <c r="D138" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="E138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="3"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E139" s="1"/>
+        <v>439</v>
+      </c>
+      <c r="E139" s="3"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="E140" s="1"/>
+        <v>442</v>
+      </c>
+      <c r="E140" s="3"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="E141" s="1"/>
+        <v>445</v>
+      </c>
+      <c r="E141" s="3"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="E142" s="1"/>
+        <v>448</v>
+      </c>
+      <c r="E142" s="3"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="E143" s="1"/>
+        <v>451</v>
+      </c>
+      <c r="E143" s="3"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="E144" s="1"/>
+        <v>454</v>
+      </c>
+      <c r="E144" s="3"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E145" s="1"/>
+        <v>457</v>
+      </c>
+      <c r="E145" s="3"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C146" s="1"/>
-      <c r="D146" s="1"/>
-      <c r="E146" s="1"/>
+      <c r="D146" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E146" s="3"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C147" s="1"/>
-      <c r="D147" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="E147" s="1"/>
+      <c r="D147" s="1"/>
+      <c r="E147" s="3"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C148" s="1"/>
       <c r="D148" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E148" s="1"/>
+        <v>465</v>
+      </c>
+      <c r="E148" s="3"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="E149" s="1"/>
+        <v>467</v>
+      </c>
+      <c r="E149" s="3"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="E150" s="1"/>
+        <v>469</v>
+      </c>
+      <c r="E150" s="3"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>669</v>
+        <v>475</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>670</v>
+        <v>470</v>
       </c>
       <c r="C151" s="1"/>
-      <c r="D151" s="1"/>
-      <c r="E151" s="1"/>
+      <c r="D151" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="E151" s="3"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>726</v>
+        <v>669</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>727</v>
+        <v>670</v>
       </c>
       <c r="C152" s="1"/>
-      <c r="D152" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="E152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="3"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>233</v>
+        <v>726</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>153</v>
-      </c>
+        <v>727</v>
+      </c>
+      <c r="C153" s="1"/>
       <c r="D153" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E153" s="1"/>
+        <v>728</v>
+      </c>
+      <c r="E153" s="3"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E154" s="3"/>
+    </row>
+    <row r="155" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E155" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E156" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="E156" s="3"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E157" s="1"/>
+        <v>164</v>
+      </c>
+      <c r="E157" s="3"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E158" s="1"/>
+        <v>167</v>
+      </c>
+      <c r="E158" s="3"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E159" s="1"/>
+        <v>169</v>
+      </c>
+      <c r="E159" s="3"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="E160" s="3"/>
+    </row>
+    <row r="161" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E161" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+      <c r="E162" s="3"/>
+    </row>
+    <row r="163" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E163" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E163" s="3" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E165" s="1"/>
+        <v>220</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="E166" s="3"/>
+    </row>
+    <row r="167" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E167" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E167" s="3" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E168" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E168" s="3" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E169" s="1"/>
+        <v>232</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E170" s="1"/>
+        <v>214</v>
+      </c>
+      <c r="E170" s="3"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>369</v>
+        <v>242</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>370</v>
+        <v>243</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="E171" s="1"/>
+        <v>244</v>
+      </c>
+      <c r="E171" s="3"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>253</v>
+        <v>369</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>4</v>
+        <v>370</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E172" s="1"/>
+        <v>371</v>
+      </c>
+      <c r="E172" s="3"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E173" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="E173" s="3"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>310</v>
+        <v>254</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>311</v>
+        <v>11</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="E174" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="E174" s="3"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>255</v>
+        <v>310</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>10</v>
+        <v>311</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E175" s="1"/>
+        <v>312</v>
+      </c>
+      <c r="E175" s="3"/>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>550</v>
+        <v>255</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>551</v>
+        <v>10</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="E176" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="E176" s="3"/>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>256</v>
+        <v>550</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>308</v>
+        <v>551</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E177" s="1"/>
+        <v>552</v>
+      </c>
+      <c r="E177" s="3"/>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>12</v>
+        <v>308</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E178" s="1"/>
+        <v>309</v>
+      </c>
+      <c r="E178" s="3"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E179" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="E179" s="3"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E180" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="E180" s="3"/>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E181" s="1"/>
+        <v>201</v>
+      </c>
+      <c r="E181" s="3"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E182" s="1"/>
+        <v>268</v>
+      </c>
+      <c r="E182" s="3"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>81</v>
+        <v>261</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E183" s="1"/>
+        <v>269</v>
+      </c>
+      <c r="E183" s="3"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E184" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="E184" s="3"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="E185" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="E185" s="3"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>528</v>
+        <v>103</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>529</v>
+        <v>22</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E186" s="1"/>
+        <v>525</v>
+      </c>
+      <c r="E186" s="3"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>316</v>
+        <v>528</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>317</v>
+        <v>529</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="E187" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="E187" s="3"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>511</v>
+        <v>316</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>512</v>
+        <v>317</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="E188" s="1"/>
+        <v>514</v>
+      </c>
+      <c r="E188" s="3"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>318</v>
+        <v>511</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>319</v>
+        <v>512</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E189" s="1"/>
+        <v>513</v>
+      </c>
+      <c r="E189" s="3"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>518</v>
+        <v>318</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>519</v>
+        <v>319</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="E190" s="1"/>
+        <v>320</v>
+      </c>
+      <c r="E190" s="3"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="E191" s="1"/>
+        <v>520</v>
+      </c>
+      <c r="E191" s="3"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="E192" s="1"/>
+        <v>524</v>
+      </c>
+      <c r="E192" s="3"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>273</v>
+        <v>522</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>13</v>
+        <v>526</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E193" s="1"/>
+        <v>527</v>
+      </c>
+      <c r="E193" s="3"/>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E194" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="E194" s="3"/>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E195" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="E195" s="3"/>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>322</v>
+        <v>48</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E196" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E196" s="3"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>321</v>
+        <v>276</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="E197" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="E197" s="3"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>277</v>
+        <v>321</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>52</v>
+        <v>323</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E198" s="1"/>
+        <v>324</v>
+      </c>
+      <c r="E198" s="3"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E199" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E199" s="3"/>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E200" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="E200" s="3"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>326</v>
+        <v>279</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>327</v>
+        <v>105</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="E201" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E201" s="3"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>280</v>
+        <v>326</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>106</v>
+        <v>327</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E202" s="1"/>
+        <v>328</v>
+      </c>
+      <c r="E202" s="3"/>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E203" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="E203" s="3"/>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>110</v>
+        <v>281</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E204" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="E204" s="3"/>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E205" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="E205" s="3"/>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E206" s="1"/>
+        <v>113</v>
+      </c>
+      <c r="E206" s="3"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E207" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="E207" s="3"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E208" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="E208" s="3"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>182</v>
+        <v>122</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>183</v>
+        <v>39</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E209" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="E209" s="3"/>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>375</v>
+        <v>182</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>376</v>
+        <v>183</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D210" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E210" s="3"/>
+    </row>
+    <row r="211" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A211" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D211" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="E210" s="1" t="s">
+      <c r="E211" s="3" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A211" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C211" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E211" s="1"/>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E212" s="1"/>
+        <v>102</v>
+      </c>
+      <c r="E212" s="3"/>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E213" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E213" s="3"/>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E214" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="E214" s="3"/>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E215" s="1"/>
+        <v>101</v>
+      </c>
+      <c r="E215" s="3"/>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E216" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E216" s="3"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E217" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E217" s="3"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E218" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="E218" s="3"/>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>297</v>
+        <v>99</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E219" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E219" s="3"/>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E220" s="1"/>
+        <v>298</v>
+      </c>
+      <c r="E220" s="3"/>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>325</v>
+        <v>299</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>367</v>
+        <v>300</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="E221" s="1"/>
+        <v>301</v>
+      </c>
+      <c r="E221" s="3"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="E222" s="1"/>
+        <v>368</v>
+      </c>
+      <c r="E222" s="3"/>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>303</v>
+        <v>381</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E223" s="1"/>
+        <v>382</v>
+      </c>
+      <c r="E223" s="3"/>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>361</v>
+        <v>303</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E224" s="1"/>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+      <c r="E224" s="3"/>
+    </row>
+    <row r="225" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>363</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>306</v>
+        <v>361</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E225" s="1"/>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+        <v>362</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>378</v>
       </c>
@@ -6264,191 +6304,225 @@
       <c r="D226" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="E226" s="1"/>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E226" s="3" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>693</v>
+        <v>746</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>694</v>
+        <v>747</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>681</v>
+        <v>380</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>137</v>
+        <v>745</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>138</v>
+        <v>306</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>139</v>
+        <v>94</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+        <v>307</v>
+      </c>
+      <c r="E228" s="3"/>
+    </row>
+    <row r="229" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>142</v>
+        <v>693</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>143</v>
+        <v>694</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E229" s="1"/>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+        <v>695</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>398</v>
+        <v>137</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>399</v>
+        <v>138</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="E230" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>202</v>
+        <v>142</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E231" s="1"/>
+        <v>397</v>
+      </c>
+      <c r="E231" s="3"/>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>245</v>
+        <v>398</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>246</v>
+        <v>399</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E232" s="1"/>
+        <v>400</v>
+      </c>
+      <c r="E232" s="3"/>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>248</v>
+        <v>202</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>249</v>
+        <v>203</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E233" s="1"/>
+        <v>204</v>
+      </c>
+      <c r="E233" s="3"/>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>482</v>
+        <v>245</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>476</v>
+        <v>246</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="E234" s="1"/>
+        <v>247</v>
+      </c>
+      <c r="E234" s="3"/>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>478</v>
+        <v>248</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>479</v>
+        <v>249</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="E235" s="1"/>
+        <v>250</v>
+      </c>
+      <c r="E235" s="3"/>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="E236" s="1"/>
+        <v>477</v>
+      </c>
+      <c r="E236" s="3"/>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>270</v>
+        <v>478</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>271</v>
+        <v>479</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E237" s="1"/>
+        <v>483</v>
+      </c>
+      <c r="E237" s="3"/>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D238" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="E238" s="3"/>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A239" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E239" s="3"/>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A240" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D240" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="E238" s="1"/>
+      <c r="E240" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New composite outcome added
Hospitalization (ever/never) or death within 30 days
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66947100-5CCF-1C42-8A17-26BA0B501764}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A073A574-773D-F943-BCCE-F2C7398D12BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-41680" yWindow="2880" windowWidth="40940" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="762">
   <si>
     <t>Variable #</t>
   </si>
@@ -272,9 +272,6 @@
     <t>Combined days to death</t>
   </si>
   <si>
-    <t>O10</t>
-  </si>
-  <si>
     <t>severe3</t>
   </si>
   <si>
@@ -809,9 +806,6 @@
     <t>O07</t>
   </si>
   <si>
-    <t>O08</t>
-  </si>
-  <si>
     <t>O09</t>
   </si>
   <si>
@@ -2301,6 +2295,24 @@
   </si>
   <si>
     <t xml:space="preserve">Metastatic to lung </t>
+  </si>
+  <si>
+    <t>1 = ER+; 2 = ER+/HER2+; 3 = HER2+; 4 = triple negative; 99 = Unknown</t>
+  </si>
+  <si>
+    <t>O08b</t>
+  </si>
+  <si>
+    <t>O08c</t>
+  </si>
+  <si>
+    <t>O08a</t>
+  </si>
+  <si>
+    <t>composite_hosp_death</t>
+  </si>
+  <si>
+    <t>Composite outcome of hospitalization (ever/never) and death within 30 days</t>
   </si>
 </sst>
 </file>
@@ -2456,10 +2468,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E242" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E242" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E241">
-    <sortCondition ref="A1:A241"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E243" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E243" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E242">
+    <sortCondition ref="A1:A242"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #" dataDxfId="4"/>
@@ -2793,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E242"/>
+  <dimension ref="A1:E243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C49" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2822,80 +2834,80 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>27</v>
@@ -2907,12 +2919,12 @@
         <v>28</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>46</v>
@@ -2924,29 +2936,29 @@
         <v>47</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>37</v>
@@ -2958,12 +2970,12 @@
         <v>65</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>38</v>
@@ -2975,29 +2987,29 @@
         <v>66</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>40</v>
@@ -3009,12 +3021,12 @@
         <v>67</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>41</v>
@@ -3023,15 +3035,15 @@
         <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>53</v>
@@ -3043,97 +3055,97 @@
         <v>54</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>60</v>
@@ -3142,52 +3154,52 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>348</v>
       </c>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>567</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>569</v>
       </c>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>24</v>
@@ -3196,15 +3208,15 @@
         <v>49</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>70</v>
@@ -3216,18 +3228,18 @@
         <v>71</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>35</v>
@@ -3236,58 +3248,58 @@
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>717</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>719</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>720</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>724</v>
-      </c>
       <c r="E28" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>721</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>725</v>
-      </c>
       <c r="E29" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>8</v>
@@ -3302,10 +3314,10 @@
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
@@ -3314,748 +3326,748 @@
         <v>64</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="E44" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="E45" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>374</v>
-      </c>
       <c r="E46" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>555</v>
-      </c>
       <c r="E47" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>751</v>
-      </c>
       <c r="E48" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>671</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>673</v>
-      </c>
       <c r="C49" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="E53" s="3"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>498</v>
       </c>
       <c r="E54" s="3"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E55" s="3"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>502</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>504</v>
       </c>
       <c r="E56" s="3"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>505</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>507</v>
       </c>
       <c r="E57" s="3"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>510</v>
       </c>
       <c r="E58" s="3"/>
     </row>
     <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E61" s="3"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E62" s="3"/>
     </row>
     <row r="63" spans="1:5" ht="46" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>572</v>
-      </c>
       <c r="E63" s="3" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E64" s="3"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E66" s="3"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E67" s="3"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E68" s="3"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E69" s="3"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E70" s="3"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E71" s="3"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E72" s="3"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E73" s="3"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E74" s="3"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E75" s="3"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E76" s="3"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E77" s="3"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>36</v>
@@ -4064,28 +4076,28 @@
         <v>33</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E78" s="3"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E79" s="3"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>50</v>
@@ -4100,544 +4112,544 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E81" s="3"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E82" s="3"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E83" s="3"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E84" s="3"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E85" s="3"/>
     </row>
     <row r="86" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
@@ -4646,29 +4658,29 @@
         <v>44</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>42</v>
@@ -4683,41 +4695,41 @@
     </row>
     <row r="116" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>17</v>
@@ -4732,25 +4744,25 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E119" s="3"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>5</v>
@@ -4760,7 +4772,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>20</v>
@@ -4775,7 +4787,7 @@
     </row>
     <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>3</v>
@@ -4787,227 +4799,227 @@
         <v>7</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E126" s="3"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E127" s="3"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>406</v>
-      </c>
       <c r="D128" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E128" s="3"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D129" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>409</v>
       </c>
       <c r="E129" s="3"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>412</v>
       </c>
       <c r="E130" s="3"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>415</v>
       </c>
       <c r="E131" s="3"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D132" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="E132" s="3"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="3"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>423</v>
       </c>
       <c r="E134" s="3"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D135" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="E135" s="3"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D136" s="1" t="s">
         <v>427</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>429</v>
       </c>
       <c r="E136" s="3"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
@@ -5015,23 +5027,23 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E138" s="3"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
@@ -5039,114 +5051,114 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E140" s="3"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E141" s="3"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E142" s="3"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E143" s="3"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E144" s="3"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E145" s="3"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E146" s="3"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E147" s="3"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
@@ -5154,62 +5166,62 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E149" s="3"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E150" s="3"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C151" s="1"/>
       <c r="D151" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E151" s="3"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C152" s="1"/>
       <c r="D152" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E152" s="3"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
@@ -5217,321 +5229,321 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C154" s="1"/>
       <c r="D154" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E154" s="3"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B155" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C155" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C155" s="1" t="s">
+      <c r="D155" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="E155" s="3"/>
     </row>
     <row r="156" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B156" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D156" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C156" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="E156" s="3" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B157" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D157" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="E157" s="3"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E158" s="3"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B159" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D159" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="E159" s="3"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B160" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D160" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E160" s="3"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B161" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D161" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="E161" s="3"/>
     </row>
     <row r="162" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B162" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D162" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C162" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="E162" s="3" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B163" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D163" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="E163" s="3"/>
     </row>
     <row r="164" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B164" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="C164" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D164" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C164" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="E164" s="3" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B165" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D165" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C165" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="E165" s="3" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="C166" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D166" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C166" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="E166" s="3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="C167" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D167" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="E167" s="3"/>
     </row>
     <row r="168" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B168" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="C168" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D168" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C168" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="E168" s="3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B169" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="C169" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D169" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C169" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>229</v>
-      </c>
       <c r="E169" s="3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B170" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B170" s="1" t="s">
+      <c r="C170" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D170" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C170" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>232</v>
-      </c>
       <c r="E170" s="3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B171" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D171" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="E171" s="3"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B172" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="C172" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D172" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="E172" s="3"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D173" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="E173" s="3"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>4</v>
@@ -5546,7 +5558,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>11</v>
@@ -5561,22 +5573,22 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E176" s="3"/>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>10</v>
@@ -5591,37 +5603,37 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E178" s="3"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E179" s="3"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>12</v>
@@ -5636,7 +5648,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>79</v>
@@ -5651,7 +5663,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>25</v>
@@ -5660,13 +5672,13 @@
         <v>6</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E182" s="3"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>260</v>
+        <v>759</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>26</v>
@@ -5675,13 +5687,13 @@
         <v>6</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E183" s="3"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>261</v>
+        <v>757</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>45</v>
@@ -5690,892 +5702,909 @@
         <v>6</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E184" s="3"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B185" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E185" s="3"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>84</v>
+        <v>259</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>32</v>
+        <v>760</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>69</v>
+        <v>761</v>
       </c>
       <c r="E186" s="3"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>525</v>
+        <v>69</v>
       </c>
       <c r="E187" s="3"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>528</v>
+        <v>102</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>529</v>
+        <v>22</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>63</v>
+        <v>523</v>
       </c>
       <c r="E188" s="3"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>316</v>
+        <v>526</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>317</v>
+        <v>527</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>514</v>
+        <v>63</v>
       </c>
       <c r="E189" s="3"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>511</v>
+        <v>314</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>512</v>
+        <v>315</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E190" s="3"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>318</v>
+        <v>509</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>319</v>
+        <v>510</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>320</v>
+        <v>511</v>
       </c>
       <c r="E191" s="3"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>518</v>
+        <v>316</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>519</v>
+        <v>317</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>520</v>
+        <v>318</v>
       </c>
       <c r="E192" s="3"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E193" s="3"/>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="E194" s="3"/>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>273</v>
+        <v>520</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>13</v>
+        <v>524</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>59</v>
+        <v>525</v>
       </c>
       <c r="E195" s="3"/>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E196" s="3"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E197" s="3"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>322</v>
+        <v>48</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="E198" s="3"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>321</v>
+        <v>274</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>324</v>
+        <v>103</v>
       </c>
       <c r="E199" s="3"/>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>52</v>
+        <v>321</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>74</v>
+        <v>322</v>
       </c>
       <c r="E200" s="3"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E201" s="3"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E202" s="3"/>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>326</v>
+        <v>277</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>327</v>
+        <v>104</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>328</v>
+        <v>77</v>
       </c>
       <c r="E203" s="3"/>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>280</v>
+        <v>324</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>106</v>
+        <v>325</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>107</v>
+        <v>326</v>
       </c>
       <c r="E204" s="3"/>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E205" s="3"/>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>110</v>
+        <v>279</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E206" s="3"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E207" s="3"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E208" s="3"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E209" s="3"/>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="E210" s="3"/>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>182</v>
+        <v>121</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>183</v>
+        <v>39</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>184</v>
+        <v>76</v>
       </c>
       <c r="E211" s="3"/>
     </row>
-    <row r="212" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>375</v>
+        <v>181</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>376</v>
+        <v>182</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="E212" s="3" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+      <c r="E212" s="3"/>
+    </row>
+    <row r="213" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>288</v>
+        <v>373</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>93</v>
+        <v>374</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E213" s="3"/>
+        <v>375</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>679</v>
+      </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="E214" s="3"/>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E215" s="3"/>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E216" s="3"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E217" s="3"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E218" s="3"/>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="E219" s="3"/>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B220" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D220" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E220" s="3"/>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>297</v>
+        <v>98</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
       </c>
       <c r="E221" s="3"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E222" s="3"/>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>325</v>
+        <v>297</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>367</v>
+        <v>298</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>368</v>
+        <v>299</v>
       </c>
       <c r="E223" s="3"/>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>302</v>
+        <v>323</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="E224" s="3"/>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B225" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E225" s="3"/>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C225" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D225" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E225" s="3"/>
-    </row>
-    <row r="226" spans="1:5" ht="31" x14ac:dyDescent="0.2">
-      <c r="A226" s="1" t="s">
-        <v>363</v>
-      </c>
       <c r="B226" s="1" t="s">
-        <v>361</v>
+        <v>301</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E226" s="3" t="s">
-        <v>743</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="E226" s="3"/>
     </row>
     <row r="227" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="228" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>746</v>
+        <v>376</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>747</v>
+        <v>377</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B229" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="B229" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="C229" s="1" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E229" s="3"/>
-    </row>
-    <row r="230" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>693</v>
+        <v>743</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>694</v>
+        <v>304</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="E230" s="3" t="s">
-        <v>681</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="E230" s="3"/>
     </row>
     <row r="231" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="E231" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A232" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B232" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B231" s="1" t="s">
+      <c r="C232" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C231" s="1" t="s">
+      <c r="D232" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D231" s="1" t="s">
+      <c r="E232" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E231" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A232" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C232" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D232" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E232" s="3"/>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>398</v>
+        <v>141</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>399</v>
+        <v>142</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="E233" s="3"/>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>202</v>
+        <v>396</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>203</v>
+        <v>397</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>204</v>
+        <v>398</v>
       </c>
       <c r="E234" s="3"/>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>245</v>
+        <v>201</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>246</v>
+        <v>202</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>247</v>
+        <v>203</v>
       </c>
       <c r="E235" s="3"/>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E236" s="3"/>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>482</v>
+        <v>247</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>476</v>
+        <v>248</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>477</v>
+        <v>249</v>
       </c>
       <c r="E237" s="3"/>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="E238" s="3"/>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B239" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D239" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="C239" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D239" s="1" t="s">
-        <v>484</v>
       </c>
       <c r="E239" s="3"/>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E240" s="3"/>
+    </row>
+    <row r="241" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A241" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D241" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B240" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E240" s="3"/>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A241" s="1" t="s">
+      <c r="E241" s="3" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A242" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D242" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B241" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="C241" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D241" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="E241" s="3"/>
-    </row>
-    <row r="242" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A242" s="1" t="s">
+      <c r="E242" s="3"/>
+    </row>
+    <row r="243" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A243" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D243" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="B242" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="C242" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D242" s="1" t="s">
-        <v>754</v>
-      </c>
-      <c r="E242" s="3" t="s">
-        <v>681</v>
+      <c r="E243" s="3" t="s">
+        <v>679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up drug code, added PD-1/PD-L1 derived variable
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B0D842-59DF-5F43-9CE6-C5AD8C1E83D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E40CB38-3A08-4248-8674-B1FAC8E85C50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41680" yWindow="3540" windowWidth="40940" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="814">
   <si>
     <t>Variable #</t>
   </si>
@@ -2459,6 +2459,15 @@
   </si>
   <si>
     <t>Any surgery (cancer or otherwise) in the month prior to COVID-19</t>
+  </si>
+  <si>
+    <t>Ca04k</t>
+  </si>
+  <si>
+    <t>pd1_l1</t>
+  </si>
+  <si>
+    <t>Most recent line of therapy includes a PD-1/PD-L1 antibody</t>
   </si>
 </sst>
 </file>
@@ -2614,10 +2623,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E259" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E259" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E259">
-    <sortCondition ref="A1:A259"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E260" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E260" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E260">
+    <sortCondition ref="A1:A260"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #" dataDxfId="4"/>
@@ -2951,10 +2960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E259"/>
+  <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="199" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="199" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3564,101 +3573,101 @@
         <v>703</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>699</v>
-      </c>
+      <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>382</v>
+        <v>360</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>361</v>
+        <v>134</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>362</v>
+        <v>64</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>488</v>
+        <v>382</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>283</v>
+        <v>488</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>142</v>
+        <v>383</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>144</v>
+        <v>384</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>703</v>
@@ -3666,33 +3675,33 @@
     </row>
     <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>153</v>
+        <v>284</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>526</v>
+        <v>18</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>552</v>
+        <v>145</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>677</v>
+        <v>703</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>804</v>
+        <v>153</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>806</v>
+        <v>157</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>805</v>
+        <v>552</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>677</v>
@@ -3700,16 +3709,16 @@
     </row>
     <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>191</v>
+        <v>804</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>192</v>
+        <v>806</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>553</v>
+        <v>805</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>677</v>
@@ -3717,16 +3726,16 @@
     </row>
     <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>352</v>
+        <v>192</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>677</v>
@@ -3734,16 +3743,16 @@
     </row>
     <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>677</v>
@@ -3751,16 +3760,16 @@
     </row>
     <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>348</v>
+        <v>196</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>677</v>
@@ -3768,16 +3777,16 @@
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>677</v>
@@ -3785,16 +3794,16 @@
     </row>
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>807</v>
+        <v>355</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>677</v>
@@ -3802,16 +3811,16 @@
     </row>
     <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>808</v>
+        <v>350</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>810</v>
+        <v>558</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>677</v>
@@ -3819,16 +3828,16 @@
     </row>
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>351</v>
+        <v>808</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>356</v>
+        <v>809</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>559</v>
+        <v>810</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>677</v>
@@ -3836,16 +3845,16 @@
     </row>
     <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>194</v>
+        <v>356</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>195</v>
+        <v>559</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>677</v>
@@ -3853,16 +3862,16 @@
     </row>
     <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>677</v>
@@ -3870,16 +3879,16 @@
     </row>
     <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>368</v>
+        <v>347</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>369</v>
+        <v>197</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>370</v>
+        <v>198</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>677</v>
@@ -3887,16 +3896,16 @@
     </row>
     <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>549</v>
+        <v>368</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>550</v>
+        <v>369</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>551</v>
+        <v>370</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>677</v>
@@ -3904,16 +3913,16 @@
     </row>
     <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>745</v>
+        <v>549</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>746</v>
+        <v>550</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>747</v>
+        <v>551</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>677</v>
@@ -3921,617 +3930,617 @@
     </row>
     <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>667</v>
+        <v>745</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>669</v>
+        <v>746</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D58" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="31" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>399</v>
-      </c>
       <c r="E59" s="3" t="s">
-        <v>688</v>
+        <v>677</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>685</v>
+        <v>185</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>686</v>
+        <v>186</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>687</v>
+        <v>399</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>204</v>
+        <v>685</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>205</v>
+        <v>686</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>526</v>
+        <v>18</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E61" s="3"/>
+        <v>687</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E62" s="3"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>492</v>
+        <v>207</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>493</v>
+        <v>208</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>494</v>
+        <v>209</v>
       </c>
       <c r="E63" s="3"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E64" s="3"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E66" s="3"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D67" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="E67" s="3"/>
-    </row>
-    <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>677</v>
-      </c>
+      <c r="E68" s="3"/>
     </row>
     <row r="69" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>751</v>
+        <v>511</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>752</v>
+        <v>512</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>753</v>
+        <v>513</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>527</v>
+        <v>751</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>528</v>
+        <v>752</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="E70" s="3"/>
+        <v>753</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D71" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="E71" s="3"/>
-    </row>
-    <row r="72" spans="1:5" ht="46" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" ht="46" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>567</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>801</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>802</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D73" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E74" s="3"/>
+      <c r="E74" s="3" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>533</v>
+        <v>83</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>534</v>
+        <v>89</v>
       </c>
       <c r="E75" s="3"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>84</v>
+        <v>533</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>88</v>
+        <v>534</v>
       </c>
       <c r="E76" s="3"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E77" s="3"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>535</v>
+        <v>85</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>536</v>
+        <v>87</v>
       </c>
       <c r="E78" s="3"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>86</v>
+        <v>536</v>
       </c>
       <c r="E79" s="3"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>539</v>
+        <v>86</v>
       </c>
       <c r="E80" s="3"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>146</v>
+        <v>538</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>147</v>
+        <v>539</v>
       </c>
       <c r="E81" s="3"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>397</v>
+        <v>146</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>398</v>
+        <v>147</v>
       </c>
       <c r="E82" s="3"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>540</v>
+        <v>397</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>541</v>
+        <v>398</v>
       </c>
       <c r="E83" s="3"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>148</v>
+        <v>540</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>149</v>
+        <v>541</v>
       </c>
       <c r="E84" s="3"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>542</v>
+        <v>148</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>543</v>
+        <v>149</v>
       </c>
       <c r="E85" s="3"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>385</v>
+        <v>542</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>386</v>
+        <v>543</v>
       </c>
       <c r="E86" s="3"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>544</v>
+        <v>385</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>545</v>
+        <v>386</v>
       </c>
       <c r="E87" s="3"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>36</v>
+        <v>544</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>634</v>
+        <v>545</v>
       </c>
       <c r="E88" s="3"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>259</v>
+        <v>36</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>260</v>
+        <v>634</v>
       </c>
       <c r="E89" s="3"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>50</v>
+        <v>259</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>51</v>
+        <v>260</v>
       </c>
       <c r="E90" s="3"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>587</v>
+        <v>50</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>588</v>
+        <v>51</v>
       </c>
       <c r="E91" s="3"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E92" s="3"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E93" s="3"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E94" s="3"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E95" s="3"/>
     </row>
-    <row r="96" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>603</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>677</v>
-      </c>
+        <v>600</v>
+      </c>
+      <c r="E96" s="3"/>
     </row>
     <row r="97" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>677</v>
@@ -4539,16 +4548,16 @@
     </row>
     <row r="98" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>677</v>
@@ -4556,16 +4565,16 @@
     </row>
     <row r="99" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>677</v>
@@ -4573,16 +4582,16 @@
     </row>
     <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>677</v>
@@ -4590,16 +4599,16 @@
     </row>
     <row r="101" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>677</v>
@@ -4607,16 +4616,16 @@
     </row>
     <row r="102" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>677</v>
@@ -4624,16 +4633,16 @@
     </row>
     <row r="103" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>677</v>
@@ -4641,16 +4650,16 @@
     </row>
     <row r="104" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>677</v>
@@ -4658,16 +4667,16 @@
     </row>
     <row r="105" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>677</v>
@@ -4675,16 +4684,16 @@
     </row>
     <row r="106" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>677</v>
@@ -4692,16 +4701,16 @@
     </row>
     <row r="107" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>677</v>
@@ -4709,16 +4718,16 @@
     </row>
     <row r="108" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>677</v>
@@ -4726,16 +4735,16 @@
     </row>
     <row r="109" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>677</v>
@@ -4743,16 +4752,16 @@
     </row>
     <row r="110" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>677</v>
@@ -4760,16 +4769,16 @@
     </row>
     <row r="111" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>677</v>
@@ -4777,16 +4786,16 @@
     </row>
     <row r="112" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>677</v>
@@ -4794,16 +4803,16 @@
     </row>
     <row r="113" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>677</v>
@@ -4811,16 +4820,16 @@
     </row>
     <row r="114" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>677</v>
@@ -4828,16 +4837,16 @@
     </row>
     <row r="115" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>677</v>
@@ -4845,16 +4854,16 @@
     </row>
     <row r="116" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>677</v>
@@ -4862,16 +4871,16 @@
     </row>
     <row r="117" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>704</v>
+        <v>662</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>705</v>
+        <v>663</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>709</v>
+        <v>664</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>677</v>
@@ -4879,16 +4888,16 @@
     </row>
     <row r="118" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>677</v>
@@ -4896,16 +4905,16 @@
     </row>
     <row r="119" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>725</v>
+        <v>706</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>726</v>
+        <v>707</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>727</v>
+        <v>708</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>677</v>
@@ -4913,16 +4922,16 @@
     </row>
     <row r="120" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>677</v>
@@ -4930,16 +4939,16 @@
     </row>
     <row r="121" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>710</v>
+        <v>728</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>711</v>
+        <v>729</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>712</v>
+        <v>730</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>677</v>
@@ -4947,800 +4956,800 @@
     </row>
     <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>735</v>
+        <v>710</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>736</v>
+        <v>711</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D122" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="E122" s="3" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
+      <c r="E123" s="3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B124" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C124" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E123" s="3"/>
-    </row>
-    <row r="124" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>675</v>
-      </c>
+      <c r="E124" s="3"/>
     </row>
     <row r="125" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>731</v>
+        <v>261</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>732</v>
+        <v>121</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>733</v>
+        <v>44</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>262</v>
+        <v>731</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>42</v>
+        <v>732</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D126" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D127" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E126" s="3"/>
-    </row>
-    <row r="127" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E127" s="3" t="s">
-        <v>693</v>
-      </c>
+      <c r="E127" s="3"/>
     </row>
     <row r="128" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B129" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E128" s="3" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E129" s="3"/>
+        <v>132</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>487</v>
+        <v>263</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>187</v>
+        <v>17</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>188</v>
+        <v>61</v>
       </c>
       <c r="E130" s="3"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>482</v>
+        <v>187</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D131" s="1"/>
+      <c r="D131" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="E131" s="3"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132" s="1"/>
+      <c r="E132" s="3"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B133" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="C133" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="D133" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E132" s="3"/>
-    </row>
-    <row r="133" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E133" s="3" t="s">
-        <v>738</v>
-      </c>
+      <c r="E133" s="3"/>
     </row>
     <row r="134" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>310</v>
+        <v>125</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>311</v>
+        <v>3</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>312</v>
+        <v>7</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>680</v>
+        <v>738</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>681</v>
+        <v>310</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>682</v>
+        <v>311</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>683</v>
+        <v>312</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>126</v>
+        <v>681</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>127</v>
+        <v>682</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E136" s="3"/>
+        <v>683</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="E137" s="3"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="E138" s="3"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>400</v>
+        <v>177</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>401</v>
+        <v>178</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>402</v>
+        <v>5</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>468</v>
+        <v>179</v>
       </c>
       <c r="E139" s="3"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>405</v>
+        <v>468</v>
       </c>
       <c r="E140" s="3"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E141" s="3"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E142" s="3"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E143" s="3"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="D144" s="1"/>
+      <c r="D144" s="1" t="s">
+        <v>414</v>
+      </c>
       <c r="E144" s="3"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="D145" s="1" t="s">
-        <v>419</v>
-      </c>
+      <c r="D145" s="1"/>
       <c r="E145" s="3"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E146" s="3"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E147" s="3"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="C148" s="1"/>
-      <c r="D148" s="1"/>
+        <v>424</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="E148" s="3"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C149" s="1"/>
-      <c r="D149" s="1" t="s">
-        <v>430</v>
-      </c>
+      <c r="D149" s="1"/>
       <c r="E149" s="3"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C150" s="1"/>
-      <c r="D150" s="1"/>
+      <c r="D150" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="E150" s="3"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C151" s="1"/>
-      <c r="D151" s="1" t="s">
-        <v>435</v>
-      </c>
+      <c r="D151" s="1"/>
       <c r="E151" s="3"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C152" s="1"/>
       <c r="D152" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E152" s="3"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C153" s="1"/>
       <c r="D153" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E153" s="3"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C154" s="1"/>
       <c r="D154" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="E154" s="3"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C155" s="1"/>
       <c r="D155" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="E155" s="3"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C156" s="1"/>
       <c r="D156" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="E156" s="3"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="E157" s="3"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E158" s="3"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C159" s="1"/>
-      <c r="D159" s="1"/>
+      <c r="D159" s="1" t="s">
+        <v>456</v>
+      </c>
       <c r="E159" s="3"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C160" s="1"/>
-      <c r="D160" s="1" t="s">
-        <v>461</v>
-      </c>
+      <c r="D160" s="1"/>
       <c r="E160" s="3"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C161" s="1"/>
       <c r="D161" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E161" s="3"/>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E162" s="3"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C163" s="1"/>
       <c r="D163" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E163" s="3"/>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>665</v>
+        <v>471</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>666</v>
+        <v>466</v>
       </c>
       <c r="C164" s="1"/>
-      <c r="D164" s="1"/>
+      <c r="D164" s="1" t="s">
+        <v>467</v>
+      </c>
       <c r="E164" s="3"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>722</v>
+        <v>665</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>723</v>
+        <v>666</v>
       </c>
       <c r="C165" s="1"/>
-      <c r="D165" s="1" t="s">
-        <v>724</v>
-      </c>
+      <c r="D165" s="1"/>
       <c r="E165" s="3"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="E166" s="3"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="B167" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E166" s="3"/>
-    </row>
-    <row r="167" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A167" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E167" s="3" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+      <c r="E167" s="3"/>
+    </row>
+    <row r="168" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E168" s="3"/>
+        <v>159</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E169" s="3"/>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E170" s="3"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E171" s="3"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E172" s="3"/>
     </row>
-    <row r="173" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E173" s="3" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="E173" s="3"/>
+    </row>
+    <row r="174" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E174" s="3"/>
-    </row>
-    <row r="175" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>174</v>
+        <v>239</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E175" s="3" t="s">
-        <v>692</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="E175" s="3"/>
     </row>
     <row r="176" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>692</v>
@@ -5748,65 +5757,65 @@
     </row>
     <row r="177" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E178" s="3"/>
-    </row>
-    <row r="179" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E179" s="3" t="s">
-        <v>676</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="E179" s="3"/>
     </row>
     <row r="180" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>676</v>
@@ -5814,545 +5823,545 @@
     </row>
     <row r="181" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="E182" s="3"/>
+        <v>230</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>240</v>
+        <v>213</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="E183" s="3"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>365</v>
+        <v>240</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>366</v>
+        <v>241</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>367</v>
+        <v>242</v>
       </c>
       <c r="E184" s="3"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>251</v>
+        <v>365</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>4</v>
+        <v>366</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>55</v>
+        <v>367</v>
       </c>
       <c r="E185" s="3"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E186" s="3"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>307</v>
+        <v>252</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>308</v>
+        <v>11</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>309</v>
+        <v>56</v>
       </c>
       <c r="E187" s="3"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>253</v>
+        <v>307</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>10</v>
+        <v>308</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>57</v>
+        <v>309</v>
       </c>
       <c r="E188" s="3"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>546</v>
+        <v>253</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>547</v>
+        <v>10</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>548</v>
+        <v>57</v>
       </c>
       <c r="E189" s="3"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>254</v>
+        <v>546</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>305</v>
+        <v>547</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>306</v>
+        <v>548</v>
       </c>
       <c r="E190" s="3"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>12</v>
+        <v>305</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>58</v>
+        <v>306</v>
       </c>
       <c r="E191" s="3"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E192" s="3"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>199</v>
+        <v>80</v>
       </c>
       <c r="E193" s="3"/>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>757</v>
+        <v>257</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>265</v>
+        <v>199</v>
       </c>
       <c r="E194" s="3"/>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E195" s="3"/>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>82</v>
+        <v>266</v>
       </c>
       <c r="E196" s="3"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>258</v>
+        <v>756</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>758</v>
+        <v>81</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>759</v>
+        <v>82</v>
       </c>
       <c r="E197" s="3"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>101</v>
+        <v>258</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>22</v>
+        <v>758</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>521</v>
+        <v>759</v>
       </c>
       <c r="E198" s="3"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>524</v>
+        <v>101</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>525</v>
+        <v>22</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>63</v>
+        <v>521</v>
       </c>
       <c r="E199" s="3"/>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>313</v>
+        <v>524</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>314</v>
+        <v>525</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>510</v>
+        <v>63</v>
       </c>
       <c r="E200" s="3"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>507</v>
+        <v>313</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>508</v>
+        <v>314</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E201" s="3"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>315</v>
+        <v>507</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>316</v>
+        <v>508</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>317</v>
+        <v>509</v>
       </c>
       <c r="E202" s="3"/>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>514</v>
+        <v>315</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>515</v>
+        <v>316</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>516</v>
+        <v>317</v>
       </c>
       <c r="E203" s="3"/>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="E204" s="3"/>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E205" s="3"/>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>270</v>
+        <v>518</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>13</v>
+        <v>522</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>59</v>
+        <v>523</v>
       </c>
       <c r="E206" s="3"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E207" s="3"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E208" s="3"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>319</v>
+        <v>48</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="E209" s="3"/>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>318</v>
+        <v>273</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>321</v>
+        <v>102</v>
       </c>
       <c r="E210" s="3"/>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>274</v>
+        <v>318</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>52</v>
+        <v>320</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>74</v>
+        <v>321</v>
       </c>
       <c r="E211" s="3"/>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E212" s="3"/>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E213" s="3"/>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>323</v>
+        <v>276</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>324</v>
+        <v>103</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>325</v>
+        <v>77</v>
       </c>
       <c r="E214" s="3"/>
     </row>
-    <row r="215" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>277</v>
+        <v>323</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>104</v>
+        <v>324</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E215" s="3" t="s">
-        <v>677</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="E215" s="3"/>
     </row>
     <row r="216" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E216" s="3" t="s">
         <v>677</v>
@@ -6360,16 +6369,16 @@
     </row>
     <row r="217" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>108</v>
+        <v>278</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E217" s="3" t="s">
         <v>677</v>
@@ -6377,16 +6386,16 @@
     </row>
     <row r="218" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E218" s="3" t="s">
         <v>677</v>
@@ -6394,16 +6403,16 @@
     </row>
     <row r="219" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E219" s="3" t="s">
         <v>677</v>
@@ -6411,16 +6420,16 @@
     </row>
     <row r="220" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E220" s="3" t="s">
         <v>677</v>
@@ -6428,16 +6437,16 @@
     </row>
     <row r="221" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>785</v>
+        <v>119</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>786</v>
+        <v>118</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>787</v>
+        <v>117</v>
       </c>
       <c r="E221" s="3" t="s">
         <v>677</v>
@@ -6445,16 +6454,16 @@
     </row>
     <row r="222" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="E222" s="3" t="s">
         <v>677</v>
@@ -6462,16 +6471,16 @@
     </row>
     <row r="223" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>120</v>
+        <v>788</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>39</v>
+        <v>789</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>76</v>
+        <v>790</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>677</v>
@@ -6479,16 +6488,16 @@
     </row>
     <row r="224" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>181</v>
+        <v>39</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>182</v>
+        <v>76</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>677</v>
@@ -6496,16 +6505,16 @@
     </row>
     <row r="225" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>371</v>
+        <v>180</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>372</v>
+        <v>181</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>373</v>
+        <v>182</v>
       </c>
       <c r="E225" s="3" t="s">
         <v>677</v>
@@ -6513,16 +6522,16 @@
     </row>
     <row r="226" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>760</v>
+        <v>371</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>761</v>
+        <v>372</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>762</v>
+        <v>373</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>677</v>
@@ -6530,16 +6539,16 @@
     </row>
     <row r="227" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>791</v>
+        <v>760</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>792</v>
+        <v>761</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>793</v>
+        <v>762</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>677</v>
@@ -6547,16 +6556,16 @@
     </row>
     <row r="228" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="E228" s="3" t="s">
         <v>677</v>
@@ -6564,16 +6573,16 @@
     </row>
     <row r="229" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>677</v>
@@ -6581,241 +6590,241 @@
     </row>
     <row r="230" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A231" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B230" s="1" t="s">
+      <c r="B231" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C230" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D230" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E230" s="3" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A231" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E231" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="E231" s="3" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E232" s="3"/>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
       <c r="E233" s="3"/>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="E234" s="3"/>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E235" s="3"/>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="E236" s="3"/>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="E237" s="3"/>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>294</v>
+        <v>97</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>295</v>
+        <v>21</v>
       </c>
       <c r="E238" s="3"/>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E239" s="3"/>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
-        <v>322</v>
+        <v>296</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>363</v>
+        <v>297</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>364</v>
+        <v>298</v>
       </c>
       <c r="E240" s="3"/>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="E241" s="3"/>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>300</v>
+        <v>377</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D242" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E242" s="3"/>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A243" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D243" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="E242" s="3"/>
-    </row>
-    <row r="243" spans="1:5" ht="31" x14ac:dyDescent="0.2">
-      <c r="A243" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B243" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C243" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D243" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="E243" s="3" t="s">
-        <v>739</v>
-      </c>
+      <c r="E243" s="3"/>
     </row>
     <row r="244" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="E244" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="245" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
-        <v>742</v>
+        <v>374</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>743</v>
+        <v>375</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>18</v>
@@ -6824,224 +6833,241 @@
         <v>376</v>
       </c>
       <c r="E245" s="3" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+      <c r="A246" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="E246" s="3" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A246" s="1" t="s">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A247" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="B246" s="1" t="s">
+      <c r="B247" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C246" s="1" t="s">
+      <c r="C247" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D246" s="1" t="s">
+      <c r="D247" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="E246" s="3"/>
-    </row>
-    <row r="247" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A247" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="B247" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="C247" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D247" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="E247" s="3" t="s">
-        <v>677</v>
-      </c>
+      <c r="E247" s="3"/>
     </row>
     <row r="248" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
-        <v>135</v>
+        <v>689</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>136</v>
+        <v>690</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>138</v>
+        <v>691</v>
       </c>
       <c r="E248" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="E249" s="3"/>
+        <v>138</v>
+      </c>
+      <c r="E249" s="3" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
-        <v>394</v>
+        <v>140</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>395</v>
+        <v>141</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E250" s="3"/>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
-        <v>200</v>
+        <v>394</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>201</v>
+        <v>395</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>202</v>
+        <v>396</v>
       </c>
       <c r="E251" s="3"/>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
-        <v>243</v>
+        <v>200</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>244</v>
+        <v>201</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>245</v>
+        <v>202</v>
       </c>
       <c r="E252" s="3"/>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E253" s="3"/>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
-        <v>478</v>
+        <v>246</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>472</v>
+        <v>247</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>473</v>
+        <v>248</v>
       </c>
       <c r="E254" s="3"/>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="E255" s="3"/>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E256" s="3"/>
     </row>
-    <row r="257" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
-        <v>267</v>
+        <v>476</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>268</v>
+        <v>477</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E257" s="3" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+        <v>480</v>
+      </c>
+      <c r="E257" s="3"/>
+    </row>
+    <row r="258" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
-        <v>489</v>
+        <v>267</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>490</v>
+        <v>268</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="E258" s="3"/>
-    </row>
-    <row r="259" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+      <c r="E258" s="3" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
-        <v>748</v>
+        <v>489</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>749</v>
+        <v>490</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D259" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="E259" s="3"/>
+    </row>
+    <row r="260" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A260" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D260" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="E259" s="3" t="s">
+      <c r="E260" s="3" t="s">
         <v>677</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to QA tracker
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E40CB38-3A08-4248-8674-B1FAC8E85C50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E1F78B-59EB-9442-B3D7-B6E83294538D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-49380" yWindow="580" windowWidth="41000" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="814">
   <si>
     <t>Variable #</t>
   </si>
@@ -2962,8 +2962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="199" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="199" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C245" sqref="C245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2971,8 +2971,8 @@
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="48.83203125" customWidth="1"/>
-    <col min="5" max="5" width="70.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="44.1640625" customWidth="1"/>
+    <col min="5" max="5" width="55.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -3709,16 +3709,16 @@
     </row>
     <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>804</v>
+        <v>191</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>806</v>
+        <v>192</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>805</v>
+        <v>553</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>677</v>
@@ -3726,16 +3726,16 @@
     </row>
     <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>192</v>
+        <v>352</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>677</v>
@@ -3743,16 +3743,16 @@
     </row>
     <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>677</v>
@@ -3760,16 +3760,16 @@
     </row>
     <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>196</v>
+        <v>348</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>677</v>
@@ -3777,16 +3777,16 @@
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>677</v>
@@ -3794,16 +3794,16 @@
     </row>
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>355</v>
+        <v>807</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>677</v>
@@ -3811,16 +3811,16 @@
     </row>
     <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>350</v>
+        <v>808</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>558</v>
+        <v>810</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>677</v>
@@ -3828,16 +3828,16 @@
     </row>
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>808</v>
+        <v>351</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>809</v>
+        <v>356</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>810</v>
+        <v>559</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>677</v>
@@ -3845,16 +3845,16 @@
     </row>
     <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>356</v>
+        <v>194</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>559</v>
+        <v>195</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>677</v>
@@ -3862,16 +3862,16 @@
     </row>
     <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>677</v>
@@ -3879,16 +3879,16 @@
     </row>
     <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>347</v>
+        <v>368</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>197</v>
+        <v>369</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>198</v>
+        <v>370</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>677</v>
@@ -3896,16 +3896,16 @@
     </row>
     <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>368</v>
+        <v>549</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>369</v>
+        <v>550</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>370</v>
+        <v>551</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>677</v>
@@ -3913,16 +3913,16 @@
     </row>
     <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>549</v>
+        <v>745</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>550</v>
+        <v>746</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>551</v>
+        <v>747</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>677</v>
@@ -3930,16 +3930,16 @@
     </row>
     <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>745</v>
+        <v>667</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>746</v>
+        <v>669</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>747</v>
+        <v>668</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>677</v>
@@ -3947,16 +3947,16 @@
     </row>
     <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>667</v>
+        <v>804</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>669</v>
+        <v>806</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>526</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>668</v>
+        <v>805</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>677</v>
@@ -5380,7 +5380,9 @@
       <c r="B149" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="C149" s="1"/>
+      <c r="C149" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D149" s="1"/>
       <c r="E149" s="3"/>
     </row>
@@ -5391,7 +5393,9 @@
       <c r="B150" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="C150" s="1"/>
+      <c r="C150" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D150" s="1" t="s">
         <v>430</v>
       </c>
@@ -5404,7 +5408,9 @@
       <c r="B151" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="C151" s="1"/>
+      <c r="C151" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D151" s="1"/>
       <c r="E151" s="3"/>
     </row>
@@ -5415,7 +5421,9 @@
       <c r="B152" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C152" s="1"/>
+      <c r="C152" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D152" s="1" t="s">
         <v>435</v>
       </c>
@@ -5428,7 +5436,9 @@
       <c r="B153" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="C153" s="1"/>
+      <c r="C153" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D153" s="1" t="s">
         <v>438</v>
       </c>
@@ -5441,7 +5451,9 @@
       <c r="B154" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="C154" s="1"/>
+      <c r="C154" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D154" s="1" t="s">
         <v>441</v>
       </c>
@@ -5454,7 +5466,9 @@
       <c r="B155" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="C155" s="1"/>
+      <c r="C155" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D155" s="1" t="s">
         <v>444</v>
       </c>
@@ -5467,7 +5481,9 @@
       <c r="B156" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="C156" s="1"/>
+      <c r="C156" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D156" s="1" t="s">
         <v>447</v>
       </c>
@@ -5480,7 +5496,9 @@
       <c r="B157" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="C157" s="1"/>
+      <c r="C157" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D157" s="1" t="s">
         <v>450</v>
       </c>
@@ -5493,7 +5511,9 @@
       <c r="B158" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="C158" s="1"/>
+      <c r="C158" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D158" s="1" t="s">
         <v>453</v>
       </c>
@@ -5506,7 +5526,9 @@
       <c r="B159" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="C159" s="1"/>
+      <c r="C159" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D159" s="1" t="s">
         <v>456</v>
       </c>
@@ -5519,7 +5541,9 @@
       <c r="B160" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="C160" s="1"/>
+      <c r="C160" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D160" s="1"/>
       <c r="E160" s="3"/>
     </row>
@@ -5530,7 +5554,9 @@
       <c r="B161" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="C161" s="1"/>
+      <c r="C161" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D161" s="1" t="s">
         <v>461</v>
       </c>
@@ -5543,7 +5569,9 @@
       <c r="B162" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="C162" s="1"/>
+      <c r="C162" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D162" s="1" t="s">
         <v>463</v>
       </c>
@@ -5556,7 +5584,9 @@
       <c r="B163" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="C163" s="1"/>
+      <c r="C163" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D163" s="1" t="s">
         <v>465</v>
       </c>
@@ -5569,7 +5599,9 @@
       <c r="B164" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C164" s="1"/>
+      <c r="C164" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D164" s="1" t="s">
         <v>467</v>
       </c>
@@ -5582,7 +5614,9 @@
       <c r="B165" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="C165" s="1"/>
+      <c r="C165" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D165" s="1"/>
       <c r="E165" s="3"/>
     </row>
@@ -5593,7 +5627,9 @@
       <c r="B166" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="C166" s="1"/>
+      <c r="C166" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D166" s="1" t="s">
         <v>724</v>
       </c>
@@ -5631,7 +5667,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>233</v>
       </c>
@@ -5644,9 +5680,11 @@
       <c r="D169" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E169" s="3"/>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E169" s="3" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>234</v>
       </c>
@@ -5659,9 +5697,11 @@
       <c r="D170" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E170" s="3"/>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E170" s="3" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>235</v>
       </c>
@@ -5674,9 +5714,11 @@
       <c r="D171" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E171" s="3"/>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E171" s="3" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>236</v>
       </c>
@@ -5689,9 +5731,11 @@
       <c r="D172" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E172" s="3"/>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E172" s="3" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>237</v>
       </c>
@@ -5704,7 +5748,9 @@
       <c r="D173" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E173" s="3"/>
+      <c r="E173" s="3" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="174" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
@@ -5723,7 +5769,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>239</v>
       </c>
@@ -5736,7 +5782,9 @@
       <c r="D175" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E175" s="3"/>
+      <c r="E175" s="3" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="176" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
@@ -5789,7 +5837,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>219</v>
       </c>
@@ -5802,7 +5850,9 @@
       <c r="D179" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E179" s="3"/>
+      <c r="E179" s="3" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="180" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
@@ -5855,7 +5905,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>213</v>
       </c>
@@ -5868,7 +5918,9 @@
       <c r="D183" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E183" s="3"/>
+      <c r="E183" s="3" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">

</xml_diff>

<commit_message>
Added lab normalization codes
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4522DEF-C18D-0746-B690-D0F0DDAB9137}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EE0E69-C7BD-6942-88DB-604E5C12B73C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-42640" yWindow="1960" windowWidth="41000" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="854">
   <si>
     <t>Variable #</t>
   </si>
@@ -2510,6 +2510,84 @@
   </si>
   <si>
     <t>Any endocrine therapy in the 12 months prior to COVID-19</t>
+  </si>
+  <si>
+    <t>L20</t>
+  </si>
+  <si>
+    <t>transformed_wbc</t>
+  </si>
+  <si>
+    <t>Normalized WBC</t>
+  </si>
+  <si>
+    <t>cells*10^9/L</t>
+  </si>
+  <si>
+    <t>L21</t>
+  </si>
+  <si>
+    <t>transformed_alc</t>
+  </si>
+  <si>
+    <t>Normalized ALC</t>
+  </si>
+  <si>
+    <t>cells/uL</t>
+  </si>
+  <si>
+    <t>L22</t>
+  </si>
+  <si>
+    <t>transformed_anc</t>
+  </si>
+  <si>
+    <t>Normalized ANC</t>
+  </si>
+  <si>
+    <t>L23</t>
+  </si>
+  <si>
+    <t>transformed_aec</t>
+  </si>
+  <si>
+    <t>Normalized AEC</t>
+  </si>
+  <si>
+    <t>L24</t>
+  </si>
+  <si>
+    <t>transformed_hgb</t>
+  </si>
+  <si>
+    <t>Normalized hemoglobin</t>
+  </si>
+  <si>
+    <t>g/dL</t>
+  </si>
+  <si>
+    <t>10^3/uL</t>
+  </si>
+  <si>
+    <t>Normalized platelet count</t>
+  </si>
+  <si>
+    <t>L25</t>
+  </si>
+  <si>
+    <t>transformed_plt</t>
+  </si>
+  <si>
+    <t>L26</t>
+  </si>
+  <si>
+    <t>transformed_creat</t>
+  </si>
+  <si>
+    <t>Normalized creatinine</t>
+  </si>
+  <si>
+    <t>mg/dL</t>
   </si>
 </sst>
 </file>
@@ -2665,10 +2743,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E263" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E263" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E263">
-    <sortCondition ref="A1:A263"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E270" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E270" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E270">
+    <sortCondition ref="A1:A270"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #" dataDxfId="4"/>
@@ -3002,10 +3080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E263"/>
+  <dimension ref="A1:E270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="199" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="199" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A194" sqref="A194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6030,610 +6108,610 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>251</v>
+        <v>828</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>4</v>
+        <v>829</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E188" s="3"/>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+        <v>830</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>252</v>
+        <v>836</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>11</v>
+        <v>837</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E189" s="3"/>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+        <v>838</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>307</v>
+        <v>839</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>308</v>
+        <v>840</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E190" s="3"/>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+        <v>841</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>253</v>
+        <v>842</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>10</v>
+        <v>843</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E191" s="3"/>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+        <v>844</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>543</v>
+        <v>848</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>544</v>
+        <v>849</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="E192" s="3"/>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+        <v>847</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>254</v>
+        <v>850</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>305</v>
+        <v>851</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E193" s="3"/>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+        <v>852</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>255</v>
+        <v>832</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>12</v>
+        <v>833</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E194" s="3"/>
+        <v>834</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>835</v>
+      </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E195" s="3"/>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>199</v>
+        <v>56</v>
       </c>
       <c r="E196" s="3"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>754</v>
+        <v>307</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>26</v>
+        <v>308</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>265</v>
+        <v>309</v>
       </c>
       <c r="E197" s="3"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>752</v>
+        <v>253</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>266</v>
+        <v>57</v>
       </c>
       <c r="E198" s="3"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>753</v>
+        <v>543</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>81</v>
+        <v>544</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>82</v>
+        <v>545</v>
       </c>
       <c r="E199" s="3"/>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>755</v>
+        <v>305</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>756</v>
+        <v>306</v>
       </c>
       <c r="E200" s="3"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>101</v>
+        <v>255</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>518</v>
+        <v>58</v>
       </c>
       <c r="E201" s="3"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>521</v>
+        <v>256</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>522</v>
+        <v>79</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="E202" s="3"/>
     </row>
-    <row r="203" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>313</v>
+        <v>257</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>314</v>
+        <v>25</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="E203" s="3" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+      <c r="E203" s="3"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>507</v>
+        <v>754</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>508</v>
+        <v>26</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="E204" s="3" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+      <c r="E204" s="3"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>315</v>
+        <v>752</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>316</v>
+        <v>45</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="E205" s="3" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" ht="46" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+      <c r="E205" s="3"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>811</v>
+        <v>753</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>812</v>
+        <v>81</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>813</v>
-      </c>
-      <c r="E206" s="3" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" ht="46" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="E206" s="3"/>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>815</v>
+        <v>258</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>816</v>
+        <v>755</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="E207" s="3" t="s">
-        <v>818</v>
-      </c>
+        <v>756</v>
+      </c>
+      <c r="E207" s="3"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>514</v>
+        <v>101</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>516</v>
+        <v>22</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E208" s="3"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>520</v>
+        <v>63</v>
       </c>
       <c r="E209" s="3"/>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>270</v>
+        <v>313</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>13</v>
+        <v>314</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E210" s="3"/>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+        <v>510</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>271</v>
+        <v>507</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>29</v>
+        <v>508</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E211" s="3"/>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+        <v>509</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>272</v>
+        <v>315</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>48</v>
+        <v>316</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E212" s="3"/>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" ht="46" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>273</v>
+        <v>811</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>319</v>
+        <v>812</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E213" s="3"/>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+        <v>813</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" ht="46" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>318</v>
+        <v>815</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>320</v>
+        <v>816</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E214" s="3"/>
+        <v>817</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>818</v>
+      </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>274</v>
+        <v>514</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>52</v>
+        <v>516</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>74</v>
+        <v>517</v>
       </c>
       <c r="E215" s="3"/>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>275</v>
+        <v>515</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>72</v>
+        <v>519</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>73</v>
+        <v>520</v>
       </c>
       <c r="E216" s="3"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E217" s="3"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>323</v>
+        <v>271</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>324</v>
+        <v>29</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>325</v>
+        <v>68</v>
       </c>
       <c r="E218" s="3"/>
     </row>
-    <row r="219" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E219" s="3" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="E219" s="3"/>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>106</v>
+        <v>319</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E220" s="3" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="E220" s="3"/>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>108</v>
+        <v>318</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>109</v>
+        <v>320</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E221" s="3" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+      <c r="E221" s="3"/>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>112</v>
+        <v>274</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E222" s="3" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="E222" s="3"/>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>115</v>
+        <v>275</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E223" s="3" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="E223" s="3"/>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>119</v>
+        <v>276</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E224" s="3" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="E224" s="3"/>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>782</v>
+        <v>323</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>783</v>
+        <v>324</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="E225" s="3" t="s">
-        <v>674</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="E225" s="3"/>
     </row>
     <row r="226" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>785</v>
+        <v>277</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>786</v>
+        <v>104</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>787</v>
+        <v>105</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>674</v>
@@ -6641,16 +6719,16 @@
     </row>
     <row r="227" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>120</v>
+        <v>278</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>674</v>
@@ -6658,16 +6736,16 @@
     </row>
     <row r="228" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>180</v>
+        <v>108</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>181</v>
+        <v>109</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>182</v>
+        <v>110</v>
       </c>
       <c r="E228" s="3" t="s">
         <v>674</v>
@@ -6675,16 +6753,16 @@
     </row>
     <row r="229" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>371</v>
+        <v>112</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>372</v>
+        <v>113</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>373</v>
+        <v>111</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>674</v>
@@ -6692,16 +6770,16 @@
     </row>
     <row r="230" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>757</v>
+        <v>115</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>758</v>
+        <v>116</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>759</v>
+        <v>114</v>
       </c>
       <c r="E230" s="3" t="s">
         <v>674</v>
@@ -6709,16 +6787,16 @@
     </row>
     <row r="231" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>788</v>
+        <v>119</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>789</v>
+        <v>118</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>790</v>
+        <v>117</v>
       </c>
       <c r="E231" s="3" t="s">
         <v>674</v>
@@ -6726,16 +6804,16 @@
     </row>
     <row r="232" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>791</v>
+        <v>782</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>792</v>
+        <v>783</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>793</v>
+        <v>784</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>674</v>
@@ -6743,16 +6821,16 @@
     </row>
     <row r="233" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>795</v>
+        <v>785</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>796</v>
+        <v>786</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>797</v>
+        <v>787</v>
       </c>
       <c r="E233" s="3" t="s">
         <v>674</v>
@@ -6760,467 +6838,586 @@
     </row>
     <row r="234" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A235" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E236" s="3" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A237" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A238" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A239" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="E239" s="3" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A240" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="E240" s="3" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A241" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B234" s="1" t="s">
+      <c r="B241" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C234" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D234" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E234" s="3" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A235" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C235" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D235" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E235" s="3"/>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A236" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E236" s="3"/>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A237" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B237" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C237" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D237" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E237" s="3"/>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A238" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D238" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E238" s="3"/>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A239" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C239" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D239" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E239" s="3"/>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A240" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E240" s="3"/>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A241" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E241" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="E241" s="3" t="s">
+        <v>794</v>
+      </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>294</v>
+        <v>90</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>295</v>
+        <v>21</v>
       </c>
       <c r="E242" s="3"/>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>297</v>
+        <v>93</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>298</v>
+        <v>23</v>
       </c>
       <c r="E243" s="3"/>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>363</v>
+        <v>95</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>364</v>
+        <v>99</v>
       </c>
       <c r="E244" s="3"/>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>377</v>
+        <v>94</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>378</v>
+        <v>21</v>
       </c>
       <c r="E245" s="3"/>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>301</v>
+        <v>31</v>
       </c>
       <c r="E246" s="3"/>
     </row>
-    <row r="247" spans="1:5" ht="46" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
-        <v>359</v>
+        <v>291</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>357</v>
+        <v>96</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="E247" s="3" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="E247" s="3"/>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
-        <v>374</v>
+        <v>292</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>375</v>
+        <v>97</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="E248" s="3" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="E248" s="3"/>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
-        <v>739</v>
+        <v>293</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>740</v>
+        <v>294</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="E249" s="3" t="s">
-        <v>741</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="E249" s="3"/>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
-        <v>738</v>
+        <v>296</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E250" s="3"/>
     </row>
-    <row r="251" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
-        <v>686</v>
+        <v>322</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>687</v>
+        <v>363</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="E251" s="3" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+      <c r="E251" s="3"/>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
-        <v>135</v>
+        <v>299</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>136</v>
+        <v>377</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E252" s="3" t="s">
-        <v>139</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="E252" s="3"/>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
-        <v>140</v>
+        <v>302</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>141</v>
+        <v>300</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>393</v>
+        <v>301</v>
       </c>
       <c r="E253" s="3"/>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:5" ht="46" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
-        <v>394</v>
+        <v>359</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>395</v>
+        <v>357</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>137</v>
+        <v>18</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="E254" s="3"/>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+      <c r="E254" s="3" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
-        <v>200</v>
+        <v>374</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>201</v>
+        <v>375</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>137</v>
+        <v>18</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E255" s="3"/>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+      <c r="E255" s="3" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
-        <v>243</v>
+        <v>739</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>244</v>
+        <v>740</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>137</v>
+        <v>18</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E256" s="3"/>
+        <v>376</v>
+      </c>
+      <c r="E256" s="3" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
-        <v>246</v>
+        <v>738</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>247</v>
+        <v>303</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>248</v>
+        <v>304</v>
       </c>
       <c r="E257" s="3"/>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
-        <v>478</v>
+        <v>686</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>472</v>
+        <v>687</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="E258" s="3"/>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+        <v>688</v>
+      </c>
+      <c r="E258" s="3" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
-        <v>474</v>
+        <v>135</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>475</v>
+        <v>136</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="E259" s="3"/>
+        <v>138</v>
+      </c>
+      <c r="E259" s="3" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
-        <v>476</v>
+        <v>140</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>477</v>
+        <v>141</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>480</v>
+        <v>393</v>
       </c>
       <c r="E260" s="3"/>
     </row>
-    <row r="261" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
-        <v>267</v>
+        <v>394</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>268</v>
+        <v>395</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E261" s="3" t="s">
-        <v>751</v>
-      </c>
+        <v>396</v>
+      </c>
+      <c r="E261" s="3"/>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
-        <v>489</v>
+        <v>200</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>490</v>
+        <v>201</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>491</v>
+        <v>202</v>
       </c>
       <c r="E262" s="3"/>
     </row>
-    <row r="263" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
-        <v>745</v>
+        <v>243</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>746</v>
+        <v>244</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D263" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E263" s="3"/>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A264" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E264" s="3"/>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A265" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="E265" s="3"/>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A266" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="E266" s="3"/>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A267" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E267" s="3"/>
+    </row>
+    <row r="268" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+      <c r="A268" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E268" s="3" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A269" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="E269" s="3"/>
+    </row>
+    <row r="270" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A270" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D270" s="1" t="s">
         <v>747</v>
       </c>
-      <c r="E263" s="3" t="s">
+      <c r="E270" s="3" t="s">
         <v>674</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes, new derived variables
1. Tweaked logic for outcomes to include the no symptoms/no complications choices
2. new cancer type variables.
</commit_message>
<xml_diff>
--- a/CCC19_Derived_Variables_Spreadsheet.xlsx
+++ b/CCC19_Derived_Variables_Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EE0E69-C7BD-6942-88DB-604E5C12B73C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48F8A9F-FF8B-3A43-A33A-EE4B16F7AC9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-42640" yWindow="1960" windowWidth="41000" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="872">
   <si>
     <t>Variable #</t>
   </si>
@@ -2588,6 +2588,60 @@
   </si>
   <si>
     <t>mg/dL</t>
+  </si>
+  <si>
+    <t>Dx15a</t>
+  </si>
+  <si>
+    <t>colorectal</t>
+  </si>
+  <si>
+    <t>Colorectal cancers</t>
+  </si>
+  <si>
+    <t>anal</t>
+  </si>
+  <si>
+    <t>Anal cancer</t>
+  </si>
+  <si>
+    <t>Dx15b</t>
+  </si>
+  <si>
+    <t>Dx16a</t>
+  </si>
+  <si>
+    <t>hepatobiliary</t>
+  </si>
+  <si>
+    <t>Hepatobiliary cancers (excluding pancreas)</t>
+  </si>
+  <si>
+    <t>Dx16b</t>
+  </si>
+  <si>
+    <t>pancreaticohepatobiliary</t>
+  </si>
+  <si>
+    <t>Pancreaticohepatobiliary cancers</t>
+  </si>
+  <si>
+    <t>Dx16c</t>
+  </si>
+  <si>
+    <t>esophagogastric</t>
+  </si>
+  <si>
+    <t>Esophagogastric cancers</t>
+  </si>
+  <si>
+    <t>Dx19a</t>
+  </si>
+  <si>
+    <t>NET</t>
+  </si>
+  <si>
+    <t>Neuroendocrine cancers</t>
   </si>
 </sst>
 </file>
@@ -2743,10 +2797,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E270" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E270" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E270">
-    <sortCondition ref="A1:A270"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B205C10F-4E67-834B-A4D6-A760A2ED6F23}" name="Table1" displayName="Table1" ref="A1:E276" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E276" xr:uid="{519BB424-49E2-B043-A086-21F2D36AA3AD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E276">
+    <sortCondition ref="A1:A276"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{709F3135-248E-8647-8E63-4DE472082F6A}" name="Variable #" dataDxfId="4"/>
@@ -3080,10 +3134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E270"/>
+  <dimension ref="A1:E276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="199" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A194" sqref="A194"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="199" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E166" sqref="E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5409,7 +5463,7 @@
       </c>
       <c r="E142" s="3"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>403</v>
       </c>
@@ -5422,9 +5476,11 @@
       <c r="D143" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="E143" s="3"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E143" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>406</v>
       </c>
@@ -5437,9 +5493,11 @@
       <c r="D144" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="E144" s="3"/>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E144" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>409</v>
       </c>
@@ -5452,9 +5510,11 @@
       <c r="D145" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="E145" s="3"/>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E145" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>412</v>
       </c>
@@ -5467,9 +5527,11 @@
       <c r="D146" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="E146" s="3"/>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E146" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>415</v>
       </c>
@@ -5480,9 +5542,11 @@
         <v>402</v>
       </c>
       <c r="D147" s="1"/>
-      <c r="E147" s="3"/>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E147" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>417</v>
       </c>
@@ -5495,9 +5559,11 @@
       <c r="D148" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E148" s="3"/>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E148" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>420</v>
       </c>
@@ -5510,9 +5576,11 @@
       <c r="D149" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="E149" s="3"/>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E149" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>423</v>
       </c>
@@ -5525,9 +5593,11 @@
       <c r="D150" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="E150" s="3"/>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E150" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>426</v>
       </c>
@@ -5538,9 +5608,11 @@
         <v>402</v>
       </c>
       <c r="D151" s="1"/>
-      <c r="E151" s="3"/>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E151" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>428</v>
       </c>
@@ -5553,9 +5625,11 @@
       <c r="D152" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="E152" s="3"/>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E152" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>431</v>
       </c>
@@ -5566,9 +5640,11 @@
         <v>402</v>
       </c>
       <c r="D153" s="1"/>
-      <c r="E153" s="3"/>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E153" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>433</v>
       </c>
@@ -5581,9 +5657,11 @@
       <c r="D154" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="E154" s="3"/>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E154" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>436</v>
       </c>
@@ -5596,9 +5674,11 @@
       <c r="D155" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="E155" s="3"/>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E155" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>439</v>
       </c>
@@ -5611,313 +5691,339 @@
       <c r="D156" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="E156" s="3"/>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E156" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>442</v>
+        <v>854</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>443</v>
+        <v>855</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="E157" s="3"/>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+        <v>856</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>445</v>
+        <v>859</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>446</v>
+        <v>857</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="E158" s="3"/>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+        <v>858</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="E159" s="3"/>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+        <v>444</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>451</v>
+        <v>860</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>452</v>
+        <v>861</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="E160" s="3"/>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+        <v>862</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>454</v>
+        <v>863</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>455</v>
+        <v>864</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="E161" s="3"/>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+        <v>865</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>457</v>
+        <v>866</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>458</v>
+        <v>867</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="D162" s="1"/>
-      <c r="E162" s="3"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D162" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="E163" s="3"/>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+        <v>447</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="E164" s="3"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+        <v>450</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>470</v>
+        <v>451</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="E165" s="3"/>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+        <v>453</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>471</v>
+        <v>869</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>466</v>
+        <v>870</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E166" s="3"/>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+        <v>871</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>662</v>
+        <v>454</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>663</v>
+        <v>455</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="D167" s="1"/>
-      <c r="E167" s="3"/>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D167" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>719</v>
+        <v>457</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>720</v>
+        <v>458</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="D168" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="E168" s="3"/>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D168" s="1"/>
+      <c r="E168" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>231</v>
+        <v>459</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>150</v>
+        <v>460</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>151</v>
+        <v>402</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E169" s="3"/>
+        <v>461</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="170" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>232</v>
+        <v>469</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>158</v>
+        <v>462</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>151</v>
+        <v>402</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>159</v>
+        <v>463</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>689</v>
+        <v>700</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>233</v>
+        <v>470</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>160</v>
+        <v>464</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>151</v>
+        <v>402</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>161</v>
+        <v>465</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>689</v>
+        <v>700</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>234</v>
+        <v>471</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>163</v>
+        <v>466</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>151</v>
+        <v>402</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>162</v>
+        <v>467</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>689</v>
+        <v>700</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>235</v>
+        <v>662</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>164</v>
+        <v>663</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>165</v>
-      </c>
+        <v>402</v>
+      </c>
+      <c r="D173" s="1"/>
       <c r="E173" s="3" t="s">
-        <v>689</v>
+        <v>700</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>236</v>
+        <v>719</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>166</v>
+        <v>720</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>151</v>
+        <v>402</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>167</v>
+        <v>721</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E175" s="3" t="s">
-        <v>689</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="E175" s="3"/>
     </row>
     <row r="176" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>689</v>
@@ -5925,16 +6031,16 @@
     </row>
     <row r="177" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="E177" s=